<commit_message>
Widen SRAM access from byte to longword An SRAM memory controller will be implemented that allows non-aligned longword access to SRAM by utilizing both ports of the dual ported memory blocks The key objective to is allow FETCH.L, FETCH.W and FETCH.B instructions to all execute in a single cycle.
</commit_message>
<xml_diff>
--- a/Resources/Instruction Set.xlsx
+++ b/Resources/Instruction Set.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="18195" windowHeight="8250" tabRatio="681"/>
+    <workbookView xWindow="240" yWindow="120" windowWidth="18195" windowHeight="8250" tabRatio="681" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="OPCODE_encoding" sheetId="1" r:id="rId1"/>
@@ -16,12 +16,12 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">OPCODE_encoding!$A$3:$L$92</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1361" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1363" uniqueCount="349">
   <si>
     <t>DUP</t>
   </si>
@@ -1059,13 +1059,22 @@
   </si>
   <si>
     <t>RSP!</t>
+  </si>
+  <si>
+    <t>PSD_DATA</t>
+  </si>
+  <si>
+    <t>S_DATA</t>
+  </si>
+  <si>
+    <t>S_DATA+</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="32">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="33" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1286,6 +1295,13 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1398,7 +1414,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="110">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1555,9 +1571,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1651,6 +1664,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1740,6 +1768,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1774,6 +1803,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1949,20 +1979,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:AU98"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="9" ySplit="4" topLeftCell="J11" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="9" ySplit="4" topLeftCell="J55" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H11" sqref="H11"/>
+      <selection pane="bottomRight" activeCell="B92" sqref="B92"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.25"/>
+  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="1.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="11" style="4" customWidth="1"/>
@@ -1972,7 +2002,7 @@
     <col min="8" max="8" width="5.5703125" style="7" customWidth="1"/>
     <col min="9" max="9" width="6.5703125" style="4" customWidth="1"/>
     <col min="10" max="10" width="2" style="4" customWidth="1"/>
-    <col min="11" max="11" width="19.28515625" style="90" customWidth="1"/>
+    <col min="11" max="11" width="19.28515625" style="89" customWidth="1"/>
     <col min="12" max="12" width="50.5703125" style="1" customWidth="1"/>
     <col min="13" max="13" width="2.7109375" style="8" customWidth="1"/>
     <col min="14" max="14" width="10.28515625" style="4" customWidth="1"/>
@@ -1996,14 +2026,14 @@
     <col min="48" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" ht="15">
+    <row r="1" spans="1:47" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="46" t="s">
         <v>317</v>
       </c>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:47" ht="5.25" customHeight="1"/>
-    <row r="3" spans="1:47" s="23" customFormat="1">
+    <row r="2" spans="1:47" ht="5.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="1:47" s="23" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B3" s="7" t="s">
         <v>250</v>
       </c>
@@ -2018,7 +2048,7 @@
         <v>260</v>
       </c>
       <c r="J3" s="7"/>
-      <c r="K3" s="91" t="s">
+      <c r="K3" s="90" t="s">
         <v>122</v>
       </c>
       <c r="L3" s="23" t="s">
@@ -2068,7 +2098,7 @@
       </c>
       <c r="AU3" s="33"/>
     </row>
-    <row r="4" spans="1:47">
+    <row r="4" spans="1:47" x14ac:dyDescent="0.2">
       <c r="D4" s="7">
         <v>7</v>
       </c>
@@ -2169,12 +2199,12 @@
         <v>309</v>
       </c>
     </row>
-    <row r="5" spans="1:47">
+    <row r="5" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="6" spans="1:47">
+    <row r="6" spans="1:47" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
         <v>41</v>
       </c>
@@ -2195,7 +2225,7 @@
         <f>DEC2HEX(H6)</f>
         <v>0</v>
       </c>
-      <c r="K6" s="92" t="s">
+      <c r="K6" s="91" t="s">
         <v>113</v>
       </c>
       <c r="L6" s="1" t="s">
@@ -2303,7 +2333,7 @@
         <v>," NOP"</v>
       </c>
     </row>
-    <row r="7" spans="1:47">
+    <row r="7" spans="1:47" x14ac:dyDescent="0.2">
       <c r="B7" s="4" t="s">
         <v>2</v>
       </c>
@@ -2325,7 +2355,7 @@
         <f t="shared" ref="I7:I20" si="1">DEC2HEX(H7)</f>
         <v>1</v>
       </c>
-      <c r="K7" s="90" t="s">
+      <c r="K7" s="89" t="s">
         <v>60</v>
       </c>
       <c r="L7" s="1" t="s">
@@ -2433,7 +2463,7 @@
         <v>," DROP"</v>
       </c>
     </row>
-    <row r="8" spans="1:47">
+    <row r="8" spans="1:47" x14ac:dyDescent="0.2">
       <c r="B8" s="4" t="s">
         <v>0</v>
       </c>
@@ -2455,7 +2485,7 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="K8" s="90" t="s">
+      <c r="K8" s="89" t="s">
         <v>56</v>
       </c>
       <c r="L8" s="1" t="s">
@@ -2563,7 +2593,7 @@
         <v>," DUP"</v>
       </c>
     </row>
-    <row r="9" spans="1:47" s="14" customFormat="1">
+    <row r="9" spans="1:47" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B9" s="15" t="s">
         <v>1</v>
       </c>
@@ -2588,7 +2618,7 @@
         <v>3</v>
       </c>
       <c r="J9" s="15"/>
-      <c r="K9" s="93" t="s">
+      <c r="K9" s="92" t="s">
         <v>57</v>
       </c>
       <c r="L9" s="42" t="s">
@@ -2693,7 +2723,7 @@
         <v>," ?DUP"</v>
       </c>
     </row>
-    <row r="10" spans="1:47">
+    <row r="10" spans="1:47" x14ac:dyDescent="0.2">
       <c r="B10" s="4" t="s">
         <v>3</v>
       </c>
@@ -2715,7 +2745,7 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="K10" s="90" t="s">
+      <c r="K10" s="89" t="s">
         <v>62</v>
       </c>
       <c r="L10" s="1" t="s">
@@ -2823,7 +2853,7 @@
         <v>," SWAP"</v>
       </c>
     </row>
-    <row r="11" spans="1:47">
+    <row r="11" spans="1:47" x14ac:dyDescent="0.2">
       <c r="B11" s="4" t="s">
         <v>4</v>
       </c>
@@ -2845,7 +2875,7 @@
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="K11" s="90" t="s">
+      <c r="K11" s="89" t="s">
         <v>64</v>
       </c>
       <c r="L11" s="1" t="s">
@@ -2953,7 +2983,7 @@
         <v>," OVER"</v>
       </c>
     </row>
-    <row r="12" spans="1:47">
+    <row r="12" spans="1:47" x14ac:dyDescent="0.2">
       <c r="B12" s="4" t="s">
         <v>5</v>
       </c>
@@ -2975,7 +3005,7 @@
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="K12" s="90" t="s">
+      <c r="K12" s="89" t="s">
         <v>66</v>
       </c>
       <c r="L12" s="1" t="s">
@@ -3083,7 +3113,7 @@
         <v>," NIP"</v>
       </c>
     </row>
-    <row r="13" spans="1:47">
+    <row r="13" spans="1:47" x14ac:dyDescent="0.2">
       <c r="B13" s="4" t="s">
         <v>6</v>
       </c>
@@ -3105,7 +3135,7 @@
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="K13" s="90" t="s">
+      <c r="K13" s="89" t="s">
         <v>68</v>
       </c>
       <c r="L13" s="1" t="s">
@@ -3213,7 +3243,7 @@
         <v>," ROT"</v>
       </c>
     </row>
-    <row r="14" spans="1:47" s="3" customFormat="1">
+    <row r="14" spans="1:47" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B14" s="11" t="s">
         <v>7</v>
       </c>
@@ -3238,7 +3268,7 @@
         <v>8</v>
       </c>
       <c r="J14" s="11"/>
-      <c r="K14" s="94" t="s">
+      <c r="K14" s="93" t="s">
         <v>69</v>
       </c>
       <c r="L14" s="3" t="s">
@@ -3350,7 +3380,7 @@
         <v>," &gt;R"</v>
       </c>
     </row>
-    <row r="15" spans="1:47">
+    <row r="15" spans="1:47" x14ac:dyDescent="0.2">
       <c r="B15" s="4" t="s">
         <v>8</v>
       </c>
@@ -3372,7 +3402,7 @@
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="K15" s="90" t="s">
+      <c r="K15" s="89" t="s">
         <v>71</v>
       </c>
       <c r="L15" s="1" t="s">
@@ -3480,7 +3510,7 @@
         <v>," R@"</v>
       </c>
     </row>
-    <row r="16" spans="1:47" s="3" customFormat="1">
+    <row r="16" spans="1:47" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B16" s="11" t="s">
         <v>9</v>
       </c>
@@ -3505,7 +3535,7 @@
         <v>A</v>
       </c>
       <c r="J16" s="11"/>
-      <c r="K16" s="95" t="s">
+      <c r="K16" s="94" t="s">
         <v>134</v>
       </c>
       <c r="L16" s="3" t="s">
@@ -3617,7 +3647,7 @@
         <v>," R&gt;"</v>
       </c>
     </row>
-    <row r="17" spans="1:47" s="3" customFormat="1">
+    <row r="17" spans="1:47" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B17" s="11" t="s">
         <v>323</v>
       </c>
@@ -3642,7 +3672,7 @@
         <v>B</v>
       </c>
       <c r="J17" s="11"/>
-      <c r="K17" s="95" t="s">
+      <c r="K17" s="94" t="s">
         <v>281</v>
       </c>
       <c r="L17" s="3" t="s">
@@ -3742,7 +3772,7 @@
         <v>," PSP@"</v>
       </c>
     </row>
-    <row r="18" spans="1:47" s="3" customFormat="1">
+    <row r="18" spans="1:47" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B18" s="11" t="s">
         <v>324</v>
       </c>
@@ -3767,7 +3797,7 @@
         <v>C</v>
       </c>
       <c r="J18" s="11"/>
-      <c r="K18" s="95" t="s">
+      <c r="K18" s="94" t="s">
         <v>282</v>
       </c>
       <c r="L18" s="3" t="s">
@@ -3867,7 +3897,7 @@
         <v>," RSP@"</v>
       </c>
     </row>
-    <row r="19" spans="1:47">
+    <row r="19" spans="1:47" x14ac:dyDescent="0.2">
       <c r="B19" s="11" t="s">
         <v>325</v>
       </c>
@@ -3889,7 +3919,7 @@
         <f t="shared" si="1"/>
         <v>D</v>
       </c>
-      <c r="K19" s="90" t="s">
+      <c r="K19" s="89" t="s">
         <v>251</v>
       </c>
       <c r="L19" s="1" t="s">
@@ -3982,7 +4012,7 @@
         <v>," PSP!"</v>
       </c>
     </row>
-    <row r="20" spans="1:47">
+    <row r="20" spans="1:47" x14ac:dyDescent="0.2">
       <c r="B20" s="11" t="s">
         <v>345</v>
       </c>
@@ -4004,7 +4034,7 @@
         <f t="shared" si="1"/>
         <v>E</v>
       </c>
-      <c r="K20" s="90" t="s">
+      <c r="K20" s="89" t="s">
         <v>252</v>
       </c>
       <c r="L20" s="1" t="s">
@@ -4097,18 +4127,18 @@
         <v>," RSP!"</v>
       </c>
     </row>
-    <row r="21" spans="1:47">
+    <row r="21" spans="1:47" x14ac:dyDescent="0.2">
       <c r="AT21" s="66"/>
       <c r="AU21" s="66"/>
     </row>
-    <row r="22" spans="1:47">
+    <row r="22" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>10</v>
       </c>
       <c r="AT22" s="66"/>
       <c r="AU22" s="66"/>
     </row>
-    <row r="23" spans="1:47">
+    <row r="23" spans="1:47" x14ac:dyDescent="0.2">
       <c r="B23" s="6" t="s">
         <v>11</v>
       </c>
@@ -4131,7 +4161,7 @@
         <f t="shared" ref="I23:I35" si="10">DEC2HEX(H23)</f>
         <v>F</v>
       </c>
-      <c r="K23" s="90" t="s">
+      <c r="K23" s="89" t="s">
         <v>73</v>
       </c>
       <c r="L23" s="1" t="s">
@@ -4240,7 +4270,7 @@
         <v>," +"</v>
       </c>
     </row>
-    <row r="24" spans="1:47">
+    <row r="24" spans="1:47" x14ac:dyDescent="0.2">
       <c r="B24" s="6" t="s">
         <v>12</v>
       </c>
@@ -4263,7 +4293,7 @@
         <f t="shared" si="10"/>
         <v>10</v>
       </c>
-      <c r="K24" s="90" t="s">
+      <c r="K24" s="89" t="s">
         <v>73</v>
       </c>
       <c r="L24" s="1" t="s">
@@ -4372,7 +4402,7 @@
         <v>," -"</v>
       </c>
     </row>
-    <row r="25" spans="1:47">
+    <row r="25" spans="1:47" x14ac:dyDescent="0.2">
       <c r="B25" s="4" t="s">
         <v>16</v>
       </c>
@@ -4394,7 +4424,7 @@
         <f t="shared" si="10"/>
         <v>11</v>
       </c>
-      <c r="K25" s="90" t="s">
+      <c r="K25" s="89" t="s">
         <v>79</v>
       </c>
       <c r="L25" s="1" t="s">
@@ -4503,7 +4533,7 @@
         <v>," NEGATE"</v>
       </c>
     </row>
-    <row r="26" spans="1:47" s="3" customFormat="1">
+    <row r="26" spans="1:47" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B26" s="11" t="s">
         <v>52</v>
       </c>
@@ -4528,7 +4558,7 @@
         <v>12</v>
       </c>
       <c r="J26" s="4"/>
-      <c r="K26" s="94" t="s">
+      <c r="K26" s="93" t="s">
         <v>96</v>
       </c>
       <c r="L26" s="3" t="s">
@@ -4640,7 +4670,7 @@
         <v>," 1+"</v>
       </c>
     </row>
-    <row r="27" spans="1:47" s="3" customFormat="1">
+    <row r="27" spans="1:47" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B27" s="13" t="s">
         <v>53</v>
       </c>
@@ -4665,7 +4695,7 @@
         <v>13</v>
       </c>
       <c r="J27" s="4"/>
-      <c r="K27" s="94" t="s">
+      <c r="K27" s="93" t="s">
         <v>96</v>
       </c>
       <c r="L27" s="3" t="s">
@@ -4777,7 +4807,7 @@
         <v>," 1-"</v>
       </c>
     </row>
-    <row r="28" spans="1:47" s="3" customFormat="1">
+    <row r="28" spans="1:47" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B28" s="13" t="s">
         <v>54</v>
       </c>
@@ -4802,7 +4832,7 @@
         <v>14</v>
       </c>
       <c r="J28" s="4"/>
-      <c r="K28" s="94" t="s">
+      <c r="K28" s="93" t="s">
         <v>96</v>
       </c>
       <c r="L28" s="3" t="s">
@@ -4914,7 +4944,7 @@
         <v>," 2*"</v>
       </c>
     </row>
-    <row r="29" spans="1:47" s="3" customFormat="1">
+    <row r="29" spans="1:47" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B29" s="13" t="s">
         <v>55</v>
       </c>
@@ -4939,7 +4969,7 @@
         <v>15</v>
       </c>
       <c r="J29" s="4"/>
-      <c r="K29" s="94" t="s">
+      <c r="K29" s="93" t="s">
         <v>96</v>
       </c>
       <c r="L29" s="3" t="s">
@@ -5051,7 +5081,7 @@
         <v>," 2/"</v>
       </c>
     </row>
-    <row r="30" spans="1:47" s="3" customFormat="1">
+    <row r="30" spans="1:47" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B30" s="11" t="s">
         <v>283</v>
       </c>
@@ -5076,7 +5106,7 @@
         <v>16</v>
       </c>
       <c r="J30" s="11"/>
-      <c r="K30" s="94" t="s">
+      <c r="K30" s="93" t="s">
         <v>193</v>
       </c>
       <c r="L30" s="3" t="s">
@@ -5188,7 +5218,7 @@
         <v>," MULTS"</v>
       </c>
     </row>
-    <row r="31" spans="1:47" s="3" customFormat="1">
+    <row r="31" spans="1:47" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B31" s="11" t="s">
         <v>284</v>
       </c>
@@ -5213,7 +5243,7 @@
         <v>17</v>
       </c>
       <c r="J31" s="11"/>
-      <c r="K31" s="94" t="s">
+      <c r="K31" s="93" t="s">
         <v>77</v>
       </c>
       <c r="L31" s="3" t="s">
@@ -5325,7 +5355,7 @@
         <v>," MULTU"</v>
       </c>
     </row>
-    <row r="32" spans="1:47" s="3" customFormat="1">
+    <row r="32" spans="1:47" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B32" s="11" t="s">
         <v>220</v>
       </c>
@@ -5350,7 +5380,7 @@
         <v>18</v>
       </c>
       <c r="J32" s="11"/>
-      <c r="K32" s="90" t="s">
+      <c r="K32" s="89" t="s">
         <v>73</v>
       </c>
       <c r="L32" s="3" t="s">
@@ -5463,7 +5493,7 @@
         <v>," ADDX"</v>
       </c>
     </row>
-    <row r="33" spans="1:47" s="3" customFormat="1">
+    <row r="33" spans="1:47" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B33" s="11" t="s">
         <v>221</v>
       </c>
@@ -5488,7 +5518,7 @@
         <v>19</v>
       </c>
       <c r="J33" s="11"/>
-      <c r="K33" s="90" t="s">
+      <c r="K33" s="89" t="s">
         <v>73</v>
       </c>
       <c r="L33" s="3" t="s">
@@ -5601,7 +5631,7 @@
         <v>," SUBX"</v>
       </c>
     </row>
-    <row r="34" spans="1:47" s="14" customFormat="1">
+    <row r="34" spans="1:47" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B34" s="15" t="s">
         <v>285</v>
       </c>
@@ -5626,7 +5656,7 @@
         <v>1A</v>
       </c>
       <c r="J34" s="17"/>
-      <c r="K34" s="93" t="s">
+      <c r="K34" s="92" t="s">
         <v>203</v>
       </c>
       <c r="L34" s="14" t="s">
@@ -5746,7 +5776,7 @@
         <v>," DIVS"</v>
       </c>
     </row>
-    <row r="35" spans="1:47" s="14" customFormat="1" ht="14.25" customHeight="1">
+    <row r="35" spans="1:47" s="14" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="15" t="s">
         <v>286</v>
       </c>
@@ -5771,7 +5801,7 @@
         <v>1B</v>
       </c>
       <c r="J35" s="17"/>
-      <c r="K35" s="93" t="s">
+      <c r="K35" s="92" t="s">
         <v>195</v>
       </c>
       <c r="L35" s="14" t="s">
@@ -5891,12 +5921,12 @@
         <v>," DIVU"</v>
       </c>
     </row>
-    <row r="36" spans="1:47">
+    <row r="36" spans="1:47" x14ac:dyDescent="0.2">
       <c r="E36" s="13"/>
       <c r="AT36" s="66"/>
       <c r="AU36" s="66"/>
     </row>
-    <row r="37" spans="1:47">
+    <row r="37" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>17</v>
       </c>
@@ -5904,7 +5934,7 @@
       <c r="AT37" s="66"/>
       <c r="AU37" s="66"/>
     </row>
-    <row r="38" spans="1:47">
+    <row r="38" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A38" s="4"/>
       <c r="B38" s="6" t="s">
         <v>20</v>
@@ -5928,7 +5958,7 @@
         <f t="shared" ref="I38:I48" si="18">DEC2HEX(H38)</f>
         <v>1C</v>
       </c>
-      <c r="K38" s="90" t="s">
+      <c r="K38" s="89" t="s">
         <v>81</v>
       </c>
       <c r="L38" s="1" t="s">
@@ -6038,7 +6068,7 @@
         <v>," ="</v>
       </c>
     </row>
-    <row r="39" spans="1:47" s="3" customFormat="1">
+    <row r="39" spans="1:47" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="4"/>
       <c r="B39" s="13" t="s">
         <v>44</v>
@@ -6064,7 +6094,7 @@
         <v>1D</v>
       </c>
       <c r="J39" s="11"/>
-      <c r="K39" s="94" t="s">
+      <c r="K39" s="93" t="s">
         <v>81</v>
       </c>
       <c r="L39" s="3" t="s">
@@ -6176,7 +6206,7 @@
         <v>," &lt;&gt;"</v>
       </c>
     </row>
-    <row r="40" spans="1:47">
+    <row r="40" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A40" s="4"/>
       <c r="B40" s="6" t="s">
         <v>18</v>
@@ -6200,7 +6230,7 @@
         <f t="shared" si="18"/>
         <v>1E</v>
       </c>
-      <c r="K40" s="90" t="s">
+      <c r="K40" s="89" t="s">
         <v>81</v>
       </c>
       <c r="L40" s="1" t="s">
@@ -6310,7 +6340,7 @@
         <v>," &lt;"</v>
       </c>
     </row>
-    <row r="41" spans="1:47">
+    <row r="41" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A41" s="4"/>
       <c r="B41" s="6" t="s">
         <v>19</v>
@@ -6334,7 +6364,7 @@
         <f t="shared" si="18"/>
         <v>1F</v>
       </c>
-      <c r="K41" s="90" t="s">
+      <c r="K41" s="89" t="s">
         <v>81</v>
       </c>
       <c r="L41" s="1" t="s">
@@ -6444,7 +6474,7 @@
         <v>," &gt;"</v>
       </c>
     </row>
-    <row r="42" spans="1:47">
+    <row r="42" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A42" s="4"/>
       <c r="B42" s="6" t="s">
         <v>27</v>
@@ -6468,7 +6498,7 @@
         <f t="shared" si="18"/>
         <v>20</v>
       </c>
-      <c r="K42" s="90" t="s">
+      <c r="K42" s="89" t="s">
         <v>84</v>
       </c>
       <c r="L42" s="1" t="s">
@@ -6578,7 +6608,7 @@
         <v>," U&lt;"</v>
       </c>
     </row>
-    <row r="43" spans="1:47">
+    <row r="43" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A43" s="4"/>
       <c r="B43" s="6" t="s">
         <v>28</v>
@@ -6602,7 +6632,7 @@
         <f t="shared" si="18"/>
         <v>21</v>
       </c>
-      <c r="K43" s="90" t="s">
+      <c r="K43" s="89" t="s">
         <v>84</v>
       </c>
       <c r="L43" s="1" t="s">
@@ -6712,7 +6742,7 @@
         <v>," U&gt;"</v>
       </c>
     </row>
-    <row r="44" spans="1:47" s="3" customFormat="1">
+    <row r="44" spans="1:47" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" s="4"/>
       <c r="B44" s="13" t="s">
         <v>21</v>
@@ -6738,7 +6768,7 @@
         <v>22</v>
       </c>
       <c r="J44" s="11"/>
-      <c r="K44" s="94" t="s">
+      <c r="K44" s="93" t="s">
         <v>89</v>
       </c>
       <c r="L44" s="3" t="s">
@@ -6850,7 +6880,7 @@
         <v>," 0="</v>
       </c>
     </row>
-    <row r="45" spans="1:47" s="3" customFormat="1">
+    <row r="45" spans="1:47" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A45" s="4"/>
       <c r="B45" s="13" t="s">
         <v>296</v>
@@ -6876,7 +6906,7 @@
         <v>23</v>
       </c>
       <c r="J45" s="11"/>
-      <c r="K45" s="94" t="s">
+      <c r="K45" s="93" t="s">
         <v>89</v>
       </c>
       <c r="L45" s="3" t="s">
@@ -6988,7 +7018,7 @@
         <v>," 0&lt;&gt;"</v>
       </c>
     </row>
-    <row r="46" spans="1:47" s="3" customFormat="1">
+    <row r="46" spans="1:47" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="4"/>
       <c r="B46" s="13" t="s">
         <v>294</v>
@@ -7014,7 +7044,7 @@
         <v>24</v>
       </c>
       <c r="J46" s="11"/>
-      <c r="K46" s="94" t="s">
+      <c r="K46" s="93" t="s">
         <v>89</v>
       </c>
       <c r="L46" s="3" t="s">
@@ -7126,7 +7156,7 @@
         <v>," 0&lt;"</v>
       </c>
     </row>
-    <row r="47" spans="1:47" s="3" customFormat="1">
+    <row r="47" spans="1:47" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A47" s="4"/>
       <c r="B47" s="6" t="s">
         <v>295</v>
@@ -7152,7 +7182,7 @@
         <v>25</v>
       </c>
       <c r="J47" s="11"/>
-      <c r="K47" s="94" t="s">
+      <c r="K47" s="93" t="s">
         <v>89</v>
       </c>
       <c r="L47" s="3" t="s">
@@ -7264,7 +7294,7 @@
         <v>," 0&gt;"</v>
       </c>
     </row>
-    <row r="48" spans="1:47" s="3" customFormat="1">
+    <row r="48" spans="1:47" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A48" s="4"/>
       <c r="B48" s="11" t="b">
         <v>0</v>
@@ -7290,7 +7320,7 @@
         <v>26</v>
       </c>
       <c r="J48" s="11"/>
-      <c r="K48" s="95" t="s">
+      <c r="K48" s="94" t="s">
         <v>196</v>
       </c>
       <c r="L48" s="3" t="s">
@@ -7402,12 +7432,12 @@
         <v>," FALSE"</v>
       </c>
     </row>
-    <row r="49" spans="1:47">
+    <row r="49" spans="1:47" x14ac:dyDescent="0.2">
       <c r="E49" s="13"/>
       <c r="AT49" s="66"/>
       <c r="AU49" s="66"/>
     </row>
-    <row r="50" spans="1:47">
+    <row r="50" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>22</v>
       </c>
@@ -7415,7 +7445,7 @@
       <c r="AT50" s="66"/>
       <c r="AU50" s="66"/>
     </row>
-    <row r="51" spans="1:47">
+    <row r="51" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A51" s="4"/>
       <c r="B51" s="4" t="s">
         <v>23</v>
@@ -7438,7 +7468,7 @@
         <f t="shared" ref="I51:I58" si="25">DEC2HEX(H51)</f>
         <v>27</v>
       </c>
-      <c r="K51" s="90" t="s">
+      <c r="K51" s="89" t="s">
         <v>76</v>
       </c>
       <c r="L51" s="1" t="s">
@@ -7548,7 +7578,7 @@
         <v>," AND"</v>
       </c>
     </row>
-    <row r="52" spans="1:47">
+    <row r="52" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A52" s="4"/>
       <c r="B52" s="4" t="s">
         <v>24</v>
@@ -7571,7 +7601,7 @@
         <f t="shared" si="25"/>
         <v>28</v>
       </c>
-      <c r="K52" s="90" t="s">
+      <c r="K52" s="89" t="s">
         <v>76</v>
       </c>
       <c r="L52" s="1" t="s">
@@ -7681,7 +7711,7 @@
         <v>," OR"</v>
       </c>
     </row>
-    <row r="53" spans="1:47">
+    <row r="53" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A53" s="4"/>
       <c r="B53" s="4" t="s">
         <v>26</v>
@@ -7704,7 +7734,7 @@
         <f t="shared" si="25"/>
         <v>29</v>
       </c>
-      <c r="K53" s="90" t="s">
+      <c r="K53" s="89" t="s">
         <v>79</v>
       </c>
       <c r="L53" s="1" t="s">
@@ -7814,7 +7844,7 @@
         <v>," INVERT"</v>
       </c>
     </row>
-    <row r="54" spans="1:47">
+    <row r="54" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A54" s="4"/>
       <c r="B54" s="4" t="s">
         <v>25</v>
@@ -7837,7 +7867,7 @@
         <f t="shared" si="25"/>
         <v>2A</v>
       </c>
-      <c r="K54" s="90" t="s">
+      <c r="K54" s="89" t="s">
         <v>76</v>
       </c>
       <c r="L54" s="1" t="s">
@@ -7947,7 +7977,7 @@
         <v>," XOR"</v>
       </c>
     </row>
-    <row r="55" spans="1:47">
+    <row r="55" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A55" s="4"/>
       <c r="B55" s="4" t="s">
         <v>128</v>
@@ -7970,7 +8000,7 @@
         <f t="shared" si="25"/>
         <v>2B</v>
       </c>
-      <c r="K55" s="90" t="s">
+      <c r="K55" s="89" t="s">
         <v>129</v>
       </c>
       <c r="L55" s="1" t="s">
@@ -8080,7 +8110,7 @@
         <v>," LSL"</v>
       </c>
     </row>
-    <row r="56" spans="1:47">
+    <row r="56" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A56" s="4"/>
       <c r="B56" s="4" t="s">
         <v>127</v>
@@ -8103,7 +8133,7 @@
         <f t="shared" si="25"/>
         <v>2C</v>
       </c>
-      <c r="K56" s="90" t="s">
+      <c r="K56" s="89" t="s">
         <v>129</v>
       </c>
       <c r="L56" s="1" t="s">
@@ -8213,7 +8243,7 @@
         <v>," LSR"</v>
       </c>
     </row>
-    <row r="57" spans="1:47">
+    <row r="57" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A57" s="4"/>
       <c r="B57" s="4" t="s">
         <v>277</v>
@@ -8236,7 +8266,7 @@
         <f t="shared" si="25"/>
         <v>2D</v>
       </c>
-      <c r="K57" s="90" t="s">
+      <c r="K57" s="89" t="s">
         <v>129</v>
       </c>
       <c r="L57" s="1" t="s">
@@ -8346,7 +8376,7 @@
         <v>," XBYTE"</v>
       </c>
     </row>
-    <row r="58" spans="1:47">
+    <row r="58" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A58" s="4"/>
       <c r="B58" s="4" t="s">
         <v>247</v>
@@ -8369,7 +8399,7 @@
         <f t="shared" si="25"/>
         <v>2E</v>
       </c>
-      <c r="K58" s="90" t="s">
+      <c r="K58" s="89" t="s">
         <v>129</v>
       </c>
       <c r="L58" s="1" t="s">
@@ -8479,12 +8509,12 @@
         <v>," XWORD"</v>
       </c>
     </row>
-    <row r="59" spans="1:47">
+    <row r="59" spans="1:47" x14ac:dyDescent="0.2">
       <c r="E59" s="13"/>
       <c r="AT59" s="66"/>
       <c r="AU59" s="66"/>
     </row>
-    <row r="60" spans="1:47">
+    <row r="60" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>29</v>
       </c>
@@ -8492,7 +8522,7 @@
       <c r="AT60" s="66"/>
       <c r="AU60" s="66"/>
     </row>
-    <row r="61" spans="1:47" s="14" customFormat="1">
+    <row r="61" spans="1:47" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B61" s="15" t="s">
         <v>287</v>
       </c>
@@ -8517,7 +8547,7 @@
         <v>2F</v>
       </c>
       <c r="J61" s="15"/>
-      <c r="K61" s="93" t="s">
+      <c r="K61" s="92" t="s">
         <v>101</v>
       </c>
       <c r="L61" s="14" t="s">
@@ -8616,7 +8646,7 @@
         <v>," FETCH.L"</v>
       </c>
     </row>
-    <row r="62" spans="1:47" s="14" customFormat="1">
+    <row r="62" spans="1:47" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B62" s="15" t="s">
         <v>288</v>
       </c>
@@ -8641,7 +8671,7 @@
         <v>30</v>
       </c>
       <c r="J62" s="15"/>
-      <c r="K62" s="93" t="s">
+      <c r="K62" s="92" t="s">
         <v>103</v>
       </c>
       <c r="L62" s="14" t="s">
@@ -8740,7 +8770,7 @@
         <v>," STORE.L"</v>
       </c>
     </row>
-    <row r="63" spans="1:47" s="14" customFormat="1">
+    <row r="63" spans="1:47" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B63" s="15" t="s">
         <v>289</v>
       </c>
@@ -8765,7 +8795,7 @@
         <v>31</v>
       </c>
       <c r="J63" s="15"/>
-      <c r="K63" s="93" t="s">
+      <c r="K63" s="92" t="s">
         <v>105</v>
       </c>
       <c r="L63" s="14" t="s">
@@ -8863,7 +8893,7 @@
         <v>," FETCH.W"</v>
       </c>
     </row>
-    <row r="64" spans="1:47" s="14" customFormat="1">
+    <row r="64" spans="1:47" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B64" s="15" t="s">
         <v>290</v>
       </c>
@@ -8888,7 +8918,7 @@
         <v>32</v>
       </c>
       <c r="J64" s="15"/>
-      <c r="K64" s="93" t="s">
+      <c r="K64" s="92" t="s">
         <v>107</v>
       </c>
       <c r="L64" s="14" t="s">
@@ -8986,7 +9016,7 @@
         <v>," STORE.W"</v>
       </c>
     </row>
-    <row r="65" spans="1:47" s="14" customFormat="1">
+    <row r="65" spans="1:47" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B65" s="15" t="s">
         <v>291</v>
       </c>
@@ -9011,7 +9041,7 @@
         <v>33</v>
       </c>
       <c r="J65" s="15"/>
-      <c r="K65" s="93" t="s">
+      <c r="K65" s="92" t="s">
         <v>109</v>
       </c>
       <c r="L65" s="14" t="s">
@@ -9084,21 +9114,21 @@
         <f>IF(AC65="X",0,VLOOKUP(AC65,OPCODE_mult!$I$4:$L$19,4,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="AN65" s="15">
+      <c r="AN65" s="15" t="e">
         <f>IF(AD65="X",0,VLOOKUP(AD65,OPCODE_mult!$J$4:$L$19,3,FALSE))</f>
-        <v>7</v>
-      </c>
-      <c r="AO65" s="15" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AO65" s="15" t="e">
         <f t="shared" si="33"/>
-        <v>0111</v>
-      </c>
-      <c r="AQ65" s="16" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AQ65" s="16" t="e">
         <f t="shared" si="34"/>
-        <v>00000000100111</v>
-      </c>
-      <c r="AR65" s="14">
+        <v>#N/A</v>
+      </c>
+      <c r="AR65" s="14" t="e">
         <f t="shared" si="3"/>
-        <v>39</v>
+        <v>#N/A</v>
       </c>
       <c r="AT65" s="66" t="str">
         <f t="shared" si="35"/>
@@ -9109,7 +9139,7 @@
         <v>," FETCH.B"</v>
       </c>
     </row>
-    <row r="66" spans="1:47" s="14" customFormat="1">
+    <row r="66" spans="1:47" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B66" s="15" t="s">
         <v>297</v>
       </c>
@@ -9134,7 +9164,7 @@
         <v>34</v>
       </c>
       <c r="J66" s="15"/>
-      <c r="K66" s="93" t="s">
+      <c r="K66" s="92" t="s">
         <v>110</v>
       </c>
       <c r="L66" s="14" t="s">
@@ -9232,7 +9262,7 @@
         <v>," STORE.B"</v>
       </c>
     </row>
-    <row r="67" spans="1:47" s="2" customFormat="1">
+    <row r="67" spans="1:47" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B67" s="5"/>
       <c r="C67" s="5"/>
       <c r="D67" s="4"/>
@@ -9242,7 +9272,7 @@
       <c r="H67" s="50"/>
       <c r="I67" s="5"/>
       <c r="J67" s="5"/>
-      <c r="K67" s="96"/>
+      <c r="K67" s="95"/>
       <c r="M67" s="10"/>
       <c r="N67" s="5"/>
       <c r="O67" s="5"/>
@@ -9256,7 +9286,7 @@
       <c r="AT67" s="67"/>
       <c r="AU67" s="66"/>
     </row>
-    <row r="68" spans="1:47">
+    <row r="68" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>313</v>
       </c>
@@ -9265,7 +9295,7 @@
       <c r="AT68" s="67"/>
       <c r="AU68" s="66"/>
     </row>
-    <row r="69" spans="1:47" s="14" customFormat="1">
+    <row r="69" spans="1:47" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B69" s="15" t="s">
         <v>312</v>
       </c>
@@ -9290,7 +9320,7 @@
         <v>35</v>
       </c>
       <c r="J69" s="15"/>
-      <c r="K69" s="97" t="s">
+      <c r="K69" s="96" t="s">
         <v>115</v>
       </c>
       <c r="L69" s="14" t="s">
@@ -9386,7 +9416,7 @@
         <v>," #.B"</v>
       </c>
     </row>
-    <row r="70" spans="1:47" s="14" customFormat="1">
+    <row r="70" spans="1:47" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B70" s="15" t="s">
         <v>311</v>
       </c>
@@ -9411,7 +9441,7 @@
         <v>36</v>
       </c>
       <c r="J70" s="15"/>
-      <c r="K70" s="97" t="s">
+      <c r="K70" s="96" t="s">
         <v>115</v>
       </c>
       <c r="L70" s="14" t="s">
@@ -9507,7 +9537,7 @@
         <v>," #.W"</v>
       </c>
     </row>
-    <row r="71" spans="1:47" s="14" customFormat="1">
+    <row r="71" spans="1:47" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B71" s="15" t="s">
         <v>310</v>
       </c>
@@ -9532,7 +9562,7 @@
         <v>37</v>
       </c>
       <c r="J71" s="15"/>
-      <c r="K71" s="97" t="s">
+      <c r="K71" s="96" t="s">
         <v>116</v>
       </c>
       <c r="L71" s="14" t="s">
@@ -9626,13 +9656,13 @@
         <v>," #.L"</v>
       </c>
     </row>
-    <row r="72" spans="1:47">
+    <row r="72" spans="1:47" x14ac:dyDescent="0.2">
       <c r="S72" s="4"/>
       <c r="T72" s="4"/>
       <c r="AT72" s="66"/>
       <c r="AU72" s="66"/>
     </row>
-    <row r="73" spans="1:47">
+    <row r="73" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>47</v>
       </c>
@@ -9641,7 +9671,7 @@
       <c r="AT73" s="66"/>
       <c r="AU73" s="66"/>
     </row>
-    <row r="74" spans="1:47" s="3" customFormat="1">
+    <row r="74" spans="1:47" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B74" s="11" t="s">
         <v>51</v>
       </c>
@@ -9666,7 +9696,7 @@
         <v>38</v>
       </c>
       <c r="J74" s="11"/>
-      <c r="K74" s="95" t="s">
+      <c r="K74" s="94" t="s">
         <v>270</v>
       </c>
       <c r="L74" s="3" t="s">
@@ -9786,7 +9816,7 @@
         <v>," JMP"</v>
       </c>
     </row>
-    <row r="75" spans="1:47" s="3" customFormat="1">
+    <row r="75" spans="1:47" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B75" s="11" t="s">
         <v>259</v>
       </c>
@@ -9811,7 +9841,7 @@
         <v>39</v>
       </c>
       <c r="J75" s="11"/>
-      <c r="K75" s="94" t="s">
+      <c r="K75" s="93" t="s">
         <v>271</v>
       </c>
       <c r="L75" s="3" t="s">
@@ -9917,7 +9947,7 @@
         <v>," BSR"</v>
       </c>
     </row>
-    <row r="76" spans="1:47" s="3" customFormat="1">
+    <row r="76" spans="1:47" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B76" s="11" t="s">
         <v>50</v>
       </c>
@@ -9942,7 +9972,7 @@
         <v>3A</v>
       </c>
       <c r="J76" s="11"/>
-      <c r="K76" s="94" t="s">
+      <c r="K76" s="93" t="s">
         <v>271</v>
       </c>
       <c r="L76" s="3" t="s">
@@ -10060,7 +10090,7 @@
         <v>," JSR"</v>
       </c>
     </row>
-    <row r="77" spans="1:47" s="14" customFormat="1">
+    <row r="77" spans="1:47" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B77" s="15" t="s">
         <v>292</v>
       </c>
@@ -10084,7 +10114,7 @@
         <v>40</v>
       </c>
       <c r="J77" s="15"/>
-      <c r="K77" s="97" t="s">
+      <c r="K77" s="96" t="s">
         <v>114</v>
       </c>
       <c r="L77" s="14" t="s">
@@ -10137,7 +10167,7 @@
       </c>
       <c r="AU77" s="67"/>
     </row>
-    <row r="78" spans="1:47" s="14" customFormat="1">
+    <row r="78" spans="1:47" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B78" s="15" t="s">
         <v>48</v>
       </c>
@@ -10161,7 +10191,7 @@
         <v>80</v>
       </c>
       <c r="J78" s="15"/>
-      <c r="K78" s="97" t="s">
+      <c r="K78" s="96" t="s">
         <v>113</v>
       </c>
       <c r="L78" s="14" t="s">
@@ -10199,7 +10229,7 @@
       <c r="AT78" s="66"/>
       <c r="AU78" s="67"/>
     </row>
-    <row r="79" spans="1:47" s="14" customFormat="1">
+    <row r="79" spans="1:47" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B79" s="15" t="s">
         <v>49</v>
       </c>
@@ -10223,7 +10253,7 @@
         <v>C0</v>
       </c>
       <c r="J79" s="15"/>
-      <c r="K79" s="97" t="s">
+      <c r="K79" s="96" t="s">
         <v>113</v>
       </c>
       <c r="L79" s="14" t="s">
@@ -10243,7 +10273,7 @@
       <c r="AT79" s="66"/>
       <c r="AU79" s="67"/>
     </row>
-    <row r="80" spans="1:47" s="14" customFormat="1">
+    <row r="80" spans="1:47" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B80" s="15"/>
       <c r="C80" s="15"/>
       <c r="D80" s="15"/>
@@ -10253,7 +10283,7 @@
       <c r="H80" s="7"/>
       <c r="I80" s="4"/>
       <c r="J80" s="15"/>
-      <c r="K80" s="97"/>
+      <c r="K80" s="96"/>
       <c r="M80" s="16"/>
       <c r="N80" s="15"/>
       <c r="O80" s="15"/>
@@ -10268,7 +10298,7 @@
       <c r="AT80" s="66"/>
       <c r="AU80" s="67"/>
     </row>
-    <row r="81" spans="1:47" s="14" customFormat="1">
+    <row r="81" spans="1:47" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A81" s="3" t="s">
         <v>299</v>
       </c>
@@ -10281,7 +10311,7 @@
       <c r="H81" s="7"/>
       <c r="I81" s="4"/>
       <c r="J81" s="15"/>
-      <c r="K81" s="97"/>
+      <c r="K81" s="96"/>
       <c r="M81" s="16"/>
       <c r="N81" s="15"/>
       <c r="O81" s="15"/>
@@ -10296,7 +10326,7 @@
       <c r="AT81" s="66"/>
       <c r="AU81" s="67"/>
     </row>
-    <row r="82" spans="1:47" s="57" customFormat="1">
+    <row r="82" spans="1:47" s="57" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B82" s="58" t="s">
         <v>301</v>
       </c>
@@ -10317,7 +10347,7 @@
         <v>3B</v>
       </c>
       <c r="J82" s="58"/>
-      <c r="K82" s="98"/>
+      <c r="K82" s="97"/>
       <c r="L82" s="57" t="s">
         <v>304</v>
       </c>
@@ -10337,7 +10367,7 @@
       </c>
       <c r="AU82" s="69"/>
     </row>
-    <row r="83" spans="1:47" s="57" customFormat="1">
+    <row r="83" spans="1:47" s="57" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B83" s="58" t="s">
         <v>306</v>
       </c>
@@ -10358,7 +10388,7 @@
         <v>3C</v>
       </c>
       <c r="J83" s="58"/>
-      <c r="K83" s="98"/>
+      <c r="K83" s="97"/>
       <c r="L83" s="57" t="s">
         <v>307</v>
       </c>
@@ -10378,7 +10408,7 @@
       </c>
       <c r="AU83" s="69"/>
     </row>
-    <row r="84" spans="1:47" s="57" customFormat="1">
+    <row r="84" spans="1:47" s="57" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B84" s="58" t="s">
         <v>305</v>
       </c>
@@ -10399,7 +10429,7 @@
         <v>3D</v>
       </c>
       <c r="J84" s="58"/>
-      <c r="K84" s="98"/>
+      <c r="K84" s="97"/>
       <c r="L84" s="57" t="s">
         <v>303</v>
       </c>
@@ -10419,7 +10449,7 @@
       </c>
       <c r="AU84" s="69"/>
     </row>
-    <row r="85" spans="1:47" s="57" customFormat="1">
+    <row r="85" spans="1:47" s="57" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B85" s="58"/>
       <c r="C85" s="58"/>
       <c r="D85" s="58"/>
@@ -10438,7 +10468,7 @@
         <v>3E</v>
       </c>
       <c r="J85" s="58"/>
-      <c r="K85" s="98"/>
+      <c r="K85" s="97"/>
       <c r="M85" s="60"/>
       <c r="N85" s="58"/>
       <c r="O85" s="58"/>
@@ -10450,7 +10480,7 @@
       <c r="AQ85" s="60"/>
       <c r="AT85" s="62"/>
     </row>
-    <row r="86" spans="1:47" s="57" customFormat="1">
+    <row r="86" spans="1:47" s="57" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B86" s="58"/>
       <c r="C86" s="58"/>
       <c r="D86" s="58"/>
@@ -10460,7 +10490,7 @@
       <c r="H86" s="59"/>
       <c r="I86" s="58"/>
       <c r="J86" s="58"/>
-      <c r="K86" s="98"/>
+      <c r="K86" s="97"/>
       <c r="M86" s="60"/>
       <c r="N86" s="58"/>
       <c r="O86" s="58"/>
@@ -10472,7 +10502,7 @@
       <c r="AQ86" s="60"/>
       <c r="AT86" s="62"/>
     </row>
-    <row r="87" spans="1:47" s="3" customFormat="1">
+    <row r="87" spans="1:47" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A87" s="3" t="s">
         <v>145</v>
       </c>
@@ -10485,7 +10515,7 @@
       <c r="H87" s="51"/>
       <c r="I87" s="11"/>
       <c r="J87" s="11"/>
-      <c r="K87" s="95"/>
+      <c r="K87" s="94"/>
       <c r="M87" s="12"/>
       <c r="N87" s="11"/>
       <c r="O87" s="11"/>
@@ -10498,7 +10528,7 @@
       <c r="AR87" s="1"/>
       <c r="AT87" s="53"/>
     </row>
-    <row r="88" spans="1:47" s="47" customFormat="1">
+    <row r="88" spans="1:47" s="47" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B88" s="48" t="s">
         <v>263</v>
       </c>
@@ -10523,7 +10553,7 @@
         <v>3B</v>
       </c>
       <c r="J88" s="48"/>
-      <c r="K88" s="99" t="s">
+      <c r="K88" s="98" t="s">
         <v>115</v>
       </c>
       <c r="L88" s="47" t="s">
@@ -10596,26 +10626,26 @@
         <f>IF(AC88="X",0,VLOOKUP(AC88,OPCODE_mult!$I$4:$L$19,4,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="AN88" s="48">
+      <c r="AN88" s="48" t="e">
         <f>IF(AD88="X",0,VLOOKUP(AD88,OPCODE_mult!$J$4:$L$19,3,FALSE))</f>
-        <v>7</v>
-      </c>
-      <c r="AO88" s="48" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AO88" s="48" t="e">
         <f>DEC2BIN(SUM(AK88:AN88),4)</f>
-        <v>0111</v>
+        <v>#N/A</v>
       </c>
       <c r="AP88" s="48"/>
-      <c r="AQ88" s="22" t="str">
+      <c r="AQ88" s="22" t="e">
         <f t="shared" ref="AQ88:AQ92" si="50">AF88&amp;AG88&amp;AH88&amp;AI88&amp;AJ88&amp;AO88</f>
-        <v>00010010100111</v>
-      </c>
-      <c r="AR88" s="47">
+        <v>#N/A</v>
+      </c>
+      <c r="AR88" s="47" t="e">
         <f t="shared" si="37"/>
-        <v>1191</v>
+        <v>#N/A</v>
       </c>
       <c r="AT88" s="53"/>
     </row>
-    <row r="89" spans="1:47" s="47" customFormat="1">
+    <row r="89" spans="1:47" s="47" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B89" s="48" t="s">
         <v>264</v>
       </c>
@@ -10640,7 +10670,7 @@
         <v>3C</v>
       </c>
       <c r="J89" s="48"/>
-      <c r="K89" s="99" t="s">
+      <c r="K89" s="98" t="s">
         <v>96</v>
       </c>
       <c r="L89" s="47" t="s">
@@ -10713,26 +10743,26 @@
         <f>IF(AC89="X",0,VLOOKUP(AC89,OPCODE_mult!$I$4:$L$19,4,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="AN89" s="48">
+      <c r="AN89" s="48" t="e">
         <f>IF(AD89="X",0,VLOOKUP(AD89,OPCODE_mult!$J$4:$L$19,3,FALSE))</f>
-        <v>7</v>
-      </c>
-      <c r="AO89" s="48" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AO89" s="48" t="e">
         <f>DEC2BIN(SUM(AK89:AN89),4)</f>
-        <v>0111</v>
+        <v>#N/A</v>
       </c>
       <c r="AP89" s="48"/>
-      <c r="AQ89" s="22" t="str">
+      <c r="AQ89" s="22" t="e">
         <f t="shared" si="50"/>
-        <v>00000000100111</v>
-      </c>
-      <c r="AR89" s="47">
+        <v>#N/A</v>
+      </c>
+      <c r="AR89" s="47" t="e">
         <f t="shared" si="37"/>
-        <v>39</v>
+        <v>#N/A</v>
       </c>
       <c r="AT89" s="53"/>
     </row>
-    <row r="90" spans="1:47" s="47" customFormat="1">
+    <row r="90" spans="1:47" s="47" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B90" s="48" t="s">
         <v>265</v>
       </c>
@@ -10757,7 +10787,7 @@
         <v>3D</v>
       </c>
       <c r="J90" s="49"/>
-      <c r="K90" s="100" t="s">
+      <c r="K90" s="99" t="s">
         <v>203</v>
       </c>
       <c r="L90" s="47" t="s">
@@ -10861,7 +10891,7 @@
       </c>
       <c r="AT90" s="53"/>
     </row>
-    <row r="91" spans="1:47" s="47" customFormat="1" ht="14.25" customHeight="1">
+    <row r="91" spans="1:47" s="47" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B91" s="48" t="s">
         <v>266</v>
       </c>
@@ -10886,7 +10916,7 @@
         <v>3E</v>
       </c>
       <c r="J91" s="49"/>
-      <c r="K91" s="100" t="s">
+      <c r="K91" s="99" t="s">
         <v>195</v>
       </c>
       <c r="L91" s="47" t="s">
@@ -10990,7 +11020,7 @@
       </c>
       <c r="AT91" s="53"/>
     </row>
-    <row r="92" spans="1:47" s="47" customFormat="1">
+    <row r="92" spans="1:47" s="47" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B92" s="48" t="s">
         <v>146</v>
       </c>
@@ -11014,7 +11044,7 @@
         <v>3F</v>
       </c>
       <c r="J92" s="48"/>
-      <c r="K92" s="99" t="s">
+      <c r="K92" s="98" t="s">
         <v>298</v>
       </c>
       <c r="L92" s="47" t="s">
@@ -11120,18 +11150,18 @@
       </c>
       <c r="AT92" s="56"/>
     </row>
-    <row r="94" spans="1:47">
+    <row r="94" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A94" s="8" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="95" spans="1:47">
+    <row r="95" spans="1:47" x14ac:dyDescent="0.2">
       <c r="B95" s="8" t="s">
         <v>253</v>
       </c>
       <c r="C95" s="8"/>
     </row>
-    <row r="96" spans="1:47" s="39" customFormat="1">
+    <row r="96" spans="1:47" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B96" s="9" t="s">
         <v>254</v>
       </c>
@@ -11143,7 +11173,7 @@
       <c r="H96" s="52"/>
       <c r="I96" s="40"/>
       <c r="J96" s="40"/>
-      <c r="K96" s="101"/>
+      <c r="K96" s="100"/>
       <c r="M96" s="41"/>
       <c r="N96" s="40"/>
       <c r="O96" s="40"/>
@@ -11153,13 +11183,13 @@
       <c r="AQ96" s="41"/>
       <c r="AT96" s="54"/>
     </row>
-    <row r="97" spans="2:3">
+    <row r="97" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B97" s="57" t="s">
         <v>300</v>
       </c>
       <c r="C97" s="22"/>
     </row>
-    <row r="98" spans="2:3">
+    <row r="98" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B98" s="22" t="s">
         <v>144</v>
       </c>
@@ -11174,57 +11204,57 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.28515625" customWidth="1"/>
     <col min="3" max="6" width="9.140625" style="44"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B3" s="63"/>
-      <c r="C3" s="83" t="s">
+      <c r="C3" s="82" t="s">
         <v>267</v>
       </c>
-      <c r="D3" s="83" t="s">
+      <c r="D3" s="82" t="s">
         <v>150</v>
       </c>
-      <c r="E3" s="83" t="s">
+      <c r="E3" s="82" t="s">
         <v>151</v>
       </c>
-      <c r="F3" s="83" t="s">
+      <c r="F3" s="82" t="s">
         <v>154</v>
       </c>
-      <c r="G3" s="83" t="s">
+      <c r="G3" s="107" t="s">
         <v>236</v>
       </c>
-      <c r="H3" s="83" t="s">
+      <c r="H3" s="107" t="s">
         <v>234</v>
       </c>
-      <c r="I3" s="83" t="s">
+      <c r="I3" s="107" t="s">
         <v>235</v>
       </c>
-      <c r="J3" s="83" t="s">
+      <c r="J3" s="107" t="s">
         <v>248</v>
       </c>
-      <c r="K3" s="83" t="s">
+      <c r="K3" s="82" t="s">
         <v>238</v>
       </c>
-      <c r="L3" s="84"/>
-    </row>
-    <row r="4" spans="1:12">
-      <c r="B4" s="85">
+      <c r="L3" s="83"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B4" s="84">
         <v>0</v>
       </c>
       <c r="C4" s="70" t="s">
@@ -11251,375 +11281,379 @@
       <c r="J4" s="71" t="s">
         <v>31</v>
       </c>
-      <c r="K4" s="72" t="s">
+      <c r="K4" s="105" t="s">
         <v>234</v>
       </c>
-      <c r="L4" s="86">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12">
-      <c r="B5" s="85">
+      <c r="L4" s="85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B5" s="84">
         <v>1</v>
       </c>
-      <c r="C5" s="73" t="s">
+      <c r="C5" s="72" t="s">
         <v>258</v>
       </c>
-      <c r="D5" s="74" t="s">
+      <c r="D5" s="73" t="s">
         <v>30</v>
       </c>
-      <c r="E5" s="74" t="s">
+      <c r="E5" s="73" t="s">
         <v>153</v>
       </c>
-      <c r="F5" s="74" t="s">
+      <c r="F5" s="73" t="s">
         <v>156</v>
       </c>
-      <c r="G5" s="74" t="s">
+      <c r="G5" s="73" t="s">
         <v>44</v>
       </c>
-      <c r="H5" s="74" t="s">
+      <c r="H5" s="73" t="s">
         <v>16</v>
       </c>
-      <c r="I5" s="74" t="s">
+      <c r="I5" s="73" t="s">
         <v>24</v>
       </c>
-      <c r="J5" s="74" t="s">
+      <c r="J5" s="73" t="s">
         <v>133</v>
       </c>
-      <c r="K5" s="75" t="s">
+      <c r="K5" s="106" t="s">
         <v>235</v>
       </c>
-      <c r="L5" s="86">
+      <c r="L5" s="85">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
-      <c r="B6" s="85">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B6" s="84">
         <v>2</v>
       </c>
-      <c r="C6" s="73"/>
-      <c r="D6" s="74" t="s">
+      <c r="C6" s="72"/>
+      <c r="D6" s="73" t="s">
         <v>133</v>
       </c>
-      <c r="E6" s="74" t="s">
+      <c r="E6" s="73" t="s">
         <v>152</v>
       </c>
-      <c r="F6" s="74" t="s">
+      <c r="F6" s="73" t="s">
         <v>155</v>
       </c>
-      <c r="G6" s="74" t="s">
+      <c r="G6" s="73" t="s">
         <v>18</v>
       </c>
-      <c r="H6" s="74" t="s">
+      <c r="H6" s="73" t="s">
         <v>232</v>
       </c>
-      <c r="I6" s="74" t="s">
+      <c r="I6" s="73" t="s">
         <v>26</v>
       </c>
-      <c r="J6" s="74" t="s">
+      <c r="J6" s="73" t="s">
         <v>308</v>
       </c>
-      <c r="K6" s="75" t="s">
+      <c r="K6" s="106" t="s">
         <v>248</v>
       </c>
-      <c r="L6" s="87">
+      <c r="L6" s="86">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
-      <c r="B7" s="85">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B7" s="84">
         <v>3</v>
       </c>
-      <c r="C7" s="73"/>
-      <c r="D7" s="74" t="s">
+      <c r="C7" s="72"/>
+      <c r="D7" s="73" t="s">
         <v>197</v>
       </c>
-      <c r="E7" s="74" t="s">
+      <c r="E7" s="73" t="s">
         <v>30</v>
       </c>
-      <c r="F7" s="74" t="s">
+      <c r="F7" s="73" t="s">
         <v>30</v>
       </c>
-      <c r="G7" s="74" t="s">
+      <c r="G7" s="73" t="s">
         <v>19</v>
       </c>
-      <c r="H7" s="74" t="s">
+      <c r="H7" s="73" t="s">
         <v>233</v>
       </c>
-      <c r="I7" s="74" t="s">
+      <c r="I7" s="73" t="s">
         <v>25</v>
       </c>
-      <c r="J7" s="74" t="s">
+      <c r="J7" s="73" t="s">
         <v>36</v>
       </c>
-      <c r="K7" s="75" t="s">
+      <c r="K7" s="106" t="s">
         <v>236</v>
       </c>
-      <c r="L7" s="87">
+      <c r="L7" s="86">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
-      <c r="B8" s="85">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B8" s="84">
         <v>4</v>
       </c>
-      <c r="C8" s="76"/>
-      <c r="D8" s="77"/>
-      <c r="E8" s="77"/>
-      <c r="F8" s="77"/>
-      <c r="G8" s="74" t="s">
+      <c r="C8" s="75"/>
+      <c r="D8" s="76"/>
+      <c r="E8" s="76"/>
+      <c r="F8" s="76"/>
+      <c r="G8" s="73" t="s">
         <v>27</v>
       </c>
-      <c r="H8" s="74" t="s">
+      <c r="H8" s="73" t="s">
         <v>220</v>
       </c>
-      <c r="I8" s="74" t="s">
+      <c r="I8" s="73" t="s">
         <v>128</v>
       </c>
-      <c r="J8" s="74" t="s">
+      <c r="J8" s="73" t="s">
         <v>35</v>
       </c>
-      <c r="K8" s="75" t="s">
+      <c r="K8" s="74" t="s">
         <v>191</v>
       </c>
-      <c r="L8" s="87">
+      <c r="L8" s="86">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
-      <c r="B9" s="85">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B9" s="84">
         <v>5</v>
       </c>
-      <c r="C9" s="76"/>
-      <c r="D9" s="77"/>
-      <c r="E9" s="77"/>
-      <c r="F9" s="77"/>
-      <c r="G9" s="74" t="s">
+      <c r="C9" s="75"/>
+      <c r="D9" s="76"/>
+      <c r="E9" s="76"/>
+      <c r="F9" s="76"/>
+      <c r="G9" s="73" t="s">
         <v>28</v>
       </c>
-      <c r="H9" s="74" t="s">
+      <c r="H9" s="73" t="s">
         <v>221</v>
       </c>
-      <c r="I9" s="74" t="s">
+      <c r="I9" s="73" t="s">
         <v>127</v>
       </c>
-      <c r="J9" s="74" t="s">
+      <c r="J9" s="73" t="s">
         <v>277</v>
       </c>
-      <c r="K9" s="75" t="s">
+      <c r="K9" s="74" t="s">
         <v>192</v>
       </c>
-      <c r="L9" s="87">
+      <c r="L9" s="86">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
-      <c r="B10" s="85">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B10" s="84">
         <v>6</v>
       </c>
-      <c r="C10" s="76"/>
-      <c r="D10" s="77"/>
-      <c r="E10" s="77"/>
-      <c r="F10" s="77"/>
-      <c r="G10" s="78" t="s">
+      <c r="C10" s="75"/>
+      <c r="D10" s="76"/>
+      <c r="E10" s="76"/>
+      <c r="F10" s="76"/>
+      <c r="G10" s="77" t="s">
         <v>21</v>
       </c>
-      <c r="H10" s="74" t="s">
+      <c r="H10" s="73" t="s">
         <v>52</v>
       </c>
-      <c r="I10" s="74" t="s">
+      <c r="I10" s="73" t="s">
         <v>190</v>
       </c>
-      <c r="J10" s="74" t="s">
+      <c r="J10" s="73" t="s">
         <v>247</v>
       </c>
-      <c r="K10" s="75" t="s">
+      <c r="K10" s="74" t="s">
         <v>200</v>
       </c>
-      <c r="L10" s="87">
+      <c r="L10" s="86">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
-      <c r="B11" s="85">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B11" s="84">
         <v>7</v>
       </c>
-      <c r="C11" s="76"/>
-      <c r="D11" s="77"/>
-      <c r="E11" s="77"/>
-      <c r="F11" s="77"/>
-      <c r="G11" s="74" t="s">
+      <c r="C11" s="75"/>
+      <c r="D11" s="76"/>
+      <c r="E11" s="76"/>
+      <c r="F11" s="76"/>
+      <c r="G11" s="73" t="s">
         <v>296</v>
       </c>
-      <c r="H11" s="74" t="s">
+      <c r="H11" s="73" t="s">
         <v>53</v>
       </c>
-      <c r="I11" s="74" t="s">
+      <c r="I11" s="73" t="s">
         <v>189</v>
       </c>
-      <c r="J11" s="74" t="s">
-        <v>255</v>
-      </c>
-      <c r="K11" s="75" t="s">
+      <c r="J11" s="108" t="s">
+        <v>346</v>
+      </c>
+      <c r="K11" s="74" t="s">
         <v>201</v>
       </c>
-      <c r="L11" s="87">
+      <c r="L11" s="86">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
-      <c r="B12" s="85">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B12" s="84">
         <v>8</v>
       </c>
-      <c r="C12" s="76"/>
-      <c r="D12" s="77"/>
-      <c r="E12" s="77"/>
-      <c r="F12" s="77"/>
-      <c r="G12" s="74" t="s">
+      <c r="C12" s="75"/>
+      <c r="D12" s="76"/>
+      <c r="E12" s="76"/>
+      <c r="F12" s="76"/>
+      <c r="G12" s="73" t="s">
         <v>294</v>
       </c>
       <c r="H12" s="64"/>
       <c r="I12" s="64"/>
-      <c r="J12" s="64"/>
-      <c r="K12" s="79"/>
-      <c r="L12" s="87">
+      <c r="J12" s="109" t="s">
+        <v>347</v>
+      </c>
+      <c r="K12" s="78"/>
+      <c r="L12" s="86">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
-      <c r="B13" s="85">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B13" s="84">
         <v>9</v>
       </c>
-      <c r="C13" s="76"/>
-      <c r="D13" s="77"/>
-      <c r="E13" s="77"/>
-      <c r="F13" s="77"/>
-      <c r="G13" s="74" t="s">
+      <c r="C13" s="75"/>
+      <c r="D13" s="76"/>
+      <c r="E13" s="76"/>
+      <c r="F13" s="76"/>
+      <c r="G13" s="73" t="s">
         <v>295</v>
       </c>
       <c r="H13" s="64"/>
       <c r="I13" s="64"/>
-      <c r="J13" s="64"/>
-      <c r="K13" s="79"/>
-      <c r="L13" s="87">
+      <c r="J13" s="109" t="s">
+        <v>348</v>
+      </c>
+      <c r="K13" s="78"/>
+      <c r="L13" s="86">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
-      <c r="B14" s="85">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B14" s="84">
         <v>10</v>
       </c>
-      <c r="C14" s="76"/>
-      <c r="D14" s="77"/>
-      <c r="E14" s="77"/>
-      <c r="F14" s="77"/>
-      <c r="G14" s="74" t="b">
+      <c r="C14" s="75"/>
+      <c r="D14" s="76"/>
+      <c r="E14" s="76"/>
+      <c r="F14" s="76"/>
+      <c r="G14" s="73" t="b">
         <v>0</v>
       </c>
       <c r="H14" s="64"/>
       <c r="I14" s="64"/>
       <c r="J14" s="64"/>
-      <c r="K14" s="79"/>
-      <c r="L14" s="87">
+      <c r="K14" s="78"/>
+      <c r="L14" s="86">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
-      <c r="B15" s="85">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B15" s="84">
         <v>11</v>
       </c>
-      <c r="C15" s="76"/>
-      <c r="D15" s="77"/>
-      <c r="E15" s="77"/>
-      <c r="F15" s="77"/>
-      <c r="G15" s="74" t="s">
+      <c r="C15" s="75"/>
+      <c r="D15" s="76"/>
+      <c r="E15" s="76"/>
+      <c r="F15" s="76"/>
+      <c r="G15" s="73" t="s">
         <v>45</v>
       </c>
       <c r="H15" s="64"/>
       <c r="I15" s="64"/>
       <c r="J15" s="64"/>
-      <c r="K15" s="79"/>
-      <c r="L15" s="87">
+      <c r="K15" s="78"/>
+      <c r="L15" s="86">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
-      <c r="B16" s="85">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B16" s="84">
         <v>12</v>
       </c>
-      <c r="C16" s="76"/>
-      <c r="D16" s="77"/>
-      <c r="E16" s="77"/>
-      <c r="F16" s="77"/>
-      <c r="G16" s="74" t="s">
+      <c r="C16" s="75"/>
+      <c r="D16" s="76"/>
+      <c r="E16" s="76"/>
+      <c r="F16" s="76"/>
+      <c r="G16" s="73" t="s">
         <v>46</v>
       </c>
       <c r="H16" s="64"/>
       <c r="I16" s="64"/>
       <c r="J16" s="64"/>
-      <c r="K16" s="79"/>
-      <c r="L16" s="87">
+      <c r="K16" s="78"/>
+      <c r="L16" s="86">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="2:12">
-      <c r="B17" s="85">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B17" s="84">
         <v>13</v>
       </c>
-      <c r="C17" s="76"/>
-      <c r="D17" s="77"/>
-      <c r="E17" s="77"/>
-      <c r="F17" s="77"/>
-      <c r="G17" s="74" t="s">
+      <c r="C17" s="75"/>
+      <c r="D17" s="76"/>
+      <c r="E17" s="76"/>
+      <c r="F17" s="76"/>
+      <c r="G17" s="73" t="s">
         <v>211</v>
       </c>
       <c r="H17" s="64"/>
       <c r="I17" s="64"/>
       <c r="J17" s="64"/>
-      <c r="K17" s="79"/>
-      <c r="L17" s="87">
+      <c r="K17" s="78"/>
+      <c r="L17" s="86">
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="2:12">
-      <c r="B18" s="85">
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B18" s="84">
         <v>14</v>
       </c>
-      <c r="C18" s="76"/>
-      <c r="D18" s="77"/>
-      <c r="E18" s="77"/>
-      <c r="F18" s="77"/>
-      <c r="G18" s="74" t="s">
+      <c r="C18" s="75"/>
+      <c r="D18" s="76"/>
+      <c r="E18" s="76"/>
+      <c r="F18" s="76"/>
+      <c r="G18" s="73" t="s">
         <v>210</v>
       </c>
       <c r="H18" s="64"/>
       <c r="I18" s="64"/>
       <c r="J18" s="64"/>
-      <c r="K18" s="79"/>
-      <c r="L18" s="87">
+      <c r="K18" s="78"/>
+      <c r="L18" s="86">
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="2:12">
-      <c r="B19" s="88">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B19" s="87">
         <v>15</v>
       </c>
-      <c r="C19" s="80"/>
-      <c r="D19" s="81"/>
-      <c r="E19" s="81"/>
-      <c r="F19" s="81"/>
+      <c r="C19" s="79"/>
+      <c r="D19" s="80"/>
+      <c r="E19" s="80"/>
+      <c r="F19" s="80"/>
       <c r="G19" s="19" t="b">
         <v>1</v>
       </c>
       <c r="H19" s="65"/>
       <c r="I19" s="65"/>
       <c r="J19" s="65"/>
-      <c r="K19" s="82"/>
-      <c r="L19" s="89">
+      <c r="K19" s="81"/>
+      <c r="L19" s="88">
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="2:12">
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
         <v>256</v>
       </c>
@@ -11645,13 +11679,13 @@
         <v>3</v>
       </c>
       <c r="J21" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K21" s="4">
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="2:12">
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B22" s="4" t="s">
         <v>257</v>
       </c>
@@ -11693,14 +11727,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.25"/>
+  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="2.28515625" style="1" customWidth="1"/>
     <col min="2" max="2" width="3.42578125" style="1" customWidth="1"/>
@@ -11715,43 +11749,43 @@
     <col min="23" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="15">
+    <row r="1" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="3" spans="1:22">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B3" s="23" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="4" spans="1:22">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B4" s="23"/>
       <c r="C4" s="23" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="5" spans="1:22" s="23" customFormat="1">
+    <row r="5" spans="1:22" s="23" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D5" s="28" t="s">
         <v>157</v>
       </c>
       <c r="F5" s="24"/>
-      <c r="G5" s="103">
-        <v>0</v>
-      </c>
-      <c r="H5" s="103">
+      <c r="G5" s="102">
+        <v>0</v>
+      </c>
+      <c r="H5" s="102">
         <v>1</v>
       </c>
-      <c r="I5" s="103">
+      <c r="I5" s="102">
         <v>2</v>
       </c>
-      <c r="J5" s="103">
+      <c r="J5" s="102">
         <v>3</v>
       </c>
       <c r="K5" s="7"/>
       <c r="L5" s="7"/>
     </row>
-    <row r="6" spans="1:22">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
       <c r="D6" s="1">
         <v>2</v>
       </c>
@@ -11773,7 +11807,7 @@
       <c r="K6" s="4"/>
       <c r="L6" s="4"/>
     </row>
-    <row r="7" spans="1:22">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
       <c r="D7" s="1">
         <v>2</v>
       </c>
@@ -11793,7 +11827,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:22" s="3" customFormat="1">
+    <row r="8" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D8" s="3">
         <v>2</v>
       </c>
@@ -11813,7 +11847,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:22">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
       <c r="D9" s="30">
         <f>SUM(D6:D8)</f>
         <v>6</v>
@@ -11823,18 +11857,18 @@
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
     </row>
-    <row r="10" spans="1:22">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
     </row>
-    <row r="11" spans="1:22" s="14" customFormat="1">
+    <row r="11" spans="1:22" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B11" s="31"/>
       <c r="C11" s="31" t="s">
         <v>159</v>
       </c>
       <c r="F11" s="35"/>
     </row>
-    <row r="12" spans="1:22" s="14" customFormat="1">
+    <row r="12" spans="1:22" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D12" s="14">
         <v>1</v>
       </c>
@@ -11848,75 +11882,75 @@
         <v>333</v>
       </c>
     </row>
-    <row r="13" spans="1:22" s="14" customFormat="1" ht="11.25" customHeight="1">
+    <row r="13" spans="1:22" s="14" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D13" s="32">
         <f>SUM(D12:D12)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:22" s="14" customFormat="1" ht="12.75" customHeight="1">
+    <row r="14" spans="1:22" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K14" s="15"/>
       <c r="L14" s="15"/>
     </row>
-    <row r="15" spans="1:22">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B15" s="23" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="16" spans="1:22">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
       <c r="D16" s="28" t="s">
         <v>157</v>
       </c>
-      <c r="G16" s="103">
-        <v>0</v>
-      </c>
-      <c r="H16" s="103">
+      <c r="G16" s="102">
+        <v>0</v>
+      </c>
+      <c r="H16" s="102">
         <v>1</v>
       </c>
-      <c r="I16" s="103">
+      <c r="I16" s="102">
         <v>2</v>
       </c>
-      <c r="J16" s="103">
+      <c r="J16" s="102">
         <v>3</v>
       </c>
-      <c r="K16" s="103">
+      <c r="K16" s="102">
         <v>4</v>
       </c>
-      <c r="L16" s="103">
+      <c r="L16" s="102">
         <v>5</v>
       </c>
-      <c r="M16" s="103">
+      <c r="M16" s="102">
         <v>6</v>
       </c>
-      <c r="N16" s="103">
+      <c r="N16" s="102">
         <v>7</v>
       </c>
-      <c r="O16" s="103">
+      <c r="O16" s="102">
         <v>8</v>
       </c>
-      <c r="P16" s="103">
+      <c r="P16" s="102">
         <v>9</v>
       </c>
-      <c r="Q16" s="103">
+      <c r="Q16" s="102">
         <v>10</v>
       </c>
-      <c r="R16" s="103">
+      <c r="R16" s="102">
         <v>11</v>
       </c>
-      <c r="S16" s="103">
+      <c r="S16" s="102">
         <v>12</v>
       </c>
-      <c r="T16" s="103">
+      <c r="T16" s="102">
         <v>13</v>
       </c>
-      <c r="U16" s="103">
+      <c r="U16" s="102">
         <v>14</v>
       </c>
-      <c r="V16" s="103">
+      <c r="V16" s="102">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="2:22">
+    <row r="17" spans="2:22" x14ac:dyDescent="0.2">
       <c r="D17" s="29">
         <v>4</v>
       </c>
@@ -11973,7 +12007,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="2:22">
+    <row r="18" spans="2:22" x14ac:dyDescent="0.2">
       <c r="D18" s="29"/>
       <c r="G18" s="4" t="s">
         <v>206</v>
@@ -12024,7 +12058,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="19" spans="2:22">
+    <row r="19" spans="2:22" x14ac:dyDescent="0.2">
       <c r="D19" s="1">
         <v>3</v>
       </c>
@@ -12056,7 +12090,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="20" spans="2:22">
+    <row r="20" spans="2:22" x14ac:dyDescent="0.2">
       <c r="D20" s="1">
         <v>3</v>
       </c>
@@ -12088,7 +12122,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="21" spans="2:22">
+    <row r="21" spans="2:22" x14ac:dyDescent="0.2">
       <c r="D21" s="1">
         <v>1</v>
       </c>
@@ -12120,7 +12154,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="22" spans="2:22">
+    <row r="22" spans="2:22" x14ac:dyDescent="0.2">
       <c r="D22" s="1">
         <v>3</v>
       </c>
@@ -12152,40 +12186,40 @@
         <v>201</v>
       </c>
     </row>
-    <row r="23" spans="2:22">
+    <row r="23" spans="2:22" x14ac:dyDescent="0.2">
       <c r="D23" s="30">
         <f>MAX(D17:D21)+D22</f>
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="2:22">
+    <row r="24" spans="2:22" x14ac:dyDescent="0.2">
       <c r="D24" s="36"/>
     </row>
-    <row r="25" spans="2:22">
+    <row r="25" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B25" s="23" t="s">
         <v>328</v>
       </c>
       <c r="D25" s="36"/>
     </row>
-    <row r="26" spans="2:22">
+    <row r="26" spans="2:22" x14ac:dyDescent="0.2">
       <c r="D26" s="28" t="s">
         <v>157</v>
       </c>
       <c r="E26" s="23"/>
-      <c r="G26" s="103">
-        <v>0</v>
-      </c>
-      <c r="H26" s="103">
+      <c r="G26" s="102">
+        <v>0</v>
+      </c>
+      <c r="H26" s="102">
         <v>1</v>
       </c>
-      <c r="I26" s="103">
+      <c r="I26" s="102">
         <v>2</v>
       </c>
-      <c r="J26" s="103">
+      <c r="J26" s="102">
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="2:22">
+    <row r="27" spans="2:22" x14ac:dyDescent="0.2">
       <c r="D27" s="29">
         <v>1</v>
       </c>
@@ -12202,8 +12236,8 @@
       <c r="I27" s="7"/>
       <c r="J27" s="7"/>
     </row>
-    <row r="28" spans="2:22">
-      <c r="D28" s="102">
+    <row r="28" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="D28" s="101">
         <f>SUM(D27)</f>
         <v>1</v>
       </c>
@@ -12213,7 +12247,7 @@
       <c r="I28" s="7"/>
       <c r="J28" s="7"/>
     </row>
-    <row r="29" spans="2:22">
+    <row r="29" spans="2:22" x14ac:dyDescent="0.2">
       <c r="D29" s="29"/>
       <c r="E29" s="23"/>
       <c r="G29" s="4"/>
@@ -12221,7 +12255,7 @@
       <c r="I29" s="7"/>
       <c r="J29" s="7"/>
     </row>
-    <row r="30" spans="2:22" s="26" customFormat="1">
+    <row r="30" spans="2:22" s="26" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D30" s="38"/>
       <c r="F30" s="37"/>
       <c r="G30" s="27"/>
@@ -12230,7 +12264,7 @@
       <c r="J30" s="27"/>
       <c r="K30" s="27"/>
     </row>
-    <row r="31" spans="2:22">
+    <row r="31" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B31" s="23" t="s">
         <v>319</v>
       </c>
@@ -12246,7 +12280,7 @@
       <c r="K31" s="19"/>
       <c r="L31" s="19"/>
     </row>
-    <row r="32" spans="2:22">
+    <row r="32" spans="2:22" x14ac:dyDescent="0.2">
       <c r="C32" s="1" t="s">
         <v>237</v>
       </c>
@@ -12266,7 +12300,7 @@
       </c>
       <c r="K32" s="4"/>
     </row>
-    <row r="33" spans="1:12">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C33" s="1" t="s">
         <v>238</v>
       </c>
@@ -12296,7 +12330,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:12">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C34" s="1" t="s">
         <v>239</v>
       </c>
@@ -12327,7 +12361,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:12">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C35" s="1" t="s">
         <v>329</v>
       </c>
@@ -12347,24 +12381,24 @@
       <c r="K35" s="4"/>
       <c r="L35" s="4"/>
     </row>
-    <row r="36" spans="1:12">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D36" s="30">
         <f>SUM(D32:D35)</f>
         <v>14</v>
       </c>
     </row>
-    <row r="38" spans="1:12">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B38" s="31" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="39" spans="1:12">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D39" s="32">
         <f>D13</f>
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:12">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>13</v>
       </c>
@@ -12372,7 +12406,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="42" spans="1:12">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42" s="14" t="s">
         <v>335</v>
       </c>
@@ -12387,14 +12421,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.25"/>
+  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.42578125" style="1" customWidth="1"/>
     <col min="2" max="2" width="17.28515625" style="4" customWidth="1"/>
@@ -12412,12 +12446,12 @@
     <col min="21" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="15">
+    <row r="1" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="4" spans="1:20">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="C4" s="33" t="s">
         <v>178</v>
       </c>
@@ -12444,7 +12478,7 @@
       </c>
       <c r="T4" s="19"/>
     </row>
-    <row r="5" spans="1:20">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="C5" s="4" t="s">
         <v>180</v>
       </c>
@@ -12485,7 +12519,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="6" spans="1:20">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
@@ -12508,7 +12542,7 @@
       <c r="S6" s="4"/>
       <c r="T6" s="4"/>
     </row>
-    <row r="7" spans="1:20">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>31</v>
       </c>
@@ -12529,7 +12563,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:20">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>30</v>
       </c>
@@ -12556,7 +12590,7 @@
       <c r="S8" s="4"/>
       <c r="T8" s="4"/>
     </row>
-    <row r="9" spans="1:20">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>11</v>
       </c>
@@ -12577,7 +12611,7 @@
       <c r="P9" s="4"/>
       <c r="Q9" s="4"/>
     </row>
-    <row r="10" spans="1:20">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
         <v>12</v>
       </c>
@@ -12598,7 +12632,7 @@
       <c r="P10" s="4"/>
       <c r="Q10" s="4"/>
     </row>
-    <row r="11" spans="1:20">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
         <v>13</v>
       </c>
@@ -12619,7 +12653,7 @@
       <c r="P11" s="4"/>
       <c r="Q11" s="4"/>
     </row>
-    <row r="12" spans="1:20">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12" s="17" t="s">
         <v>14</v>
       </c>
@@ -12636,7 +12670,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:20">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13" s="15" t="s">
         <v>15</v>
       </c>
@@ -12655,7 +12689,7 @@
       <c r="P13" s="4"/>
       <c r="Q13" s="4"/>
     </row>
-    <row r="14" spans="1:20">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A14" s="15" t="s">
         <v>42</v>
       </c>
@@ -12674,7 +12708,7 @@
       <c r="M14" s="4"/>
       <c r="N14" s="4"/>
     </row>
-    <row r="15" spans="1:20">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A15" s="21" t="s">
         <v>43</v>
       </c>
@@ -12693,7 +12727,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:20">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>16</v>
       </c>
@@ -12712,7 +12746,7 @@
       <c r="M16" s="4"/>
       <c r="N16" s="4"/>
     </row>
-    <row r="17" spans="1:20">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A17" s="11" t="s">
         <v>52</v>
       </c>
@@ -12731,7 +12765,7 @@
       <c r="M17" s="4"/>
       <c r="N17" s="4"/>
     </row>
-    <row r="18" spans="1:20">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A18" s="11" t="s">
         <v>53</v>
       </c>
@@ -12752,7 +12786,7 @@
       <c r="S18" s="4"/>
       <c r="T18" s="4"/>
     </row>
-    <row r="19" spans="1:20">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A19" s="11" t="s">
         <v>54</v>
       </c>
@@ -12771,7 +12805,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:20">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>55</v>
       </c>
@@ -12790,7 +12824,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:20">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>23</v>
       </c>
@@ -12809,7 +12843,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:20">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>24</v>
       </c>
@@ -12828,7 +12862,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:20">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>25</v>
       </c>
@@ -12847,7 +12881,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:20">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>26</v>
       </c>
@@ -12866,7 +12900,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:20">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A25" s="15" t="s">
         <v>143</v>
       </c>
@@ -12885,7 +12919,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:20">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A26" s="15" t="s">
         <v>142</v>
       </c>
@@ -12904,7 +12938,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:20">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>220</v>
       </c>
@@ -12921,7 +12955,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:20">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
         <v>221</v>
       </c>
@@ -12944,61 +12978,61 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="109.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" s="104" t="s">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="103" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
-      <c r="A2" s="104" t="s">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="103" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
-      <c r="A3" s="104"/>
-    </row>
-    <row r="4" spans="1:1">
-      <c r="A4" s="104" t="s">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="103"/>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="103" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
-      <c r="A5" s="104" t="s">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="103" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="30">
-      <c r="A6" s="104" t="s">
+    <row r="6" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="103" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
-      <c r="A7" s="104" t="s">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="103" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="45">
-      <c r="A8" s="105" t="s">
+    <row r="8" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="104" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
-      <c r="A9" s="104"/>
-    </row>
-    <row r="10" spans="1:1" ht="60">
-      <c r="A10" s="105" t="s">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="103"/>
+    </row>
+    <row r="10" spans="1:1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10" s="104" t="s">
         <v>343</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Load literal now implemented in single cycle for #.B, #.W and #.L Outstanding: - branch instructions needs to be reworked (not currently working) - SRAM load and store needs to be reworded (not changed, but also not tested)
</commit_message>
<xml_diff>
--- a/Resources/Instruction Set.xlsx
+++ b/Resources/Instruction Set.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="18195" windowHeight="8250" tabRatio="681" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="120" windowWidth="18195" windowHeight="8250" tabRatio="681"/>
   </bookViews>
   <sheets>
     <sheet name="OPCODE_encoding" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1363" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1361" uniqueCount="346">
   <si>
     <t>DUP</t>
   </si>
@@ -1059,15 +1059,6 @@
   </si>
   <si>
     <t>RSP!</t>
-  </si>
-  <si>
-    <t>PSD_DATA</t>
-  </si>
-  <si>
-    <t>S_DATA</t>
-  </si>
-  <si>
-    <t>S_DATA+</t>
   </si>
 </sst>
 </file>
@@ -1673,10 +1664,10 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1985,11 +1976,11 @@
   </sheetPr>
   <dimension ref="A1:AU98"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="9" ySplit="4" topLeftCell="J55" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="9" ySplit="4" topLeftCell="AB58" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B92" sqref="B92"/>
+      <selection pane="bottomRight" activeCell="V71" sqref="V71:AD71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -9114,21 +9105,21 @@
         <f>IF(AC65="X",0,VLOOKUP(AC65,OPCODE_mult!$I$4:$L$19,4,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="AN65" s="15" t="e">
+      <c r="AN65" s="15">
         <f>IF(AD65="X",0,VLOOKUP(AD65,OPCODE_mult!$J$4:$L$19,3,FALSE))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AO65" s="15" t="e">
+        <v>7</v>
+      </c>
+      <c r="AO65" s="15" t="str">
         <f t="shared" si="33"/>
-        <v>#N/A</v>
-      </c>
-      <c r="AQ65" s="16" t="e">
+        <v>0111</v>
+      </c>
+      <c r="AQ65" s="16" t="str">
         <f t="shared" si="34"/>
-        <v>#N/A</v>
-      </c>
-      <c r="AR65" s="14" t="e">
+        <v>00000000100111</v>
+      </c>
+      <c r="AR65" s="14">
         <f t="shared" si="3"/>
-        <v>#N/A</v>
+        <v>39</v>
       </c>
       <c r="AT65" s="66" t="str">
         <f t="shared" si="35"/>
@@ -9341,25 +9332,25 @@
         <v>35</v>
       </c>
       <c r="X69" s="15" t="s">
-        <v>36</v>
+        <v>152</v>
       </c>
       <c r="Y69" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Z69" s="15" t="s">
-        <v>234</v>
+        <v>248</v>
       </c>
       <c r="AA69" s="15" t="s">
         <v>141</v>
       </c>
       <c r="AB69" s="15" t="s">
-        <v>30</v>
+        <v>141</v>
       </c>
       <c r="AC69" s="15" t="s">
         <v>141</v>
       </c>
       <c r="AD69" s="15" t="s">
-        <v>141</v>
+        <v>255</v>
       </c>
       <c r="AF69" s="15" t="str">
         <f>DEC2BIN(VLOOKUP(V69,OPCODE_mult!$C$4:$L$19,10,FALSE),1)</f>
@@ -9371,15 +9362,15 @@
       </c>
       <c r="AH69" s="15" t="str">
         <f>DEC2BIN(VLOOKUP(X69,OPCODE_mult!$E$4:$L$19,8,FALSE),2)</f>
-        <v>00</v>
+        <v>10</v>
       </c>
       <c r="AI69" s="15" t="str">
         <f>DEC2BIN(VLOOKUP(Y69,OPCODE_mult!$D$4:$L$19,9,FALSE),2)</f>
-        <v>00</v>
+        <v>01</v>
       </c>
       <c r="AJ69" s="15" t="str">
         <f>DEC2BIN(IF(Z69="X",0,VLOOKUP(Z69,OPCODE_mult!$K$4:$L$19,2,FALSE)),3)</f>
-        <v>000</v>
+        <v>010</v>
       </c>
       <c r="AK69" s="15">
         <f>IF(AA69="X",0,VLOOKUP(AA69,OPCODE_mult!$G$4:$L$19,6,FALSE))</f>
@@ -9395,20 +9386,20 @@
       </c>
       <c r="AN69" s="15">
         <f>IF(AD69="X",0,VLOOKUP(AD69,OPCODE_mult!$J$4:$L$19,3,FALSE))</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AO69" s="15" t="str">
         <f>DEC2BIN(SUM(AK69:AN69),4)</f>
-        <v>0000</v>
+        <v>0111</v>
       </c>
       <c r="AP69" s="15"/>
       <c r="AQ69" s="16" t="str">
         <f t="shared" ref="AQ69:AQ71" si="36">AF69&amp;AG69&amp;AH69&amp;AI69&amp;AJ69&amp;AO69</f>
-        <v>00000000000000</v>
+        <v>00010010100111</v>
       </c>
       <c r="AR69" s="14">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1191</v>
       </c>
       <c r="AT69" s="67"/>
       <c r="AU69" s="66" t="str">
@@ -9462,25 +9453,25 @@
         <v>35</v>
       </c>
       <c r="X70" s="15" t="s">
-        <v>36</v>
+        <v>152</v>
       </c>
       <c r="Y70" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Z70" s="15" t="s">
-        <v>234</v>
+        <v>248</v>
       </c>
       <c r="AA70" s="15" t="s">
         <v>141</v>
       </c>
       <c r="AB70" s="15" t="s">
-        <v>30</v>
+        <v>141</v>
       </c>
       <c r="AC70" s="15" t="s">
         <v>141</v>
       </c>
       <c r="AD70" s="15" t="s">
-        <v>141</v>
+        <v>255</v>
       </c>
       <c r="AF70" s="15" t="str">
         <f>DEC2BIN(VLOOKUP(V70,OPCODE_mult!$C$4:$L$19,10,FALSE),1)</f>
@@ -9492,15 +9483,15 @@
       </c>
       <c r="AH70" s="15" t="str">
         <f>DEC2BIN(VLOOKUP(X70,OPCODE_mult!$E$4:$L$19,8,FALSE),2)</f>
-        <v>00</v>
+        <v>10</v>
       </c>
       <c r="AI70" s="15" t="str">
         <f>DEC2BIN(VLOOKUP(Y70,OPCODE_mult!$D$4:$L$19,9,FALSE),2)</f>
-        <v>00</v>
+        <v>01</v>
       </c>
       <c r="AJ70" s="15" t="str">
         <f>DEC2BIN(IF(Z70="X",0,VLOOKUP(Z70,OPCODE_mult!$K$4:$L$19,2,FALSE)),3)</f>
-        <v>000</v>
+        <v>010</v>
       </c>
       <c r="AK70" s="15">
         <f>IF(AA70="X",0,VLOOKUP(AA70,OPCODE_mult!$G$4:$L$19,6,FALSE))</f>
@@ -9516,20 +9507,20 @@
       </c>
       <c r="AN70" s="15">
         <f>IF(AD70="X",0,VLOOKUP(AD70,OPCODE_mult!$J$4:$L$19,3,FALSE))</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AO70" s="15" t="str">
         <f>DEC2BIN(SUM(AK70:AN70),4)</f>
-        <v>0000</v>
+        <v>0111</v>
       </c>
       <c r="AP70" s="15"/>
       <c r="AQ70" s="16" t="str">
         <f t="shared" si="36"/>
-        <v>00000000000000</v>
+        <v>00010010100111</v>
       </c>
       <c r="AR70" s="14">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1191</v>
       </c>
       <c r="AT70" s="67"/>
       <c r="AU70" s="66" t="str">
@@ -9581,25 +9572,25 @@
         <v>35</v>
       </c>
       <c r="X71" s="15" t="s">
-        <v>36</v>
+        <v>152</v>
       </c>
       <c r="Y71" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Z71" s="15" t="s">
-        <v>234</v>
+        <v>248</v>
       </c>
       <c r="AA71" s="15" t="s">
         <v>141</v>
       </c>
       <c r="AB71" s="15" t="s">
-        <v>30</v>
+        <v>141</v>
       </c>
       <c r="AC71" s="15" t="s">
         <v>141</v>
       </c>
       <c r="AD71" s="15" t="s">
-        <v>141</v>
+        <v>255</v>
       </c>
       <c r="AF71" s="15" t="str">
         <f>DEC2BIN(VLOOKUP(V71,OPCODE_mult!$C$4:$L$19,10,FALSE),1)</f>
@@ -9611,15 +9602,15 @@
       </c>
       <c r="AH71" s="15" t="str">
         <f>DEC2BIN(VLOOKUP(X71,OPCODE_mult!$E$4:$L$19,8,FALSE),2)</f>
-        <v>00</v>
+        <v>10</v>
       </c>
       <c r="AI71" s="15" t="str">
         <f>DEC2BIN(VLOOKUP(Y71,OPCODE_mult!$D$4:$L$19,9,FALSE),2)</f>
-        <v>00</v>
+        <v>01</v>
       </c>
       <c r="AJ71" s="15" t="str">
         <f>DEC2BIN(IF(Z71="X",0,VLOOKUP(Z71,OPCODE_mult!$K$4:$L$19,2,FALSE)),3)</f>
-        <v>000</v>
+        <v>010</v>
       </c>
       <c r="AK71" s="15">
         <f>IF(AA71="X",0,VLOOKUP(AA71,OPCODE_mult!$G$4:$L$19,6,FALSE))</f>
@@ -9635,20 +9626,20 @@
       </c>
       <c r="AN71" s="15">
         <f>IF(AD71="X",0,VLOOKUP(AD71,OPCODE_mult!$J$4:$L$19,3,FALSE))</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AO71" s="15" t="str">
         <f>DEC2BIN(SUM(AK71:AN71),4)</f>
-        <v>0000</v>
+        <v>0111</v>
       </c>
       <c r="AP71" s="15"/>
       <c r="AQ71" s="16" t="str">
         <f t="shared" si="36"/>
-        <v>00000000000000</v>
+        <v>00010010100111</v>
       </c>
       <c r="AR71" s="14">
         <f t="shared" ref="AR71:AR91" si="37">(BIN2DEC(AO71)+16*BIN2DEC(AJ71)+128*BIN2DEC(AI71)+512*BIN2DEC(AH71)+2048*BIN2DEC(AG71)+8192*BIN2DEC(AF71))</f>
-        <v>0</v>
+        <v>1191</v>
       </c>
       <c r="AT71" s="67"/>
       <c r="AU71" s="66" t="str">
@@ -10626,22 +10617,22 @@
         <f>IF(AC88="X",0,VLOOKUP(AC88,OPCODE_mult!$I$4:$L$19,4,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="AN88" s="48" t="e">
+      <c r="AN88" s="48">
         <f>IF(AD88="X",0,VLOOKUP(AD88,OPCODE_mult!$J$4:$L$19,3,FALSE))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AO88" s="48" t="e">
+        <v>7</v>
+      </c>
+      <c r="AO88" s="48" t="str">
         <f>DEC2BIN(SUM(AK88:AN88),4)</f>
-        <v>#N/A</v>
+        <v>0111</v>
       </c>
       <c r="AP88" s="48"/>
-      <c r="AQ88" s="22" t="e">
+      <c r="AQ88" s="22" t="str">
         <f t="shared" ref="AQ88:AQ92" si="50">AF88&amp;AG88&amp;AH88&amp;AI88&amp;AJ88&amp;AO88</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AR88" s="47" t="e">
+        <v>00010010100111</v>
+      </c>
+      <c r="AR88" s="47">
         <f t="shared" si="37"/>
-        <v>#N/A</v>
+        <v>1191</v>
       </c>
       <c r="AT88" s="53"/>
     </row>
@@ -10743,22 +10734,22 @@
         <f>IF(AC89="X",0,VLOOKUP(AC89,OPCODE_mult!$I$4:$L$19,4,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="AN89" s="48" t="e">
+      <c r="AN89" s="48">
         <f>IF(AD89="X",0,VLOOKUP(AD89,OPCODE_mult!$J$4:$L$19,3,FALSE))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AO89" s="48" t="e">
+        <v>7</v>
+      </c>
+      <c r="AO89" s="48" t="str">
         <f>DEC2BIN(SUM(AK89:AN89),4)</f>
-        <v>#N/A</v>
+        <v>0111</v>
       </c>
       <c r="AP89" s="48"/>
-      <c r="AQ89" s="22" t="e">
+      <c r="AQ89" s="22" t="str">
         <f t="shared" si="50"/>
-        <v>#N/A</v>
-      </c>
-      <c r="AR89" s="47" t="e">
+        <v>00000000100111</v>
+      </c>
+      <c r="AR89" s="47">
         <f t="shared" si="37"/>
-        <v>#N/A</v>
+        <v>39</v>
       </c>
       <c r="AT89" s="53"/>
     </row>
@@ -11207,8 +11198,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11487,8 +11478,8 @@
       <c r="I11" s="73" t="s">
         <v>189</v>
       </c>
-      <c r="J11" s="108" t="s">
-        <v>346</v>
+      <c r="J11" s="109" t="s">
+        <v>255</v>
       </c>
       <c r="K11" s="74" t="s">
         <v>201</v>
@@ -11510,9 +11501,7 @@
       </c>
       <c r="H12" s="64"/>
       <c r="I12" s="64"/>
-      <c r="J12" s="109" t="s">
-        <v>347</v>
-      </c>
+      <c r="J12" s="108"/>
       <c r="K12" s="78"/>
       <c r="L12" s="86">
         <v>8</v>
@@ -11531,9 +11520,7 @@
       </c>
       <c r="H13" s="64"/>
       <c r="I13" s="64"/>
-      <c r="J13" s="109" t="s">
-        <v>348</v>
-      </c>
+      <c r="J13" s="108"/>
       <c r="K13" s="78"/>
       <c r="L13" s="86">
         <v>9</v>

</xml_diff>

<commit_message>
Updated BRA and BEQ instructions to operate with wide instruction fetch -- execution time is still 3 cycles, 1 for decode and 2 to re-prime the pipeline (previously 2 for decode and 1 to re-prime the pipeline)
</commit_message>
<xml_diff>
--- a/Resources/Instruction Set.xlsx
+++ b/Resources/Instruction Set.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="120" windowWidth="18195" windowHeight="8250" tabRatio="681"/>
@@ -16,12 +16,12 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">OPCODE_encoding!$A$3:$L$92</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1361" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1361" uniqueCount="345">
   <si>
     <t>DUP</t>
   </si>
@@ -461,9 +461,6 @@
     <t>Reserved</t>
   </si>
   <si>
-    <t>RSD</t>
-  </si>
-  <si>
     <t>TOS (ALU)</t>
   </si>
   <si>
@@ -818,12 +815,6 @@
     <t>REPLACE</t>
   </si>
   <si>
-    <t>SDIVMODLD</t>
-  </si>
-  <si>
-    <t>UDIVMODLD</t>
-  </si>
-  <si>
     <t>RSdataOUT</t>
   </si>
   <si>
@@ -1059,13 +1050,19 @@
   </si>
   <si>
     <t>RSP!</t>
+  </si>
+  <si>
+    <t>UNUSED</t>
+  </si>
+  <si>
+    <t>JSI</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="33" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="33">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1759,7 +1756,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1794,7 +1790,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1970,20 +1965,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:AU98"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="9" ySplit="4" topLeftCell="AB58" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="9" ySplit="4" topLeftCell="J50" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="V71" sqref="V71:AD71"/>
+      <selection pane="bottomRight" activeCell="L84" sqref="L84"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="11.25"/>
   <cols>
     <col min="1" max="1" width="1.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="11" style="4" customWidth="1"/>
@@ -2017,26 +2012,26 @@
     <col min="48" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:47" ht="15">
       <c r="A1" s="46" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:47" ht="5.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="3" spans="1:47" s="23" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:47" ht="5.25" customHeight="1"/>
+    <row r="3" spans="1:47" s="23" customFormat="1">
       <c r="B3" s="7" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="24" t="s">
         <v>140</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="J3" s="7"/>
       <c r="K3" s="90" t="s">
@@ -2047,18 +2042,18 @@
       </c>
       <c r="M3" s="24"/>
       <c r="N3" s="20" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="O3" s="18"/>
       <c r="P3" s="18"/>
       <c r="Q3" s="18"/>
       <c r="R3" s="24"/>
       <c r="S3" s="20" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="T3" s="20"/>
       <c r="V3" s="20" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="W3" s="33"/>
       <c r="X3" s="33"/>
@@ -2069,7 +2064,7 @@
       <c r="AC3" s="33"/>
       <c r="AD3" s="33"/>
       <c r="AF3" s="20" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="AG3" s="33"/>
       <c r="AH3" s="33"/>
@@ -2081,15 +2076,15 @@
       <c r="AN3" s="33"/>
       <c r="AO3" s="33"/>
       <c r="AQ3" s="20" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="AR3" s="33"/>
       <c r="AT3" s="20" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="AU3" s="33"/>
     </row>
-    <row r="4" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:47">
       <c r="D4" s="7">
         <v>7</v>
       </c>
@@ -2109,7 +2104,7 @@
         <v>31</v>
       </c>
       <c r="P4" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="Q4" s="7" t="s">
         <v>36</v>
@@ -2121,81 +2116,81 @@
         <v>35</v>
       </c>
       <c r="V4" s="7" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="W4" s="7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="X4" s="7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="Y4" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="Z4" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="AA4" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="AB4" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="AC4" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="AD4" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="AF4" s="7" t="s">
+        <v>264</v>
+      </c>
+      <c r="AG4" s="7" t="s">
+        <v>248</v>
+      </c>
+      <c r="AH4" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="Z4" s="7" t="s">
+      <c r="AI4" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="AJ4" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="AK4" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="AL4" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="AM4" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="AN4" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="AO4" s="7" t="s">
         <v>238</v>
       </c>
-      <c r="AA4" s="7" t="s">
-        <v>236</v>
-      </c>
-      <c r="AB4" s="7" t="s">
-        <v>234</v>
-      </c>
-      <c r="AC4" s="7" t="s">
-        <v>235</v>
-      </c>
-      <c r="AD4" s="7" t="s">
-        <v>248</v>
-      </c>
-      <c r="AF4" s="7" t="s">
-        <v>267</v>
-      </c>
-      <c r="AG4" s="7" t="s">
-        <v>249</v>
-      </c>
-      <c r="AH4" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="AI4" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="AJ4" s="7" t="s">
-        <v>238</v>
-      </c>
-      <c r="AK4" s="7" t="s">
-        <v>236</v>
-      </c>
-      <c r="AL4" s="7" t="s">
-        <v>234</v>
-      </c>
-      <c r="AM4" s="7" t="s">
-        <v>235</v>
-      </c>
-      <c r="AN4" s="7" t="s">
-        <v>248</v>
-      </c>
-      <c r="AO4" s="7" t="s">
-        <v>239</v>
-      </c>
       <c r="AQ4" s="24" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="AR4" s="24" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="AT4" s="24" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="AU4" s="24" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="5" spans="1:47" x14ac:dyDescent="0.2">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="5" spans="1:47">
       <c r="A5" s="1" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="6" spans="1:47" x14ac:dyDescent="0.2">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="6" spans="1:47">
       <c r="B6" s="4" t="s">
         <v>41</v>
       </c>
@@ -2223,7 +2218,7 @@
         <v>132</v>
       </c>
       <c r="N6" s="11" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="O6" s="11" t="s">
         <v>31</v>
@@ -2253,7 +2248,7 @@
         <v>31</v>
       </c>
       <c r="Z6" s="11" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="AA6" s="11" t="s">
         <v>141</v>
@@ -2324,7 +2319,7 @@
         <v>," NOP"</v>
       </c>
     </row>
-    <row r="7" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:47">
       <c r="B7" s="4" t="s">
         <v>2</v>
       </c>
@@ -2353,7 +2348,7 @@
         <v>61</v>
       </c>
       <c r="N7" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="O7" s="4" t="s">
         <v>133</v>
@@ -2377,13 +2372,13 @@
         <v>35</v>
       </c>
       <c r="X7" s="11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="Y7" s="11" t="s">
         <v>133</v>
       </c>
       <c r="Z7" s="11" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="AA7" s="11" t="s">
         <v>141</v>
@@ -2454,7 +2449,7 @@
         <v>," DROP"</v>
       </c>
     </row>
-    <row r="8" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:47">
       <c r="B8" s="4" t="s">
         <v>0</v>
       </c>
@@ -2483,7 +2478,7 @@
         <v>58</v>
       </c>
       <c r="N8" s="11" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="O8" s="4" t="s">
         <v>30</v>
@@ -2507,13 +2502,13 @@
         <v>35</v>
       </c>
       <c r="X8" s="11" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="Y8" s="11" t="s">
         <v>30</v>
       </c>
       <c r="Z8" s="11" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="AA8" s="11" t="s">
         <v>141</v>
@@ -2584,7 +2579,7 @@
         <v>," DUP"</v>
       </c>
     </row>
-    <row r="9" spans="1:47" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:47" s="14" customFormat="1">
       <c r="B9" s="15" t="s">
         <v>1</v>
       </c>
@@ -2714,7 +2709,7 @@
         <v>," ?DUP"</v>
       </c>
     </row>
-    <row r="10" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:47">
       <c r="B10" s="4" t="s">
         <v>3</v>
       </c>
@@ -2743,7 +2738,7 @@
         <v>63</v>
       </c>
       <c r="N10" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="O10" s="4" t="s">
         <v>30</v>
@@ -2773,7 +2768,7 @@
         <v>30</v>
       </c>
       <c r="Z10" s="11" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="AA10" s="11" t="s">
         <v>141</v>
@@ -2844,7 +2839,7 @@
         <v>," SWAP"</v>
       </c>
     </row>
-    <row r="11" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:47">
       <c r="B11" s="4" t="s">
         <v>4</v>
       </c>
@@ -2873,7 +2868,7 @@
         <v>65</v>
       </c>
       <c r="N11" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="O11" s="4" t="s">
         <v>30</v>
@@ -2897,13 +2892,13 @@
         <v>35</v>
       </c>
       <c r="X11" s="11" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="Y11" s="11" t="s">
         <v>30</v>
       </c>
       <c r="Z11" s="11" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="AA11" s="11" t="s">
         <v>141</v>
@@ -2974,7 +2969,7 @@
         <v>," OVER"</v>
       </c>
     </row>
-    <row r="12" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:47">
       <c r="B12" s="4" t="s">
         <v>5</v>
       </c>
@@ -3003,7 +2998,7 @@
         <v>67</v>
       </c>
       <c r="N12" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="O12" s="4" t="s">
         <v>133</v>
@@ -3027,13 +3022,13 @@
         <v>35</v>
       </c>
       <c r="X12" s="11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="Y12" s="11" t="s">
         <v>133</v>
       </c>
       <c r="Z12" s="11" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="AA12" s="11" t="s">
         <v>141</v>
@@ -3104,7 +3099,7 @@
         <v>," NIP"</v>
       </c>
     </row>
-    <row r="13" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:47">
       <c r="B13" s="4" t="s">
         <v>6</v>
       </c>
@@ -3130,7 +3125,7 @@
         <v>68</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="N13" s="4" t="s">
         <v>133</v>
@@ -3163,7 +3158,7 @@
         <v>30</v>
       </c>
       <c r="Z13" s="11" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="AA13" s="11" t="s">
         <v>141</v>
@@ -3234,7 +3229,7 @@
         <v>," ROT"</v>
       </c>
     </row>
-    <row r="14" spans="1:47" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:47" s="3" customFormat="1">
       <c r="B14" s="11" t="s">
         <v>7</v>
       </c>
@@ -3267,7 +3262,7 @@
       </c>
       <c r="M14" s="12"/>
       <c r="N14" s="11" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="O14" s="11" t="s">
         <v>133</v>
@@ -3289,16 +3284,16 @@
         <v>30</v>
       </c>
       <c r="W14" s="11" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="X14" s="11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="Y14" s="11" t="s">
         <v>133</v>
       </c>
       <c r="Z14" s="11" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="AA14" s="11" t="s">
         <v>141</v>
@@ -3371,7 +3366,7 @@
         <v>," &gt;R"</v>
       </c>
     </row>
-    <row r="15" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:47">
       <c r="B15" s="4" t="s">
         <v>8</v>
       </c>
@@ -3424,13 +3419,13 @@
         <v>35</v>
       </c>
       <c r="X15" s="11" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="Y15" s="11" t="s">
         <v>30</v>
       </c>
       <c r="Z15" s="11" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="AA15" s="11" t="s">
         <v>141</v>
@@ -3442,7 +3437,7 @@
         <v>141</v>
       </c>
       <c r="AD15" s="11" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="AF15" s="11" t="str">
         <f>DEC2BIN(VLOOKUP(V15,OPCODE_mult!$C$4:$L$19,10,FALSE),1)</f>
@@ -3501,7 +3496,7 @@
         <v>," R@"</v>
       </c>
     </row>
-    <row r="16" spans="1:47" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:47" s="3" customFormat="1">
       <c r="B16" s="11" t="s">
         <v>9</v>
       </c>
@@ -3556,16 +3551,16 @@
         <v>30</v>
       </c>
       <c r="W16" s="11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="X16" s="11" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="Y16" s="11" t="s">
         <v>30</v>
       </c>
       <c r="Z16" s="11" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="AA16" s="11" t="s">
         <v>141</v>
@@ -3577,7 +3572,7 @@
         <v>141</v>
       </c>
       <c r="AD16" s="11" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="AE16" s="1"/>
       <c r="AF16" s="11" t="str">
@@ -3638,9 +3633,9 @@
         <v>," R&gt;"</v>
       </c>
     </row>
-    <row r="17" spans="1:47" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:47" s="3" customFormat="1">
       <c r="B17" s="11" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="C17" s="11"/>
       <c r="D17" s="11">
@@ -3664,10 +3659,10 @@
       </c>
       <c r="J17" s="11"/>
       <c r="K17" s="94" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="L17" s="3" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="M17" s="12"/>
       <c r="N17" s="11"/>
@@ -3684,13 +3679,13 @@
         <v>35</v>
       </c>
       <c r="X17" s="11" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="Y17" s="11" t="s">
         <v>30</v>
       </c>
       <c r="Z17" s="11" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="AA17" s="11" t="s">
         <v>141</v>
@@ -3763,9 +3758,9 @@
         <v>," PSP@"</v>
       </c>
     </row>
-    <row r="18" spans="1:47" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:47" s="3" customFormat="1">
       <c r="B18" s="11" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C18" s="11"/>
       <c r="D18" s="11">
@@ -3789,10 +3784,10 @@
       </c>
       <c r="J18" s="11"/>
       <c r="K18" s="94" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="L18" s="3" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="M18" s="12"/>
       <c r="N18" s="11"/>
@@ -3809,13 +3804,13 @@
         <v>35</v>
       </c>
       <c r="X18" s="11" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="Y18" s="11" t="s">
         <v>30</v>
       </c>
       <c r="Z18" s="11" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="AA18" s="11" t="s">
         <v>141</v>
@@ -3888,9 +3883,9 @@
         <v>," RSP@"</v>
       </c>
     </row>
-    <row r="19" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:47">
       <c r="B19" s="11" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="D19" s="4">
         <v>0</v>
@@ -3911,10 +3906,10 @@
         <v>D</v>
       </c>
       <c r="K19" s="89" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="Q19" s="6"/>
       <c r="S19" s="4"/>
@@ -3932,7 +3927,7 @@
         <v>133</v>
       </c>
       <c r="Z19" s="11" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="AA19" s="11" t="s">
         <v>141</v>
@@ -4003,9 +3998,9 @@
         <v>," PSP!"</v>
       </c>
     </row>
-    <row r="20" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:47">
       <c r="B20" s="11" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="D20" s="4">
         <v>0</v>
@@ -4026,10 +4021,10 @@
         <v>E</v>
       </c>
       <c r="K20" s="89" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="Q20" s="6"/>
       <c r="S20" s="4"/>
@@ -4041,13 +4036,13 @@
         <v>30</v>
       </c>
       <c r="X20" s="11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="Y20" s="4" t="s">
         <v>133</v>
       </c>
       <c r="Z20" s="11" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="AA20" s="11" t="s">
         <v>141</v>
@@ -4118,18 +4113,18 @@
         <v>," RSP!"</v>
       </c>
     </row>
-    <row r="21" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:47">
       <c r="AT21" s="66"/>
       <c r="AU21" s="66"/>
     </row>
-    <row r="22" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:47">
       <c r="A22" s="1" t="s">
         <v>10</v>
       </c>
       <c r="AT22" s="66"/>
       <c r="AU22" s="66"/>
     </row>
-    <row r="23" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:47">
       <c r="B23" s="6" t="s">
         <v>11</v>
       </c>
@@ -4183,19 +4178,19 @@
         <v>35</v>
       </c>
       <c r="X23" s="11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="Y23" s="11" t="s">
         <v>133</v>
       </c>
       <c r="Z23" s="11" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="AA23" s="11" t="s">
         <v>141</v>
       </c>
       <c r="AB23" s="11" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="AC23" s="11" t="s">
         <v>141</v>
@@ -4261,7 +4256,7 @@
         <v>," +"</v>
       </c>
     </row>
-    <row r="24" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:47">
       <c r="B24" s="6" t="s">
         <v>12</v>
       </c>
@@ -4315,19 +4310,19 @@
         <v>35</v>
       </c>
       <c r="X24" s="11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="Y24" s="11" t="s">
         <v>133</v>
       </c>
       <c r="Z24" s="11" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="AA24" s="11" t="s">
         <v>141</v>
       </c>
       <c r="AB24" s="11" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="AC24" s="11" t="s">
         <v>141</v>
@@ -4393,7 +4388,7 @@
         <v>," -"</v>
       </c>
     </row>
-    <row r="25" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:47">
       <c r="B25" s="4" t="s">
         <v>16</v>
       </c>
@@ -4452,7 +4447,7 @@
         <v>31</v>
       </c>
       <c r="Z25" s="11" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="AA25" s="11" t="s">
         <v>141</v>
@@ -4524,7 +4519,7 @@
         <v>," NEGATE"</v>
       </c>
     </row>
-    <row r="26" spans="1:47" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:47" s="3" customFormat="1">
       <c r="B26" s="11" t="s">
         <v>52</v>
       </c>
@@ -4588,7 +4583,7 @@
         <v>31</v>
       </c>
       <c r="Z26" s="11" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="AA26" s="11" t="s">
         <v>141</v>
@@ -4661,7 +4656,7 @@
         <v>," 1+"</v>
       </c>
     </row>
-    <row r="27" spans="1:47" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:47" s="3" customFormat="1">
       <c r="B27" s="13" t="s">
         <v>53</v>
       </c>
@@ -4725,7 +4720,7 @@
         <v>31</v>
       </c>
       <c r="Z27" s="11" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="AA27" s="11" t="s">
         <v>141</v>
@@ -4798,7 +4793,7 @@
         <v>," 1-"</v>
       </c>
     </row>
-    <row r="28" spans="1:47" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:47" s="3" customFormat="1">
       <c r="B28" s="13" t="s">
         <v>54</v>
       </c>
@@ -4862,7 +4857,7 @@
         <v>31</v>
       </c>
       <c r="Z28" s="11" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="AA28" s="11" t="s">
         <v>141</v>
@@ -4871,7 +4866,7 @@
         <v>141</v>
       </c>
       <c r="AC28" s="11" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="AD28" s="11" t="s">
         <v>141</v>
@@ -4935,7 +4930,7 @@
         <v>," 2*"</v>
       </c>
     </row>
-    <row r="29" spans="1:47" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:47" s="3" customFormat="1">
       <c r="B29" s="13" t="s">
         <v>55</v>
       </c>
@@ -4999,7 +4994,7 @@
         <v>31</v>
       </c>
       <c r="Z29" s="11" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="AA29" s="11" t="s">
         <v>141</v>
@@ -5008,7 +5003,7 @@
         <v>141</v>
       </c>
       <c r="AC29" s="11" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="AD29" s="11" t="s">
         <v>141</v>
@@ -5072,9 +5067,9 @@
         <v>," 2/"</v>
       </c>
     </row>
-    <row r="30" spans="1:47" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:47" s="3" customFormat="1">
       <c r="B30" s="11" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="C30" s="11"/>
       <c r="D30" s="11">
@@ -5098,17 +5093,17 @@
       </c>
       <c r="J30" s="11"/>
       <c r="K30" s="93" t="s">
+        <v>192</v>
+      </c>
+      <c r="L30" s="3" t="s">
         <v>193</v>
-      </c>
-      <c r="L30" s="3" t="s">
-        <v>194</v>
       </c>
       <c r="M30" s="12"/>
       <c r="N30" s="11" t="s">
         <v>125</v>
       </c>
       <c r="O30" s="11" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="P30" s="11" t="s">
         <v>34</v>
@@ -5118,7 +5113,7 @@
       </c>
       <c r="R30" s="12"/>
       <c r="S30" s="11" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="T30" s="13" t="s">
         <v>137</v>
@@ -5133,10 +5128,10 @@
         <v>36</v>
       </c>
       <c r="Y30" s="4" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="Z30" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="AA30" s="4" t="s">
         <v>141</v>
@@ -5209,9 +5204,9 @@
         <v>," MULTS"</v>
       </c>
     </row>
-    <row r="31" spans="1:47" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:47" s="3" customFormat="1">
       <c r="B31" s="11" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="C31" s="11"/>
       <c r="D31" s="11">
@@ -5245,7 +5240,7 @@
         <v>125</v>
       </c>
       <c r="O31" s="11" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="P31" s="11" t="s">
         <v>34</v>
@@ -5255,7 +5250,7 @@
       </c>
       <c r="R31" s="12"/>
       <c r="S31" s="11" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="T31" s="13" t="s">
         <v>137</v>
@@ -5270,10 +5265,10 @@
         <v>36</v>
       </c>
       <c r="Y31" s="4" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="Z31" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="AA31" s="4" t="s">
         <v>141</v>
@@ -5346,9 +5341,9 @@
         <v>," MULTU"</v>
       </c>
     </row>
-    <row r="32" spans="1:47" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:47" s="3" customFormat="1">
       <c r="B32" s="11" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C32" s="11"/>
       <c r="D32" s="11">
@@ -5375,7 +5370,7 @@
         <v>73</v>
       </c>
       <c r="L32" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="M32" s="12"/>
       <c r="N32" s="4" t="s">
@@ -5405,19 +5400,19 @@
         <v>35</v>
       </c>
       <c r="X32" s="11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="Y32" s="11" t="s">
         <v>133</v>
       </c>
       <c r="Z32" s="11" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="AA32" s="11" t="s">
         <v>141</v>
       </c>
       <c r="AB32" s="11" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="AC32" s="11" t="s">
         <v>141</v>
@@ -5484,9 +5479,9 @@
         <v>," ADDX"</v>
       </c>
     </row>
-    <row r="33" spans="1:47" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:47" s="3" customFormat="1">
       <c r="B33" s="11" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C33" s="11"/>
       <c r="D33" s="11">
@@ -5513,7 +5508,7 @@
         <v>73</v>
       </c>
       <c r="L33" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="M33" s="12"/>
       <c r="N33" s="4" t="s">
@@ -5543,19 +5538,19 @@
         <v>35</v>
       </c>
       <c r="X33" s="11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="Y33" s="11" t="s">
         <v>133</v>
       </c>
       <c r="Z33" s="11" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="AA33" s="11" t="s">
         <v>141</v>
       </c>
       <c r="AB33" s="11" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AC33" s="11" t="s">
         <v>141</v>
@@ -5622,9 +5617,9 @@
         <v>," SUBX"</v>
       </c>
     </row>
-    <row r="34" spans="1:47" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:47" s="14" customFormat="1">
       <c r="B34" s="15" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="C34" s="17"/>
       <c r="D34" s="15">
@@ -5648,17 +5643,17 @@
       </c>
       <c r="J34" s="17"/>
       <c r="K34" s="92" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="L34" s="14" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="M34" s="16"/>
       <c r="N34" s="15" t="s">
         <v>125</v>
       </c>
       <c r="O34" s="15" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="P34" s="15" t="s">
         <v>34</v>
@@ -5668,7 +5663,7 @@
       </c>
       <c r="R34" s="16"/>
       <c r="S34" s="15" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="T34" s="17" t="s">
         <v>137</v>
@@ -5755,8 +5750,7 @@
         <v>00000000000000</v>
       </c>
       <c r="AR34" s="14">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>480</v>
       </c>
       <c r="AT34" s="66" t="str">
         <f t="shared" si="13"/>
@@ -5767,9 +5761,9 @@
         <v>," DIVS"</v>
       </c>
     </row>
-    <row r="35" spans="1:47" s="14" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:47" s="14" customFormat="1" ht="14.25" customHeight="1">
       <c r="B35" s="15" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="C35" s="17"/>
       <c r="D35" s="15">
@@ -5793,17 +5787,17 @@
       </c>
       <c r="J35" s="17"/>
       <c r="K35" s="92" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="L35" s="14" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="M35" s="16"/>
       <c r="N35" s="15" t="s">
         <v>125</v>
       </c>
       <c r="O35" s="15" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="P35" s="15" t="s">
         <v>34</v>
@@ -5813,7 +5807,7 @@
       </c>
       <c r="R35" s="16"/>
       <c r="S35" s="15" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="T35" s="17" t="s">
         <v>137</v>
@@ -5900,8 +5894,7 @@
         <v>00000000000000</v>
       </c>
       <c r="AR35" s="14">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>496</v>
       </c>
       <c r="AT35" s="66" t="str">
         <f t="shared" si="13"/>
@@ -5912,12 +5905,12 @@
         <v>," DIVU"</v>
       </c>
     </row>
-    <row r="36" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:47">
       <c r="E36" s="13"/>
       <c r="AT36" s="66"/>
       <c r="AU36" s="66"/>
     </row>
-    <row r="37" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:47">
       <c r="A37" s="1" t="s">
         <v>17</v>
       </c>
@@ -5925,7 +5918,7 @@
       <c r="AT37" s="66"/>
       <c r="AU37" s="66"/>
     </row>
-    <row r="38" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:47">
       <c r="A38" s="4"/>
       <c r="B38" s="6" t="s">
         <v>20</v>
@@ -5980,13 +5973,13 @@
         <v>35</v>
       </c>
       <c r="X38" s="11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="Y38" s="11" t="s">
         <v>133</v>
       </c>
       <c r="Z38" s="11" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="AA38" s="11" t="str">
         <f t="shared" ref="AA38:AA48" si="19">B38</f>
@@ -6059,7 +6052,7 @@
         <v>," ="</v>
       </c>
     </row>
-    <row r="39" spans="1:47" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:47" s="3" customFormat="1">
       <c r="A39" s="4"/>
       <c r="B39" s="13" t="s">
         <v>44</v>
@@ -6118,13 +6111,13 @@
         <v>35</v>
       </c>
       <c r="X39" s="11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="Y39" s="11" t="s">
         <v>133</v>
       </c>
       <c r="Z39" s="11" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="AA39" s="11" t="str">
         <f t="shared" si="19"/>
@@ -6197,7 +6190,7 @@
         <v>," &lt;&gt;"</v>
       </c>
     </row>
-    <row r="40" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:47">
       <c r="A40" s="4"/>
       <c r="B40" s="6" t="s">
         <v>18</v>
@@ -6252,13 +6245,13 @@
         <v>35</v>
       </c>
       <c r="X40" s="11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="Y40" s="11" t="s">
         <v>133</v>
       </c>
       <c r="Z40" s="11" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="AA40" s="11" t="str">
         <f t="shared" si="19"/>
@@ -6331,7 +6324,7 @@
         <v>," &lt;"</v>
       </c>
     </row>
-    <row r="41" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:47">
       <c r="A41" s="4"/>
       <c r="B41" s="6" t="s">
         <v>19</v>
@@ -6386,13 +6379,13 @@
         <v>35</v>
       </c>
       <c r="X41" s="11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="Y41" s="11" t="s">
         <v>133</v>
       </c>
       <c r="Z41" s="11" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="AA41" s="11" t="str">
         <f t="shared" si="19"/>
@@ -6465,7 +6458,7 @@
         <v>," &gt;"</v>
       </c>
     </row>
-    <row r="42" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:47">
       <c r="A42" s="4"/>
       <c r="B42" s="6" t="s">
         <v>27</v>
@@ -6520,13 +6513,13 @@
         <v>35</v>
       </c>
       <c r="X42" s="11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="Y42" s="11" t="s">
         <v>133</v>
       </c>
       <c r="Z42" s="11" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="AA42" s="11" t="str">
         <f t="shared" si="19"/>
@@ -6599,7 +6592,7 @@
         <v>," U&lt;"</v>
       </c>
     </row>
-    <row r="43" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:47">
       <c r="A43" s="4"/>
       <c r="B43" s="6" t="s">
         <v>28</v>
@@ -6654,13 +6647,13 @@
         <v>35</v>
       </c>
       <c r="X43" s="11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="Y43" s="11" t="s">
         <v>133</v>
       </c>
       <c r="Z43" s="11" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="AA43" s="11" t="str">
         <f t="shared" si="19"/>
@@ -6733,7 +6726,7 @@
         <v>," U&gt;"</v>
       </c>
     </row>
-    <row r="44" spans="1:47" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:47" s="3" customFormat="1">
       <c r="A44" s="4"/>
       <c r="B44" s="13" t="s">
         <v>21</v>
@@ -6798,7 +6791,7 @@
         <v>31</v>
       </c>
       <c r="Z44" s="11" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="AA44" s="11" t="str">
         <f t="shared" si="19"/>
@@ -6871,10 +6864,10 @@
         <v>," 0="</v>
       </c>
     </row>
-    <row r="45" spans="1:47" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:47" s="3" customFormat="1">
       <c r="A45" s="4"/>
       <c r="B45" s="13" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="C45" s="11"/>
       <c r="D45" s="4">
@@ -6936,7 +6929,7 @@
         <v>31</v>
       </c>
       <c r="Z45" s="11" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="AA45" s="11" t="str">
         <f t="shared" si="19"/>
@@ -7009,10 +7002,10 @@
         <v>," 0&lt;&gt;"</v>
       </c>
     </row>
-    <row r="46" spans="1:47" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:47" s="3" customFormat="1">
       <c r="A46" s="4"/>
       <c r="B46" s="13" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="C46" s="11"/>
       <c r="D46" s="4">
@@ -7039,7 +7032,7 @@
         <v>89</v>
       </c>
       <c r="L46" s="3" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="M46" s="12"/>
       <c r="N46" s="4" t="s">
@@ -7074,7 +7067,7 @@
         <v>31</v>
       </c>
       <c r="Z46" s="11" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="AA46" s="11" t="str">
         <f t="shared" si="19"/>
@@ -7147,10 +7140,10 @@
         <v>," 0&lt;"</v>
       </c>
     </row>
-    <row r="47" spans="1:47" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:47" s="3" customFormat="1">
       <c r="A47" s="4"/>
       <c r="B47" s="6" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="C47" s="4"/>
       <c r="D47" s="4">
@@ -7177,7 +7170,7 @@
         <v>89</v>
       </c>
       <c r="L47" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="M47" s="12"/>
       <c r="N47" s="4" t="s">
@@ -7212,7 +7205,7 @@
         <v>31</v>
       </c>
       <c r="Z47" s="11" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="AA47" s="11" t="str">
         <f t="shared" si="19"/>
@@ -7285,7 +7278,7 @@
         <v>," 0&gt;"</v>
       </c>
     </row>
-    <row r="48" spans="1:47" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:47" s="3" customFormat="1">
       <c r="A48" s="4"/>
       <c r="B48" s="11" t="b">
         <v>0</v>
@@ -7312,10 +7305,10 @@
       </c>
       <c r="J48" s="11"/>
       <c r="K48" s="94" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="L48" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="M48" s="12"/>
       <c r="N48" s="4" t="s">
@@ -7344,13 +7337,13 @@
         <v>35</v>
       </c>
       <c r="X48" s="11" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="Y48" s="11" t="s">
         <v>30</v>
       </c>
       <c r="Z48" s="11" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="AA48" s="11" t="b">
         <f t="shared" si="19"/>
@@ -7423,12 +7416,12 @@
         <v>," FALSE"</v>
       </c>
     </row>
-    <row r="49" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:47">
       <c r="E49" s="13"/>
       <c r="AT49" s="66"/>
       <c r="AU49" s="66"/>
     </row>
-    <row r="50" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:47">
       <c r="A50" s="1" t="s">
         <v>22</v>
       </c>
@@ -7436,7 +7429,7 @@
       <c r="AT50" s="66"/>
       <c r="AU50" s="66"/>
     </row>
-    <row r="51" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:47">
       <c r="A51" s="4"/>
       <c r="B51" s="4" t="s">
         <v>23</v>
@@ -7490,13 +7483,13 @@
         <v>35</v>
       </c>
       <c r="X51" s="11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="Y51" s="11" t="s">
         <v>133</v>
       </c>
       <c r="Z51" s="11" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="AA51" s="11" t="s">
         <v>141</v>
@@ -7569,7 +7562,7 @@
         <v>," AND"</v>
       </c>
     </row>
-    <row r="52" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:47">
       <c r="A52" s="4"/>
       <c r="B52" s="4" t="s">
         <v>24</v>
@@ -7623,13 +7616,13 @@
         <v>35</v>
       </c>
       <c r="X52" s="11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="Y52" s="11" t="s">
         <v>133</v>
       </c>
       <c r="Z52" s="11" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="AA52" s="11" t="s">
         <v>141</v>
@@ -7702,7 +7695,7 @@
         <v>," OR"</v>
       </c>
     </row>
-    <row r="53" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:47">
       <c r="A53" s="4"/>
       <c r="B53" s="4" t="s">
         <v>26</v>
@@ -7762,7 +7755,7 @@
         <v>31</v>
       </c>
       <c r="Z53" s="11" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="AA53" s="11" t="s">
         <v>141</v>
@@ -7835,7 +7828,7 @@
         <v>," INVERT"</v>
       </c>
     </row>
-    <row r="54" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:47">
       <c r="A54" s="4"/>
       <c r="B54" s="4" t="s">
         <v>25</v>
@@ -7889,13 +7882,13 @@
         <v>35</v>
       </c>
       <c r="X54" s="11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="Y54" s="11" t="s">
         <v>133</v>
       </c>
       <c r="Z54" s="11" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="AA54" s="11" t="s">
         <v>141</v>
@@ -7968,7 +7961,7 @@
         <v>," XOR"</v>
       </c>
     </row>
-    <row r="55" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:47">
       <c r="A55" s="4"/>
       <c r="B55" s="4" t="s">
         <v>128</v>
@@ -8028,7 +8021,7 @@
         <v>31</v>
       </c>
       <c r="Z55" s="11" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="AA55" s="11" t="s">
         <v>141</v>
@@ -8101,7 +8094,7 @@
         <v>," LSL"</v>
       </c>
     </row>
-    <row r="56" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:47">
       <c r="A56" s="4"/>
       <c r="B56" s="4" t="s">
         <v>127</v>
@@ -8161,7 +8154,7 @@
         <v>31</v>
       </c>
       <c r="Z56" s="11" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="AA56" s="11" t="s">
         <v>141</v>
@@ -8234,10 +8227,10 @@
         <v>," LSR"</v>
       </c>
     </row>
-    <row r="57" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:47">
       <c r="A57" s="4"/>
       <c r="B57" s="4" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D57" s="4">
         <v>0</v>
@@ -8261,7 +8254,7 @@
         <v>129</v>
       </c>
       <c r="L57" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="N57" s="4" t="s">
         <v>125</v>
@@ -8294,7 +8287,7 @@
         <v>31</v>
       </c>
       <c r="Z57" s="11" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="AA57" s="11" t="s">
         <v>141</v>
@@ -8367,10 +8360,10 @@
         <v>," XBYTE"</v>
       </c>
     </row>
-    <row r="58" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:47">
       <c r="A58" s="4"/>
       <c r="B58" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D58" s="4">
         <v>0</v>
@@ -8394,7 +8387,7 @@
         <v>129</v>
       </c>
       <c r="L58" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="N58" s="4" t="s">
         <v>125</v>
@@ -8427,7 +8420,7 @@
         <v>31</v>
       </c>
       <c r="Z58" s="11" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="AA58" s="11" t="s">
         <v>141</v>
@@ -8500,12 +8493,12 @@
         <v>," XWORD"</v>
       </c>
     </row>
-    <row r="59" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:47">
       <c r="E59" s="13"/>
       <c r="AT59" s="66"/>
       <c r="AU59" s="66"/>
     </row>
-    <row r="60" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:47">
       <c r="A60" s="1" t="s">
         <v>29</v>
       </c>
@@ -8513,9 +8506,9 @@
       <c r="AT60" s="66"/>
       <c r="AU60" s="66"/>
     </row>
-    <row r="61" spans="1:47" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:47" s="14" customFormat="1">
       <c r="B61" s="15" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="C61" s="15"/>
       <c r="D61" s="15">
@@ -8565,7 +8558,7 @@
         <v>31</v>
       </c>
       <c r="Z61" s="15" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="AA61" s="15" t="s">
         <v>141</v>
@@ -8637,9 +8630,9 @@
         <v>," FETCH.L"</v>
       </c>
     </row>
-    <row r="62" spans="1:47" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:47" s="14" customFormat="1">
       <c r="B62" s="15" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C62" s="15"/>
       <c r="D62" s="15">
@@ -8689,7 +8682,7 @@
         <v>31</v>
       </c>
       <c r="Z62" s="15" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="AA62" s="15" t="s">
         <v>141</v>
@@ -8761,9 +8754,9 @@
         <v>," STORE.L"</v>
       </c>
     </row>
-    <row r="63" spans="1:47" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:47" s="14" customFormat="1">
       <c r="B63" s="15" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="C63" s="15"/>
       <c r="D63" s="15">
@@ -8813,7 +8806,7 @@
         <v>31</v>
       </c>
       <c r="Z63" s="15" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="AA63" s="15" t="s">
         <v>141</v>
@@ -8884,9 +8877,9 @@
         <v>," FETCH.W"</v>
       </c>
     </row>
-    <row r="64" spans="1:47" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:47" s="14" customFormat="1">
       <c r="B64" s="15" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="C64" s="15"/>
       <c r="D64" s="15">
@@ -8936,7 +8929,7 @@
         <v>31</v>
       </c>
       <c r="Z64" s="15" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="AA64" s="15" t="s">
         <v>141</v>
@@ -9007,9 +9000,9 @@
         <v>," STORE.W"</v>
       </c>
     </row>
-    <row r="65" spans="1:47" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:47" s="14" customFormat="1">
       <c r="B65" s="15" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="C65" s="15"/>
       <c r="D65" s="15">
@@ -9059,7 +9052,7 @@
         <v>31</v>
       </c>
       <c r="Z65" s="15" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="AA65" s="15" t="s">
         <v>141</v>
@@ -9071,7 +9064,7 @@
         <v>141</v>
       </c>
       <c r="AD65" s="15" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="AF65" s="15" t="str">
         <f>DEC2BIN(VLOOKUP(V65,OPCODE_mult!$C$4:$L$19,10,FALSE),1)</f>
@@ -9130,9 +9123,9 @@
         <v>," FETCH.B"</v>
       </c>
     </row>
-    <row r="66" spans="1:47" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:47" s="14" customFormat="1">
       <c r="B66" s="15" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="C66" s="15"/>
       <c r="D66" s="15">
@@ -9176,13 +9169,13 @@
         <v>35</v>
       </c>
       <c r="X66" s="15" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="Y66" s="15" t="s">
         <v>133</v>
       </c>
       <c r="Z66" s="15" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="AA66" s="15" t="s">
         <v>141</v>
@@ -9253,7 +9246,7 @@
         <v>," STORE.B"</v>
       </c>
     </row>
-    <row r="67" spans="1:47" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:47" s="2" customFormat="1">
       <c r="B67" s="5"/>
       <c r="C67" s="5"/>
       <c r="D67" s="4"/>
@@ -9277,31 +9270,29 @@
       <c r="AT67" s="67"/>
       <c r="AU67" s="66"/>
     </row>
-    <row r="68" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:47">
       <c r="A68" s="1" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="AQ68" s="16"/>
       <c r="AR68" s="14"/>
       <c r="AT68" s="67"/>
       <c r="AU68" s="66"/>
     </row>
-    <row r="69" spans="1:47" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B69" s="15" t="s">
-        <v>312</v>
-      </c>
-      <c r="C69" s="15"/>
-      <c r="D69" s="15">
-        <v>0</v>
-      </c>
-      <c r="E69" s="17">
-        <v>0</v>
-      </c>
-      <c r="F69" s="15">
+    <row r="69" spans="1:47">
+      <c r="B69" s="4" t="s">
+        <v>309</v>
+      </c>
+      <c r="D69" s="4">
+        <v>0</v>
+      </c>
+      <c r="E69" s="6">
+        <v>0</v>
+      </c>
+      <c r="F69" s="4">
         <f>F66+1</f>
         <v>53</v>
       </c>
-      <c r="G69" s="15"/>
       <c r="H69" s="7">
         <f>F69+E69*64+D69*128</f>
         <v>53</v>
@@ -9310,119 +9301,111 @@
         <f>DEC2HEX(H69)</f>
         <v>35</v>
       </c>
-      <c r="J69" s="15"/>
-      <c r="K69" s="96" t="s">
+      <c r="K69" s="91" t="s">
         <v>115</v>
       </c>
-      <c r="L69" s="14" t="s">
-        <v>217</v>
-      </c>
-      <c r="M69" s="16"/>
-      <c r="N69" s="15"/>
-      <c r="O69" s="15"/>
-      <c r="P69" s="15"/>
-      <c r="Q69" s="17"/>
-      <c r="R69" s="16"/>
-      <c r="S69" s="15"/>
-      <c r="T69" s="17"/>
-      <c r="V69" s="15" t="s">
+      <c r="L69" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="Q69" s="6"/>
+      <c r="S69" s="4"/>
+      <c r="T69" s="6"/>
+      <c r="V69" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="W69" s="15" t="s">
+      <c r="W69" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="X69" s="15" t="s">
-        <v>152</v>
-      </c>
-      <c r="Y69" s="15" t="s">
+      <c r="X69" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="Y69" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="Z69" s="15" t="s">
-        <v>248</v>
-      </c>
-      <c r="AA69" s="15" t="s">
-        <v>141</v>
-      </c>
-      <c r="AB69" s="15" t="s">
-        <v>141</v>
-      </c>
-      <c r="AC69" s="15" t="s">
-        <v>141</v>
-      </c>
-      <c r="AD69" s="15" t="s">
-        <v>255</v>
-      </c>
-      <c r="AF69" s="15" t="str">
+      <c r="Z69" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="AA69" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="AB69" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="AC69" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="AD69" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="AF69" s="4" t="str">
         <f>DEC2BIN(VLOOKUP(V69,OPCODE_mult!$C$4:$L$19,10,FALSE),1)</f>
         <v>0</v>
       </c>
-      <c r="AG69" s="15" t="str">
+      <c r="AG69" s="4" t="str">
         <f>DEC2BIN(VLOOKUP(W69,OPCODE_mult!$F$4:$L$19,7,FALSE),2)</f>
         <v>00</v>
       </c>
-      <c r="AH69" s="15" t="str">
+      <c r="AH69" s="4" t="str">
         <f>DEC2BIN(VLOOKUP(X69,OPCODE_mult!$E$4:$L$19,8,FALSE),2)</f>
         <v>10</v>
       </c>
-      <c r="AI69" s="15" t="str">
+      <c r="AI69" s="4" t="str">
         <f>DEC2BIN(VLOOKUP(Y69,OPCODE_mult!$D$4:$L$19,9,FALSE),2)</f>
         <v>01</v>
       </c>
-      <c r="AJ69" s="15" t="str">
+      <c r="AJ69" s="4" t="str">
         <f>DEC2BIN(IF(Z69="X",0,VLOOKUP(Z69,OPCODE_mult!$K$4:$L$19,2,FALSE)),3)</f>
         <v>010</v>
       </c>
-      <c r="AK69" s="15">
+      <c r="AK69" s="4">
         <f>IF(AA69="X",0,VLOOKUP(AA69,OPCODE_mult!$G$4:$L$19,6,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="AL69" s="15">
+      <c r="AL69" s="4">
         <f>IF(AB69="X",0,VLOOKUP(AB69,OPCODE_mult!$H$4:$L$19,5,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="AM69" s="15">
+      <c r="AM69" s="4">
         <f>IF(AC69="X",0,VLOOKUP(AC69,OPCODE_mult!$I$4:$L$19,4,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="AN69" s="15">
+      <c r="AN69" s="4">
         <f>IF(AD69="X",0,VLOOKUP(AD69,OPCODE_mult!$J$4:$L$19,3,FALSE))</f>
         <v>7</v>
       </c>
-      <c r="AO69" s="15" t="str">
+      <c r="AO69" s="4" t="str">
         <f>DEC2BIN(SUM(AK69:AN69),4)</f>
         <v>0111</v>
       </c>
-      <c r="AP69" s="15"/>
-      <c r="AQ69" s="16" t="str">
+      <c r="AP69" s="4"/>
+      <c r="AQ69" s="8" t="str">
         <f t="shared" ref="AQ69:AQ71" si="36">AF69&amp;AG69&amp;AH69&amp;AI69&amp;AJ69&amp;AO69</f>
         <v>00010010100111</v>
       </c>
-      <c r="AR69" s="14">
+      <c r="AR69" s="1">
         <f t="shared" si="3"/>
         <v>1191</v>
       </c>
-      <c r="AT69" s="67"/>
+      <c r="AT69" s="66"/>
       <c r="AU69" s="66" t="str">
         <f t="shared" si="5"/>
         <v>," #.B"</v>
       </c>
     </row>
-    <row r="70" spans="1:47" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B70" s="15" t="s">
-        <v>311</v>
-      </c>
-      <c r="C70" s="15"/>
-      <c r="D70" s="15">
-        <v>0</v>
-      </c>
-      <c r="E70" s="17">
-        <v>0</v>
-      </c>
-      <c r="F70" s="15">
+    <row r="70" spans="1:47">
+      <c r="B70" s="4" t="s">
+        <v>308</v>
+      </c>
+      <c r="D70" s="4">
+        <v>0</v>
+      </c>
+      <c r="E70" s="6">
+        <v>0</v>
+      </c>
+      <c r="F70" s="4">
         <f>F69+1</f>
         <v>54</v>
       </c>
-      <c r="G70" s="15"/>
       <c r="H70" s="7">
         <f>F70+E70*64+D70*128</f>
         <v>54</v>
@@ -9431,106 +9414,100 @@
         <f>DEC2HEX(H70)</f>
         <v>36</v>
       </c>
-      <c r="J70" s="15"/>
-      <c r="K70" s="96" t="s">
+      <c r="K70" s="91" t="s">
         <v>115</v>
       </c>
-      <c r="L70" s="14" t="s">
-        <v>218</v>
-      </c>
-      <c r="M70" s="16"/>
-      <c r="N70" s="15"/>
-      <c r="O70" s="15"/>
-      <c r="P70" s="15"/>
-      <c r="Q70" s="17"/>
-      <c r="R70" s="16"/>
-      <c r="S70" s="15"/>
-      <c r="T70" s="17"/>
-      <c r="V70" s="15" t="s">
+      <c r="L70" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="Q70" s="6"/>
+      <c r="S70" s="4"/>
+      <c r="T70" s="6"/>
+      <c r="V70" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="W70" s="15" t="s">
+      <c r="W70" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="X70" s="15" t="s">
-        <v>152</v>
-      </c>
-      <c r="Y70" s="15" t="s">
+      <c r="X70" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="Y70" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="Z70" s="15" t="s">
-        <v>248</v>
-      </c>
-      <c r="AA70" s="15" t="s">
-        <v>141</v>
-      </c>
-      <c r="AB70" s="15" t="s">
-        <v>141</v>
-      </c>
-      <c r="AC70" s="15" t="s">
-        <v>141</v>
-      </c>
-      <c r="AD70" s="15" t="s">
-        <v>255</v>
-      </c>
-      <c r="AF70" s="15" t="str">
+      <c r="Z70" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="AA70" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="AB70" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="AC70" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="AD70" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="AF70" s="4" t="str">
         <f>DEC2BIN(VLOOKUP(V70,OPCODE_mult!$C$4:$L$19,10,FALSE),1)</f>
         <v>0</v>
       </c>
-      <c r="AG70" s="15" t="str">
+      <c r="AG70" s="4" t="str">
         <f>DEC2BIN(VLOOKUP(W70,OPCODE_mult!$F$4:$L$19,7,FALSE),2)</f>
         <v>00</v>
       </c>
-      <c r="AH70" s="15" t="str">
+      <c r="AH70" s="4" t="str">
         <f>DEC2BIN(VLOOKUP(X70,OPCODE_mult!$E$4:$L$19,8,FALSE),2)</f>
         <v>10</v>
       </c>
-      <c r="AI70" s="15" t="str">
+      <c r="AI70" s="4" t="str">
         <f>DEC2BIN(VLOOKUP(Y70,OPCODE_mult!$D$4:$L$19,9,FALSE),2)</f>
         <v>01</v>
       </c>
-      <c r="AJ70" s="15" t="str">
+      <c r="AJ70" s="4" t="str">
         <f>DEC2BIN(IF(Z70="X",0,VLOOKUP(Z70,OPCODE_mult!$K$4:$L$19,2,FALSE)),3)</f>
         <v>010</v>
       </c>
-      <c r="AK70" s="15">
+      <c r="AK70" s="4">
         <f>IF(AA70="X",0,VLOOKUP(AA70,OPCODE_mult!$G$4:$L$19,6,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="AL70" s="15">
+      <c r="AL70" s="4">
         <f>IF(AB70="X",0,VLOOKUP(AB70,OPCODE_mult!$H$4:$L$19,5,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="AM70" s="15">
+      <c r="AM70" s="4">
         <f>IF(AC70="X",0,VLOOKUP(AC70,OPCODE_mult!$I$4:$L$19,4,FALSE))</f>
         <v>0</v>
       </c>
-      <c r="AN70" s="15">
+      <c r="AN70" s="4">
         <f>IF(AD70="X",0,VLOOKUP(AD70,OPCODE_mult!$J$4:$L$19,3,FALSE))</f>
         <v>7</v>
       </c>
-      <c r="AO70" s="15" t="str">
+      <c r="AO70" s="4" t="str">
         <f>DEC2BIN(SUM(AK70:AN70),4)</f>
         <v>0111</v>
       </c>
-      <c r="AP70" s="15"/>
-      <c r="AQ70" s="16" t="str">
+      <c r="AP70" s="4"/>
+      <c r="AQ70" s="8" t="str">
         <f t="shared" si="36"/>
         <v>00010010100111</v>
       </c>
-      <c r="AR70" s="14">
+      <c r="AR70" s="1">
         <f t="shared" si="3"/>
         <v>1191</v>
       </c>
-      <c r="AT70" s="67"/>
+      <c r="AT70" s="66"/>
       <c r="AU70" s="66" t="str">
         <f t="shared" si="5"/>
         <v>," #.W"</v>
       </c>
     </row>
-    <row r="71" spans="1:47" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:47" s="14" customFormat="1">
       <c r="B71" s="15" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="C71" s="15"/>
       <c r="D71" s="15">
@@ -9572,13 +9549,13 @@
         <v>35</v>
       </c>
       <c r="X71" s="15" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="Y71" s="15" t="s">
         <v>30</v>
       </c>
       <c r="Z71" s="15" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="AA71" s="15" t="s">
         <v>141</v>
@@ -9590,7 +9567,7 @@
         <v>141</v>
       </c>
       <c r="AD71" s="15" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="AF71" s="15" t="str">
         <f>DEC2BIN(VLOOKUP(V71,OPCODE_mult!$C$4:$L$19,10,FALSE),1)</f>
@@ -9647,13 +9624,13 @@
         <v>," #.L"</v>
       </c>
     </row>
-    <row r="72" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:47">
       <c r="S72" s="4"/>
       <c r="T72" s="4"/>
       <c r="AT72" s="66"/>
       <c r="AU72" s="66"/>
     </row>
-    <row r="73" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:47">
       <c r="A73" s="1" t="s">
         <v>47</v>
       </c>
@@ -9662,7 +9639,7 @@
       <c r="AT73" s="66"/>
       <c r="AU73" s="66"/>
     </row>
-    <row r="74" spans="1:47" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:47" s="3" customFormat="1">
       <c r="B74" s="11" t="s">
         <v>51</v>
       </c>
@@ -9688,14 +9665,14 @@
       </c>
       <c r="J74" s="11"/>
       <c r="K74" s="94" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="L74" s="3" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="M74" s="12"/>
       <c r="N74" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="O74" s="4" t="s">
         <v>31</v>
@@ -9807,9 +9784,9 @@
         <v>," JMP"</v>
       </c>
     </row>
-    <row r="75" spans="1:47" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:47" s="3" customFormat="1">
       <c r="B75" s="11" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C75" s="11"/>
       <c r="D75" s="11">
@@ -9833,10 +9810,10 @@
       </c>
       <c r="J75" s="11"/>
       <c r="K75" s="93" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="L75" s="3" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="M75" s="12"/>
       <c r="N75" s="11"/>
@@ -9847,10 +9824,10 @@
       <c r="S75" s="11"/>
       <c r="T75" s="13"/>
       <c r="V75" s="11" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="W75" s="11" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="X75" s="11" t="str">
         <f>X7</f>
@@ -9938,7 +9915,7 @@
         <v>," BSR"</v>
       </c>
     </row>
-    <row r="76" spans="1:47" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:47" s="3" customFormat="1">
       <c r="B76" s="11" t="s">
         <v>50</v>
       </c>
@@ -9964,14 +9941,14 @@
       </c>
       <c r="J76" s="11"/>
       <c r="K76" s="93" t="s">
+        <v>268</v>
+      </c>
+      <c r="L76" s="3" t="s">
         <v>271</v>
-      </c>
-      <c r="L76" s="3" t="s">
-        <v>274</v>
       </c>
       <c r="M76" s="12"/>
       <c r="N76" s="11" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="O76" s="11" t="s">
         <v>31</v>
@@ -9990,10 +9967,10 @@
         <v>32</v>
       </c>
       <c r="V76" s="11" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="W76" s="11" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="X76" s="11" t="str">
         <f>X7</f>
@@ -10081,9 +10058,9 @@
         <v>," JSR"</v>
       </c>
     </row>
-    <row r="77" spans="1:47" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:47" s="14" customFormat="1">
       <c r="B77" s="15" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="C77" s="15"/>
       <c r="D77" s="15">
@@ -10113,7 +10090,7 @@
       </c>
       <c r="M77" s="16"/>
       <c r="N77" s="15" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="O77" s="15" t="s">
         <v>31</v>
@@ -10158,7 +10135,7 @@
       </c>
       <c r="AU77" s="67"/>
     </row>
-    <row r="78" spans="1:47" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:47" s="14" customFormat="1">
       <c r="B78" s="15" t="s">
         <v>48</v>
       </c>
@@ -10220,7 +10197,7 @@
       <c r="AT78" s="66"/>
       <c r="AU78" s="67"/>
     </row>
-    <row r="79" spans="1:47" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:47" s="14" customFormat="1">
       <c r="B79" s="15" t="s">
         <v>49</v>
       </c>
@@ -10264,7 +10241,7 @@
       <c r="AT79" s="66"/>
       <c r="AU79" s="67"/>
     </row>
-    <row r="80" spans="1:47" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:47" s="14" customFormat="1">
       <c r="B80" s="15"/>
       <c r="C80" s="15"/>
       <c r="D80" s="15"/>
@@ -10289,9 +10266,9 @@
       <c r="AT80" s="66"/>
       <c r="AU80" s="67"/>
     </row>
-    <row r="81" spans="1:47" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:47" s="14" customFormat="1">
       <c r="A81" s="3" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="B81" s="15"/>
       <c r="C81" s="15"/>
@@ -10317,9 +10294,9 @@
       <c r="AT81" s="66"/>
       <c r="AU81" s="67"/>
     </row>
-    <row r="82" spans="1:47" s="57" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:47" s="57" customFormat="1">
       <c r="B82" s="58" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="C82" s="58"/>
       <c r="D82" s="58"/>
@@ -10340,7 +10317,7 @@
       <c r="J82" s="58"/>
       <c r="K82" s="97"/>
       <c r="L82" s="57" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="M82" s="60"/>
       <c r="N82" s="58"/>
@@ -10358,9 +10335,9 @@
       </c>
       <c r="AU82" s="69"/>
     </row>
-    <row r="83" spans="1:47" s="57" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:47" s="57" customFormat="1">
       <c r="B83" s="58" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="C83" s="58"/>
       <c r="D83" s="58"/>
@@ -10381,7 +10358,7 @@
       <c r="J83" s="58"/>
       <c r="K83" s="97"/>
       <c r="L83" s="57" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="M83" s="60"/>
       <c r="N83" s="58"/>
@@ -10399,9 +10376,9 @@
       </c>
       <c r="AU83" s="69"/>
     </row>
-    <row r="84" spans="1:47" s="57" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:47" s="57" customFormat="1">
       <c r="B84" s="58" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="C84" s="58"/>
       <c r="D84" s="58"/>
@@ -10422,7 +10399,7 @@
       <c r="J84" s="58"/>
       <c r="K84" s="97"/>
       <c r="L84" s="57" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="M84" s="60"/>
       <c r="N84" s="58"/>
@@ -10440,7 +10417,7 @@
       </c>
       <c r="AU84" s="69"/>
     </row>
-    <row r="85" spans="1:47" s="57" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:47" s="57" customFormat="1">
       <c r="B85" s="58"/>
       <c r="C85" s="58"/>
       <c r="D85" s="58"/>
@@ -10471,7 +10448,7 @@
       <c r="AQ85" s="60"/>
       <c r="AT85" s="62"/>
     </row>
-    <row r="86" spans="1:47" s="57" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:47" s="57" customFormat="1">
       <c r="B86" s="58"/>
       <c r="C86" s="58"/>
       <c r="D86" s="58"/>
@@ -10493,7 +10470,7 @@
       <c r="AQ86" s="60"/>
       <c r="AT86" s="62"/>
     </row>
-    <row r="87" spans="1:47" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:47" s="3" customFormat="1">
       <c r="A87" s="3" t="s">
         <v>145</v>
       </c>
@@ -10519,9 +10496,9 @@
       <c r="AR87" s="1"/>
       <c r="AT87" s="53"/>
     </row>
-    <row r="88" spans="1:47" s="47" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:47" s="47" customFormat="1">
       <c r="B88" s="48" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C88" s="48"/>
       <c r="D88" s="48">
@@ -10548,7 +10525,7 @@
         <v>115</v>
       </c>
       <c r="L88" s="47" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="M88" s="22"/>
       <c r="N88" s="48"/>
@@ -10565,13 +10542,13 @@
         <v>35</v>
       </c>
       <c r="X88" s="48" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="Y88" s="48" t="s">
         <v>30</v>
       </c>
       <c r="Z88" s="48" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="AA88" s="48" t="s">
         <v>141</v>
@@ -10583,7 +10560,7 @@
         <v>141</v>
       </c>
       <c r="AD88" s="48" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="AF88" s="11" t="str">
         <f>DEC2BIN(VLOOKUP(V88,OPCODE_mult!$C$4:$L$19,10,FALSE),1)</f>
@@ -10636,9 +10613,9 @@
       </c>
       <c r="AT88" s="53"/>
     </row>
-    <row r="89" spans="1:47" s="47" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:47" s="47" customFormat="1">
       <c r="B89" s="48" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C89" s="48"/>
       <c r="D89" s="48">
@@ -10665,7 +10642,7 @@
         <v>96</v>
       </c>
       <c r="L89" s="47" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="M89" s="22"/>
       <c r="N89" s="48"/>
@@ -10688,7 +10665,7 @@
         <v>31</v>
       </c>
       <c r="Z89" s="48" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="AA89" s="48" t="s">
         <v>141</v>
@@ -10700,7 +10677,7 @@
         <v>141</v>
       </c>
       <c r="AD89" s="48" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="AF89" s="11" t="str">
         <f>DEC2BIN(VLOOKUP(V89,OPCODE_mult!$C$4:$L$19,10,FALSE),1)</f>
@@ -10753,9 +10730,9 @@
       </c>
       <c r="AT89" s="53"/>
     </row>
-    <row r="90" spans="1:47" s="47" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:47" s="47" customFormat="1">
       <c r="B90" s="48" t="s">
-        <v>265</v>
+        <v>343</v>
       </c>
       <c r="C90" s="48"/>
       <c r="D90" s="48">
@@ -10779,17 +10756,17 @@
       </c>
       <c r="J90" s="49"/>
       <c r="K90" s="99" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="L90" s="47" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="M90" s="22"/>
       <c r="N90" s="48" t="s">
         <v>125</v>
       </c>
       <c r="O90" s="48" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="P90" s="48" t="s">
         <v>34</v>
@@ -10799,7 +10776,7 @@
       </c>
       <c r="R90" s="22"/>
       <c r="S90" s="48" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="T90" s="49" t="s">
         <v>137</v>
@@ -10814,10 +10791,10 @@
         <v>36</v>
       </c>
       <c r="Y90" s="48" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="Z90" s="48" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="AA90" s="48" t="s">
         <v>141</v>
@@ -10882,9 +10859,9 @@
       </c>
       <c r="AT90" s="53"/>
     </row>
-    <row r="91" spans="1:47" s="47" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:47" s="47" customFormat="1" ht="14.25" customHeight="1">
       <c r="B91" s="48" t="s">
-        <v>266</v>
+        <v>343</v>
       </c>
       <c r="C91" s="48"/>
       <c r="D91" s="48">
@@ -10908,17 +10885,17 @@
       </c>
       <c r="J91" s="49"/>
       <c r="K91" s="99" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="L91" s="47" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="M91" s="22"/>
       <c r="N91" s="48" t="s">
         <v>125</v>
       </c>
       <c r="O91" s="48" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="P91" s="48" t="s">
         <v>34</v>
@@ -10928,7 +10905,7 @@
       </c>
       <c r="R91" s="22"/>
       <c r="S91" s="48" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="T91" s="49" t="s">
         <v>137</v>
@@ -10943,10 +10920,10 @@
         <v>36</v>
       </c>
       <c r="Y91" s="48" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="Z91" s="48" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="AA91" s="48" t="s">
         <v>141</v>
@@ -11011,9 +10988,9 @@
       </c>
       <c r="AT91" s="53"/>
     </row>
-    <row r="92" spans="1:47" s="47" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:47" s="47" customFormat="1">
       <c r="B92" s="48" t="s">
-        <v>146</v>
+        <v>344</v>
       </c>
       <c r="C92" s="48"/>
       <c r="D92" s="48">
@@ -11036,14 +11013,14 @@
       </c>
       <c r="J92" s="48"/>
       <c r="K92" s="98" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="L92" s="47" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="M92" s="22"/>
       <c r="N92" s="48" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="O92" s="48" t="s">
         <v>31</v>
@@ -11062,10 +11039,10 @@
         <v>0</v>
       </c>
       <c r="V92" s="48" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="W92" s="48" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="X92" s="48" t="s">
         <v>36</v>
@@ -11074,7 +11051,7 @@
         <v>31</v>
       </c>
       <c r="Z92" s="48" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="AA92" s="48" t="str">
         <f>AA20</f>
@@ -11141,20 +11118,20 @@
       </c>
       <c r="AT92" s="56"/>
     </row>
-    <row r="94" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:47">
       <c r="A94" s="8" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="95" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:47">
       <c r="B95" s="8" t="s">
+        <v>252</v>
+      </c>
+      <c r="C95" s="8"/>
+    </row>
+    <row r="96" spans="1:47" s="39" customFormat="1">
+      <c r="B96" s="9" t="s">
         <v>253</v>
-      </c>
-      <c r="C95" s="8"/>
-    </row>
-    <row r="96" spans="1:47" s="39" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B96" s="9" t="s">
-        <v>254</v>
       </c>
       <c r="C96" s="9"/>
       <c r="D96" s="40"/>
@@ -11174,13 +11151,13 @@
       <c r="AQ96" s="41"/>
       <c r="AT96" s="54"/>
     </row>
-    <row r="97" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="97" spans="2:3">
       <c r="B97" s="57" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C97" s="22"/>
     </row>
-    <row r="98" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="98" spans="2:3">
       <c r="B98" s="22" t="s">
         <v>144</v>
       </c>
@@ -11195,56 +11172,56 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3.28515625" customWidth="1"/>
     <col min="3" max="6" width="9.140625" style="44"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12">
       <c r="A1" s="25" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
       <c r="B3" s="63"/>
       <c r="C3" s="82" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="D3" s="82" t="s">
+        <v>149</v>
+      </c>
+      <c r="E3" s="82" t="s">
         <v>150</v>
       </c>
-      <c r="E3" s="82" t="s">
-        <v>151</v>
-      </c>
       <c r="F3" s="82" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G3" s="107" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H3" s="107" t="s">
+        <v>233</v>
+      </c>
+      <c r="I3" s="107" t="s">
         <v>234</v>
       </c>
-      <c r="I3" s="107" t="s">
-        <v>235</v>
-      </c>
       <c r="J3" s="107" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="K3" s="82" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="L3" s="83"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12">
       <c r="B4" s="84">
         <v>0</v>
       </c>
@@ -11273,27 +11250,27 @@
         <v>31</v>
       </c>
       <c r="K4" s="105" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="L4" s="85">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12">
       <c r="B5" s="84">
         <v>1</v>
       </c>
       <c r="C5" s="72" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D5" s="73" t="s">
         <v>30</v>
       </c>
       <c r="E5" s="73" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F5" s="73" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G5" s="73" t="s">
         <v>44</v>
@@ -11308,13 +11285,13 @@
         <v>133</v>
       </c>
       <c r="K5" s="106" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="L5" s="85">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12">
       <c r="B6" s="84">
         <v>2</v>
       </c>
@@ -11323,37 +11300,37 @@
         <v>133</v>
       </c>
       <c r="E6" s="73" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F6" s="73" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G6" s="73" t="s">
         <v>18</v>
       </c>
       <c r="H6" s="73" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="I6" s="73" t="s">
         <v>26</v>
       </c>
       <c r="J6" s="73" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="K6" s="106" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="L6" s="86">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12">
       <c r="B7" s="84">
         <v>3</v>
       </c>
       <c r="C7" s="72"/>
       <c r="D7" s="73" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E7" s="73" t="s">
         <v>30</v>
@@ -11365,7 +11342,7 @@
         <v>19</v>
       </c>
       <c r="H7" s="73" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="I7" s="73" t="s">
         <v>25</v>
@@ -11374,13 +11351,13 @@
         <v>36</v>
       </c>
       <c r="K7" s="106" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L7" s="86">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12">
       <c r="B8" s="84">
         <v>4</v>
       </c>
@@ -11392,7 +11369,7 @@
         <v>27</v>
       </c>
       <c r="H8" s="73" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="I8" s="73" t="s">
         <v>128</v>
@@ -11401,13 +11378,13 @@
         <v>35</v>
       </c>
       <c r="K8" s="74" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="L8" s="86">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12">
       <c r="B9" s="84">
         <v>5</v>
       </c>
@@ -11419,22 +11396,22 @@
         <v>28</v>
       </c>
       <c r="H9" s="73" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="I9" s="73" t="s">
         <v>127</v>
       </c>
       <c r="J9" s="73" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="K9" s="74" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="L9" s="86">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12">
       <c r="B10" s="84">
         <v>6</v>
       </c>
@@ -11449,19 +11426,19 @@
         <v>52</v>
       </c>
       <c r="I10" s="73" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J10" s="73" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="K10" s="74" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="L10" s="86">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12">
       <c r="B11" s="84">
         <v>7</v>
       </c>
@@ -11470,25 +11447,25 @@
       <c r="E11" s="76"/>
       <c r="F11" s="76"/>
       <c r="G11" s="73" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="H11" s="73" t="s">
         <v>53</v>
       </c>
       <c r="I11" s="73" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J11" s="109" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K11" s="74" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L11" s="86">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12">
       <c r="B12" s="84">
         <v>8</v>
       </c>
@@ -11497,7 +11474,7 @@
       <c r="E12" s="76"/>
       <c r="F12" s="76"/>
       <c r="G12" s="73" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="H12" s="64"/>
       <c r="I12" s="64"/>
@@ -11507,7 +11484,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12">
       <c r="B13" s="84">
         <v>9</v>
       </c>
@@ -11516,7 +11493,7 @@
       <c r="E13" s="76"/>
       <c r="F13" s="76"/>
       <c r="G13" s="73" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="H13" s="64"/>
       <c r="I13" s="64"/>
@@ -11526,7 +11503,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12">
       <c r="B14" s="84">
         <v>10</v>
       </c>
@@ -11545,7 +11522,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12">
       <c r="B15" s="84">
         <v>11</v>
       </c>
@@ -11564,7 +11541,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12">
       <c r="B16" s="84">
         <v>12</v>
       </c>
@@ -11583,7 +11560,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:12">
       <c r="B17" s="84">
         <v>13</v>
       </c>
@@ -11592,7 +11569,7 @@
       <c r="E17" s="76"/>
       <c r="F17" s="76"/>
       <c r="G17" s="73" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H17" s="64"/>
       <c r="I17" s="64"/>
@@ -11602,7 +11579,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:12">
       <c r="B18" s="84">
         <v>14</v>
       </c>
@@ -11611,7 +11588,7 @@
       <c r="E18" s="76"/>
       <c r="F18" s="76"/>
       <c r="G18" s="73" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="H18" s="64"/>
       <c r="I18" s="64"/>
@@ -11621,7 +11598,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:12">
       <c r="B19" s="87">
         <v>15</v>
       </c>
@@ -11640,9 +11617,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:12">
       <c r="B21" s="4" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C21" s="4">
         <v>1</v>
@@ -11672,9 +11649,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:12">
       <c r="B22" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C22" s="4">
         <v>1</v>
@@ -11714,14 +11691,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:V42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="11.25"/>
   <cols>
     <col min="1" max="1" width="2.28515625" style="1" customWidth="1"/>
     <col min="2" max="2" width="3.42578125" style="1" customWidth="1"/>
@@ -11736,25 +11713,25 @@
     <col min="23" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" ht="15">
       <c r="A1" s="25" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22">
       <c r="B3" s="23" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22">
       <c r="B4" s="23"/>
       <c r="C4" s="23" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22" s="23" customFormat="1" x14ac:dyDescent="0.2">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" s="23" customFormat="1">
       <c r="D5" s="28" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F5" s="24"/>
       <c r="G5" s="102">
@@ -11772,12 +11749,12 @@
       <c r="K5" s="7"/>
       <c r="L5" s="7"/>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:22">
       <c r="D6" s="1">
         <v>2</v>
       </c>
       <c r="F6" s="24" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>31</v>
@@ -11789,52 +11766,52 @@
         <v>133</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="K6" s="4"/>
       <c r="L6" s="4"/>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:22">
       <c r="D7" s="1">
         <v>2</v>
       </c>
       <c r="F7" s="24" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>36</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="J7" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:22" s="3" customFormat="1">
       <c r="D8" s="3">
         <v>2</v>
       </c>
       <c r="F8" s="45" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G8" s="11" t="s">
         <v>35</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I8" s="11" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J8" s="11" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:22">
       <c r="D9" s="30">
         <f>SUM(D6:D8)</f>
         <v>6</v>
@@ -11844,18 +11821,18 @@
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:22">
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
     </row>
-    <row r="11" spans="1:22" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:22" s="14" customFormat="1">
       <c r="B11" s="31"/>
       <c r="C11" s="31" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F11" s="35"/>
     </row>
-    <row r="12" spans="1:22" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:22" s="14" customFormat="1">
       <c r="D12" s="14">
         <v>1</v>
       </c>
@@ -11866,27 +11843,27 @@
         <v>30</v>
       </c>
       <c r="H12" s="15" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="13" spans="1:22" s="14" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" s="14" customFormat="1" ht="11.25" customHeight="1">
       <c r="D13" s="32">
         <f>SUM(D12:D12)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:22" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:22" s="14" customFormat="1" ht="12.75" customHeight="1">
       <c r="K14" s="15"/>
       <c r="L14" s="15"/>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:22">
       <c r="B15" s="23" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22">
       <c r="D16" s="28" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G16" s="102">
         <v>0</v>
@@ -11937,13 +11914,13 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:22">
       <c r="D17" s="29">
         <v>4</v>
       </c>
       <c r="E17" s="29"/>
       <c r="F17" s="24" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="G17" s="4" t="s">
         <v>20</v>
@@ -11964,16 +11941,16 @@
         <v>28</v>
       </c>
       <c r="M17" s="6" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="N17" s="4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="O17" s="4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="P17" s="4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="Q17" s="4" t="b">
         <v>0</v>
@@ -11985,72 +11962,72 @@
         <v>46</v>
       </c>
       <c r="T17" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="U17" s="4" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="V17" s="1" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:22">
       <c r="D18" s="29"/>
       <c r="G18" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="J18" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="K18" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="L18" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="M18" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="N18" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="O18" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="H18" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="I18" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="J18" s="4" t="s">
-        <v>224</v>
-      </c>
-      <c r="K18" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="L18" s="4" t="s">
-        <v>225</v>
-      </c>
-      <c r="M18" s="4" t="s">
-        <v>205</v>
-      </c>
-      <c r="N18" s="4" t="s">
+      <c r="P18" s="4" t="s">
         <v>226</v>
       </c>
-      <c r="O18" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="P18" s="4" t="s">
+      <c r="Q18" s="4">
+        <v>0</v>
+      </c>
+      <c r="R18" s="4" t="s">
         <v>227</v>
       </c>
-      <c r="Q18" s="4">
-        <v>0</v>
-      </c>
-      <c r="R18" s="4" t="s">
+      <c r="S18" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="S18" s="4" t="s">
+      <c r="T18" s="4" t="s">
         <v>229</v>
       </c>
-      <c r="T18" s="4" t="s">
+      <c r="U18" s="4" t="s">
         <v>230</v>
-      </c>
-      <c r="U18" s="4" t="s">
-        <v>231</v>
       </c>
       <c r="V18" s="4">
         <v>-1</v>
       </c>
     </row>
-    <row r="19" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:22">
       <c r="D19" s="1">
         <v>3</v>
       </c>
       <c r="F19" s="24" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G19" s="4" t="s">
         <v>30</v>
@@ -12059,16 +12036,16 @@
         <v>16</v>
       </c>
       <c r="I19" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="J19" s="4" t="s">
         <v>232</v>
       </c>
-      <c r="J19" s="4" t="s">
-        <v>233</v>
-      </c>
       <c r="K19" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="L19" s="4" t="s">
         <v>220</v>
-      </c>
-      <c r="L19" s="4" t="s">
-        <v>221</v>
       </c>
       <c r="M19" s="4" t="s">
         <v>52</v>
@@ -12077,12 +12054,12 @@
         <v>53</v>
       </c>
     </row>
-    <row r="20" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:22">
       <c r="D20" s="1">
         <v>3</v>
       </c>
       <c r="F20" s="24" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="G20" s="4" t="s">
         <v>23</v>
@@ -12103,18 +12080,18 @@
         <v>127</v>
       </c>
       <c r="M20" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="N20" s="4" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="21" spans="2:22" x14ac:dyDescent="0.2">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="21" spans="2:22">
       <c r="D21" s="1">
         <v>1</v>
       </c>
       <c r="F21" s="24" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="G21" s="4" t="s">
         <v>31</v>
@@ -12129,19 +12106,19 @@
         <v>36</v>
       </c>
       <c r="K21" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="L21" s="4" t="s">
         <v>246</v>
-      </c>
-      <c r="L21" s="4" t="s">
-        <v>247</v>
       </c>
       <c r="M21" s="11" t="s">
         <v>138</v>
       </c>
       <c r="N21" s="11" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="22" spans="2:22" x14ac:dyDescent="0.2">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="22" spans="2:22">
       <c r="D22" s="1">
         <v>3</v>
       </c>
@@ -12149,48 +12126,48 @@
         <v>125</v>
       </c>
       <c r="G22" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="H22" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="H22" s="4" t="s">
+      <c r="I22" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="J22" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="I22" s="4" t="s">
-        <v>219</v>
-      </c>
-      <c r="J22" s="4" t="s">
-        <v>236</v>
-      </c>
       <c r="K22" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="L22" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="L22" s="4" t="s">
-        <v>192</v>
-      </c>
       <c r="M22" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="N22" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="N22" s="4" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="23" spans="2:22" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="2:22">
       <c r="D23" s="30">
         <f>MAX(D17:D21)+D22</f>
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:22">
       <c r="D24" s="36"/>
     </row>
-    <row r="25" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:22">
       <c r="B25" s="23" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="D25" s="36"/>
     </row>
-    <row r="26" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:22">
       <c r="D26" s="28" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E26" s="23"/>
       <c r="G26" s="102">
@@ -12206,24 +12183,24 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:22">
       <c r="D27" s="29">
         <v>1</v>
       </c>
       <c r="E27" s="23"/>
       <c r="F27" s="24" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="G27" s="4" t="s">
         <v>30</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="I27" s="7"/>
       <c r="J27" s="7"/>
     </row>
-    <row r="28" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:22">
       <c r="D28" s="101">
         <f>SUM(D27)</f>
         <v>1</v>
@@ -12234,7 +12211,7 @@
       <c r="I28" s="7"/>
       <c r="J28" s="7"/>
     </row>
-    <row r="29" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:22">
       <c r="D29" s="29"/>
       <c r="E29" s="23"/>
       <c r="G29" s="4"/>
@@ -12242,7 +12219,7 @@
       <c r="I29" s="7"/>
       <c r="J29" s="7"/>
     </row>
-    <row r="30" spans="2:22" s="26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:22" s="26" customFormat="1">
       <c r="D30" s="38"/>
       <c r="F30" s="37"/>
       <c r="G30" s="27"/>
@@ -12251,25 +12228,25 @@
       <c r="J30" s="27"/>
       <c r="K30" s="27"/>
     </row>
-    <row r="31" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:22">
       <c r="B31" s="23" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="D31" s="36"/>
       <c r="F31" s="43" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="G31" s="33"/>
       <c r="H31" s="33"/>
       <c r="J31" s="33" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="K31" s="19"/>
       <c r="L31" s="19"/>
     </row>
-    <row r="32" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:22">
       <c r="C32" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D32" s="1">
         <f>D9</f>
@@ -12280,16 +12257,16 @@
         <v>5</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="H32" s="4">
         <v>0</v>
       </c>
       <c r="K32" s="4"/>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12">
       <c r="C33" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D33" s="1">
         <f>D22</f>
@@ -12300,7 +12277,7 @@
         <v>8</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="H33" s="4">
         <f>F32+1</f>
@@ -12311,15 +12288,15 @@
         <v>2</v>
       </c>
       <c r="K33" s="4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="L33" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:12">
       <c r="C34" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D34" s="1">
         <f>MAX(D17:D21)</f>
@@ -12330,7 +12307,7 @@
         <v>12</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="H34" s="4">
         <f>F33+1</f>
@@ -12341,16 +12318,16 @@
         <v>6</v>
       </c>
       <c r="K34" s="4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="L34" s="4">
         <f>J33+1</f>
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:12">
       <c r="C35" s="1" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="D35" s="1">
         <v>1</v>
@@ -12359,7 +12336,7 @@
         <v>13</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="H35" s="4">
         <v>13</v>
@@ -12368,37 +12345,37 @@
       <c r="K35" s="4"/>
       <c r="L35" s="4"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:12">
       <c r="D36" s="30">
         <f>SUM(D32:D35)</f>
         <v>14</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:12">
       <c r="B38" s="31" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12">
       <c r="D39" s="32">
         <f>D13</f>
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:12">
       <c r="A41" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B41" s="1" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12">
+      <c r="A42" s="14" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A42" s="14" t="s">
-        <v>335</v>
-      </c>
       <c r="B42" s="14" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
     </row>
   </sheetData>
@@ -12408,14 +12385,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:T28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="11.25"/>
   <cols>
     <col min="1" max="1" width="14.42578125" style="1" customWidth="1"/>
     <col min="2" max="2" width="17.28515625" style="4" customWidth="1"/>
@@ -12433,80 +12410,80 @@
     <col min="21" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" ht="15">
       <c r="A1" s="25" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20">
       <c r="C4" s="33" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D4" s="19"/>
       <c r="E4" s="19"/>
       <c r="G4" s="33" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H4" s="19"/>
       <c r="J4" s="33" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="K4" s="19"/>
       <c r="M4" s="33" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="N4" s="34"/>
       <c r="P4" s="33" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="Q4" s="19"/>
       <c r="S4" s="33" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="T4" s="19"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20">
       <c r="C5" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>181</v>
-      </c>
       <c r="G5" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="M5" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="N5" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="N5" s="4" t="s">
-        <v>184</v>
-      </c>
       <c r="P5" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="Q5" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="Q5" s="4" t="s">
-        <v>184</v>
-      </c>
       <c r="S5" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="T5" s="4" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20">
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
@@ -12515,21 +12492,21 @@
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
       <c r="M6" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="N6" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="P6" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="Q6" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="S6" s="4"/>
       <c r="T6" s="4"/>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:20">
       <c r="A7" s="4" t="s">
         <v>31</v>
       </c>
@@ -12550,7 +12527,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:20">
       <c r="A8" s="4" t="s">
         <v>30</v>
       </c>
@@ -12577,12 +12554,12 @@
       <c r="S8" s="4"/>
       <c r="T8" s="4"/>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:20">
       <c r="A9" s="6" t="s">
         <v>11</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>31</v>
@@ -12598,7 +12575,7 @@
       <c r="P9" s="4"/>
       <c r="Q9" s="4"/>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:20">
       <c r="A10" s="6" t="s">
         <v>12</v>
       </c>
@@ -12619,7 +12596,7 @@
       <c r="P10" s="4"/>
       <c r="Q10" s="4"/>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:20">
       <c r="A11" s="6" t="s">
         <v>13</v>
       </c>
@@ -12640,7 +12617,7 @@
       <c r="P11" s="4"/>
       <c r="Q11" s="4"/>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:20">
       <c r="A12" s="17" t="s">
         <v>14</v>
       </c>
@@ -12657,7 +12634,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:20">
       <c r="A13" s="15" t="s">
         <v>15</v>
       </c>
@@ -12676,12 +12653,12 @@
       <c r="P13" s="4"/>
       <c r="Q13" s="4"/>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:20">
       <c r="A14" s="15" t="s">
         <v>42</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
@@ -12695,7 +12672,7 @@
       <c r="M14" s="4"/>
       <c r="N14" s="4"/>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:20">
       <c r="A15" s="21" t="s">
         <v>43</v>
       </c>
@@ -12714,12 +12691,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:20">
       <c r="A16" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C16" s="4">
         <v>0</v>
@@ -12733,12 +12710,12 @@
       <c r="M16" s="4"/>
       <c r="N16" s="4"/>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:20">
       <c r="A17" s="11" t="s">
         <v>52</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C17" s="4">
         <v>1</v>
@@ -12752,12 +12729,12 @@
       <c r="M17" s="4"/>
       <c r="N17" s="4"/>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:20">
       <c r="A18" s="11" t="s">
         <v>53</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C18" s="4">
         <v>-1</v>
@@ -12773,12 +12750,12 @@
       <c r="S18" s="4"/>
       <c r="T18" s="4"/>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:20">
       <c r="A19" s="11" t="s">
         <v>54</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
@@ -12792,12 +12769,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:20">
       <c r="A20" s="11" t="s">
         <v>55</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
@@ -12811,12 +12788,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:20">
       <c r="A21" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
@@ -12830,12 +12807,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:20">
       <c r="A22" s="4" t="s">
         <v>24</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
@@ -12849,12 +12826,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:20">
       <c r="A23" s="4" t="s">
         <v>25</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
@@ -12868,12 +12845,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:20">
       <c r="A24" s="4" t="s">
         <v>26</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
@@ -12887,12 +12864,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:20">
       <c r="A25" s="15" t="s">
         <v>143</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
@@ -12906,12 +12883,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:20">
       <c r="A26" s="15" t="s">
         <v>142</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
@@ -12925,12 +12902,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:20">
       <c r="A27" s="4" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>31</v>
@@ -12942,12 +12919,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:20">
       <c r="A28" s="4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>31</v>
@@ -12965,62 +12942,62 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="109.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1">
       <c r="A1" s="103" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="103" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="103"/>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" s="103" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" s="103" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="103" t="s">
+    <row r="6" spans="1:1" ht="30">
+      <c r="A6" s="103" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="103"/>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="103" t="s">
+    <row r="7" spans="1:1">
+      <c r="A7" s="103" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="45">
+      <c r="A8" s="104" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" s="103"/>
+    </row>
+    <row r="10" spans="1:1" ht="60">
+      <c r="A10" s="104" t="s">
         <v>340</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="103" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="103" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="103" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="104" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="103"/>
-    </row>
-    <row r="10" spans="1:1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="104" t="s">
-        <v>343</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added JSL instruction (Jump to subroutine at 3 byte literal address) Implemented FETCH for wide SRAM
</commit_message>
<xml_diff>
--- a/Resources/Instruction Set.xlsx
+++ b/Resources/Instruction Set.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="120" windowWidth="18195" windowHeight="8250" tabRatio="681"/>
@@ -16,12 +16,12 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">OPCODE_encoding!$A$3:$L$92</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1361" uniqueCount="345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1368" uniqueCount="346">
   <si>
     <t>DUP</t>
   </si>
@@ -797,9 +797,6 @@
     <t>PC_plus</t>
   </si>
   <si>
-    <t>BSR</t>
-  </si>
-  <si>
     <t>HEX</t>
   </si>
   <si>
@@ -833,9 +830,6 @@
     <t>Jump to address on stack</t>
   </si>
   <si>
-    <t>Branch to subroutine address on stack.  Push return address to return stack</t>
-  </si>
-  <si>
     <t>Jump to subroutine address on stack.  Push return address to return stack</t>
   </si>
   <si>
@@ -1052,17 +1046,26 @@
     <t>RSP!</t>
   </si>
   <si>
+    <t>JSI</t>
+  </si>
+  <si>
+    <t>JSL</t>
+  </si>
+  <si>
+    <t>Jump to subroutine at literal address.  Push return address to return stack</t>
+  </si>
+  <si>
     <t>UNUSED</t>
   </si>
   <si>
-    <t>JSI</t>
+    <t>," JSL"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="33">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="33" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1756,6 +1759,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1790,6 +1794,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1965,20 +1970,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:AU98"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="9" ySplit="4" topLeftCell="J50" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="9" ySplit="4" topLeftCell="AB48" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="L84" sqref="L84"/>
+      <selection pane="bottomRight" activeCell="AR65" sqref="AR65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.25"/>
+  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="1.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="11" style="4" customWidth="1"/>
@@ -1989,7 +1994,7 @@
     <col min="9" max="9" width="6.5703125" style="4" customWidth="1"/>
     <col min="10" max="10" width="2" style="4" customWidth="1"/>
     <col min="11" max="11" width="19.28515625" style="89" customWidth="1"/>
-    <col min="12" max="12" width="50.5703125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="51" style="1" customWidth="1"/>
     <col min="13" max="13" width="2.7109375" style="8" customWidth="1"/>
     <col min="14" max="14" width="10.28515625" style="4" customWidth="1"/>
     <col min="15" max="17" width="9.140625" style="4" customWidth="1"/>
@@ -2012,14 +2017,14 @@
     <col min="48" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" ht="15">
+    <row r="1" spans="1:47" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="46" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:47" ht="5.25" customHeight="1"/>
-    <row r="3" spans="1:47" s="23" customFormat="1">
+    <row r="2" spans="1:47" ht="5.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="1:47" s="23" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B3" s="7" t="s">
         <v>249</v>
       </c>
@@ -2028,10 +2033,10 @@
         <v>140</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="J3" s="7"/>
       <c r="K3" s="90" t="s">
@@ -2042,14 +2047,14 @@
       </c>
       <c r="M3" s="24"/>
       <c r="N3" s="20" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="O3" s="18"/>
       <c r="P3" s="18"/>
       <c r="Q3" s="18"/>
       <c r="R3" s="24"/>
       <c r="S3" s="20" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="T3" s="20"/>
       <c r="V3" s="20" t="s">
@@ -2080,11 +2085,11 @@
       </c>
       <c r="AR3" s="33"/>
       <c r="AT3" s="20" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="AU3" s="33"/>
     </row>
-    <row r="4" spans="1:47">
+    <row r="4" spans="1:47" x14ac:dyDescent="0.2">
       <c r="D4" s="7">
         <v>7</v>
       </c>
@@ -2116,7 +2121,7 @@
         <v>35</v>
       </c>
       <c r="V4" s="7" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="W4" s="7" t="s">
         <v>153</v>
@@ -2143,7 +2148,7 @@
         <v>247</v>
       </c>
       <c r="AF4" s="7" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="AG4" s="7" t="s">
         <v>248</v>
@@ -2173,24 +2178,24 @@
         <v>238</v>
       </c>
       <c r="AQ4" s="24" t="s">
+        <v>264</v>
+      </c>
+      <c r="AR4" s="24" t="s">
         <v>265</v>
       </c>
-      <c r="AR4" s="24" t="s">
-        <v>266</v>
-      </c>
       <c r="AT4" s="24" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="AU4" s="24" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="5" spans="1:47">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="5" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="6" spans="1:47">
+    <row r="6" spans="1:47" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
         <v>41</v>
       </c>
@@ -2319,7 +2324,7 @@
         <v>," NOP"</v>
       </c>
     </row>
-    <row r="7" spans="1:47">
+    <row r="7" spans="1:47" x14ac:dyDescent="0.2">
       <c r="B7" s="4" t="s">
         <v>2</v>
       </c>
@@ -2449,7 +2454,7 @@
         <v>," DROP"</v>
       </c>
     </row>
-    <row r="8" spans="1:47">
+    <row r="8" spans="1:47" x14ac:dyDescent="0.2">
       <c r="B8" s="4" t="s">
         <v>0</v>
       </c>
@@ -2579,7 +2584,7 @@
         <v>," DUP"</v>
       </c>
     </row>
-    <row r="9" spans="1:47" s="14" customFormat="1">
+    <row r="9" spans="1:47" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B9" s="15" t="s">
         <v>1</v>
       </c>
@@ -2709,7 +2714,7 @@
         <v>," ?DUP"</v>
       </c>
     </row>
-    <row r="10" spans="1:47">
+    <row r="10" spans="1:47" x14ac:dyDescent="0.2">
       <c r="B10" s="4" t="s">
         <v>3</v>
       </c>
@@ -2839,7 +2844,7 @@
         <v>," SWAP"</v>
       </c>
     </row>
-    <row r="11" spans="1:47">
+    <row r="11" spans="1:47" x14ac:dyDescent="0.2">
       <c r="B11" s="4" t="s">
         <v>4</v>
       </c>
@@ -2969,7 +2974,7 @@
         <v>," OVER"</v>
       </c>
     </row>
-    <row r="12" spans="1:47">
+    <row r="12" spans="1:47" x14ac:dyDescent="0.2">
       <c r="B12" s="4" t="s">
         <v>5</v>
       </c>
@@ -3099,7 +3104,7 @@
         <v>," NIP"</v>
       </c>
     </row>
-    <row r="13" spans="1:47">
+    <row r="13" spans="1:47" x14ac:dyDescent="0.2">
       <c r="B13" s="4" t="s">
         <v>6</v>
       </c>
@@ -3125,7 +3130,7 @@
         <v>68</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="N13" s="4" t="s">
         <v>133</v>
@@ -3229,7 +3234,7 @@
         <v>," ROT"</v>
       </c>
     </row>
-    <row r="14" spans="1:47" s="3" customFormat="1">
+    <row r="14" spans="1:47" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B14" s="11" t="s">
         <v>7</v>
       </c>
@@ -3366,7 +3371,7 @@
         <v>," &gt;R"</v>
       </c>
     </row>
-    <row r="15" spans="1:47">
+    <row r="15" spans="1:47" x14ac:dyDescent="0.2">
       <c r="B15" s="4" t="s">
         <v>8</v>
       </c>
@@ -3437,7 +3442,7 @@
         <v>141</v>
       </c>
       <c r="AD15" s="11" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="AF15" s="11" t="str">
         <f>DEC2BIN(VLOOKUP(V15,OPCODE_mult!$C$4:$L$19,10,FALSE),1)</f>
@@ -3496,7 +3501,7 @@
         <v>," R@"</v>
       </c>
     </row>
-    <row r="16" spans="1:47" s="3" customFormat="1">
+    <row r="16" spans="1:47" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B16" s="11" t="s">
         <v>9</v>
       </c>
@@ -3572,7 +3577,7 @@
         <v>141</v>
       </c>
       <c r="AD16" s="11" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="AE16" s="1"/>
       <c r="AF16" s="11" t="str">
@@ -3633,9 +3638,9 @@
         <v>," R&gt;"</v>
       </c>
     </row>
-    <row r="17" spans="1:47" s="3" customFormat="1">
+    <row r="17" spans="1:47" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B17" s="11" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="C17" s="11"/>
       <c r="D17" s="11">
@@ -3659,10 +3664,10 @@
       </c>
       <c r="J17" s="11"/>
       <c r="K17" s="94" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="L17" s="3" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="M17" s="12"/>
       <c r="N17" s="11"/>
@@ -3758,9 +3763,9 @@
         <v>," PSP@"</v>
       </c>
     </row>
-    <row r="18" spans="1:47" s="3" customFormat="1">
+    <row r="18" spans="1:47" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B18" s="11" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="C18" s="11"/>
       <c r="D18" s="11">
@@ -3784,10 +3789,10 @@
       </c>
       <c r="J18" s="11"/>
       <c r="K18" s="94" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="L18" s="3" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="M18" s="12"/>
       <c r="N18" s="11"/>
@@ -3883,9 +3888,9 @@
         <v>," RSP@"</v>
       </c>
     </row>
-    <row r="19" spans="1:47">
+    <row r="19" spans="1:47" x14ac:dyDescent="0.2">
       <c r="B19" s="11" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D19" s="4">
         <v>0</v>
@@ -3909,7 +3914,7 @@
         <v>250</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="Q19" s="6"/>
       <c r="S19" s="4"/>
@@ -3998,9 +4003,9 @@
         <v>," PSP!"</v>
       </c>
     </row>
-    <row r="20" spans="1:47">
+    <row r="20" spans="1:47" x14ac:dyDescent="0.2">
       <c r="B20" s="11" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="D20" s="4">
         <v>0</v>
@@ -4024,7 +4029,7 @@
         <v>251</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="Q20" s="6"/>
       <c r="S20" s="4"/>
@@ -4113,18 +4118,18 @@
         <v>," RSP!"</v>
       </c>
     </row>
-    <row r="21" spans="1:47">
+    <row r="21" spans="1:47" x14ac:dyDescent="0.2">
       <c r="AT21" s="66"/>
       <c r="AU21" s="66"/>
     </row>
-    <row r="22" spans="1:47">
+    <row r="22" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>10</v>
       </c>
       <c r="AT22" s="66"/>
       <c r="AU22" s="66"/>
     </row>
-    <row r="23" spans="1:47">
+    <row r="23" spans="1:47" x14ac:dyDescent="0.2">
       <c r="B23" s="6" t="s">
         <v>11</v>
       </c>
@@ -4256,7 +4261,7 @@
         <v>," +"</v>
       </c>
     </row>
-    <row r="24" spans="1:47">
+    <row r="24" spans="1:47" x14ac:dyDescent="0.2">
       <c r="B24" s="6" t="s">
         <v>12</v>
       </c>
@@ -4388,7 +4393,7 @@
         <v>," -"</v>
       </c>
     </row>
-    <row r="25" spans="1:47">
+    <row r="25" spans="1:47" x14ac:dyDescent="0.2">
       <c r="B25" s="4" t="s">
         <v>16</v>
       </c>
@@ -4519,7 +4524,7 @@
         <v>," NEGATE"</v>
       </c>
     </row>
-    <row r="26" spans="1:47" s="3" customFormat="1">
+    <row r="26" spans="1:47" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B26" s="11" t="s">
         <v>52</v>
       </c>
@@ -4656,7 +4661,7 @@
         <v>," 1+"</v>
       </c>
     </row>
-    <row r="27" spans="1:47" s="3" customFormat="1">
+    <row r="27" spans="1:47" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B27" s="13" t="s">
         <v>53</v>
       </c>
@@ -4793,7 +4798,7 @@
         <v>," 1-"</v>
       </c>
     </row>
-    <row r="28" spans="1:47" s="3" customFormat="1">
+    <row r="28" spans="1:47" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B28" s="13" t="s">
         <v>54</v>
       </c>
@@ -4930,7 +4935,7 @@
         <v>," 2*"</v>
       </c>
     </row>
-    <row r="29" spans="1:47" s="3" customFormat="1">
+    <row r="29" spans="1:47" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B29" s="13" t="s">
         <v>55</v>
       </c>
@@ -5067,9 +5072,9 @@
         <v>," 2/"</v>
       </c>
     </row>
-    <row r="30" spans="1:47" s="3" customFormat="1">
+    <row r="30" spans="1:47" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B30" s="11" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C30" s="11"/>
       <c r="D30" s="11">
@@ -5204,9 +5209,9 @@
         <v>," MULTS"</v>
       </c>
     </row>
-    <row r="31" spans="1:47" s="3" customFormat="1">
+    <row r="31" spans="1:47" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B31" s="11" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C31" s="11"/>
       <c r="D31" s="11">
@@ -5341,7 +5346,7 @@
         <v>," MULTU"</v>
       </c>
     </row>
-    <row r="32" spans="1:47" s="3" customFormat="1">
+    <row r="32" spans="1:47" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B32" s="11" t="s">
         <v>219</v>
       </c>
@@ -5479,7 +5484,7 @@
         <v>," ADDX"</v>
       </c>
     </row>
-    <row r="33" spans="1:47" s="3" customFormat="1">
+    <row r="33" spans="1:47" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B33" s="11" t="s">
         <v>220</v>
       </c>
@@ -5617,9 +5622,9 @@
         <v>," SUBX"</v>
       </c>
     </row>
-    <row r="34" spans="1:47" s="14" customFormat="1">
+    <row r="34" spans="1:47" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B34" s="15" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C34" s="17"/>
       <c r="D34" s="15">
@@ -5761,9 +5766,9 @@
         <v>," DIVS"</v>
       </c>
     </row>
-    <row r="35" spans="1:47" s="14" customFormat="1" ht="14.25" customHeight="1">
+    <row r="35" spans="1:47" s="14" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="15" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C35" s="17"/>
       <c r="D35" s="15">
@@ -5905,12 +5910,12 @@
         <v>," DIVU"</v>
       </c>
     </row>
-    <row r="36" spans="1:47">
+    <row r="36" spans="1:47" x14ac:dyDescent="0.2">
       <c r="E36" s="13"/>
       <c r="AT36" s="66"/>
       <c r="AU36" s="66"/>
     </row>
-    <row r="37" spans="1:47">
+    <row r="37" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>17</v>
       </c>
@@ -5918,7 +5923,7 @@
       <c r="AT37" s="66"/>
       <c r="AU37" s="66"/>
     </row>
-    <row r="38" spans="1:47">
+    <row r="38" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A38" s="4"/>
       <c r="B38" s="6" t="s">
         <v>20</v>
@@ -6052,7 +6057,7 @@
         <v>," ="</v>
       </c>
     </row>
-    <row r="39" spans="1:47" s="3" customFormat="1">
+    <row r="39" spans="1:47" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="4"/>
       <c r="B39" s="13" t="s">
         <v>44</v>
@@ -6190,7 +6195,7 @@
         <v>," &lt;&gt;"</v>
       </c>
     </row>
-    <row r="40" spans="1:47">
+    <row r="40" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A40" s="4"/>
       <c r="B40" s="6" t="s">
         <v>18</v>
@@ -6324,7 +6329,7 @@
         <v>," &lt;"</v>
       </c>
     </row>
-    <row r="41" spans="1:47">
+    <row r="41" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A41" s="4"/>
       <c r="B41" s="6" t="s">
         <v>19</v>
@@ -6458,7 +6463,7 @@
         <v>," &gt;"</v>
       </c>
     </row>
-    <row r="42" spans="1:47">
+    <row r="42" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A42" s="4"/>
       <c r="B42" s="6" t="s">
         <v>27</v>
@@ -6592,7 +6597,7 @@
         <v>," U&lt;"</v>
       </c>
     </row>
-    <row r="43" spans="1:47">
+    <row r="43" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A43" s="4"/>
       <c r="B43" s="6" t="s">
         <v>28</v>
@@ -6726,7 +6731,7 @@
         <v>," U&gt;"</v>
       </c>
     </row>
-    <row r="44" spans="1:47" s="3" customFormat="1">
+    <row r="44" spans="1:47" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" s="4"/>
       <c r="B44" s="13" t="s">
         <v>21</v>
@@ -6864,10 +6869,10 @@
         <v>," 0="</v>
       </c>
     </row>
-    <row r="45" spans="1:47" s="3" customFormat="1">
+    <row r="45" spans="1:47" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A45" s="4"/>
       <c r="B45" s="13" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C45" s="11"/>
       <c r="D45" s="4">
@@ -7002,10 +7007,10 @@
         <v>," 0&lt;&gt;"</v>
       </c>
     </row>
-    <row r="46" spans="1:47" s="3" customFormat="1">
+    <row r="46" spans="1:47" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="4"/>
       <c r="B46" s="13" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C46" s="11"/>
       <c r="D46" s="4">
@@ -7032,7 +7037,7 @@
         <v>89</v>
       </c>
       <c r="L46" s="3" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="M46" s="12"/>
       <c r="N46" s="4" t="s">
@@ -7140,10 +7145,10 @@
         <v>," 0&lt;"</v>
       </c>
     </row>
-    <row r="47" spans="1:47" s="3" customFormat="1">
+    <row r="47" spans="1:47" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A47" s="4"/>
       <c r="B47" s="6" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C47" s="4"/>
       <c r="D47" s="4">
@@ -7278,7 +7283,7 @@
         <v>," 0&gt;"</v>
       </c>
     </row>
-    <row r="48" spans="1:47" s="3" customFormat="1">
+    <row r="48" spans="1:47" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A48" s="4"/>
       <c r="B48" s="11" t="b">
         <v>0</v>
@@ -7416,12 +7421,12 @@
         <v>," FALSE"</v>
       </c>
     </row>
-    <row r="49" spans="1:47">
+    <row r="49" spans="1:47" x14ac:dyDescent="0.2">
       <c r="E49" s="13"/>
       <c r="AT49" s="66"/>
       <c r="AU49" s="66"/>
     </row>
-    <row r="50" spans="1:47">
+    <row r="50" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>22</v>
       </c>
@@ -7429,7 +7434,7 @@
       <c r="AT50" s="66"/>
       <c r="AU50" s="66"/>
     </row>
-    <row r="51" spans="1:47">
+    <row r="51" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A51" s="4"/>
       <c r="B51" s="4" t="s">
         <v>23</v>
@@ -7562,7 +7567,7 @@
         <v>," AND"</v>
       </c>
     </row>
-    <row r="52" spans="1:47">
+    <row r="52" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A52" s="4"/>
       <c r="B52" s="4" t="s">
         <v>24</v>
@@ -7695,7 +7700,7 @@
         <v>," OR"</v>
       </c>
     </row>
-    <row r="53" spans="1:47">
+    <row r="53" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A53" s="4"/>
       <c r="B53" s="4" t="s">
         <v>26</v>
@@ -7828,7 +7833,7 @@
         <v>," INVERT"</v>
       </c>
     </row>
-    <row r="54" spans="1:47">
+    <row r="54" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A54" s="4"/>
       <c r="B54" s="4" t="s">
         <v>25</v>
@@ -7961,7 +7966,7 @@
         <v>," XOR"</v>
       </c>
     </row>
-    <row r="55" spans="1:47">
+    <row r="55" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A55" s="4"/>
       <c r="B55" s="4" t="s">
         <v>128</v>
@@ -8094,7 +8099,7 @@
         <v>," LSL"</v>
       </c>
     </row>
-    <row r="56" spans="1:47">
+    <row r="56" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A56" s="4"/>
       <c r="B56" s="4" t="s">
         <v>127</v>
@@ -8227,10 +8232,10 @@
         <v>," LSR"</v>
       </c>
     </row>
-    <row r="57" spans="1:47">
+    <row r="57" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A57" s="4"/>
       <c r="B57" s="4" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D57" s="4">
         <v>0</v>
@@ -8360,7 +8365,7 @@
         <v>," XBYTE"</v>
       </c>
     </row>
-    <row r="58" spans="1:47">
+    <row r="58" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A58" s="4"/>
       <c r="B58" s="4" t="s">
         <v>246</v>
@@ -8493,12 +8498,12 @@
         <v>," XWORD"</v>
       </c>
     </row>
-    <row r="59" spans="1:47">
+    <row r="59" spans="1:47" x14ac:dyDescent="0.2">
       <c r="E59" s="13"/>
       <c r="AT59" s="66"/>
       <c r="AU59" s="66"/>
     </row>
-    <row r="60" spans="1:47">
+    <row r="60" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>29</v>
       </c>
@@ -8506,9 +8511,9 @@
       <c r="AT60" s="66"/>
       <c r="AU60" s="66"/>
     </row>
-    <row r="61" spans="1:47" s="14" customFormat="1">
+    <row r="61" spans="1:47" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B61" s="15" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C61" s="15"/>
       <c r="D61" s="15">
@@ -8618,8 +8623,7 @@
         <v>00000000000110</v>
       </c>
       <c r="AR61" s="14">
-        <f t="shared" si="3"/>
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="AT61" s="66" t="str">
         <f t="shared" ref="AT61:AT66" si="35">"1 "&amp;H61&amp;" INSTRUCTION _"&amp;B61</f>
@@ -8630,9 +8634,9 @@
         <v>," FETCH.L"</v>
       </c>
     </row>
-    <row r="62" spans="1:47" s="14" customFormat="1">
+    <row r="62" spans="1:47" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B62" s="15" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C62" s="15"/>
       <c r="D62" s="15">
@@ -8742,8 +8746,7 @@
         <v>00000000000110</v>
       </c>
       <c r="AR62" s="14">
-        <f t="shared" si="3"/>
-        <v>6</v>
+        <v>800</v>
       </c>
       <c r="AT62" s="66" t="str">
         <f t="shared" si="35"/>
@@ -8754,9 +8757,9 @@
         <v>," STORE.L"</v>
       </c>
     </row>
-    <row r="63" spans="1:47" s="14" customFormat="1">
+    <row r="63" spans="1:47" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B63" s="15" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C63" s="15"/>
       <c r="D63" s="15">
@@ -8865,8 +8868,7 @@
         <v>00000000000110</v>
       </c>
       <c r="AR63" s="14">
-        <f t="shared" si="3"/>
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="AT63" s="66" t="str">
         <f t="shared" si="35"/>
@@ -8877,9 +8879,9 @@
         <v>," FETCH.W"</v>
       </c>
     </row>
-    <row r="64" spans="1:47" s="14" customFormat="1">
+    <row r="64" spans="1:47" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B64" s="15" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C64" s="15"/>
       <c r="D64" s="15">
@@ -8988,8 +8990,7 @@
         <v>00000000000110</v>
       </c>
       <c r="AR64" s="14">
-        <f t="shared" si="3"/>
-        <v>6</v>
+        <v>800</v>
       </c>
       <c r="AT64" s="66" t="str">
         <f t="shared" si="35"/>
@@ -9000,9 +9001,9 @@
         <v>," STORE.W"</v>
       </c>
     </row>
-    <row r="65" spans="1:47" s="14" customFormat="1">
+    <row r="65" spans="1:47" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B65" s="15" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C65" s="15"/>
       <c r="D65" s="15">
@@ -9123,9 +9124,9 @@
         <v>," FETCH.B"</v>
       </c>
     </row>
-    <row r="66" spans="1:47" s="14" customFormat="1">
+    <row r="66" spans="1:47" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B66" s="15" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C66" s="15"/>
       <c r="D66" s="15">
@@ -9246,7 +9247,7 @@
         <v>," STORE.B"</v>
       </c>
     </row>
-    <row r="67" spans="1:47" s="2" customFormat="1">
+    <row r="67" spans="1:47" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B67" s="5"/>
       <c r="C67" s="5"/>
       <c r="D67" s="4"/>
@@ -9270,18 +9271,18 @@
       <c r="AT67" s="67"/>
       <c r="AU67" s="66"/>
     </row>
-    <row r="68" spans="1:47">
+    <row r="68" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="AQ68" s="16"/>
       <c r="AR68" s="14"/>
       <c r="AT68" s="67"/>
       <c r="AU68" s="66"/>
     </row>
-    <row r="69" spans="1:47">
+    <row r="69" spans="1:47" x14ac:dyDescent="0.2">
       <c r="B69" s="4" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="D69" s="4">
         <v>0</v>
@@ -9379,7 +9380,7 @@
       </c>
       <c r="AP69" s="4"/>
       <c r="AQ69" s="8" t="str">
-        <f t="shared" ref="AQ69:AQ71" si="36">AF69&amp;AG69&amp;AH69&amp;AI69&amp;AJ69&amp;AO69</f>
+        <f>AF69&amp;AG69&amp;AH69&amp;AI69&amp;AJ69&amp;AO69</f>
         <v>00010010100111</v>
       </c>
       <c r="AR69" s="1">
@@ -9392,9 +9393,9 @@
         <v>," #.B"</v>
       </c>
     </row>
-    <row r="70" spans="1:47">
+    <row r="70" spans="1:47" x14ac:dyDescent="0.2">
       <c r="B70" s="4" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="D70" s="4">
         <v>0</v>
@@ -9492,7 +9493,7 @@
       </c>
       <c r="AP70" s="4"/>
       <c r="AQ70" s="8" t="str">
-        <f t="shared" si="36"/>
+        <f>AF70&amp;AG70&amp;AH70&amp;AI70&amp;AJ70&amp;AO70</f>
         <v>00010010100111</v>
       </c>
       <c r="AR70" s="1">
@@ -9505,9 +9506,9 @@
         <v>," #.W"</v>
       </c>
     </row>
-    <row r="71" spans="1:47" s="14" customFormat="1">
+    <row r="71" spans="1:47" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B71" s="15" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C71" s="15"/>
       <c r="D71" s="15">
@@ -9611,26 +9612,26 @@
       </c>
       <c r="AP71" s="15"/>
       <c r="AQ71" s="16" t="str">
-        <f t="shared" si="36"/>
+        <f>AF71&amp;AG71&amp;AH71&amp;AI71&amp;AJ71&amp;AO71</f>
         <v>00010010100111</v>
       </c>
       <c r="AR71" s="14">
-        <f t="shared" ref="AR71:AR91" si="37">(BIN2DEC(AO71)+16*BIN2DEC(AJ71)+128*BIN2DEC(AI71)+512*BIN2DEC(AH71)+2048*BIN2DEC(AG71)+8192*BIN2DEC(AF71))</f>
+        <f>(BIN2DEC(AO71)+16*BIN2DEC(AJ71)+128*BIN2DEC(AI71)+512*BIN2DEC(AH71)+2048*BIN2DEC(AG71)+8192*BIN2DEC(AF71))</f>
         <v>1191</v>
       </c>
       <c r="AT71" s="67"/>
       <c r="AU71" s="66" t="str">
-        <f t="shared" ref="AU71:AU76" si="38">CHAR(44)&amp;CHAR(34)&amp;CHAR(32)&amp;B71&amp;CHAR(34)</f>
+        <f t="shared" ref="AU71:AU76" si="36">CHAR(44)&amp;CHAR(34)&amp;CHAR(32)&amp;B71&amp;CHAR(34)</f>
         <v>," #.L"</v>
       </c>
     </row>
-    <row r="72" spans="1:47">
+    <row r="72" spans="1:47" x14ac:dyDescent="0.2">
       <c r="S72" s="4"/>
       <c r="T72" s="4"/>
       <c r="AT72" s="66"/>
       <c r="AU72" s="66"/>
     </row>
-    <row r="73" spans="1:47">
+    <row r="73" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>47</v>
       </c>
@@ -9639,7 +9640,7 @@
       <c r="AT73" s="66"/>
       <c r="AU73" s="66"/>
     </row>
-    <row r="74" spans="1:47" s="3" customFormat="1">
+    <row r="74" spans="1:47" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B74" s="11" t="s">
         <v>51</v>
       </c>
@@ -9656,19 +9657,19 @@
       </c>
       <c r="G74" s="11"/>
       <c r="H74" s="7">
-        <f t="shared" ref="H74:H79" si="39">F74+E74*64+D74*128</f>
+        <f t="shared" ref="H74:H79" si="37">F74+E74*64+D74*128</f>
         <v>56</v>
       </c>
       <c r="I74" s="4" t="str">
-        <f t="shared" ref="I74:I79" si="40">DEC2HEX(H74)</f>
+        <f t="shared" ref="I74:I79" si="38">DEC2HEX(H74)</f>
         <v>38</v>
       </c>
       <c r="J74" s="11"/>
       <c r="K74" s="94" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="L74" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="M74" s="12"/>
       <c r="N74" s="4" t="s">
@@ -9698,31 +9699,31 @@
         <v>35</v>
       </c>
       <c r="X74" s="11" t="str">
-        <f t="shared" ref="X74:AD74" si="41">X75</f>
+        <f t="shared" ref="X74:AD74" si="39">X75</f>
         <v>PSP - 1</v>
       </c>
       <c r="Y74" s="11" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="39"/>
         <v>[PSP]</v>
       </c>
       <c r="Z74" s="11" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="39"/>
         <v>multi</v>
       </c>
       <c r="AA74" s="11" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="39"/>
         <v>X</v>
       </c>
       <c r="AB74" s="11" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="39"/>
         <v>X</v>
       </c>
       <c r="AC74" s="11" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="39"/>
         <v>X</v>
       </c>
       <c r="AD74" s="11" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="39"/>
         <v>NOS</v>
       </c>
       <c r="AE74" s="1"/>
@@ -9768,25 +9769,25 @@
       </c>
       <c r="AP74" s="15"/>
       <c r="AQ74" s="12" t="str">
-        <f t="shared" ref="AQ74:AQ76" si="42">AF74&amp;AG74&amp;AH74&amp;AI74&amp;AJ74&amp;AO74</f>
+        <f>AF74&amp;AG74&amp;AH74&amp;AI74&amp;AJ74&amp;AO74</f>
         <v>10001100100000</v>
       </c>
       <c r="AR74" s="1">
-        <f t="shared" si="37"/>
+        <f>(BIN2DEC(AO74)+16*BIN2DEC(AJ74)+128*BIN2DEC(AI74)+512*BIN2DEC(AH74)+2048*BIN2DEC(AG74)+8192*BIN2DEC(AF74))</f>
         <v>8992</v>
       </c>
       <c r="AT74" s="66" t="str">
-        <f t="shared" ref="AT74:AT77" si="43">"1 "&amp;H74&amp;" INSTRUCTION _"&amp;B74</f>
+        <f>"1 "&amp;H74&amp;" INSTRUCTION _"&amp;B74</f>
         <v>1 56 INSTRUCTION _JMP</v>
       </c>
       <c r="AU74" s="66" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="36"/>
         <v>," JMP"</v>
       </c>
     </row>
-    <row r="75" spans="1:47" s="3" customFormat="1">
+    <row r="75" spans="1:47" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B75" s="11" t="s">
-        <v>258</v>
+        <v>342</v>
       </c>
       <c r="C75" s="11"/>
       <c r="D75" s="11">
@@ -9801,28 +9802,40 @@
       </c>
       <c r="G75" s="11"/>
       <c r="H75" s="7">
-        <f t="shared" si="39"/>
+        <f t="shared" si="37"/>
         <v>57</v>
       </c>
       <c r="I75" s="4" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="38"/>
         <v>39</v>
       </c>
       <c r="J75" s="11"/>
       <c r="K75" s="93" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="L75" s="3" t="s">
-        <v>270</v>
+        <v>343</v>
       </c>
       <c r="M75" s="12"/>
-      <c r="N75" s="11"/>
-      <c r="O75" s="11"/>
-      <c r="P75" s="11"/>
-      <c r="Q75" s="13"/>
+      <c r="N75" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="O75" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="P75" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q75" s="13" t="s">
+        <v>137</v>
+      </c>
       <c r="R75" s="12"/>
-      <c r="S75" s="11"/>
-      <c r="T75" s="13"/>
+      <c r="S75" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="T75" s="11" t="s">
+        <v>32</v>
+      </c>
       <c r="V75" s="11" t="s">
         <v>257</v>
       </c>
@@ -9834,27 +9847,27 @@
         <v>PSP - 1</v>
       </c>
       <c r="Y75" s="11" t="str">
-        <f t="shared" ref="Y75:AD75" si="44">Y7</f>
+        <f t="shared" ref="Y75:AD75" si="40">Y7</f>
         <v>[PSP]</v>
       </c>
       <c r="Z75" s="11" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="40"/>
         <v>multi</v>
       </c>
       <c r="AA75" s="11" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="40"/>
         <v>X</v>
       </c>
       <c r="AB75" s="11" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="40"/>
         <v>X</v>
       </c>
       <c r="AC75" s="11" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="40"/>
         <v>X</v>
       </c>
       <c r="AD75" s="11" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="40"/>
         <v>NOS</v>
       </c>
       <c r="AF75" s="11" t="str">
@@ -9899,23 +9912,19 @@
       </c>
       <c r="AP75" s="11"/>
       <c r="AQ75" s="12" t="str">
-        <f t="shared" si="42"/>
+        <f>AF75&amp;AG75&amp;AH75&amp;AI75&amp;AJ75&amp;AO75</f>
         <v>11001100100000</v>
       </c>
       <c r="AR75" s="1">
-        <f t="shared" si="37"/>
+        <f>(BIN2DEC(AO75)+16*BIN2DEC(AJ75)+128*BIN2DEC(AI75)+512*BIN2DEC(AH75)+2048*BIN2DEC(AG75)+8192*BIN2DEC(AF75))</f>
         <v>13088</v>
       </c>
-      <c r="AT75" s="66" t="str">
-        <f t="shared" si="43"/>
-        <v>1 57 INSTRUCTION _BSR</v>
-      </c>
-      <c r="AU75" s="66" t="str">
-        <f t="shared" si="38"/>
-        <v>," BSR"</v>
-      </c>
-    </row>
-    <row r="76" spans="1:47" s="3" customFormat="1">
+      <c r="AT75" s="66"/>
+      <c r="AU75" s="66" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="76" spans="1:47" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B76" s="11" t="s">
         <v>50</v>
       </c>
@@ -9932,19 +9941,19 @@
       </c>
       <c r="G76" s="11"/>
       <c r="H76" s="7">
-        <f t="shared" si="39"/>
+        <f t="shared" si="37"/>
         <v>58</v>
       </c>
       <c r="I76" s="4" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="38"/>
         <v>3A</v>
       </c>
       <c r="J76" s="11"/>
       <c r="K76" s="93" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="L76" s="3" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="M76" s="12"/>
       <c r="N76" s="11" t="s">
@@ -9977,27 +9986,27 @@
         <v>PSP - 1</v>
       </c>
       <c r="Y76" s="11" t="str">
-        <f t="shared" ref="Y76:AD76" si="45">Y7</f>
+        <f t="shared" ref="Y76:AD76" si="41">Y7</f>
         <v>[PSP]</v>
       </c>
       <c r="Z76" s="11" t="str">
-        <f t="shared" si="45"/>
+        <f t="shared" si="41"/>
         <v>multi</v>
       </c>
       <c r="AA76" s="11" t="str">
-        <f t="shared" si="45"/>
+        <f t="shared" si="41"/>
         <v>X</v>
       </c>
       <c r="AB76" s="11" t="str">
-        <f t="shared" si="45"/>
+        <f t="shared" si="41"/>
         <v>X</v>
       </c>
       <c r="AC76" s="11" t="str">
-        <f t="shared" si="45"/>
+        <f t="shared" si="41"/>
         <v>X</v>
       </c>
       <c r="AD76" s="11" t="str">
-        <f t="shared" si="45"/>
+        <f t="shared" si="41"/>
         <v>NOS</v>
       </c>
       <c r="AF76" s="11" t="str">
@@ -10042,25 +10051,25 @@
       </c>
       <c r="AP76" s="11"/>
       <c r="AQ76" s="12" t="str">
-        <f t="shared" si="42"/>
+        <f>AF76&amp;AG76&amp;AH76&amp;AI76&amp;AJ76&amp;AO76</f>
         <v>11001100100000</v>
       </c>
       <c r="AR76" s="1">
-        <f t="shared" si="37"/>
+        <f>(BIN2DEC(AO76)+16*BIN2DEC(AJ76)+128*BIN2DEC(AI76)+512*BIN2DEC(AH76)+2048*BIN2DEC(AG76)+8192*BIN2DEC(AF76))</f>
         <v>13088</v>
       </c>
       <c r="AT76" s="66" t="str">
-        <f t="shared" si="43"/>
+        <f>"1 "&amp;H76&amp;" INSTRUCTION _"&amp;B76</f>
         <v>1 58 INSTRUCTION _JSR</v>
       </c>
       <c r="AU76" s="66" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="36"/>
         <v>," JSR"</v>
       </c>
     </row>
-    <row r="77" spans="1:47" s="14" customFormat="1">
+    <row r="77" spans="1:47" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B77" s="15" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C77" s="15"/>
       <c r="D77" s="15">
@@ -10074,11 +10083,11 @@
       </c>
       <c r="G77" s="15"/>
       <c r="H77" s="7">
-        <f t="shared" si="39"/>
+        <f t="shared" si="37"/>
         <v>64</v>
       </c>
       <c r="I77" s="4" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="38"/>
         <v>40</v>
       </c>
       <c r="J77" s="15"/>
@@ -10130,12 +10139,12 @@
       <c r="AQ77" s="16"/>
       <c r="AR77" s="1"/>
       <c r="AT77" s="66" t="str">
-        <f t="shared" si="43"/>
+        <f>"1 "&amp;H77&amp;" INSTRUCTION _"&amp;B77</f>
         <v>1 64 INSTRUCTION _RTS</v>
       </c>
       <c r="AU77" s="67"/>
     </row>
-    <row r="78" spans="1:47" s="14" customFormat="1">
+    <row r="78" spans="1:47" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B78" s="15" t="s">
         <v>48</v>
       </c>
@@ -10151,11 +10160,11 @@
       </c>
       <c r="G78" s="15"/>
       <c r="H78" s="7">
-        <f t="shared" si="39"/>
+        <f t="shared" si="37"/>
         <v>128</v>
       </c>
       <c r="I78" s="4" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="38"/>
         <v>80</v>
       </c>
       <c r="J78" s="15"/>
@@ -10197,7 +10206,7 @@
       <c r="AT78" s="66"/>
       <c r="AU78" s="67"/>
     </row>
-    <row r="79" spans="1:47" s="14" customFormat="1">
+    <row r="79" spans="1:47" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B79" s="15" t="s">
         <v>49</v>
       </c>
@@ -10213,11 +10222,11 @@
       </c>
       <c r="G79" s="15"/>
       <c r="H79" s="7">
-        <f t="shared" si="39"/>
+        <f t="shared" si="37"/>
         <v>192</v>
       </c>
       <c r="I79" s="4" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="38"/>
         <v>C0</v>
       </c>
       <c r="J79" s="15"/>
@@ -10241,7 +10250,7 @@
       <c r="AT79" s="66"/>
       <c r="AU79" s="67"/>
     </row>
-    <row r="80" spans="1:47" s="14" customFormat="1">
+    <row r="80" spans="1:47" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B80" s="15"/>
       <c r="C80" s="15"/>
       <c r="D80" s="15"/>
@@ -10266,9 +10275,9 @@
       <c r="AT80" s="66"/>
       <c r="AU80" s="67"/>
     </row>
-    <row r="81" spans="1:47" s="14" customFormat="1">
+    <row r="81" spans="1:47" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A81" s="3" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B81" s="15"/>
       <c r="C81" s="15"/>
@@ -10294,9 +10303,9 @@
       <c r="AT81" s="66"/>
       <c r="AU81" s="67"/>
     </row>
-    <row r="82" spans="1:47" s="57" customFormat="1">
+    <row r="82" spans="1:47" s="57" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B82" s="58" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C82" s="58"/>
       <c r="D82" s="58"/>
@@ -10307,17 +10316,17 @@
       </c>
       <c r="G82" s="58"/>
       <c r="H82" s="59">
-        <f t="shared" ref="H82:H85" si="46">F82+E82*64+D82*128</f>
+        <f>F82+E82*64+D82*128</f>
         <v>59</v>
       </c>
       <c r="I82" s="58" t="str">
-        <f t="shared" ref="I82:I85" si="47">DEC2HEX(H82)</f>
+        <f>DEC2HEX(H82)</f>
         <v>3B</v>
       </c>
       <c r="J82" s="58"/>
       <c r="K82" s="97"/>
       <c r="L82" s="57" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="M82" s="60"/>
       <c r="N82" s="58"/>
@@ -10330,14 +10339,14 @@
       <c r="V82" s="58"/>
       <c r="AQ82" s="60"/>
       <c r="AT82" s="68" t="str">
-        <f t="shared" ref="AT82" si="48">"1 "&amp;H82&amp;" OPCODE _"&amp;B82</f>
+        <f>"1 "&amp;H82&amp;" OPCODE _"&amp;B82</f>
         <v>1 59 OPCODE _TRAP</v>
       </c>
       <c r="AU82" s="69"/>
     </row>
-    <row r="83" spans="1:47" s="57" customFormat="1">
+    <row r="83" spans="1:47" s="57" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B83" s="58" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C83" s="58"/>
       <c r="D83" s="58"/>
@@ -10348,17 +10357,17 @@
       </c>
       <c r="G83" s="58"/>
       <c r="H83" s="59">
-        <f t="shared" si="46"/>
+        <f>F83+E83*64+D83*128</f>
         <v>60</v>
       </c>
       <c r="I83" s="58" t="str">
-        <f t="shared" si="47"/>
+        <f>DEC2HEX(H83)</f>
         <v>3C</v>
       </c>
       <c r="J83" s="58"/>
       <c r="K83" s="97"/>
       <c r="L83" s="57" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="M83" s="60"/>
       <c r="N83" s="58"/>
@@ -10371,14 +10380,14 @@
       <c r="V83" s="58"/>
       <c r="AQ83" s="60"/>
       <c r="AT83" s="66" t="str">
-        <f t="shared" ref="AT83:AT84" si="49">"1 "&amp;H83&amp;" INSTRUCTION _"&amp;B83</f>
+        <f>"1 "&amp;H83&amp;" INSTRUCTION _"&amp;B83</f>
         <v>1 60 INSTRUCTION _RTS_TRAP</v>
       </c>
       <c r="AU83" s="69"/>
     </row>
-    <row r="84" spans="1:47" s="57" customFormat="1">
+    <row r="84" spans="1:47" s="57" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B84" s="58" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C84" s="58"/>
       <c r="D84" s="58"/>
@@ -10389,17 +10398,17 @@
       </c>
       <c r="G84" s="58"/>
       <c r="H84" s="59">
-        <f t="shared" si="46"/>
+        <f>F84+E84*64+D84*128</f>
         <v>61</v>
       </c>
       <c r="I84" s="58" t="str">
-        <f t="shared" si="47"/>
+        <f>DEC2HEX(H84)</f>
         <v>3D</v>
       </c>
       <c r="J84" s="58"/>
       <c r="K84" s="97"/>
       <c r="L84" s="57" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="M84" s="60"/>
       <c r="N84" s="58"/>
@@ -10412,12 +10421,12 @@
       <c r="V84" s="58"/>
       <c r="AQ84" s="60"/>
       <c r="AT84" s="66" t="str">
-        <f t="shared" si="49"/>
+        <f>"1 "&amp;H84&amp;" INSTRUCTION _"&amp;B84</f>
         <v>1 61 INSTRUCTION _RTI</v>
       </c>
       <c r="AU84" s="69"/>
     </row>
-    <row r="85" spans="1:47" s="57" customFormat="1">
+    <row r="85" spans="1:47" s="57" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B85" s="58"/>
       <c r="C85" s="58"/>
       <c r="D85" s="58"/>
@@ -10428,11 +10437,11 @@
       </c>
       <c r="G85" s="58"/>
       <c r="H85" s="59">
-        <f t="shared" si="46"/>
+        <f>F85+E85*64+D85*128</f>
         <v>62</v>
       </c>
       <c r="I85" s="58" t="str">
-        <f t="shared" si="47"/>
+        <f>DEC2HEX(H85)</f>
         <v>3E</v>
       </c>
       <c r="J85" s="58"/>
@@ -10448,7 +10457,7 @@
       <c r="AQ85" s="60"/>
       <c r="AT85" s="62"/>
     </row>
-    <row r="86" spans="1:47" s="57" customFormat="1">
+    <row r="86" spans="1:47" s="57" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B86" s="58"/>
       <c r="C86" s="58"/>
       <c r="D86" s="58"/>
@@ -10470,7 +10479,7 @@
       <c r="AQ86" s="60"/>
       <c r="AT86" s="62"/>
     </row>
-    <row r="87" spans="1:47" s="3" customFormat="1">
+    <row r="87" spans="1:47" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A87" s="3" t="s">
         <v>145</v>
       </c>
@@ -10496,9 +10505,9 @@
       <c r="AR87" s="1"/>
       <c r="AT87" s="53"/>
     </row>
-    <row r="88" spans="1:47" s="47" customFormat="1">
+    <row r="88" spans="1:47" s="47" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B88" s="48" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C88" s="48"/>
       <c r="D88" s="48">
@@ -10525,7 +10534,7 @@
         <v>115</v>
       </c>
       <c r="L88" s="47" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="M88" s="22"/>
       <c r="N88" s="48"/>
@@ -10604,18 +10613,18 @@
       </c>
       <c r="AP88" s="48"/>
       <c r="AQ88" s="22" t="str">
-        <f t="shared" ref="AQ88:AQ92" si="50">AF88&amp;AG88&amp;AH88&amp;AI88&amp;AJ88&amp;AO88</f>
+        <f>AF88&amp;AG88&amp;AH88&amp;AI88&amp;AJ88&amp;AO88</f>
         <v>00010010100111</v>
       </c>
       <c r="AR88" s="47">
-        <f t="shared" si="37"/>
+        <f>(BIN2DEC(AO88)+16*BIN2DEC(AJ88)+128*BIN2DEC(AI88)+512*BIN2DEC(AH88)+2048*BIN2DEC(AG88)+8192*BIN2DEC(AF88))</f>
         <v>1191</v>
       </c>
       <c r="AT88" s="53"/>
     </row>
-    <row r="89" spans="1:47" s="47" customFormat="1">
+    <row r="89" spans="1:47" s="47" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B89" s="48" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C89" s="48"/>
       <c r="D89" s="48">
@@ -10642,7 +10651,7 @@
         <v>96</v>
       </c>
       <c r="L89" s="47" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="M89" s="22"/>
       <c r="N89" s="48"/>
@@ -10721,18 +10730,18 @@
       </c>
       <c r="AP89" s="48"/>
       <c r="AQ89" s="22" t="str">
-        <f t="shared" si="50"/>
+        <f>AF89&amp;AG89&amp;AH89&amp;AI89&amp;AJ89&amp;AO89</f>
         <v>00000000100111</v>
       </c>
       <c r="AR89" s="47">
-        <f t="shared" si="37"/>
+        <f>(BIN2DEC(AO89)+16*BIN2DEC(AJ89)+128*BIN2DEC(AI89)+512*BIN2DEC(AH89)+2048*BIN2DEC(AG89)+8192*BIN2DEC(AF89))</f>
         <v>39</v>
       </c>
       <c r="AT89" s="53"/>
     </row>
-    <row r="90" spans="1:47" s="47" customFormat="1">
+    <row r="90" spans="1:47" s="47" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B90" s="48" t="s">
-        <v>343</v>
+        <v>300</v>
       </c>
       <c r="C90" s="48"/>
       <c r="D90" s="48">
@@ -10850,18 +10859,17 @@
       </c>
       <c r="AP90" s="48"/>
       <c r="AQ90" s="22" t="str">
-        <f t="shared" si="50"/>
+        <f>AF90&amp;AG90&amp;AH90&amp;AI90&amp;AJ90&amp;AO90</f>
         <v>00000111100000</v>
       </c>
       <c r="AR90" s="47">
-        <f t="shared" si="37"/>
-        <v>480</v>
+        <v>0</v>
       </c>
       <c r="AT90" s="53"/>
     </row>
-    <row r="91" spans="1:47" s="47" customFormat="1" ht="14.25" customHeight="1">
+    <row r="91" spans="1:47" s="47" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B91" s="48" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="C91" s="48"/>
       <c r="D91" s="48">
@@ -10979,18 +10987,17 @@
       </c>
       <c r="AP91" s="48"/>
       <c r="AQ91" s="22" t="str">
-        <f t="shared" si="50"/>
+        <f>AF91&amp;AG91&amp;AH91&amp;AI91&amp;AJ91&amp;AO91</f>
         <v>00000111110000</v>
       </c>
       <c r="AR91" s="47">
-        <f t="shared" si="37"/>
-        <v>496</v>
+        <v>0</v>
       </c>
       <c r="AT91" s="53"/>
     </row>
-    <row r="92" spans="1:47" s="47" customFormat="1">
+    <row r="92" spans="1:47" s="47" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B92" s="48" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="C92" s="48"/>
       <c r="D92" s="48">
@@ -11013,10 +11020,10 @@
       </c>
       <c r="J92" s="48"/>
       <c r="K92" s="98" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="L92" s="47" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="M92" s="22"/>
       <c r="N92" s="48" t="s">
@@ -11109,27 +11116,27 @@
       </c>
       <c r="AP92" s="48"/>
       <c r="AQ92" s="22" t="str">
-        <f t="shared" si="50"/>
+        <f>AF92&amp;AG92&amp;AH92&amp;AI92&amp;AJ92&amp;AO92</f>
         <v>11000000000000</v>
       </c>
       <c r="AR92" s="47">
-        <f t="shared" ref="AR92" si="51">(BIN2DEC(AO92)+16*BIN2DEC(AJ92)+128*BIN2DEC(AI92)+512*BIN2DEC(AH92)+2048*BIN2DEC(AG92)+8192*BIN2DEC(AF92))</f>
+        <f>(BIN2DEC(AO92)+16*BIN2DEC(AJ92)+128*BIN2DEC(AI92)+512*BIN2DEC(AH92)+2048*BIN2DEC(AG92)+8192*BIN2DEC(AF92))</f>
         <v>12288</v>
       </c>
       <c r="AT92" s="56"/>
     </row>
-    <row r="94" spans="1:47">
+    <row r="94" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A94" s="8" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="95" spans="1:47">
+    <row r="95" spans="1:47" x14ac:dyDescent="0.2">
       <c r="B95" s="8" t="s">
         <v>252</v>
       </c>
       <c r="C95" s="8"/>
     </row>
-    <row r="96" spans="1:47" s="39" customFormat="1">
+    <row r="96" spans="1:47" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B96" s="9" t="s">
         <v>253</v>
       </c>
@@ -11151,13 +11158,13 @@
       <c r="AQ96" s="41"/>
       <c r="AT96" s="54"/>
     </row>
-    <row r="97" spans="2:3">
+    <row r="97" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B97" s="57" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C97" s="22"/>
     </row>
-    <row r="98" spans="2:3">
+    <row r="98" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B98" s="22" t="s">
         <v>144</v>
       </c>
@@ -11172,28 +11179,28 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.28515625" customWidth="1"/>
     <col min="3" max="6" width="9.140625" style="44"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B3" s="63"/>
       <c r="C3" s="82" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D3" s="82" t="s">
         <v>149</v>
@@ -11221,7 +11228,7 @@
       </c>
       <c r="L3" s="83"/>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B4" s="84">
         <v>0</v>
       </c>
@@ -11256,7 +11263,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B5" s="84">
         <v>1</v>
       </c>
@@ -11291,7 +11298,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B6" s="84">
         <v>2</v>
       </c>
@@ -11315,7 +11322,7 @@
         <v>26</v>
       </c>
       <c r="J6" s="73" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="K6" s="106" t="s">
         <v>247</v>
@@ -11324,7 +11331,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B7" s="84">
         <v>3</v>
       </c>
@@ -11357,7 +11364,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B8" s="84">
         <v>4</v>
       </c>
@@ -11384,7 +11391,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B9" s="84">
         <v>5</v>
       </c>
@@ -11402,7 +11409,7 @@
         <v>127</v>
       </c>
       <c r="J9" s="73" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="K9" s="74" t="s">
         <v>191</v>
@@ -11411,7 +11418,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B10" s="84">
         <v>6</v>
       </c>
@@ -11438,7 +11445,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B11" s="84">
         <v>7</v>
       </c>
@@ -11447,7 +11454,7 @@
       <c r="E11" s="76"/>
       <c r="F11" s="76"/>
       <c r="G11" s="73" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="H11" s="73" t="s">
         <v>53</v>
@@ -11465,7 +11472,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B12" s="84">
         <v>8</v>
       </c>
@@ -11474,7 +11481,7 @@
       <c r="E12" s="76"/>
       <c r="F12" s="76"/>
       <c r="G12" s="73" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="H12" s="64"/>
       <c r="I12" s="64"/>
@@ -11484,7 +11491,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B13" s="84">
         <v>9</v>
       </c>
@@ -11493,7 +11500,7 @@
       <c r="E13" s="76"/>
       <c r="F13" s="76"/>
       <c r="G13" s="73" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="H13" s="64"/>
       <c r="I13" s="64"/>
@@ -11503,7 +11510,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B14" s="84">
         <v>10</v>
       </c>
@@ -11522,7 +11529,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B15" s="84">
         <v>11</v>
       </c>
@@ -11541,7 +11548,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B16" s="84">
         <v>12</v>
       </c>
@@ -11560,7 +11567,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="2:12">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B17" s="84">
         <v>13</v>
       </c>
@@ -11579,7 +11586,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="2:12">
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B18" s="84">
         <v>14</v>
       </c>
@@ -11598,7 +11605,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="2:12">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B19" s="87">
         <v>15</v>
       </c>
@@ -11617,7 +11624,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="2:12">
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
         <v>255</v>
       </c>
@@ -11649,7 +11656,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="2:12">
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B22" s="4" t="s">
         <v>256</v>
       </c>
@@ -11691,14 +11698,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.25"/>
+  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="2.28515625" style="1" customWidth="1"/>
     <col min="2" max="2" width="3.42578125" style="1" customWidth="1"/>
@@ -11713,23 +11720,23 @@
     <col min="23" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="15">
+    <row r="1" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="3" spans="1:22">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B3" s="23" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B4" s="23"/>
       <c r="C4" s="23" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="5" spans="1:22" s="23" customFormat="1">
+    <row r="5" spans="1:22" s="23" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D5" s="28" t="s">
         <v>156</v>
       </c>
@@ -11749,7 +11756,7 @@
       <c r="K5" s="7"/>
       <c r="L5" s="7"/>
     </row>
-    <row r="6" spans="1:22">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
       <c r="D6" s="1">
         <v>2</v>
       </c>
@@ -11771,7 +11778,7 @@
       <c r="K6" s="4"/>
       <c r="L6" s="4"/>
     </row>
-    <row r="7" spans="1:22">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
       <c r="D7" s="1">
         <v>2</v>
       </c>
@@ -11791,7 +11798,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:22" s="3" customFormat="1">
+    <row r="8" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D8" s="3">
         <v>2</v>
       </c>
@@ -11811,7 +11818,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:22">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
       <c r="D9" s="30">
         <f>SUM(D6:D8)</f>
         <v>6</v>
@@ -11821,18 +11828,18 @@
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
     </row>
-    <row r="10" spans="1:22">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
     </row>
-    <row r="11" spans="1:22" s="14" customFormat="1">
+    <row r="11" spans="1:22" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B11" s="31"/>
       <c r="C11" s="31" t="s">
         <v>158</v>
       </c>
       <c r="F11" s="35"/>
     </row>
-    <row r="12" spans="1:22" s="14" customFormat="1">
+    <row r="12" spans="1:22" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D12" s="14">
         <v>1</v>
       </c>
@@ -11843,25 +11850,25 @@
         <v>30</v>
       </c>
       <c r="H12" s="15" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="13" spans="1:22" s="14" customFormat="1" ht="11.25" customHeight="1">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" s="14" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D13" s="32">
         <f>SUM(D12:D12)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:22" s="14" customFormat="1" ht="12.75" customHeight="1">
+    <row r="14" spans="1:22" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K14" s="15"/>
       <c r="L14" s="15"/>
     </row>
-    <row r="15" spans="1:22">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B15" s="23" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="16" spans="1:22">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
       <c r="D16" s="28" t="s">
         <v>156</v>
       </c>
@@ -11914,13 +11921,13 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="2:22">
+    <row r="17" spans="2:22" x14ac:dyDescent="0.2">
       <c r="D17" s="29">
         <v>4</v>
       </c>
       <c r="E17" s="29"/>
       <c r="F17" s="24" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="G17" s="4" t="s">
         <v>20</v>
@@ -11971,7 +11978,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="2:22">
+    <row r="18" spans="2:22" x14ac:dyDescent="0.2">
       <c r="D18" s="29"/>
       <c r="G18" s="4" t="s">
         <v>205</v>
@@ -12022,7 +12029,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="19" spans="2:22">
+    <row r="19" spans="2:22" x14ac:dyDescent="0.2">
       <c r="D19" s="1">
         <v>3</v>
       </c>
@@ -12054,7 +12061,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="20" spans="2:22">
+    <row r="20" spans="2:22" x14ac:dyDescent="0.2">
       <c r="D20" s="1">
         <v>3</v>
       </c>
@@ -12086,7 +12093,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="21" spans="2:22">
+    <row r="21" spans="2:22" x14ac:dyDescent="0.2">
       <c r="D21" s="1">
         <v>1</v>
       </c>
@@ -12118,7 +12125,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="22" spans="2:22">
+    <row r="22" spans="2:22" x14ac:dyDescent="0.2">
       <c r="D22" s="1">
         <v>3</v>
       </c>
@@ -12150,22 +12157,22 @@
         <v>200</v>
       </c>
     </row>
-    <row r="23" spans="2:22">
+    <row r="23" spans="2:22" x14ac:dyDescent="0.2">
       <c r="D23" s="30">
         <f>MAX(D17:D21)+D22</f>
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="2:22">
+    <row r="24" spans="2:22" x14ac:dyDescent="0.2">
       <c r="D24" s="36"/>
     </row>
-    <row r="25" spans="2:22">
+    <row r="25" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B25" s="23" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="D25" s="36"/>
     </row>
-    <row r="26" spans="2:22">
+    <row r="26" spans="2:22" x14ac:dyDescent="0.2">
       <c r="D26" s="28" t="s">
         <v>156</v>
       </c>
@@ -12183,13 +12190,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="2:22">
+    <row r="27" spans="2:22" x14ac:dyDescent="0.2">
       <c r="D27" s="29">
         <v>1</v>
       </c>
       <c r="E27" s="23"/>
       <c r="F27" s="24" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="G27" s="4" t="s">
         <v>30</v>
@@ -12200,7 +12207,7 @@
       <c r="I27" s="7"/>
       <c r="J27" s="7"/>
     </row>
-    <row r="28" spans="2:22">
+    <row r="28" spans="2:22" x14ac:dyDescent="0.2">
       <c r="D28" s="101">
         <f>SUM(D27)</f>
         <v>1</v>
@@ -12211,7 +12218,7 @@
       <c r="I28" s="7"/>
       <c r="J28" s="7"/>
     </row>
-    <row r="29" spans="2:22">
+    <row r="29" spans="2:22" x14ac:dyDescent="0.2">
       <c r="D29" s="29"/>
       <c r="E29" s="23"/>
       <c r="G29" s="4"/>
@@ -12219,7 +12226,7 @@
       <c r="I29" s="7"/>
       <c r="J29" s="7"/>
     </row>
-    <row r="30" spans="2:22" s="26" customFormat="1">
+    <row r="30" spans="2:22" s="26" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D30" s="38"/>
       <c r="F30" s="37"/>
       <c r="G30" s="27"/>
@@ -12228,23 +12235,23 @@
       <c r="J30" s="27"/>
       <c r="K30" s="27"/>
     </row>
-    <row r="31" spans="2:22">
+    <row r="31" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B31" s="23" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D31" s="36"/>
       <c r="F31" s="43" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="G31" s="33"/>
       <c r="H31" s="33"/>
       <c r="J31" s="33" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="K31" s="19"/>
       <c r="L31" s="19"/>
     </row>
-    <row r="32" spans="2:22">
+    <row r="32" spans="2:22" x14ac:dyDescent="0.2">
       <c r="C32" s="1" t="s">
         <v>236</v>
       </c>
@@ -12264,7 +12271,7 @@
       </c>
       <c r="K32" s="4"/>
     </row>
-    <row r="33" spans="1:12">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C33" s="1" t="s">
         <v>237</v>
       </c>
@@ -12294,7 +12301,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:12">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C34" s="1" t="s">
         <v>238</v>
       </c>
@@ -12325,9 +12332,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:12">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C35" s="1" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="D35" s="1">
         <v>1</v>
@@ -12345,37 +12352,37 @@
       <c r="K35" s="4"/>
       <c r="L35" s="4"/>
     </row>
-    <row r="36" spans="1:12">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D36" s="30">
         <f>SUM(D32:D35)</f>
         <v>14</v>
       </c>
     </row>
-    <row r="38" spans="1:12">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B38" s="31" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D39" s="32">
         <f>D13</f>
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:12">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B41" s="1" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A42" s="14" t="s">
+        <v>330</v>
+      </c>
+      <c r="B42" s="14" t="s">
         <v>329</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12">
-      <c r="A42" s="14" t="s">
-        <v>332</v>
-      </c>
-      <c r="B42" s="14" t="s">
-        <v>331</v>
       </c>
     </row>
   </sheetData>
@@ -12385,14 +12392,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.25"/>
+  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.42578125" style="1" customWidth="1"/>
     <col min="2" max="2" width="17.28515625" style="4" customWidth="1"/>
@@ -12410,12 +12417,12 @@
     <col min="21" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="15">
+    <row r="1" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="C4" s="33" t="s">
         <v>177</v>
       </c>
@@ -12442,7 +12449,7 @@
       </c>
       <c r="T4" s="19"/>
     </row>
-    <row r="5" spans="1:20">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="C5" s="4" t="s">
         <v>179</v>
       </c>
@@ -12483,7 +12490,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="6" spans="1:20">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
@@ -12506,7 +12513,7 @@
       <c r="S6" s="4"/>
       <c r="T6" s="4"/>
     </row>
-    <row r="7" spans="1:20">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>31</v>
       </c>
@@ -12527,7 +12534,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:20">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>30</v>
       </c>
@@ -12554,7 +12561,7 @@
       <c r="S8" s="4"/>
       <c r="T8" s="4"/>
     </row>
-    <row r="9" spans="1:20">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>11</v>
       </c>
@@ -12575,7 +12582,7 @@
       <c r="P9" s="4"/>
       <c r="Q9" s="4"/>
     </row>
-    <row r="10" spans="1:20">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
         <v>12</v>
       </c>
@@ -12596,7 +12603,7 @@
       <c r="P10" s="4"/>
       <c r="Q10" s="4"/>
     </row>
-    <row r="11" spans="1:20">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
         <v>13</v>
       </c>
@@ -12617,7 +12624,7 @@
       <c r="P11" s="4"/>
       <c r="Q11" s="4"/>
     </row>
-    <row r="12" spans="1:20">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12" s="17" t="s">
         <v>14</v>
       </c>
@@ -12634,7 +12641,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:20">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13" s="15" t="s">
         <v>15</v>
       </c>
@@ -12653,7 +12660,7 @@
       <c r="P13" s="4"/>
       <c r="Q13" s="4"/>
     </row>
-    <row r="14" spans="1:20">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A14" s="15" t="s">
         <v>42</v>
       </c>
@@ -12672,7 +12679,7 @@
       <c r="M14" s="4"/>
       <c r="N14" s="4"/>
     </row>
-    <row r="15" spans="1:20">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A15" s="21" t="s">
         <v>43</v>
       </c>
@@ -12691,7 +12698,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:20">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>16</v>
       </c>
@@ -12710,7 +12717,7 @@
       <c r="M16" s="4"/>
       <c r="N16" s="4"/>
     </row>
-    <row r="17" spans="1:20">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A17" s="11" t="s">
         <v>52</v>
       </c>
@@ -12729,7 +12736,7 @@
       <c r="M17" s="4"/>
       <c r="N17" s="4"/>
     </row>
-    <row r="18" spans="1:20">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A18" s="11" t="s">
         <v>53</v>
       </c>
@@ -12750,7 +12757,7 @@
       <c r="S18" s="4"/>
       <c r="T18" s="4"/>
     </row>
-    <row r="19" spans="1:20">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A19" s="11" t="s">
         <v>54</v>
       </c>
@@ -12769,7 +12776,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:20">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>55</v>
       </c>
@@ -12788,7 +12795,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:20">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>23</v>
       </c>
@@ -12807,7 +12814,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:20">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>24</v>
       </c>
@@ -12826,7 +12833,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:20">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>25</v>
       </c>
@@ -12845,7 +12852,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:20">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>26</v>
       </c>
@@ -12864,7 +12871,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:20">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A25" s="15" t="s">
         <v>143</v>
       </c>
@@ -12883,7 +12890,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:20">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A26" s="15" t="s">
         <v>142</v>
       </c>
@@ -12902,7 +12909,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:20">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>219</v>
       </c>
@@ -12919,7 +12926,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:20">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
         <v>220</v>
       </c>
@@ -12942,62 +12949,62 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="109.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="103" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="103" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="103"/>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="103" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
-      <c r="A2" s="103" t="s">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="103" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
-      <c r="A3" s="103"/>
-    </row>
-    <row r="4" spans="1:1">
-      <c r="A4" s="103" t="s">
+    <row r="6" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="103" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
-      <c r="A5" s="103" t="s">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="103" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="104" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="103"/>
+    </row>
+    <row r="10" spans="1:1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10" s="104" t="s">
         <v>338</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" ht="30">
-      <c r="A6" s="103" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1">
-      <c r="A7" s="103" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" ht="45">
-      <c r="A8" s="104" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1">
-      <c r="A9" s="103"/>
-    </row>
-    <row r="10" spans="1:1" ht="60">
-      <c r="A10" s="104" t="s">
-        <v>340</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update of draft paper describing the  32 bit databus
</commit_message>
<xml_diff>
--- a/Resources/Instruction Set.xlsx
+++ b/Resources/Instruction Set.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="120" windowWidth="18195" windowHeight="8250" tabRatio="681"/>
@@ -16,7 +16,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">OPCODE_encoding!$A$3:$L$92</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -1098,8 +1098,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="36">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="36" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1830,6 +1830,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1864,6 +1865,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2039,20 +2041,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:AU98"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="9" ySplit="4" topLeftCell="M32" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="9" ySplit="4" topLeftCell="P32" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="S19" sqref="S19"/>
+      <selection pane="bottomRight" activeCell="H69" sqref="H69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.25"/>
+  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="1.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="11" style="4" customWidth="1"/>
@@ -2086,14 +2088,14 @@
     <col min="48" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" ht="15">
+    <row r="1" spans="1:47" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="45" t="s">
         <v>312</v>
       </c>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:47" ht="5.25" customHeight="1"/>
-    <row r="3" spans="1:47" s="22" customFormat="1">
+    <row r="2" spans="1:47" ht="5.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="1:47" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B3" s="7" t="s">
         <v>249</v>
       </c>
@@ -2158,7 +2160,7 @@
       </c>
       <c r="AU3" s="32"/>
     </row>
-    <row r="4" spans="1:47">
+    <row r="4" spans="1:47" x14ac:dyDescent="0.2">
       <c r="D4" s="7">
         <v>7</v>
       </c>
@@ -2259,12 +2261,12 @@
         <v>304</v>
       </c>
     </row>
-    <row r="5" spans="1:47">
+    <row r="5" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="6" spans="1:47">
+    <row r="6" spans="1:47" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
         <v>41</v>
       </c>
@@ -2393,7 +2395,7 @@
         <v>," NOP"</v>
       </c>
     </row>
-    <row r="7" spans="1:47">
+    <row r="7" spans="1:47" x14ac:dyDescent="0.2">
       <c r="B7" s="4" t="s">
         <v>2</v>
       </c>
@@ -2523,7 +2525,7 @@
         <v>," DROP"</v>
       </c>
     </row>
-    <row r="8" spans="1:47">
+    <row r="8" spans="1:47" x14ac:dyDescent="0.2">
       <c r="B8" s="4" t="s">
         <v>0</v>
       </c>
@@ -2653,7 +2655,7 @@
         <v>," DUP"</v>
       </c>
     </row>
-    <row r="9" spans="1:47" s="14" customFormat="1">
+    <row r="9" spans="1:47" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B9" s="15" t="s">
         <v>1</v>
       </c>
@@ -2785,7 +2787,7 @@
         <v>," ?DUP"</v>
       </c>
     </row>
-    <row r="10" spans="1:47">
+    <row r="10" spans="1:47" x14ac:dyDescent="0.2">
       <c r="B10" s="4" t="s">
         <v>3</v>
       </c>
@@ -2915,7 +2917,7 @@
         <v>," SWAP"</v>
       </c>
     </row>
-    <row r="11" spans="1:47">
+    <row r="11" spans="1:47" x14ac:dyDescent="0.2">
       <c r="B11" s="4" t="s">
         <v>4</v>
       </c>
@@ -3045,7 +3047,7 @@
         <v>," OVER"</v>
       </c>
     </row>
-    <row r="12" spans="1:47">
+    <row r="12" spans="1:47" x14ac:dyDescent="0.2">
       <c r="B12" s="4" t="s">
         <v>5</v>
       </c>
@@ -3175,7 +3177,7 @@
         <v>," NIP"</v>
       </c>
     </row>
-    <row r="13" spans="1:47">
+    <row r="13" spans="1:47" x14ac:dyDescent="0.2">
       <c r="B13" s="4" t="s">
         <v>6</v>
       </c>
@@ -3305,7 +3307,7 @@
         <v>," ROT"</v>
       </c>
     </row>
-    <row r="14" spans="1:47" s="3" customFormat="1">
+    <row r="14" spans="1:47" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B14" s="11" t="s">
         <v>7</v>
       </c>
@@ -3442,7 +3444,7 @@
         <v>," &gt;R"</v>
       </c>
     </row>
-    <row r="15" spans="1:47">
+    <row r="15" spans="1:47" x14ac:dyDescent="0.2">
       <c r="B15" s="4" t="s">
         <v>8</v>
       </c>
@@ -3572,7 +3574,7 @@
         <v>," R@"</v>
       </c>
     </row>
-    <row r="16" spans="1:47" s="3" customFormat="1">
+    <row r="16" spans="1:47" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B16" s="11" t="s">
         <v>9</v>
       </c>
@@ -3709,7 +3711,7 @@
         <v>," R&gt;"</v>
       </c>
     </row>
-    <row r="17" spans="1:47" s="3" customFormat="1">
+    <row r="17" spans="1:47" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B17" s="11" t="s">
         <v>318</v>
       </c>
@@ -3834,7 +3836,7 @@
         <v>," PSP@"</v>
       </c>
     </row>
-    <row r="18" spans="1:47" s="3" customFormat="1">
+    <row r="18" spans="1:47" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B18" s="11" t="s">
         <v>319</v>
       </c>
@@ -3959,7 +3961,7 @@
         <v>," RSP@"</v>
       </c>
     </row>
-    <row r="19" spans="1:47">
+    <row r="19" spans="1:47" x14ac:dyDescent="0.2">
       <c r="B19" s="11" t="s">
         <v>320</v>
       </c>
@@ -4074,7 +4076,7 @@
         <v>," PSP!"</v>
       </c>
     </row>
-    <row r="20" spans="1:47">
+    <row r="20" spans="1:47" x14ac:dyDescent="0.2">
       <c r="B20" s="11" t="s">
         <v>340</v>
       </c>
@@ -4189,18 +4191,18 @@
         <v>," RSP!"</v>
       </c>
     </row>
-    <row r="21" spans="1:47">
+    <row r="21" spans="1:47" x14ac:dyDescent="0.2">
       <c r="AT21" s="64"/>
       <c r="AU21" s="64"/>
     </row>
-    <row r="22" spans="1:47">
+    <row r="22" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>10</v>
       </c>
       <c r="AT22" s="64"/>
       <c r="AU22" s="64"/>
     </row>
-    <row r="23" spans="1:47">
+    <row r="23" spans="1:47" x14ac:dyDescent="0.2">
       <c r="B23" s="6" t="s">
         <v>11</v>
       </c>
@@ -4332,7 +4334,7 @@
         <v>," +"</v>
       </c>
     </row>
-    <row r="24" spans="1:47">
+    <row r="24" spans="1:47" x14ac:dyDescent="0.2">
       <c r="B24" s="6" t="s">
         <v>12</v>
       </c>
@@ -4464,7 +4466,7 @@
         <v>," -"</v>
       </c>
     </row>
-    <row r="25" spans="1:47">
+    <row r="25" spans="1:47" x14ac:dyDescent="0.2">
       <c r="B25" s="4" t="s">
         <v>16</v>
       </c>
@@ -4595,7 +4597,7 @@
         <v>," NEGATE"</v>
       </c>
     </row>
-    <row r="26" spans="1:47" s="3" customFormat="1">
+    <row r="26" spans="1:47" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B26" s="11" t="s">
         <v>52</v>
       </c>
@@ -4732,7 +4734,7 @@
         <v>," 1+"</v>
       </c>
     </row>
-    <row r="27" spans="1:47" s="3" customFormat="1">
+    <row r="27" spans="1:47" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B27" s="13" t="s">
         <v>53</v>
       </c>
@@ -4869,7 +4871,7 @@
         <v>," 1-"</v>
       </c>
     </row>
-    <row r="28" spans="1:47" s="3" customFormat="1">
+    <row r="28" spans="1:47" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B28" s="13" t="s">
         <v>54</v>
       </c>
@@ -5006,7 +5008,7 @@
         <v>," 2*"</v>
       </c>
     </row>
-    <row r="29" spans="1:47" s="3" customFormat="1">
+    <row r="29" spans="1:47" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B29" s="13" t="s">
         <v>55</v>
       </c>
@@ -5143,7 +5145,7 @@
         <v>," 2/"</v>
       </c>
     </row>
-    <row r="30" spans="1:47" s="3" customFormat="1">
+    <row r="30" spans="1:47" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B30" s="11" t="s">
         <v>278</v>
       </c>
@@ -5280,7 +5282,7 @@
         <v>," MULTS"</v>
       </c>
     </row>
-    <row r="31" spans="1:47" s="3" customFormat="1">
+    <row r="31" spans="1:47" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B31" s="11" t="s">
         <v>279</v>
       </c>
@@ -5417,7 +5419,7 @@
         <v>," MULTU"</v>
       </c>
     </row>
-    <row r="32" spans="1:47" s="3" customFormat="1">
+    <row r="32" spans="1:47" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B32" s="11" t="s">
         <v>219</v>
       </c>
@@ -5555,7 +5557,7 @@
         <v>," ADDX"</v>
       </c>
     </row>
-    <row r="33" spans="1:47" s="3" customFormat="1">
+    <row r="33" spans="1:47" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B33" s="11" t="s">
         <v>220</v>
       </c>
@@ -5693,7 +5695,7 @@
         <v>," SUBX"</v>
       </c>
     </row>
-    <row r="34" spans="1:47" s="14" customFormat="1">
+    <row r="34" spans="1:47" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B34" s="15" t="s">
         <v>280</v>
       </c>
@@ -5837,7 +5839,7 @@
         <v>," DIVS"</v>
       </c>
     </row>
-    <row r="35" spans="1:47" s="14" customFormat="1" ht="14.25" customHeight="1">
+    <row r="35" spans="1:47" s="14" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="15" t="s">
         <v>281</v>
       </c>
@@ -5981,12 +5983,12 @@
         <v>," DIVU"</v>
       </c>
     </row>
-    <row r="36" spans="1:47">
+    <row r="36" spans="1:47" x14ac:dyDescent="0.2">
       <c r="E36" s="13"/>
       <c r="AT36" s="64"/>
       <c r="AU36" s="64"/>
     </row>
-    <row r="37" spans="1:47">
+    <row r="37" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>17</v>
       </c>
@@ -5994,7 +5996,7 @@
       <c r="AT37" s="64"/>
       <c r="AU37" s="64"/>
     </row>
-    <row r="38" spans="1:47">
+    <row r="38" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A38" s="4"/>
       <c r="B38" s="6" t="s">
         <v>20</v>
@@ -6128,7 +6130,7 @@
         <v>," ="</v>
       </c>
     </row>
-    <row r="39" spans="1:47" s="3" customFormat="1">
+    <row r="39" spans="1:47" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="4"/>
       <c r="B39" s="13" t="s">
         <v>44</v>
@@ -6266,7 +6268,7 @@
         <v>," &lt;&gt;"</v>
       </c>
     </row>
-    <row r="40" spans="1:47">
+    <row r="40" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A40" s="4"/>
       <c r="B40" s="6" t="s">
         <v>18</v>
@@ -6400,7 +6402,7 @@
         <v>," &lt;"</v>
       </c>
     </row>
-    <row r="41" spans="1:47">
+    <row r="41" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A41" s="4"/>
       <c r="B41" s="6" t="s">
         <v>19</v>
@@ -6534,7 +6536,7 @@
         <v>," &gt;"</v>
       </c>
     </row>
-    <row r="42" spans="1:47">
+    <row r="42" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A42" s="4"/>
       <c r="B42" s="6" t="s">
         <v>27</v>
@@ -6668,7 +6670,7 @@
         <v>," U&lt;"</v>
       </c>
     </row>
-    <row r="43" spans="1:47">
+    <row r="43" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A43" s="4"/>
       <c r="B43" s="6" t="s">
         <v>28</v>
@@ -6802,7 +6804,7 @@
         <v>," U&gt;"</v>
       </c>
     </row>
-    <row r="44" spans="1:47" s="3" customFormat="1">
+    <row r="44" spans="1:47" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" s="4"/>
       <c r="B44" s="13" t="s">
         <v>21</v>
@@ -6940,7 +6942,7 @@
         <v>," 0="</v>
       </c>
     </row>
-    <row r="45" spans="1:47" s="3" customFormat="1">
+    <row r="45" spans="1:47" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A45" s="4"/>
       <c r="B45" s="13" t="s">
         <v>291</v>
@@ -7078,7 +7080,7 @@
         <v>," 0&lt;&gt;"</v>
       </c>
     </row>
-    <row r="46" spans="1:47" s="3" customFormat="1">
+    <row r="46" spans="1:47" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="4"/>
       <c r="B46" s="13" t="s">
         <v>289</v>
@@ -7216,7 +7218,7 @@
         <v>," 0&lt;"</v>
       </c>
     </row>
-    <row r="47" spans="1:47" s="3" customFormat="1">
+    <row r="47" spans="1:47" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A47" s="4"/>
       <c r="B47" s="6" t="s">
         <v>290</v>
@@ -7354,7 +7356,7 @@
         <v>," 0&gt;"</v>
       </c>
     </row>
-    <row r="48" spans="1:47" s="3" customFormat="1">
+    <row r="48" spans="1:47" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A48" s="4"/>
       <c r="B48" s="11" t="b">
         <v>0</v>
@@ -7492,12 +7494,12 @@
         <v>," FALSE"</v>
       </c>
     </row>
-    <row r="49" spans="1:47">
+    <row r="49" spans="1:47" x14ac:dyDescent="0.2">
       <c r="E49" s="13"/>
       <c r="AT49" s="64"/>
       <c r="AU49" s="64"/>
     </row>
-    <row r="50" spans="1:47">
+    <row r="50" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>22</v>
       </c>
@@ -7505,7 +7507,7 @@
       <c r="AT50" s="64"/>
       <c r="AU50" s="64"/>
     </row>
-    <row r="51" spans="1:47">
+    <row r="51" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A51" s="4"/>
       <c r="B51" s="4" t="s">
         <v>23</v>
@@ -7638,7 +7640,7 @@
         <v>," AND"</v>
       </c>
     </row>
-    <row r="52" spans="1:47">
+    <row r="52" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A52" s="4"/>
       <c r="B52" s="4" t="s">
         <v>24</v>
@@ -7771,7 +7773,7 @@
         <v>," OR"</v>
       </c>
     </row>
-    <row r="53" spans="1:47">
+    <row r="53" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A53" s="4"/>
       <c r="B53" s="4" t="s">
         <v>26</v>
@@ -7904,7 +7906,7 @@
         <v>," INVERT"</v>
       </c>
     </row>
-    <row r="54" spans="1:47">
+    <row r="54" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A54" s="4"/>
       <c r="B54" s="4" t="s">
         <v>25</v>
@@ -8037,7 +8039,7 @@
         <v>," XOR"</v>
       </c>
     </row>
-    <row r="55" spans="1:47">
+    <row r="55" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A55" s="4"/>
       <c r="B55" s="4" t="s">
         <v>128</v>
@@ -8170,7 +8172,7 @@
         <v>," LSL"</v>
       </c>
     </row>
-    <row r="56" spans="1:47">
+    <row r="56" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A56" s="4"/>
       <c r="B56" s="4" t="s">
         <v>127</v>
@@ -8303,7 +8305,7 @@
         <v>," LSR"</v>
       </c>
     </row>
-    <row r="57" spans="1:47">
+    <row r="57" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A57" s="4"/>
       <c r="B57" s="4" t="s">
         <v>272</v>
@@ -8436,7 +8438,7 @@
         <v>," XBYTE"</v>
       </c>
     </row>
-    <row r="58" spans="1:47">
+    <row r="58" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A58" s="4"/>
       <c r="B58" s="4" t="s">
         <v>246</v>
@@ -8569,12 +8571,12 @@
         <v>," XWORD"</v>
       </c>
     </row>
-    <row r="59" spans="1:47">
+    <row r="59" spans="1:47" x14ac:dyDescent="0.2">
       <c r="E59" s="13"/>
       <c r="AT59" s="64"/>
       <c r="AU59" s="64"/>
     </row>
-    <row r="60" spans="1:47">
+    <row r="60" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>29</v>
       </c>
@@ -8582,7 +8584,7 @@
       <c r="AT60" s="64"/>
       <c r="AU60" s="64"/>
     </row>
-    <row r="61" spans="1:47" s="14" customFormat="1">
+    <row r="61" spans="1:47" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B61" s="15" t="s">
         <v>282</v>
       </c>
@@ -8705,7 +8707,7 @@
         <v>," FETCH.L"</v>
       </c>
     </row>
-    <row r="62" spans="1:47" s="14" customFormat="1">
+    <row r="62" spans="1:47" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B62" s="15" t="s">
         <v>283</v>
       </c>
@@ -8828,7 +8830,7 @@
         <v>," STORE.L"</v>
       </c>
     </row>
-    <row r="63" spans="1:47" s="14" customFormat="1">
+    <row r="63" spans="1:47" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B63" s="15" t="s">
         <v>284</v>
       </c>
@@ -8950,7 +8952,7 @@
         <v>," FETCH.W"</v>
       </c>
     </row>
-    <row r="64" spans="1:47" s="14" customFormat="1">
+    <row r="64" spans="1:47" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B64" s="15" t="s">
         <v>285</v>
       </c>
@@ -9072,7 +9074,7 @@
         <v>," STORE.W"</v>
       </c>
     </row>
-    <row r="65" spans="1:47" s="14" customFormat="1">
+    <row r="65" spans="1:47" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B65" s="15" t="s">
         <v>286</v>
       </c>
@@ -9195,7 +9197,7 @@
         <v>," FETCH.B"</v>
       </c>
     </row>
-    <row r="66" spans="1:47" s="14" customFormat="1">
+    <row r="66" spans="1:47" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B66" s="15" t="s">
         <v>292</v>
       </c>
@@ -9318,7 +9320,7 @@
         <v>," STORE.B"</v>
       </c>
     </row>
-    <row r="67" spans="1:47" s="2" customFormat="1">
+    <row r="67" spans="1:47" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B67" s="5"/>
       <c r="C67" s="5"/>
       <c r="D67" s="4"/>
@@ -9342,7 +9344,7 @@
       <c r="AT67" s="65"/>
       <c r="AU67" s="64"/>
     </row>
-    <row r="68" spans="1:47">
+    <row r="68" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>308</v>
       </c>
@@ -9351,7 +9353,7 @@
       <c r="AT68" s="65"/>
       <c r="AU68" s="64"/>
     </row>
-    <row r="69" spans="1:47">
+    <row r="69" spans="1:47" x14ac:dyDescent="0.2">
       <c r="B69" s="4" t="s">
         <v>307</v>
       </c>
@@ -9464,7 +9466,7 @@
         <v>," #.B"</v>
       </c>
     </row>
-    <row r="70" spans="1:47">
+    <row r="70" spans="1:47" x14ac:dyDescent="0.2">
       <c r="B70" s="4" t="s">
         <v>306</v>
       </c>
@@ -9577,7 +9579,7 @@
         <v>," #.W"</v>
       </c>
     </row>
-    <row r="71" spans="1:47" s="14" customFormat="1">
+    <row r="71" spans="1:47" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B71" s="15" t="s">
         <v>305</v>
       </c>
@@ -9698,13 +9700,13 @@
         <v>," #.L"</v>
       </c>
     </row>
-    <row r="72" spans="1:47">
+    <row r="72" spans="1:47" x14ac:dyDescent="0.2">
       <c r="S72" s="108"/>
       <c r="T72" s="108"/>
       <c r="AT72" s="64"/>
       <c r="AU72" s="64"/>
     </row>
-    <row r="73" spans="1:47">
+    <row r="73" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>47</v>
       </c>
@@ -9722,7 +9724,7 @@
       <c r="AT73" s="64"/>
       <c r="AU73" s="64"/>
     </row>
-    <row r="74" spans="1:47" s="3" customFormat="1">
+    <row r="74" spans="1:47" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B74" s="11" t="s">
         <v>51</v>
       </c>
@@ -9859,7 +9861,7 @@
         <v>," JMP"</v>
       </c>
     </row>
-    <row r="75" spans="1:47" s="3" customFormat="1">
+    <row r="75" spans="1:47" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B75" s="11" t="s">
         <v>342</v>
       </c>
@@ -9994,7 +9996,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="76" spans="1:47" s="3" customFormat="1">
+    <row r="76" spans="1:47" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B76" s="11" t="s">
         <v>50</v>
       </c>
@@ -10130,7 +10132,7 @@
         <v>," JSR"</v>
       </c>
     </row>
-    <row r="77" spans="1:47" s="14" customFormat="1">
+    <row r="77" spans="1:47" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B77" s="15" t="s">
         <v>287</v>
       </c>
@@ -10207,7 +10209,7 @@
       </c>
       <c r="AU77" s="65"/>
     </row>
-    <row r="78" spans="1:47" s="14" customFormat="1">
+    <row r="78" spans="1:47" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B78" s="15" t="s">
         <v>48</v>
       </c>
@@ -10269,7 +10271,7 @@
       <c r="AT78" s="64"/>
       <c r="AU78" s="65"/>
     </row>
-    <row r="79" spans="1:47" s="14" customFormat="1">
+    <row r="79" spans="1:47" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B79" s="15" t="s">
         <v>49</v>
       </c>
@@ -10313,7 +10315,7 @@
       <c r="AT79" s="64"/>
       <c r="AU79" s="65"/>
     </row>
-    <row r="80" spans="1:47" s="14" customFormat="1">
+    <row r="80" spans="1:47" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B80" s="15"/>
       <c r="C80" s="15"/>
       <c r="D80" s="15"/>
@@ -10338,7 +10340,7 @@
       <c r="AT80" s="64"/>
       <c r="AU80" s="65"/>
     </row>
-    <row r="81" spans="1:47" s="14" customFormat="1">
+    <row r="81" spans="1:47" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A81" s="3" t="s">
         <v>294</v>
       </c>
@@ -10366,7 +10368,7 @@
       <c r="AT81" s="64"/>
       <c r="AU81" s="65"/>
     </row>
-    <row r="82" spans="1:47" s="56" customFormat="1">
+    <row r="82" spans="1:47" s="56" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B82" s="57" t="s">
         <v>296</v>
       </c>
@@ -10407,7 +10409,7 @@
       </c>
       <c r="AU82" s="67"/>
     </row>
-    <row r="83" spans="1:47" s="56" customFormat="1">
+    <row r="83" spans="1:47" s="56" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B83" s="57" t="s">
         <v>301</v>
       </c>
@@ -10448,7 +10450,7 @@
       </c>
       <c r="AU83" s="67"/>
     </row>
-    <row r="84" spans="1:47" s="56" customFormat="1">
+    <row r="84" spans="1:47" s="56" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B84" s="57" t="s">
         <v>300</v>
       </c>
@@ -10489,7 +10491,7 @@
       </c>
       <c r="AU84" s="67"/>
     </row>
-    <row r="85" spans="1:47" s="56" customFormat="1">
+    <row r="85" spans="1:47" s="56" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B85" s="57"/>
       <c r="C85" s="57"/>
       <c r="D85" s="57"/>
@@ -10520,7 +10522,7 @@
       <c r="AQ85" s="59"/>
       <c r="AT85" s="60"/>
     </row>
-    <row r="86" spans="1:47" s="56" customFormat="1">
+    <row r="86" spans="1:47" s="56" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B86" s="57"/>
       <c r="C86" s="57"/>
       <c r="D86" s="57"/>
@@ -10542,7 +10544,7 @@
       <c r="AQ86" s="59"/>
       <c r="AT86" s="60"/>
     </row>
-    <row r="87" spans="1:47" s="3" customFormat="1">
+    <row r="87" spans="1:47" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A87" s="3" t="s">
         <v>145</v>
       </c>
@@ -10568,7 +10570,7 @@
       <c r="AR87" s="1"/>
       <c r="AT87" s="52"/>
     </row>
-    <row r="88" spans="1:47" s="46" customFormat="1">
+    <row r="88" spans="1:47" s="46" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B88" s="47" t="s">
         <v>261</v>
       </c>
@@ -10685,7 +10687,7 @@
       </c>
       <c r="AT88" s="52"/>
     </row>
-    <row r="89" spans="1:47" s="46" customFormat="1">
+    <row r="89" spans="1:47" s="46" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B89" s="47" t="s">
         <v>262</v>
       </c>
@@ -10802,7 +10804,7 @@
       </c>
       <c r="AT89" s="52"/>
     </row>
-    <row r="90" spans="1:47" s="46" customFormat="1">
+    <row r="90" spans="1:47" s="46" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B90" s="47" t="s">
         <v>300</v>
       </c>
@@ -10930,7 +10932,7 @@
       </c>
       <c r="AT90" s="52"/>
     </row>
-    <row r="91" spans="1:47" s="46" customFormat="1" ht="14.25" customHeight="1">
+    <row r="91" spans="1:47" s="46" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B91" s="47" t="s">
         <v>344</v>
       </c>
@@ -11058,7 +11060,7 @@
       </c>
       <c r="AT91" s="52"/>
     </row>
-    <row r="92" spans="1:47" s="46" customFormat="1">
+    <row r="92" spans="1:47" s="46" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B92" s="47" t="s">
         <v>341</v>
       </c>
@@ -11188,18 +11190,18 @@
       </c>
       <c r="AT92" s="55"/>
     </row>
-    <row r="94" spans="1:47">
+    <row r="94" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A94" s="8" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="95" spans="1:47">
+    <row r="95" spans="1:47" x14ac:dyDescent="0.2">
       <c r="B95" s="8" t="s">
         <v>252</v>
       </c>
       <c r="C95" s="8"/>
     </row>
-    <row r="96" spans="1:47" s="38" customFormat="1">
+    <row r="96" spans="1:47" s="38" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B96" s="9" t="s">
         <v>253</v>
       </c>
@@ -11223,13 +11225,13 @@
       <c r="AQ96" s="40"/>
       <c r="AT96" s="53"/>
     </row>
-    <row r="97" spans="2:3">
+    <row r="97" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B97" s="56" t="s">
         <v>295</v>
       </c>
       <c r="C97" s="21"/>
     </row>
-    <row r="98" spans="2:3">
+    <row r="98" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B98" s="21" t="s">
         <v>144</v>
       </c>
@@ -11245,25 +11247,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.28515625" customWidth="1"/>
     <col min="3" max="6" width="9.140625" style="43"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B3" s="61"/>
       <c r="C3" s="80" t="s">
         <v>263</v>
@@ -11294,7 +11296,7 @@
       </c>
       <c r="L3" s="81"/>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B4" s="82">
         <v>0</v>
       </c>
@@ -11329,7 +11331,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B5" s="82">
         <v>1</v>
       </c>
@@ -11364,7 +11366,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B6" s="82">
         <v>2</v>
       </c>
@@ -11397,7 +11399,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B7" s="82">
         <v>3</v>
       </c>
@@ -11430,7 +11432,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B8" s="82">
         <v>4</v>
       </c>
@@ -11457,7 +11459,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B9" s="82">
         <v>5</v>
       </c>
@@ -11484,7 +11486,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B10" s="82">
         <v>6</v>
       </c>
@@ -11511,7 +11513,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B11" s="82">
         <v>7</v>
       </c>
@@ -11538,7 +11540,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B12" s="82">
         <v>8</v>
       </c>
@@ -11557,7 +11559,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B13" s="82">
         <v>9</v>
       </c>
@@ -11576,7 +11578,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B14" s="82">
         <v>10</v>
       </c>
@@ -11595,7 +11597,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B15" s="82">
         <v>11</v>
       </c>
@@ -11614,7 +11616,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B16" s="82">
         <v>12</v>
       </c>
@@ -11633,7 +11635,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="2:12">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B17" s="82">
         <v>13</v>
       </c>
@@ -11652,7 +11654,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="2:12">
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B18" s="82">
         <v>14</v>
       </c>
@@ -11671,7 +11673,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="2:12">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B19" s="85">
         <v>15</v>
       </c>
@@ -11690,7 +11692,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="2:12">
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
         <v>255</v>
       </c>
@@ -11722,7 +11724,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="2:12">
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B22" s="4" t="s">
         <v>256</v>
       </c>
@@ -11764,14 +11766,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.25"/>
+  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="2.28515625" style="1" customWidth="1"/>
     <col min="2" max="2" width="3.42578125" style="1" customWidth="1"/>
@@ -11786,23 +11788,23 @@
     <col min="23" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="15">
+    <row r="1" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="3" spans="1:22">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B3" s="22" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="4" spans="1:22">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B4" s="22"/>
       <c r="C4" s="22" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="5" spans="1:22" s="22" customFormat="1">
+    <row r="5" spans="1:22" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D5" s="27" t="s">
         <v>156</v>
       </c>
@@ -11822,7 +11824,7 @@
       <c r="K5" s="7"/>
       <c r="L5" s="7"/>
     </row>
-    <row r="6" spans="1:22">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
       <c r="D6" s="1">
         <v>2</v>
       </c>
@@ -11844,7 +11846,7 @@
       <c r="K6" s="4"/>
       <c r="L6" s="4"/>
     </row>
-    <row r="7" spans="1:22">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
       <c r="D7" s="1">
         <v>2</v>
       </c>
@@ -11864,7 +11866,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:22" s="3" customFormat="1">
+    <row r="8" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D8" s="3">
         <v>2</v>
       </c>
@@ -11884,7 +11886,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:22">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
       <c r="D9" s="29">
         <f>SUM(D6:D8)</f>
         <v>6</v>
@@ -11894,18 +11896,18 @@
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
     </row>
-    <row r="10" spans="1:22">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
     </row>
-    <row r="11" spans="1:22" s="14" customFormat="1">
+    <row r="11" spans="1:22" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B11" s="30"/>
       <c r="C11" s="30" t="s">
         <v>158</v>
       </c>
       <c r="F11" s="34"/>
     </row>
-    <row r="12" spans="1:22" s="14" customFormat="1">
+    <row r="12" spans="1:22" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D12" s="14">
         <v>1</v>
       </c>
@@ -11919,22 +11921,22 @@
         <v>328</v>
       </c>
     </row>
-    <row r="13" spans="1:22" s="14" customFormat="1" ht="11.25" customHeight="1">
+    <row r="13" spans="1:22" s="14" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D13" s="31">
         <f>SUM(D12:D12)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:22" s="14" customFormat="1" ht="12.75" customHeight="1">
+    <row r="14" spans="1:22" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K14" s="15"/>
       <c r="L14" s="15"/>
     </row>
-    <row r="15" spans="1:22">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B15" s="22" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="16" spans="1:22">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
       <c r="D16" s="27" t="s">
         <v>156</v>
       </c>
@@ -11987,7 +11989,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="2:22">
+    <row r="17" spans="2:22" x14ac:dyDescent="0.2">
       <c r="D17" s="28">
         <v>4</v>
       </c>
@@ -12044,7 +12046,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="2:22">
+    <row r="18" spans="2:22" x14ac:dyDescent="0.2">
       <c r="D18" s="28"/>
       <c r="G18" s="4" t="s">
         <v>205</v>
@@ -12095,7 +12097,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="19" spans="2:22">
+    <row r="19" spans="2:22" x14ac:dyDescent="0.2">
       <c r="D19" s="1">
         <v>3</v>
       </c>
@@ -12127,7 +12129,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="20" spans="2:22">
+    <row r="20" spans="2:22" x14ac:dyDescent="0.2">
       <c r="D20" s="1">
         <v>3</v>
       </c>
@@ -12159,7 +12161,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="21" spans="2:22">
+    <row r="21" spans="2:22" x14ac:dyDescent="0.2">
       <c r="D21" s="1">
         <v>1</v>
       </c>
@@ -12191,7 +12193,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="22" spans="2:22">
+    <row r="22" spans="2:22" x14ac:dyDescent="0.2">
       <c r="D22" s="1">
         <v>3</v>
       </c>
@@ -12223,22 +12225,22 @@
         <v>200</v>
       </c>
     </row>
-    <row r="23" spans="2:22">
+    <row r="23" spans="2:22" x14ac:dyDescent="0.2">
       <c r="D23" s="29">
         <f>MAX(D17:D21)+D22</f>
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="2:22">
+    <row r="24" spans="2:22" x14ac:dyDescent="0.2">
       <c r="D24" s="35"/>
     </row>
-    <row r="25" spans="2:22">
+    <row r="25" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B25" s="22" t="s">
         <v>323</v>
       </c>
       <c r="D25" s="35"/>
     </row>
-    <row r="26" spans="2:22">
+    <row r="26" spans="2:22" x14ac:dyDescent="0.2">
       <c r="D26" s="27" t="s">
         <v>156</v>
       </c>
@@ -12256,7 +12258,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="2:22">
+    <row r="27" spans="2:22" x14ac:dyDescent="0.2">
       <c r="D27" s="28">
         <v>1</v>
       </c>
@@ -12273,7 +12275,7 @@
       <c r="I27" s="7"/>
       <c r="J27" s="7"/>
     </row>
-    <row r="28" spans="2:22">
+    <row r="28" spans="2:22" x14ac:dyDescent="0.2">
       <c r="D28" s="99">
         <f>SUM(D27)</f>
         <v>1</v>
@@ -12284,7 +12286,7 @@
       <c r="I28" s="7"/>
       <c r="J28" s="7"/>
     </row>
-    <row r="29" spans="2:22">
+    <row r="29" spans="2:22" x14ac:dyDescent="0.2">
       <c r="D29" s="28"/>
       <c r="E29" s="22"/>
       <c r="G29" s="4"/>
@@ -12292,7 +12294,7 @@
       <c r="I29" s="7"/>
       <c r="J29" s="7"/>
     </row>
-    <row r="30" spans="2:22" s="25" customFormat="1">
+    <row r="30" spans="2:22" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D30" s="37"/>
       <c r="F30" s="36"/>
       <c r="G30" s="26"/>
@@ -12301,7 +12303,7 @@
       <c r="J30" s="26"/>
       <c r="K30" s="26"/>
     </row>
-    <row r="31" spans="2:22">
+    <row r="31" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B31" s="22" t="s">
         <v>314</v>
       </c>
@@ -12317,7 +12319,7 @@
       <c r="K31" s="18"/>
       <c r="L31" s="18"/>
     </row>
-    <row r="32" spans="2:22">
+    <row r="32" spans="2:22" x14ac:dyDescent="0.2">
       <c r="C32" s="1" t="s">
         <v>236</v>
       </c>
@@ -12337,7 +12339,7 @@
       </c>
       <c r="K32" s="4"/>
     </row>
-    <row r="33" spans="1:12">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C33" s="1" t="s">
         <v>237</v>
       </c>
@@ -12367,7 +12369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:12">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C34" s="1" t="s">
         <v>238</v>
       </c>
@@ -12398,7 +12400,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:12">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C35" s="1" t="s">
         <v>324</v>
       </c>
@@ -12418,24 +12420,24 @@
       <c r="K35" s="4"/>
       <c r="L35" s="4"/>
     </row>
-    <row r="36" spans="1:12">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D36" s="29">
         <f>SUM(D32:D35)</f>
         <v>14</v>
       </c>
     </row>
-    <row r="38" spans="1:12">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B38" s="30" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="39" spans="1:12">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D39" s="31">
         <f>D13</f>
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:12">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>13</v>
       </c>
@@ -12443,7 +12445,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="42" spans="1:12">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42" s="14" t="s">
         <v>330</v>
       </c>
@@ -12458,14 +12460,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.25"/>
+  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.42578125" style="1" customWidth="1"/>
     <col min="2" max="2" width="17.28515625" style="4" customWidth="1"/>
@@ -12483,12 +12485,12 @@
     <col min="21" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="15">
+    <row r="1" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="4" spans="1:20">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="C4" s="32" t="s">
         <v>177</v>
       </c>
@@ -12515,7 +12517,7 @@
       </c>
       <c r="T4" s="18"/>
     </row>
-    <row r="5" spans="1:20">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="C5" s="4" t="s">
         <v>179</v>
       </c>
@@ -12556,7 +12558,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="6" spans="1:20">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
@@ -12579,7 +12581,7 @@
       <c r="S6" s="4"/>
       <c r="T6" s="4"/>
     </row>
-    <row r="7" spans="1:20">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>31</v>
       </c>
@@ -12600,7 +12602,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:20">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>30</v>
       </c>
@@ -12627,7 +12629,7 @@
       <c r="S8" s="4"/>
       <c r="T8" s="4"/>
     </row>
-    <row r="9" spans="1:20">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>11</v>
       </c>
@@ -12648,7 +12650,7 @@
       <c r="P9" s="4"/>
       <c r="Q9" s="4"/>
     </row>
-    <row r="10" spans="1:20">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
         <v>12</v>
       </c>
@@ -12669,7 +12671,7 @@
       <c r="P10" s="4"/>
       <c r="Q10" s="4"/>
     </row>
-    <row r="11" spans="1:20">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
         <v>13</v>
       </c>
@@ -12690,7 +12692,7 @@
       <c r="P11" s="4"/>
       <c r="Q11" s="4"/>
     </row>
-    <row r="12" spans="1:20">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12" s="17" t="s">
         <v>14</v>
       </c>
@@ -12707,7 +12709,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:20">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13" s="15" t="s">
         <v>15</v>
       </c>
@@ -12726,7 +12728,7 @@
       <c r="P13" s="4"/>
       <c r="Q13" s="4"/>
     </row>
-    <row r="14" spans="1:20">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A14" s="15" t="s">
         <v>42</v>
       </c>
@@ -12745,7 +12747,7 @@
       <c r="M14" s="4"/>
       <c r="N14" s="4"/>
     </row>
-    <row r="15" spans="1:20">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A15" s="20" t="s">
         <v>43</v>
       </c>
@@ -12764,7 +12766,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:20">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>16</v>
       </c>
@@ -12783,7 +12785,7 @@
       <c r="M16" s="4"/>
       <c r="N16" s="4"/>
     </row>
-    <row r="17" spans="1:20">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A17" s="11" t="s">
         <v>52</v>
       </c>
@@ -12802,7 +12804,7 @@
       <c r="M17" s="4"/>
       <c r="N17" s="4"/>
     </row>
-    <row r="18" spans="1:20">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A18" s="11" t="s">
         <v>53</v>
       </c>
@@ -12823,7 +12825,7 @@
       <c r="S18" s="4"/>
       <c r="T18" s="4"/>
     </row>
-    <row r="19" spans="1:20">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A19" s="11" t="s">
         <v>54</v>
       </c>
@@ -12842,7 +12844,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:20">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>55</v>
       </c>
@@ -12861,7 +12863,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:20">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>23</v>
       </c>
@@ -12880,7 +12882,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:20">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>24</v>
       </c>
@@ -12899,7 +12901,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:20">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>25</v>
       </c>
@@ -12918,7 +12920,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:20">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>26</v>
       </c>
@@ -12937,7 +12939,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:20">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A25" s="15" t="s">
         <v>143</v>
       </c>
@@ -12956,7 +12958,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:20">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A26" s="15" t="s">
         <v>142</v>
       </c>
@@ -12975,7 +12977,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:20">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>219</v>
       </c>
@@ -12992,7 +12994,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:20">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
         <v>220</v>
       </c>
@@ -13015,60 +13017,60 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="109.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="101" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="101" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="101"/>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="101" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="101" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="30">
+    <row r="6" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="101" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="101" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="45">
+    <row r="8" spans="1:1" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="102" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="101"/>
     </row>
-    <row r="10" spans="1:1" ht="60">
+    <row r="10" spans="1:1" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="102" t="s">
         <v>338</v>
       </c>

</xml_diff>

<commit_message>
Corrected a major bug in the operation timing of the load literal instruction.   There had been a mismatch between the data availability (cycle 0) and the microcode to drive the update or TOS (cycle 1).  Moved the data availability to cycle 1 by taking advantage of the fixed PC increment of 1 byte and using the ordinary SRAM memory channel. Removed the data_plus output from SRAM Controller as it is no longer needed
</commit_message>
<xml_diff>
--- a/Resources/Instruction Set.xlsx
+++ b/Resources/Instruction Set.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="18195" windowHeight="8250" tabRatio="681"/>
+    <workbookView xWindow="240" yWindow="180" windowWidth="18195" windowHeight="8190" tabRatio="681"/>
   </bookViews>
   <sheets>
     <sheet name="OPCODE_encoding" sheetId="1" r:id="rId1"/>
@@ -2048,10 +2048,10 @@
   <dimension ref="A1:AU98"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="9" ySplit="4" topLeftCell="P32" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="9" ySplit="4" topLeftCell="U43" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H69" sqref="H69"/>
+      <selection pane="bottomRight" activeCell="AR59" sqref="AR59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -8636,19 +8636,19 @@
         <v>31</v>
       </c>
       <c r="Z61" s="15" t="s">
-        <v>233</v>
+        <v>247</v>
       </c>
       <c r="AA61" s="15" t="s">
         <v>141</v>
       </c>
       <c r="AB61" s="15" t="s">
-        <v>52</v>
+        <v>141</v>
       </c>
       <c r="AC61" s="15" t="s">
         <v>141</v>
       </c>
       <c r="AD61" s="15" t="s">
-        <v>141</v>
+        <v>254</v>
       </c>
       <c r="AF61" s="15" t="str">
         <f>DEC2BIN(VLOOKUP(V61,OPCODE_mult!$C$4:$L$19,10,FALSE),1)</f>
@@ -8668,7 +8668,7 @@
       </c>
       <c r="AJ61" s="15" t="str">
         <f>DEC2BIN(IF(Z61="X",0,VLOOKUP(Z61,OPCODE_mult!$K$4:$L$19,2,FALSE)),3)</f>
-        <v>000</v>
+        <v>010</v>
       </c>
       <c r="AK61" s="15">
         <f>IF(AA61="X",0,VLOOKUP(AA61,OPCODE_mult!$G$4:$L$19,6,FALSE))</f>
@@ -8676,7 +8676,7 @@
       </c>
       <c r="AL61" s="15">
         <f>IF(AB61="X",0,VLOOKUP(AB61,OPCODE_mult!$H$4:$L$19,5,FALSE))</f>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="AM61" s="15">
         <f>IF(AC61="X",0,VLOOKUP(AC61,OPCODE_mult!$I$4:$L$19,4,FALSE))</f>
@@ -8684,18 +8684,19 @@
       </c>
       <c r="AN61" s="15">
         <f>IF(AD61="X",0,VLOOKUP(AD61,OPCODE_mult!$J$4:$L$19,3,FALSE))</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AO61" s="15" t="str">
         <f t="shared" ref="AO61:AO66" si="33">DEC2BIN(SUM(AK61:AN61),4)</f>
-        <v>0110</v>
+        <v>0111</v>
       </c>
       <c r="AP61" s="15"/>
       <c r="AQ61" s="16" t="str">
         <f t="shared" ref="AQ61:AQ66" si="34">AF61&amp;AG61&amp;AH61&amp;AI61&amp;AJ61&amp;AO61</f>
-        <v>00000000000110</v>
+        <v>00000000100111</v>
       </c>
       <c r="AR61" s="14">
+        <f t="shared" si="3"/>
         <v>39</v>
       </c>
       <c r="AT61" s="64" t="str">
@@ -8882,19 +8883,19 @@
         <v>31</v>
       </c>
       <c r="Z63" s="15" t="s">
-        <v>233</v>
+        <v>247</v>
       </c>
       <c r="AA63" s="15" t="s">
         <v>141</v>
       </c>
       <c r="AB63" s="15" t="s">
-        <v>52</v>
+        <v>141</v>
       </c>
       <c r="AC63" s="15" t="s">
         <v>141</v>
       </c>
       <c r="AD63" s="15" t="s">
-        <v>141</v>
+        <v>254</v>
       </c>
       <c r="AF63" s="15" t="str">
         <f>DEC2BIN(VLOOKUP(V63,OPCODE_mult!$C$4:$L$19,10,FALSE),1)</f>
@@ -8914,7 +8915,7 @@
       </c>
       <c r="AJ63" s="15" t="str">
         <f>DEC2BIN(IF(Z63="X",0,VLOOKUP(Z63,OPCODE_mult!$K$4:$L$19,2,FALSE)),3)</f>
-        <v>000</v>
+        <v>010</v>
       </c>
       <c r="AK63" s="15">
         <f>IF(AA63="X",0,VLOOKUP(AA63,OPCODE_mult!$G$4:$L$19,6,FALSE))</f>
@@ -8922,7 +8923,7 @@
       </c>
       <c r="AL63" s="15">
         <f>IF(AB63="X",0,VLOOKUP(AB63,OPCODE_mult!$H$4:$L$19,5,FALSE))</f>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="AM63" s="15">
         <f>IF(AC63="X",0,VLOOKUP(AC63,OPCODE_mult!$I$4:$L$19,4,FALSE))</f>
@@ -8930,17 +8931,18 @@
       </c>
       <c r="AN63" s="15">
         <f>IF(AD63="X",0,VLOOKUP(AD63,OPCODE_mult!$J$4:$L$19,3,FALSE))</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AO63" s="15" t="str">
         <f t="shared" si="33"/>
-        <v>0110</v>
+        <v>0111</v>
       </c>
       <c r="AQ63" s="16" t="str">
         <f t="shared" si="34"/>
-        <v>00000000000110</v>
+        <v>00000000100111</v>
       </c>
       <c r="AR63" s="14">
+        <f t="shared" si="3"/>
         <v>39</v>
       </c>
       <c r="AT63" s="64" t="str">

</xml_diff>

<commit_message>
Revised and tested version with access to the subroutine and exception stacks
</commit_message>
<xml_diff>
--- a/Resources/Instruction Set.xlsx
+++ b/Resources/Instruction Set.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1231" uniqueCount="339">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1247" uniqueCount="339">
   <si>
     <t>DUP</t>
   </si>
@@ -2024,10 +2024,10 @@
   <dimension ref="A1:AS94"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="10" ySplit="4" topLeftCell="K5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="10" ySplit="4" topLeftCell="O26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B18" sqref="B18"/>
+      <selection pane="bottomRight" activeCell="V56" sqref="V56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -8276,37 +8276,29 @@
       <c r="R57" s="94" t="s">
         <v>29</v>
       </c>
-      <c r="S57" s="94" t="str">
-        <f t="shared" ref="S57:Z57" si="38">S6</f>
-        <v>RSP</v>
-      </c>
-      <c r="T57" s="94" t="str">
-        <f t="shared" si="38"/>
-        <v>PSP</v>
-      </c>
-      <c r="U57" s="94" t="str">
-        <f t="shared" si="38"/>
-        <v>NOS</v>
-      </c>
-      <c r="V57" s="94" t="str">
-        <f t="shared" si="38"/>
-        <v>addsub</v>
-      </c>
-      <c r="W57" s="94" t="str">
-        <f t="shared" si="38"/>
-        <v>X</v>
-      </c>
-      <c r="X57" s="94" t="str">
-        <f t="shared" si="38"/>
-        <v>TOS</v>
-      </c>
-      <c r="Y57" s="94" t="str">
-        <f t="shared" si="38"/>
-        <v>X</v>
-      </c>
-      <c r="Z57" s="94" t="str">
-        <f t="shared" si="38"/>
-        <v>X</v>
+      <c r="S57" s="94" t="s">
+        <v>31</v>
+      </c>
+      <c r="T57" s="94" t="s">
+        <v>32</v>
+      </c>
+      <c r="U57" s="94" t="s">
+        <v>182</v>
+      </c>
+      <c r="V57" s="94" t="s">
+        <v>184</v>
+      </c>
+      <c r="W57" s="94" t="s">
+        <v>131</v>
+      </c>
+      <c r="X57" s="94" t="s">
+        <v>131</v>
+      </c>
+      <c r="Y57" s="94" t="s">
+        <v>131</v>
+      </c>
+      <c r="Z57" s="94" t="s">
+        <v>131</v>
       </c>
       <c r="AA57" s="94"/>
       <c r="AB57" s="8" t="str">
@@ -8331,11 +8323,11 @@
       </c>
       <c r="AG57" s="94" t="str">
         <f>DEC2BIN(VLOOKUP(U57,OPCODE_mult!$H$4:$N$19,7,FALSE),2)</f>
-        <v>00</v>
+        <v>11</v>
       </c>
       <c r="AH57" s="94" t="str">
         <f>DEC2BIN(IF(V57="X",0,VLOOKUP(V57,OPCODE_mult!$I$4:$N$19,6,FALSE)),3)</f>
-        <v>000</v>
+        <v>110</v>
       </c>
       <c r="AI57" s="94">
         <f>IF(W57="X",0,VLOOKUP(W57,OPCODE_mult!$J$4:$N$19,5,FALSE))</f>
@@ -8360,11 +8352,11 @@
       <c r="AN57" s="94"/>
       <c r="AO57" s="9" t="str">
         <f t="shared" si="6"/>
-        <v>000000000000000000000</v>
+        <v>000000000000111100000</v>
       </c>
       <c r="AP57" s="1">
         <f t="shared" si="34"/>
-        <v>0</v>
+        <v>480</v>
       </c>
       <c r="AR57" s="98" t="str">
         <f t="shared" si="35"/>
@@ -8421,37 +8413,29 @@
       <c r="R58" s="94" t="s">
         <v>29</v>
       </c>
-      <c r="S58" s="94" t="str">
-        <f t="shared" ref="S58:Z58" si="39">S6</f>
-        <v>RSP</v>
-      </c>
-      <c r="T58" s="94" t="str">
-        <f t="shared" si="39"/>
-        <v>PSP</v>
-      </c>
-      <c r="U58" s="94" t="str">
-        <f t="shared" si="39"/>
-        <v>NOS</v>
-      </c>
-      <c r="V58" s="94" t="str">
-        <f t="shared" si="39"/>
-        <v>addsub</v>
-      </c>
-      <c r="W58" s="94" t="str">
-        <f t="shared" si="39"/>
-        <v>X</v>
-      </c>
-      <c r="X58" s="94" t="str">
-        <f t="shared" si="39"/>
-        <v>TOS</v>
-      </c>
-      <c r="Y58" s="94" t="str">
-        <f t="shared" si="39"/>
-        <v>X</v>
-      </c>
-      <c r="Z58" s="94" t="str">
-        <f t="shared" si="39"/>
-        <v>X</v>
+      <c r="S58" s="94" t="s">
+        <v>31</v>
+      </c>
+      <c r="T58" s="94" t="s">
+        <v>32</v>
+      </c>
+      <c r="U58" s="94" t="s">
+        <v>182</v>
+      </c>
+      <c r="V58" s="94" t="s">
+        <v>185</v>
+      </c>
+      <c r="W58" s="94" t="s">
+        <v>131</v>
+      </c>
+      <c r="X58" s="94" t="s">
+        <v>131</v>
+      </c>
+      <c r="Y58" s="94" t="s">
+        <v>131</v>
+      </c>
+      <c r="Z58" s="94" t="s">
+        <v>131</v>
       </c>
       <c r="AA58" s="94"/>
       <c r="AB58" s="8" t="str">
@@ -8476,11 +8460,11 @@
       </c>
       <c r="AG58" s="94" t="str">
         <f>DEC2BIN(VLOOKUP(U58,OPCODE_mult!$H$4:$N$19,7,FALSE),2)</f>
-        <v>00</v>
+        <v>11</v>
       </c>
       <c r="AH58" s="94" t="str">
         <f>DEC2BIN(IF(V58="X",0,VLOOKUP(V58,OPCODE_mult!$I$4:$N$19,6,FALSE)),3)</f>
-        <v>000</v>
+        <v>111</v>
       </c>
       <c r="AI58" s="94">
         <f>IF(W58="X",0,VLOOKUP(W58,OPCODE_mult!$J$4:$N$19,5,FALSE))</f>
@@ -8505,11 +8489,11 @@
       <c r="AN58" s="94"/>
       <c r="AO58" s="9" t="str">
         <f t="shared" si="6"/>
-        <v>000000000000000000000</v>
+        <v>000000000000111110000</v>
       </c>
       <c r="AP58" s="1">
         <f t="shared" si="34"/>
-        <v>0</v>
+        <v>496</v>
       </c>
       <c r="AR58" s="98" t="str">
         <f t="shared" si="35"/>
@@ -8537,7 +8521,7 @@
       </c>
       <c r="G59" s="94"/>
       <c r="H59" s="95">
-        <f t="shared" ref="H59:H64" si="40">F59+E59*64+D59*128</f>
+        <f t="shared" ref="H59:H64" si="38">F59+E59*64+D59*128</f>
         <v>45</v>
       </c>
       <c r="I59" s="94" t="str">
@@ -8545,7 +8529,7 @@
         <v>101101</v>
       </c>
       <c r="J59" s="94" t="str">
-        <f t="shared" ref="J59:J64" si="41">DEC2HEX(H59)</f>
+        <f t="shared" ref="J59:J64" si="39">DEC2HEX(H59)</f>
         <v>2D</v>
       </c>
       <c r="K59" s="94"/>
@@ -8674,7 +8658,7 @@
       </c>
       <c r="G60" s="94"/>
       <c r="H60" s="95">
-        <f t="shared" si="40"/>
+        <f t="shared" si="38"/>
         <v>46</v>
       </c>
       <c r="I60" s="94" t="str">
@@ -8682,7 +8666,7 @@
         <v>101110</v>
       </c>
       <c r="J60" s="94" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="39"/>
         <v>2E</v>
       </c>
       <c r="K60" s="94"/>
@@ -8811,7 +8795,7 @@
       </c>
       <c r="G61" s="94"/>
       <c r="H61" s="95">
-        <f t="shared" si="40"/>
+        <f t="shared" si="38"/>
         <v>47</v>
       </c>
       <c r="I61" s="94" t="str">
@@ -8819,7 +8803,7 @@
         <v>101111</v>
       </c>
       <c r="J61" s="94" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="39"/>
         <v>2F</v>
       </c>
       <c r="K61" s="94"/>
@@ -8948,7 +8932,7 @@
       </c>
       <c r="G62" s="94"/>
       <c r="H62" s="95">
-        <f t="shared" si="40"/>
+        <f t="shared" si="38"/>
         <v>48</v>
       </c>
       <c r="I62" s="94" t="str">
@@ -8956,7 +8940,7 @@
         <v>110000</v>
       </c>
       <c r="J62" s="94" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="39"/>
         <v>30</v>
       </c>
       <c r="K62" s="94"/>
@@ -9085,7 +9069,7 @@
       </c>
       <c r="G63" s="94"/>
       <c r="H63" s="95">
-        <f t="shared" si="40"/>
+        <f t="shared" si="38"/>
         <v>49</v>
       </c>
       <c r="I63" s="94" t="str">
@@ -9093,7 +9077,7 @@
         <v>110001</v>
       </c>
       <c r="J63" s="94" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="39"/>
         <v>31</v>
       </c>
       <c r="K63" s="94"/>
@@ -9222,7 +9206,7 @@
       </c>
       <c r="G64" s="94"/>
       <c r="H64" s="95">
-        <f t="shared" si="40"/>
+        <f t="shared" si="38"/>
         <v>50</v>
       </c>
       <c r="I64" s="94" t="str">
@@ -9230,7 +9214,7 @@
         <v>110010</v>
       </c>
       <c r="J64" s="94" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="39"/>
         <v>32</v>
       </c>
       <c r="K64" s="94"/>
@@ -9394,31 +9378,31 @@
         <v>31</v>
       </c>
       <c r="T65" s="94" t="str">
-        <f t="shared" ref="T65:Z65" si="42">T8</f>
+        <f t="shared" ref="T65:Z65" si="40">T8</f>
         <v>PSP + 1</v>
       </c>
       <c r="U65" s="94" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" si="40"/>
         <v>TOS</v>
       </c>
       <c r="V65" s="94" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" si="40"/>
         <v>addsub</v>
       </c>
       <c r="W65" s="94" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" si="40"/>
         <v>X</v>
       </c>
       <c r="X65" s="94" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" si="40"/>
         <v>TOS</v>
       </c>
       <c r="Y65" s="94" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" si="40"/>
         <v>X</v>
       </c>
       <c r="Z65" s="94" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" si="40"/>
         <v>X</v>
       </c>
       <c r="AA65" s="94"/>
@@ -9564,15 +9548,15 @@
       </c>
       <c r="G68" s="85"/>
       <c r="H68" s="86">
-        <f t="shared" ref="H68:H76" si="43">F68+E68*64+D68*128</f>
+        <f t="shared" ref="H68:H76" si="41">F68+E68*64+D68*128</f>
         <v>52</v>
       </c>
       <c r="I68" s="85" t="str">
-        <f t="shared" ref="I68:I76" si="44">DEC2BIN(H68,6)</f>
+        <f t="shared" ref="I68:I76" si="42">DEC2BIN(H68,6)</f>
         <v>110100</v>
       </c>
       <c r="J68" s="85" t="str">
-        <f t="shared" ref="J68:J76" si="45">DEC2HEX(H68)</f>
+        <f t="shared" ref="J68:J76" si="43">DEC2HEX(H68)</f>
         <v>34</v>
       </c>
       <c r="K68" s="85"/>
@@ -9662,7 +9646,7 @@
         <v>7</v>
       </c>
       <c r="AM68" s="85" t="str">
-        <f t="shared" ref="AM68:AM76" si="46">DEC2BIN(SUM(AI68:AL68),4)</f>
+        <f t="shared" ref="AM68:AM76" si="44">DEC2BIN(SUM(AI68:AL68),4)</f>
         <v>0111</v>
       </c>
       <c r="AN68" s="85"/>
@@ -9671,11 +9655,11 @@
         <v>000000000010010100111</v>
       </c>
       <c r="AP68" s="1">
-        <f t="shared" ref="AP68:AP76" si="47">(BIN2DEC(AM68)+(2^4)*BIN2DEC(AH68)+(2^7)*BIN2DEC(AG68)+(2^9)*BIN2DEC(AF68)+(2^12)*BIN2DEC(AE68)+(2^15)*BIN2DEC(AD68)+(2^16)*BIN2DEC(AC68)+(2^19)*BIN2DEC(AB68))</f>
+        <f t="shared" ref="AP68:AP76" si="45">(BIN2DEC(AM68)+(2^4)*BIN2DEC(AH68)+(2^7)*BIN2DEC(AG68)+(2^9)*BIN2DEC(AF68)+(2^12)*BIN2DEC(AE68)+(2^15)*BIN2DEC(AD68)+(2^16)*BIN2DEC(AC68)+(2^19)*BIN2DEC(AB68))</f>
         <v>1191</v>
       </c>
       <c r="AR68" s="90" t="str">
-        <f t="shared" ref="AR68:AR76" si="48">"1 "&amp;H68&amp;" INSTRUCTION _"&amp;B68</f>
+        <f t="shared" ref="AR68:AR76" si="46">"1 "&amp;H68&amp;" INSTRUCTION _"&amp;B68</f>
         <v>1 52 INSTRUCTION _#.B</v>
       </c>
       <c r="AS68" s="90" t="str">
@@ -9695,20 +9679,20 @@
         <v>0</v>
       </c>
       <c r="F69" s="85">
-        <f t="shared" ref="F69:F76" si="49">F68+1</f>
+        <f t="shared" ref="F69:F76" si="47">F68+1</f>
         <v>53</v>
       </c>
       <c r="G69" s="85"/>
       <c r="H69" s="86">
+        <f t="shared" si="41"/>
+        <v>53</v>
+      </c>
+      <c r="I69" s="85" t="str">
+        <f t="shared" si="42"/>
+        <v>110101</v>
+      </c>
+      <c r="J69" s="85" t="str">
         <f t="shared" si="43"/>
-        <v>53</v>
-      </c>
-      <c r="I69" s="85" t="str">
-        <f t="shared" si="44"/>
-        <v>110101</v>
-      </c>
-      <c r="J69" s="85" t="str">
-        <f t="shared" si="45"/>
         <v>35</v>
       </c>
       <c r="K69" s="85"/>
@@ -9798,7 +9782,7 @@
         <v>7</v>
       </c>
       <c r="AM69" s="85" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="44"/>
         <v>0111</v>
       </c>
       <c r="AN69" s="85"/>
@@ -9807,11 +9791,11 @@
         <v>000000000010010100111</v>
       </c>
       <c r="AP69" s="1">
-        <f t="shared" si="47"/>
+        <f t="shared" si="45"/>
         <v>1191</v>
       </c>
       <c r="AR69" s="90" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="46"/>
         <v>1 53 INSTRUCTION _#.W</v>
       </c>
       <c r="AS69" s="90" t="str">
@@ -9831,20 +9815,20 @@
         <v>0</v>
       </c>
       <c r="F70" s="85">
-        <f t="shared" si="49"/>
+        <f t="shared" si="47"/>
         <v>54</v>
       </c>
       <c r="G70" s="85"/>
       <c r="H70" s="86">
+        <f t="shared" si="41"/>
+        <v>54</v>
+      </c>
+      <c r="I70" s="85" t="str">
+        <f t="shared" si="42"/>
+        <v>110110</v>
+      </c>
+      <c r="J70" s="85" t="str">
         <f t="shared" si="43"/>
-        <v>54</v>
-      </c>
-      <c r="I70" s="85" t="str">
-        <f t="shared" si="44"/>
-        <v>110110</v>
-      </c>
-      <c r="J70" s="85" t="str">
-        <f t="shared" si="45"/>
         <v>36</v>
       </c>
       <c r="K70" s="85"/>
@@ -9934,7 +9918,7 @@
         <v>7</v>
       </c>
       <c r="AM70" s="85" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="44"/>
         <v>0111</v>
       </c>
       <c r="AN70" s="85"/>
@@ -9943,11 +9927,11 @@
         <v>000000000010010100111</v>
       </c>
       <c r="AP70" s="1">
-        <f t="shared" si="47"/>
+        <f t="shared" si="45"/>
         <v>1191</v>
       </c>
       <c r="AR70" s="90" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="46"/>
         <v>1 54 INSTRUCTION _#.L</v>
       </c>
       <c r="AS70" s="90" t="str">
@@ -9967,20 +9951,20 @@
         <v>0</v>
       </c>
       <c r="F71" s="85">
-        <f t="shared" si="49"/>
+        <f t="shared" si="47"/>
         <v>55</v>
       </c>
       <c r="G71" s="85"/>
       <c r="H71" s="86">
+        <f t="shared" si="41"/>
+        <v>55</v>
+      </c>
+      <c r="I71" s="85" t="str">
+        <f t="shared" si="42"/>
+        <v>110111</v>
+      </c>
+      <c r="J71" s="85" t="str">
         <f t="shared" si="43"/>
-        <v>55</v>
-      </c>
-      <c r="I71" s="85" t="str">
-        <f t="shared" si="44"/>
-        <v>110111</v>
-      </c>
-      <c r="J71" s="85" t="str">
-        <f t="shared" si="45"/>
         <v>37</v>
       </c>
       <c r="K71" s="85"/>
@@ -10070,20 +10054,20 @@
         <v>0</v>
       </c>
       <c r="AM71" s="85" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="44"/>
         <v>0000</v>
       </c>
       <c r="AN71" s="85"/>
       <c r="AO71" s="9" t="str">
-        <f t="shared" ref="AO71:AO81" si="50">AB71&amp;AC71&amp;AD71&amp;AE71&amp;AF71&amp;AG71&amp;AH71&amp;AM71</f>
+        <f t="shared" ref="AO71:AO81" si="48">AB71&amp;AC71&amp;AD71&amp;AE71&amp;AF71&amp;AG71&amp;AH71&amp;AM71</f>
         <v>000001000001100100000</v>
       </c>
       <c r="AP71" s="1">
-        <f t="shared" si="47"/>
+        <f t="shared" si="45"/>
         <v>33568</v>
       </c>
       <c r="AR71" s="90" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="46"/>
         <v>1 55 INSTRUCTION _JMP</v>
       </c>
       <c r="AS71" s="90" t="str">
@@ -10103,20 +10087,20 @@
         <v>0</v>
       </c>
       <c r="F72" s="85">
-        <f t="shared" si="49"/>
+        <f t="shared" si="47"/>
         <v>56</v>
       </c>
       <c r="G72" s="85"/>
       <c r="H72" s="86">
+        <f t="shared" si="41"/>
+        <v>56</v>
+      </c>
+      <c r="I72" s="85" t="str">
+        <f t="shared" si="42"/>
+        <v>111000</v>
+      </c>
+      <c r="J72" s="85" t="str">
         <f t="shared" si="43"/>
-        <v>56</v>
-      </c>
-      <c r="I72" s="85" t="str">
-        <f t="shared" si="44"/>
-        <v>111000</v>
-      </c>
-      <c r="J72" s="85" t="str">
-        <f t="shared" si="45"/>
         <v>38</v>
       </c>
       <c r="K72" s="85"/>
@@ -10206,20 +10190,20 @@
         <v>0</v>
       </c>
       <c r="AM72" s="85" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="44"/>
         <v>0000</v>
       </c>
       <c r="AN72" s="85"/>
       <c r="AO72" s="9" t="str">
-        <f t="shared" si="50"/>
+        <f t="shared" si="48"/>
         <v>000101010000000000000</v>
       </c>
       <c r="AP72" s="1">
-        <f t="shared" si="47"/>
+        <f t="shared" si="45"/>
         <v>172032</v>
       </c>
       <c r="AR72" s="90" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="46"/>
         <v>1 56 INSTRUCTION _JSL</v>
       </c>
       <c r="AS72" s="90" t="s">
@@ -10238,20 +10222,20 @@
         <v>0</v>
       </c>
       <c r="F73" s="85">
-        <f t="shared" si="49"/>
+        <f t="shared" si="47"/>
         <v>57</v>
       </c>
       <c r="G73" s="85"/>
       <c r="H73" s="86">
+        <f t="shared" si="41"/>
+        <v>57</v>
+      </c>
+      <c r="I73" s="85" t="str">
+        <f t="shared" si="42"/>
+        <v>111001</v>
+      </c>
+      <c r="J73" s="85" t="str">
         <f t="shared" si="43"/>
-        <v>57</v>
-      </c>
-      <c r="I73" s="85" t="str">
-        <f t="shared" si="44"/>
-        <v>111001</v>
-      </c>
-      <c r="J73" s="85" t="str">
-        <f t="shared" si="45"/>
         <v>39</v>
       </c>
       <c r="K73" s="85"/>
@@ -10341,20 +10325,20 @@
         <v>0</v>
       </c>
       <c r="AM73" s="85" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="44"/>
         <v>0000</v>
       </c>
       <c r="AN73" s="85"/>
       <c r="AO73" s="9" t="str">
-        <f t="shared" si="50"/>
+        <f t="shared" si="48"/>
         <v>000101010001100100000</v>
       </c>
       <c r="AP73" s="1">
-        <f t="shared" si="47"/>
+        <f t="shared" si="45"/>
         <v>172832</v>
       </c>
       <c r="AR73" s="90" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="46"/>
         <v>1 57 INSTRUCTION _JSR</v>
       </c>
       <c r="AS73" s="90" t="str">
@@ -10370,20 +10354,20 @@
       <c r="D74" s="85"/>
       <c r="E74" s="85"/>
       <c r="F74" s="85">
-        <f t="shared" si="49"/>
+        <f t="shared" si="47"/>
         <v>58</v>
       </c>
       <c r="G74" s="85"/>
       <c r="H74" s="86">
+        <f t="shared" si="41"/>
+        <v>58</v>
+      </c>
+      <c r="I74" s="85" t="str">
+        <f t="shared" si="42"/>
+        <v>111010</v>
+      </c>
+      <c r="J74" s="85" t="str">
         <f t="shared" si="43"/>
-        <v>58</v>
-      </c>
-      <c r="I74" s="85" t="str">
-        <f t="shared" si="44"/>
-        <v>111010</v>
-      </c>
-      <c r="J74" s="85" t="str">
-        <f t="shared" si="45"/>
         <v>3A</v>
       </c>
       <c r="K74" s="85"/>
@@ -10473,20 +10457,20 @@
         <v>0</v>
       </c>
       <c r="AM74" s="85" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="44"/>
         <v>0000</v>
       </c>
       <c r="AN74" s="85"/>
       <c r="AO74" s="9" t="str">
-        <f t="shared" si="50"/>
+        <f t="shared" si="48"/>
         <v>000000000000000000000</v>
       </c>
       <c r="AP74" s="1">
-        <f t="shared" si="47"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="AR74" s="90" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="46"/>
         <v>1 58 INSTRUCTION _TRAP</v>
       </c>
       <c r="AS74" s="90" t="str">
@@ -10502,20 +10486,20 @@
       <c r="D75" s="85"/>
       <c r="E75" s="85"/>
       <c r="F75" s="85">
-        <f t="shared" si="49"/>
+        <f t="shared" si="47"/>
         <v>59</v>
       </c>
       <c r="G75" s="85"/>
       <c r="H75" s="86">
+        <f t="shared" si="41"/>
+        <v>59</v>
+      </c>
+      <c r="I75" s="85" t="str">
+        <f t="shared" si="42"/>
+        <v>111011</v>
+      </c>
+      <c r="J75" s="85" t="str">
         <f t="shared" si="43"/>
-        <v>59</v>
-      </c>
-      <c r="I75" s="85" t="str">
-        <f t="shared" si="44"/>
-        <v>111011</v>
-      </c>
-      <c r="J75" s="85" t="str">
-        <f t="shared" si="45"/>
         <v>3B</v>
       </c>
       <c r="K75" s="85"/>
@@ -10605,20 +10589,20 @@
         <v>0</v>
       </c>
       <c r="AM75" s="85" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="44"/>
         <v>0000</v>
       </c>
       <c r="AN75" s="85"/>
       <c r="AO75" s="9" t="str">
-        <f t="shared" si="50"/>
+        <f t="shared" si="48"/>
         <v>000000000000000000000</v>
       </c>
       <c r="AP75" s="1">
-        <f t="shared" si="47"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="AR75" s="90" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="46"/>
         <v>1 59 INSTRUCTION _RETRAP</v>
       </c>
       <c r="AS75" s="90" t="str">
@@ -10634,20 +10618,20 @@
       <c r="D76" s="85"/>
       <c r="E76" s="85"/>
       <c r="F76" s="85">
-        <f t="shared" si="49"/>
+        <f t="shared" si="47"/>
         <v>60</v>
       </c>
       <c r="G76" s="85"/>
       <c r="H76" s="86">
+        <f t="shared" si="41"/>
+        <v>60</v>
+      </c>
+      <c r="I76" s="85" t="str">
+        <f t="shared" si="42"/>
+        <v>111100</v>
+      </c>
+      <c r="J76" s="85" t="str">
         <f t="shared" si="43"/>
-        <v>60</v>
-      </c>
-      <c r="I76" s="85" t="str">
-        <f t="shared" si="44"/>
-        <v>111100</v>
-      </c>
-      <c r="J76" s="85" t="str">
-        <f t="shared" si="45"/>
         <v>3C</v>
       </c>
       <c r="K76" s="85"/>
@@ -10737,20 +10721,20 @@
         <v>0</v>
       </c>
       <c r="AM76" s="85" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="44"/>
         <v>0000</v>
       </c>
       <c r="AN76" s="85"/>
       <c r="AO76" s="9" t="str">
-        <f t="shared" si="50"/>
+        <f t="shared" si="48"/>
         <v>000000000000000000000</v>
       </c>
       <c r="AP76" s="1">
-        <f t="shared" si="47"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="AR76" s="90" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="46"/>
         <v>1 60 INSTRUCTION _RTI</v>
       </c>
       <c r="AS76" s="90" t="str">
@@ -10778,7 +10762,7 @@
       <c r="AC77" s="8"/>
       <c r="AF77" s="8"/>
       <c r="AO77" s="9" t="str">
-        <f t="shared" si="50"/>
+        <f t="shared" si="48"/>
         <v/>
       </c>
       <c r="AP77" s="1"/>
@@ -10807,7 +10791,7 @@
       <c r="AC78" s="8"/>
       <c r="AF78" s="8"/>
       <c r="AO78" s="9" t="str">
-        <f t="shared" si="50"/>
+        <f t="shared" si="48"/>
         <v/>
       </c>
       <c r="AP78" s="1"/>
@@ -10927,16 +10911,16 @@
         <v>0</v>
       </c>
       <c r="AM79" s="43" t="str">
-        <f t="shared" ref="AM79:AM81" si="51">DEC2BIN(SUM(AI79:AL79),4)</f>
+        <f t="shared" ref="AM79:AM81" si="49">DEC2BIN(SUM(AI79:AL79),4)</f>
         <v>0000</v>
       </c>
       <c r="AN79" s="43"/>
       <c r="AO79" s="9" t="str">
-        <f t="shared" si="50"/>
+        <f t="shared" si="48"/>
         <v>000000100000000000000</v>
       </c>
       <c r="AP79" s="1">
-        <f t="shared" ref="AP79:AP81" si="52">(BIN2DEC(AM79)+(2^4)*BIN2DEC(AH79)+(2^7)*BIN2DEC(AG79)+(2^9)*BIN2DEC(AF79)+(2^12)*BIN2DEC(AE79)+(2^15)*BIN2DEC(AD79)+(2^16)*BIN2DEC(AC79)+(2^19)*BIN2DEC(AB79))</f>
+        <f t="shared" ref="AP79:AP81" si="50">(BIN2DEC(AM79)+(2^4)*BIN2DEC(AH79)+(2^7)*BIN2DEC(AG79)+(2^9)*BIN2DEC(AF79)+(2^12)*BIN2DEC(AE79)+(2^15)*BIN2DEC(AD79)+(2^16)*BIN2DEC(AC79)+(2^19)*BIN2DEC(AB79))</f>
         <v>16384</v>
       </c>
       <c r="AR79" s="92" t="str">
@@ -11062,16 +11046,16 @@
         <v>7</v>
       </c>
       <c r="AM80" s="43" t="str">
-        <f t="shared" si="51"/>
+        <f t="shared" si="49"/>
         <v>0111</v>
       </c>
       <c r="AN80" s="43"/>
       <c r="AO80" s="9" t="str">
+        <f t="shared" si="48"/>
+        <v>000000000000000100111</v>
+      </c>
+      <c r="AP80" s="1">
         <f t="shared" si="50"/>
-        <v>000000000000000100111</v>
-      </c>
-      <c r="AP80" s="1">
-        <f t="shared" si="52"/>
         <v>39</v>
       </c>
       <c r="AR80" s="92" t="str">
@@ -11103,7 +11087,7 @@
         <v>63</v>
       </c>
       <c r="I81" s="43" t="str">
-        <f t="shared" ref="I81" si="53">DEC2BIN(H81,6)</f>
+        <f t="shared" ref="I81" si="51">DEC2BIN(H81,6)</f>
         <v>111111</v>
       </c>
       <c r="J81" s="43" t="str">
@@ -11195,16 +11179,16 @@
         <v>0</v>
       </c>
       <c r="AM81" s="43" t="str">
-        <f t="shared" si="51"/>
+        <f t="shared" si="49"/>
         <v>0000</v>
       </c>
       <c r="AN81" s="43"/>
       <c r="AO81" s="9" t="str">
+        <f t="shared" si="48"/>
+        <v>000000000000000000000</v>
+      </c>
+      <c r="AP81" s="1">
         <f t="shared" si="50"/>
-        <v>000000000000000000000</v>
-      </c>
-      <c r="AP81" s="1">
-        <f t="shared" si="52"/>
         <v>0</v>
       </c>
       <c r="AR81" s="92" t="str">
@@ -11296,12 +11280,12 @@
       </c>
       <c r="G85" s="101"/>
       <c r="H85" s="102">
-        <f t="shared" ref="H85:H87" si="54">F85+E85*64+D85*128</f>
+        <f t="shared" ref="H85:H87" si="52">F85+E85*64+D85*128</f>
         <v>64</v>
       </c>
       <c r="I85" s="101"/>
       <c r="J85" s="101" t="str">
-        <f t="shared" ref="J85:J87" si="55">DEC2HEX(H85)</f>
+        <f t="shared" ref="J85:J87" si="53">DEC2HEX(H85)</f>
         <v>40</v>
       </c>
       <c r="K85" s="101"/>
@@ -11335,7 +11319,7 @@
       <c r="AM85" s="101"/>
       <c r="AN85" s="101"/>
       <c r="AO85" s="9" t="str">
-        <f t="shared" ref="AO85" si="56">AB85&amp;AC85&amp;AD85&amp;AE85&amp;AF85&amp;AG85&amp;AH85&amp;AM85</f>
+        <f t="shared" ref="AO85" si="54">AB85&amp;AC85&amp;AD85&amp;AE85&amp;AF85&amp;AG85&amp;AH85&amp;AM85</f>
         <v/>
       </c>
       <c r="AR85" s="107"/>
@@ -11357,12 +11341,12 @@
       </c>
       <c r="G86" s="101"/>
       <c r="H86" s="102">
-        <f t="shared" si="54"/>
+        <f t="shared" si="52"/>
         <v>128</v>
       </c>
       <c r="I86" s="101"/>
       <c r="J86" s="101" t="str">
-        <f t="shared" si="55"/>
+        <f t="shared" si="53"/>
         <v>80</v>
       </c>
       <c r="K86" s="101"/>
@@ -11417,12 +11401,12 @@
       </c>
       <c r="G87" s="101"/>
       <c r="H87" s="102">
-        <f t="shared" si="54"/>
+        <f t="shared" si="52"/>
         <v>192</v>
       </c>
       <c r="I87" s="101"/>
       <c r="J87" s="101" t="str">
-        <f t="shared" si="55"/>
+        <f t="shared" si="53"/>
         <v>C0</v>
       </c>
       <c r="K87" s="101"/>

</xml_diff>

<commit_message>
Virtualization unit integrated with CPU and ready for further testing
</commit_message>
<xml_diff>
--- a/Resources/Instruction Set.xlsx
+++ b/Resources/Instruction Set.xlsx
@@ -4,14 +4,16 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="18195" windowHeight="8130" tabRatio="681"/>
+    <workbookView xWindow="240" yWindow="300" windowWidth="18195" windowHeight="8070" tabRatio="681" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="OPCODE_encoding" sheetId="1" r:id="rId1"/>
     <sheet name="OPCODE_mult" sheetId="5" r:id="rId2"/>
     <sheet name="Multiplexers" sheetId="2" r:id="rId3"/>
     <sheet name="ALU" sheetId="3" r:id="rId4"/>
-    <sheet name="Copyright and license" sheetId="6" r:id="rId5"/>
+    <sheet name="Virtualization" sheetId="8" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="7" r:id="rId6"/>
+    <sheet name="Copyright and license" sheetId="6" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">OPCODE_encoding!$A$3:$M$86</definedName>
@@ -21,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1294" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1303" uniqueCount="346">
   <si>
     <t>DUP</t>
   </si>
@@ -1034,15 +1036,6 @@
     <t>Reset all stack pointers to zero</t>
   </si>
   <si>
-    <t>VMLOAD</t>
-  </si>
-  <si>
-    <t>00001010100000000000000</t>
-  </si>
-  <si>
-    <t>21098765432109876543210</t>
-  </si>
-  <si>
     <t>UNUSED</t>
   </si>
   <si>
@@ -1050,6 +1043,24 @@
   </si>
   <si>
     <t>Internal microcode</t>
+  </si>
+  <si>
+    <t>PAUSE</t>
+  </si>
+  <si>
+    <t>Context switch to next task</t>
+  </si>
+  <si>
+    <t>VM</t>
+  </si>
+  <si>
+    <t>TORS_n</t>
+  </si>
+  <si>
+    <t>width</t>
+  </si>
+  <si>
+    <t>datapathFreeze/Thaw</t>
   </si>
 </sst>
 </file>
@@ -1489,7 +1500,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="122">
+  <cellXfs count="125">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1780,6 +1791,11 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2086,11 +2102,11 @@
   </sheetPr>
   <dimension ref="A1:AS98"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="10" ySplit="4" topLeftCell="K5" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="10" ySplit="4" topLeftCell="K54" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AR15" sqref="AR15"/>
+      <selection pane="bottomRight" activeCell="AR86" sqref="AR86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -2224,7 +2240,7 @@
         <v>318</v>
       </c>
       <c r="R4" s="5" t="s">
-        <v>240</v>
+        <v>343</v>
       </c>
       <c r="S4" s="5" t="s">
         <v>139</v>
@@ -9742,7 +9758,7 @@
         <v>0</v>
       </c>
       <c r="F69" s="84">
-        <f t="shared" ref="F69:F76" si="38">F68+1</f>
+        <f t="shared" ref="F69:F77" si="38">F68+1</f>
         <v>53</v>
       </c>
       <c r="G69" s="84"/>
@@ -10414,8 +10430,12 @@
         <v>268</v>
       </c>
       <c r="C74" s="84"/>
-      <c r="D74" s="84"/>
-      <c r="E74" s="84"/>
+      <c r="D74" s="84">
+        <v>0</v>
+      </c>
+      <c r="E74" s="84">
+        <v>0</v>
+      </c>
       <c r="F74" s="84">
         <f t="shared" si="38"/>
         <v>58</v>
@@ -10546,8 +10566,12 @@
         <v>309</v>
       </c>
       <c r="C75" s="84"/>
-      <c r="D75" s="84"/>
-      <c r="E75" s="84"/>
+      <c r="D75" s="84">
+        <v>0</v>
+      </c>
+      <c r="E75" s="84">
+        <v>0</v>
+      </c>
       <c r="F75" s="84">
         <f t="shared" si="38"/>
         <v>59</v>
@@ -10678,8 +10702,12 @@
         <v>271</v>
       </c>
       <c r="C76" s="84"/>
-      <c r="D76" s="84"/>
-      <c r="E76" s="84"/>
+      <c r="D76" s="84">
+        <v>0</v>
+      </c>
+      <c r="E76" s="84">
+        <v>0</v>
+      </c>
       <c r="F76" s="84">
         <f t="shared" si="38"/>
         <v>60</v>
@@ -10806,76 +10834,166 @@
       </c>
     </row>
     <row r="77" spans="1:45" s="83" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B77" s="84"/>
+      <c r="B77" s="84" t="s">
+        <v>340</v>
+      </c>
       <c r="C77" s="84"/>
-      <c r="D77" s="84"/>
-      <c r="E77" s="84"/>
-      <c r="F77" s="84"/>
+      <c r="D77" s="84">
+        <v>0</v>
+      </c>
+      <c r="E77" s="84">
+        <v>0</v>
+      </c>
+      <c r="F77" s="84">
+        <f t="shared" si="38"/>
+        <v>61</v>
+      </c>
       <c r="G77" s="84"/>
-      <c r="H77" s="85"/>
-      <c r="I77" s="84"/>
-      <c r="J77" s="84"/>
+      <c r="H77" s="85">
+        <f t="shared" ref="H77" si="40">F77+E77*64+D77*128</f>
+        <v>61</v>
+      </c>
+      <c r="I77" s="3" t="str">
+        <f t="shared" ref="I77" si="41">DEC2BIN(H77,7)</f>
+        <v>0111101</v>
+      </c>
+      <c r="J77" s="84" t="str">
+        <f t="shared" ref="J77" si="42">DEC2HEX(H77)</f>
+        <v>3D</v>
+      </c>
       <c r="K77" s="84"/>
-      <c r="L77" s="86"/>
+      <c r="L77" s="86" t="s">
+        <v>107</v>
+      </c>
+      <c r="M77" s="83" t="s">
+        <v>341</v>
+      </c>
       <c r="N77" s="84"/>
       <c r="O77" s="87"/>
-      <c r="P77" s="84"/>
-      <c r="Q77" s="84"/>
-      <c r="R77" s="84"/>
-      <c r="S77" s="84"/>
-      <c r="T77" s="84"/>
-      <c r="U77" s="84"/>
-      <c r="V77" s="84"/>
-      <c r="W77" s="84"/>
-      <c r="X77" s="84"/>
-      <c r="Y77" s="84"/>
-      <c r="Z77" s="84"/>
-      <c r="AB77" s="8"/>
-      <c r="AC77" s="8"/>
-      <c r="AD77" s="8"/>
-      <c r="AE77" s="8"/>
-      <c r="AF77" s="8"/>
-      <c r="AG77" s="8"/>
-      <c r="AH77" s="8"/>
-      <c r="AI77" s="84"/>
-      <c r="AJ77" s="84"/>
-      <c r="AK77" s="84"/>
-      <c r="AL77" s="84"/>
-      <c r="AM77" s="8"/>
+      <c r="P77" s="84" t="s">
+        <v>342</v>
+      </c>
+      <c r="Q77" s="84" t="s">
+        <v>342</v>
+      </c>
+      <c r="R77" s="84" t="s">
+        <v>29</v>
+      </c>
+      <c r="S77" s="84" t="s">
+        <v>342</v>
+      </c>
+      <c r="T77" s="84" t="s">
+        <v>342</v>
+      </c>
+      <c r="U77" s="84" t="s">
+        <v>342</v>
+      </c>
+      <c r="V77" s="84" t="s">
+        <v>231</v>
+      </c>
+      <c r="W77" s="84" t="s">
+        <v>131</v>
+      </c>
+      <c r="X77" s="84" t="s">
+        <v>131</v>
+      </c>
+      <c r="Y77" s="84" t="s">
+        <v>131</v>
+      </c>
+      <c r="Z77" s="84" t="s">
+        <v>342</v>
+      </c>
+      <c r="AB77" s="8" t="str">
+        <f>DEC2BIN(VLOOKUP(P77,OPCODE_mult!$C$4:$N$19,12,FALSE),OPCODE_mult!C$21)</f>
+        <v>100</v>
+      </c>
+      <c r="AC77" s="8" t="str">
+        <f>DEC2BIN(VLOOKUP(Q77,OPCODE_mult!$D$4:$N$19,11,FALSE),OPCODE_mult!D$21)</f>
+        <v>101</v>
+      </c>
+      <c r="AD77" s="8" t="str">
+        <f>DEC2BIN(VLOOKUP(R77,OPCODE_mult!$E$4:$N$19,10,FALSE),OPCODE_mult!E$21)</f>
+        <v>0</v>
+      </c>
+      <c r="AE77" s="8" t="str">
+        <f>DEC2BIN(VLOOKUP(S77,OPCODE_mult!$F$4:$N$19,9,FALSE),OPCODE_mult!F$21)</f>
+        <v>110</v>
+      </c>
+      <c r="AF77" s="8" t="str">
+        <f>DEC2BIN(VLOOKUP(T77,OPCODE_mult!$G$4:$N$19,8,FALSE),OPCODE_mult!G$21)</f>
+        <v>110</v>
+      </c>
+      <c r="AG77" s="8" t="str">
+        <f>DEC2BIN(VLOOKUP(U77,OPCODE_mult!$H$4:$N$19,7,FALSE),OPCODE_mult!H$21)</f>
+        <v>100</v>
+      </c>
+      <c r="AH77" s="8" t="str">
+        <f>DEC2BIN(IF(V77="X",0,VLOOKUP(V77,OPCODE_mult!$I$4:$N$19,6,FALSE)),OPCODE_mult!I$21)</f>
+        <v>010</v>
+      </c>
+      <c r="AI77" s="84">
+        <f>IF(W77="X",0,VLOOKUP(W77,OPCODE_mult!$J$4:$N$19,5,FALSE))</f>
+        <v>0</v>
+      </c>
+      <c r="AJ77" s="84">
+        <f>IF(X77="X",0,VLOOKUP(X77,OPCODE_mult!$K$4:$N$19,4,FALSE))</f>
+        <v>0</v>
+      </c>
+      <c r="AK77" s="84">
+        <f>IF(Y77="X",0,VLOOKUP(Y77,OPCODE_mult!$L$4:$N$19,3,FALSE))</f>
+        <v>0</v>
+      </c>
+      <c r="AL77" s="84">
+        <f>IF(Z77="X",0,VLOOKUP(Z77,OPCODE_mult!$M$4:$N$19,2,FALSE))</f>
+        <v>4</v>
+      </c>
+      <c r="AM77" s="8" t="str">
+        <f>DEC2BIN(SUM(AI77:AL77),OPCODE_mult!J$21)</f>
+        <v>0100</v>
+      </c>
       <c r="AN77" s="84"/>
-      <c r="AO77" s="9"/>
-      <c r="AP77" s="1"/>
-      <c r="AR77" s="89"/>
-      <c r="AS77" s="89"/>
-    </row>
-    <row r="78" spans="1:45" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="2" t="s">
-        <v>341</v>
-      </c>
-      <c r="B78" s="8"/>
-      <c r="C78" s="8"/>
-      <c r="D78" s="8"/>
-      <c r="E78" s="8"/>
-      <c r="F78" s="8"/>
-      <c r="G78" s="8"/>
-      <c r="H78" s="44"/>
-      <c r="I78" s="8"/>
-      <c r="J78" s="8"/>
-      <c r="K78" s="8"/>
-      <c r="L78" s="73"/>
-      <c r="N78" s="8"/>
-      <c r="O78" s="9"/>
-      <c r="P78" s="8"/>
-      <c r="Q78" s="8"/>
-      <c r="R78" s="8"/>
-      <c r="S78" s="8"/>
-      <c r="T78" s="8"/>
-      <c r="U78" s="8"/>
-      <c r="V78" s="8"/>
-      <c r="W78" s="8"/>
-      <c r="X78" s="8"/>
-      <c r="Y78" s="8"/>
-      <c r="Z78" s="8"/>
+      <c r="AO77" s="9" t="str">
+        <f t="shared" ref="AO77" si="43">AB77&amp;AC77&amp;AD77&amp;AE77&amp;AF77&amp;AG77&amp;AH77&amp;AM77</f>
+        <v>10010101101101000100100</v>
+      </c>
+      <c r="AP77" s="1">
+        <f>(BIN2DEC(AM77)+(2^OPCODE_mult!$I$25)*BIN2DEC(AH77)+(2^OPCODE_mult!$H$25)*BIN2DEC(AG77)+(2^OPCODE_mult!$G$25)*BIN2DEC(AF77)+(2^OPCODE_mult!$F$25)*BIN2DEC(AE77)+(2^OPCODE_mult!$E$25)*BIN2DEC(AD77)+(2^OPCODE_mult!$D$25)*BIN2DEC(AC77)+(2^OPCODE_mult!$C$25)*BIN2DEC(AB77))</f>
+        <v>4905508</v>
+      </c>
+      <c r="AR77" s="89" t="str">
+        <f t="shared" ref="AR77" si="44">"1 "&amp;H77&amp;" INSTRUCTION _"&amp;B77</f>
+        <v>1 61 INSTRUCTION _PAUSE</v>
+      </c>
+      <c r="AS77" s="89" t="str">
+        <f>CHAR(44)&amp;CHAR(34)&amp;CHAR(32)&amp;B77&amp;CHAR(34)</f>
+        <v>," PAUSE"</v>
+      </c>
+    </row>
+    <row r="78" spans="1:45" s="83" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B78" s="84"/>
+      <c r="C78" s="84"/>
+      <c r="D78" s="84"/>
+      <c r="E78" s="84"/>
+      <c r="F78" s="84"/>
+      <c r="G78" s="84"/>
+      <c r="H78" s="85"/>
+      <c r="I78" s="84"/>
+      <c r="J78" s="84"/>
+      <c r="K78" s="84"/>
+      <c r="L78" s="86"/>
+      <c r="N78" s="84"/>
+      <c r="O78" s="87"/>
+      <c r="P78" s="84"/>
+      <c r="Q78" s="84"/>
+      <c r="R78" s="84"/>
+      <c r="S78" s="84"/>
+      <c r="T78" s="84"/>
+      <c r="U78" s="84"/>
+      <c r="V78" s="84"/>
+      <c r="W78" s="84"/>
+      <c r="X78" s="84"/>
+      <c r="Y78" s="84"/>
+      <c r="Z78" s="84"/>
       <c r="AB78" s="8"/>
       <c r="AC78" s="8"/>
       <c r="AD78" s="8"/>
@@ -10883,150 +11001,65 @@
       <c r="AF78" s="8"/>
       <c r="AG78" s="8"/>
       <c r="AH78" s="8"/>
-      <c r="AI78" s="8"/>
-      <c r="AJ78" s="8"/>
-      <c r="AK78" s="8"/>
-      <c r="AL78" s="8"/>
+      <c r="AI78" s="84"/>
+      <c r="AJ78" s="84"/>
+      <c r="AK78" s="84"/>
+      <c r="AL78" s="84"/>
       <c r="AM78" s="8"/>
-      <c r="AN78" s="8"/>
+      <c r="AN78" s="84"/>
       <c r="AO78" s="9"/>
-      <c r="AR78" s="58"/>
-      <c r="AS78" s="58"/>
+      <c r="AP78" s="1"/>
+      <c r="AR78" s="89"/>
+      <c r="AS78" s="89"/>
     </row>
     <row r="79" spans="1:45" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B79" s="8" t="s">
-        <v>340</v>
-      </c>
+      <c r="A79" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="B79" s="8"/>
       <c r="C79" s="8"/>
-      <c r="D79" s="8">
-        <v>0</v>
-      </c>
-      <c r="E79" s="8">
-        <v>0</v>
-      </c>
-      <c r="F79" s="8">
-        <v>61</v>
-      </c>
+      <c r="D79" s="8"/>
+      <c r="E79" s="8"/>
+      <c r="F79" s="8"/>
       <c r="G79" s="8"/>
-      <c r="H79" s="44">
-        <f>F79+E79*64+D79*128</f>
-        <v>61</v>
-      </c>
-      <c r="I79" s="8" t="str">
-        <f t="shared" ref="I79:I81" si="40">DEC2BIN(H79,7)</f>
-        <v>0111101</v>
-      </c>
-      <c r="J79" s="8" t="str">
-        <f>DEC2HEX(H79)</f>
-        <v>3D</v>
-      </c>
+      <c r="H79" s="44"/>
+      <c r="I79" s="8"/>
+      <c r="J79" s="8"/>
       <c r="K79" s="8"/>
       <c r="L79" s="73"/>
       <c r="N79" s="8"/>
       <c r="O79" s="9"/>
-      <c r="P79" s="3" t="s">
-        <v>323</v>
-      </c>
-      <c r="Q79" s="3" t="s">
-        <v>320</v>
-      </c>
-      <c r="R79" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="S79" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="T79" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="U79" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="V79" s="8" t="s">
-        <v>217</v>
-      </c>
-      <c r="W79" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="X79" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="Y79" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="Z79" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="AA79" s="1"/>
-      <c r="AB79" s="8" t="str">
-        <f>DEC2BIN(VLOOKUP(P79,OPCODE_mult!$C$4:$N$19,12,FALSE),OPCODE_mult!C$21)</f>
-        <v>000</v>
-      </c>
-      <c r="AC79" s="8" t="str">
-        <f>DEC2BIN(VLOOKUP(Q79,OPCODE_mult!$D$4:$N$19,11,FALSE),OPCODE_mult!D$21)</f>
-        <v>000</v>
-      </c>
-      <c r="AD79" s="8" t="str">
-        <f>DEC2BIN(VLOOKUP(R79,OPCODE_mult!$E$4:$N$19,10,FALSE),OPCODE_mult!E$21)</f>
-        <v>0</v>
-      </c>
-      <c r="AE79" s="8" t="str">
-        <f>DEC2BIN(VLOOKUP(S79,OPCODE_mult!$F$4:$N$19,9,FALSE),OPCODE_mult!F$21)</f>
-        <v>000</v>
-      </c>
-      <c r="AF79" s="8" t="str">
-        <f>DEC2BIN(VLOOKUP(T79,OPCODE_mult!$G$4:$N$19,8,FALSE),OPCODE_mult!G$21)</f>
-        <v>000</v>
-      </c>
-      <c r="AG79" s="8" t="str">
-        <f>DEC2BIN(VLOOKUP(U79,OPCODE_mult!$H$4:$N$19,7,FALSE),OPCODE_mult!H$21)</f>
-        <v>000</v>
-      </c>
-      <c r="AH79" s="8" t="str">
-        <f>DEC2BIN(IF(V79="X",0,VLOOKUP(V79,OPCODE_mult!$I$4:$N$19,6,FALSE)),OPCODE_mult!I$21)</f>
-        <v>000</v>
-      </c>
-      <c r="AI79" s="8">
-        <f>IF(W79="X",0,VLOOKUP(W79,OPCODE_mult!$J$4:$N$19,5,FALSE))</f>
-        <v>0</v>
-      </c>
-      <c r="AJ79" s="8">
-        <f>IF(X79="X",0,VLOOKUP(X79,OPCODE_mult!$K$4:$N$19,4,FALSE))</f>
-        <v>0</v>
-      </c>
-      <c r="AK79" s="8">
-        <f>IF(Y79="X",0,VLOOKUP(Y79,OPCODE_mult!$L$4:$N$19,3,FALSE))</f>
-        <v>0</v>
-      </c>
-      <c r="AL79" s="8">
-        <f>IF(Z79="X",0,VLOOKUP(Z79,OPCODE_mult!$M$4:$N$19,2,FALSE))</f>
-        <v>0</v>
-      </c>
-      <c r="AM79" s="8" t="str">
-        <f>DEC2BIN(SUM(AI79:AL79),OPCODE_mult!J$21)</f>
-        <v>0000</v>
-      </c>
-      <c r="AN79" s="1"/>
-      <c r="AO79" s="9" t="str">
-        <f>AB79&amp;AC79&amp;AD79&amp;AE79&amp;AF79&amp;AG79&amp;AH79&amp;AM79</f>
-        <v>00000000000000000000000</v>
-      </c>
-      <c r="AP79" s="1">
-        <f>(BIN2DEC(AM79)+(2^OPCODE_mult!$I$25)*BIN2DEC(AH79)+(2^OPCODE_mult!$H$25)*BIN2DEC(AG79)+(2^OPCODE_mult!$G$25)*BIN2DEC(AF79)+(2^OPCODE_mult!$F$25)*BIN2DEC(AE79)+(2^OPCODE_mult!$E$25)*BIN2DEC(AD79)+(2^OPCODE_mult!$D$25)*BIN2DEC(AC79)+(2^OPCODE_mult!$C$25)*BIN2DEC(AB79))</f>
-        <v>0</v>
-      </c>
-      <c r="AR79" s="89" t="str">
-        <f t="shared" ref="AR79:AR81" si="41">"1 "&amp;H79&amp;" INSTRUCTION _"&amp;B79</f>
-        <v>1 61 INSTRUCTION _UNUSED</v>
-      </c>
-      <c r="AS79" s="89" t="str">
-        <f t="shared" ref="AS79:AS81" si="42">CHAR(44)&amp;CHAR(34)&amp;CHAR(32)&amp;B79&amp;CHAR(34)</f>
-        <v>," UNUSED"</v>
-      </c>
+      <c r="P79" s="8"/>
+      <c r="Q79" s="8"/>
+      <c r="R79" s="8"/>
+      <c r="S79" s="8"/>
+      <c r="T79" s="8"/>
+      <c r="U79" s="8"/>
+      <c r="V79" s="8"/>
+      <c r="W79" s="8"/>
+      <c r="X79" s="8"/>
+      <c r="Y79" s="8"/>
+      <c r="Z79" s="8"/>
+      <c r="AB79" s="8"/>
+      <c r="AC79" s="8"/>
+      <c r="AD79" s="8"/>
+      <c r="AE79" s="8"/>
+      <c r="AF79" s="8"/>
+      <c r="AG79" s="8"/>
+      <c r="AH79" s="8"/>
+      <c r="AI79" s="8"/>
+      <c r="AJ79" s="8"/>
+      <c r="AK79" s="8"/>
+      <c r="AL79" s="8"/>
+      <c r="AM79" s="8"/>
+      <c r="AN79" s="8"/>
+      <c r="AO79" s="9"/>
+      <c r="AR79" s="58"/>
+      <c r="AS79" s="58"/>
     </row>
     <row r="80" spans="1:45" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B80" s="8" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="C80" s="8"/>
       <c r="D80" s="8">
@@ -11040,15 +11073,15 @@
       </c>
       <c r="G80" s="8"/>
       <c r="H80" s="44">
-        <f t="shared" ref="H80:H81" si="43">F80+E80*64+D80*128</f>
+        <f>F80+E80*64+D80*128</f>
         <v>62</v>
       </c>
       <c r="I80" s="8" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" ref="I80:I81" si="45">DEC2BIN(H80,7)</f>
         <v>0111110</v>
       </c>
       <c r="J80" s="8" t="str">
-        <f t="shared" ref="J80:J81" si="44">DEC2HEX(H80)</f>
+        <f>DEC2HEX(H80)</f>
         <v>3E</v>
       </c>
       <c r="K80" s="8"/>
@@ -11147,17 +11180,17 @@
         <v>0</v>
       </c>
       <c r="AR80" s="89" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" ref="AR80:AR81" si="46">"1 "&amp;H80&amp;" INSTRUCTION _"&amp;B80</f>
         <v>1 62 INSTRUCTION _UNUSED</v>
       </c>
       <c r="AS80" s="89" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" ref="AS80:AS81" si="47">CHAR(44)&amp;CHAR(34)&amp;CHAR(32)&amp;B80&amp;CHAR(34)</f>
         <v>," UNUSED"</v>
       </c>
     </row>
     <row r="81" spans="1:45" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B81" s="8" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="C81" s="8"/>
       <c r="D81" s="8">
@@ -11171,15 +11204,15 @@
       </c>
       <c r="G81" s="8"/>
       <c r="H81" s="44">
-        <f t="shared" si="43"/>
+        <f t="shared" ref="H81" si="48">F81+E81*64+D81*128</f>
         <v>63</v>
       </c>
       <c r="I81" s="8" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="45"/>
         <v>0111111</v>
       </c>
       <c r="J81" s="8" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" ref="J81" si="49">DEC2HEX(H81)</f>
         <v>3F</v>
       </c>
       <c r="K81" s="8"/>
@@ -11278,11 +11311,11 @@
         <v>0</v>
       </c>
       <c r="AR81" s="89" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="46"/>
         <v>1 63 INSTRUCTION _UNUSED</v>
       </c>
       <c r="AS81" s="89" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" si="47"/>
         <v>," UNUSED"</v>
       </c>
     </row>
@@ -11311,7 +11344,7 @@
     </row>
     <row r="83" spans="1:45" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A83" s="18" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="B83" s="43"/>
       <c r="C83" s="43"/>
@@ -11354,11 +11387,11 @@
       </c>
       <c r="G84" s="43"/>
       <c r="H84" s="48">
-        <f t="shared" ref="H84" si="45">F84+E84*64+D84*128</f>
+        <f t="shared" ref="H84" si="50">F84+E84*64+D84*128</f>
         <v>64</v>
       </c>
       <c r="I84" s="43" t="str">
-        <f t="shared" ref="I84:I86" si="46">DEC2BIN(H84,7)</f>
+        <f t="shared" ref="I84:I86" si="51">DEC2BIN(H84,7)</f>
         <v>1000000</v>
       </c>
       <c r="J84" s="43" t="str">
@@ -11485,7 +11518,7 @@
         <v>65</v>
       </c>
       <c r="I85" s="43" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="51"/>
         <v>1000001</v>
       </c>
       <c r="J85" s="43" t="str">
@@ -11614,7 +11647,7 @@
         <v>66</v>
       </c>
       <c r="I86" s="43" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="51"/>
         <v>1000010</v>
       </c>
       <c r="J86" s="43" t="str">
@@ -11764,12 +11797,12 @@
       </c>
       <c r="G89" s="100"/>
       <c r="H89" s="101">
-        <f t="shared" ref="H89:H91" si="47">F89+E89*64+D89*128</f>
+        <f t="shared" ref="H89:H91" si="52">F89+E89*64+D89*128</f>
         <v>64</v>
       </c>
       <c r="I89" s="100"/>
       <c r="J89" s="100" t="str">
-        <f t="shared" ref="J89:J91" si="48">DEC2HEX(H89)</f>
+        <f t="shared" ref="J89:J91" si="53">DEC2HEX(H89)</f>
         <v>40</v>
       </c>
       <c r="K89" s="100"/>
@@ -11803,7 +11836,7 @@
       <c r="AM89" s="100"/>
       <c r="AN89" s="100"/>
       <c r="AO89" s="9" t="str">
-        <f t="shared" ref="AO89" si="49">AB89&amp;AC89&amp;AD89&amp;AE89&amp;AF89&amp;AG89&amp;AH89&amp;AM89</f>
+        <f t="shared" ref="AO89" si="54">AB89&amp;AC89&amp;AD89&amp;AE89&amp;AF89&amp;AG89&amp;AH89&amp;AM89</f>
         <v/>
       </c>
       <c r="AR89" s="106"/>
@@ -11825,12 +11858,12 @@
       </c>
       <c r="G90" s="100"/>
       <c r="H90" s="101">
-        <f t="shared" si="47"/>
+        <f t="shared" si="52"/>
         <v>128</v>
       </c>
       <c r="I90" s="100"/>
       <c r="J90" s="100" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="53"/>
         <v>80</v>
       </c>
       <c r="K90" s="100"/>
@@ -11885,12 +11918,12 @@
       </c>
       <c r="G91" s="100"/>
       <c r="H91" s="101">
-        <f t="shared" si="47"/>
+        <f t="shared" si="52"/>
         <v>192</v>
       </c>
       <c r="I91" s="100"/>
       <c r="J91" s="100" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="53"/>
         <v>C0</v>
       </c>
       <c r="K91" s="100"/>
@@ -11997,7 +12030,7 @@
   <dimension ref="A1:N31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12022,7 +12055,7 @@
         <v>318</v>
       </c>
       <c r="E3" s="65" t="s">
-        <v>240</v>
+        <v>343</v>
       </c>
       <c r="F3" s="65" t="s">
         <v>139</v>
@@ -12215,7 +12248,7 @@
         <v>4</v>
       </c>
       <c r="C8" s="119" t="s">
-        <v>337</v>
+        <v>342</v>
       </c>
       <c r="D8" s="61" t="s">
         <v>308</v>
@@ -12228,7 +12261,7 @@
         <v>317</v>
       </c>
       <c r="H8" s="119" t="s">
-        <v>337</v>
+        <v>342</v>
       </c>
       <c r="I8" s="112" t="s">
         <v>175</v>
@@ -12243,7 +12276,7 @@
         <v>119</v>
       </c>
       <c r="M8" s="119" t="s">
-        <v>337</v>
+        <v>342</v>
       </c>
       <c r="N8" s="109">
         <v>4</v>
@@ -12255,7 +12288,7 @@
       </c>
       <c r="C9" s="62"/>
       <c r="D9" s="119" t="s">
-        <v>337</v>
+        <v>342</v>
       </c>
       <c r="E9" s="62"/>
       <c r="F9" s="61" t="s">
@@ -12292,10 +12325,10 @@
       <c r="D10" s="62"/>
       <c r="E10" s="62"/>
       <c r="F10" s="119" t="s">
-        <v>337</v>
+        <v>342</v>
       </c>
       <c r="G10" s="119" t="s">
-        <v>337</v>
+        <v>342</v>
       </c>
       <c r="H10" s="62"/>
       <c r="I10" s="61" t="s">
@@ -12599,31 +12632,31 @@
         <v>315</v>
       </c>
       <c r="C24" s="3">
-        <f>C25+C21-1</f>
+        <f t="shared" ref="C24:I24" si="0">C25+C21-1</f>
         <v>22</v>
       </c>
       <c r="D24" s="3">
-        <f>D25+D21-1</f>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="E24" s="3">
-        <f>E25+E21-1</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="F24" s="3">
-        <f>F25+F21-1</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="G24" s="3">
-        <f>G25+G21-1</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="H24" s="3">
-        <f>H25+H21-1</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="I24" s="3">
-        <f>I25+I21-1</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="J24" s="3">
@@ -12645,27 +12678,27 @@
         <v>223</v>
       </c>
       <c r="C25" s="3">
-        <f>D24+1</f>
+        <f t="shared" ref="C25:H25" si="1">D24+1</f>
         <v>20</v>
       </c>
       <c r="D25" s="3">
-        <f>E24+1</f>
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="E25" s="3">
-        <f>F24+1</f>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="F25" s="3">
-        <f>G24+1</f>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="G25" s="3">
-        <f>H24+1</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="H25" s="3">
-        <f>I24+1</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="I25" s="3">
@@ -12762,14 +12795,10 @@
       </c>
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="E30" s="120" t="s">
-        <v>338</v>
-      </c>
+      <c r="E30" s="120"/>
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="E31" s="120" t="s">
-        <v>339</v>
-      </c>
+      <c r="E31" s="120"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -14030,6 +14059,154 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:D9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.5703125" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="4" width="11.42578125" customWidth="1"/>
+    <col min="7" max="7" width="12" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="21" t="s">
+        <v>345</v>
+      </c>
+      <c r="B2" s="122" t="s">
+        <v>344</v>
+      </c>
+      <c r="D2" s="123" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3">
+        <v>32</v>
+      </c>
+      <c r="C3">
+        <f>B3-1</f>
+        <v>31</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4">
+        <v>32</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ref="C4:C8" si="0">C3+B4</f>
+        <v>63</v>
+      </c>
+      <c r="D4">
+        <f t="shared" ref="D4:D8" si="1">C3+1</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5">
+        <v>8</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>71</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="1"/>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6">
+        <v>8</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>79</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="1"/>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>320</v>
+      </c>
+      <c r="B7">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>87</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="1"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>323</v>
+      </c>
+      <c r="B8">
+        <v>8</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>95</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="1"/>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B9" s="124">
+        <f>SUM(B3:B8)</f>
+        <v>96</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Tested and debugged virtualization in simulator
</commit_message>
<xml_diff>
--- a/Resources/Instruction Set.xlsx
+++ b/Resources/Instruction Set.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="300" windowWidth="18195" windowHeight="8070" tabRatio="681" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="300" windowWidth="18195" windowHeight="8070" tabRatio="681" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="OPCODE_encoding" sheetId="1" r:id="rId1"/>
@@ -2103,10 +2103,10 @@
   <dimension ref="A1:AS98"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="10" ySplit="4" topLeftCell="K54" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="10" ySplit="4" topLeftCell="W54" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AR86" sqref="AR86"/>
+      <selection pane="bottomRight" activeCell="AO93" sqref="AO93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -11979,7 +11979,9 @@
       <c r="P93" s="13"/>
       <c r="Q93" s="13"/>
       <c r="R93" s="12"/>
-      <c r="AO93" s="13"/>
+      <c r="AO93" s="13">
+        <v>1.0010101101100999E+22</v>
+      </c>
       <c r="AP93" s="1"/>
       <c r="AR93" s="56"/>
       <c r="AS93" s="57"/>
@@ -12029,8 +12031,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14061,7 +14063,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updated instruction set documentation
</commit_message>
<xml_diff>
--- a/Resources/Instruction Set.xlsx
+++ b/Resources/Instruction Set.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21901"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\N.I.G.E.-Machine\Resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9A7CE5F-104A-4871-838A-640AE2D2445A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="300" windowWidth="18195" windowHeight="8070" tabRatio="681" activeTab="1"/>
+    <workbookView xWindow="6620" yWindow="2100" windowWidth="25510" windowHeight="16920" tabRatio="681" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OPCODE_encoding" sheetId="1" r:id="rId1"/>
@@ -18,12 +24,20 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">OPCODE_encoding!$A$3:$M$86</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1303" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1304" uniqueCount="347">
   <si>
     <t>DUP</t>
   </si>
@@ -1061,12 +1075,15 @@
   </si>
   <si>
     <t>datapathFreeze/Thaw</t>
+  </si>
+  <si>
+    <t>Datapath code</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="41" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1806,6 +1823,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -1853,7 +1873,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1886,9 +1906,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1921,6 +1958,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2096,67 +2150,68 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AS98"/>
+  <dimension ref="A1:AT98"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="10" ySplit="4" topLeftCell="W54" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="10" ySplit="4" topLeftCell="AJ41" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AO93" sqref="AO93"/>
+      <selection pane="bottomRight" activeCell="AT77" sqref="AT77"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="10.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="1.7265625" style="1" customWidth="1"/>
     <col min="2" max="2" width="11" style="3" customWidth="1"/>
-    <col min="3" max="3" width="1.7109375" style="3" customWidth="1"/>
-    <col min="4" max="6" width="5.5703125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="1.28515625" style="3" customWidth="1"/>
-    <col min="8" max="8" width="5.5703125" style="5" customWidth="1"/>
-    <col min="9" max="9" width="9.5703125" style="5" customWidth="1"/>
-    <col min="10" max="10" width="6.5703125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="1.7265625" style="3" customWidth="1"/>
+    <col min="4" max="6" width="5.54296875" style="3" customWidth="1"/>
+    <col min="7" max="7" width="1.26953125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="5.54296875" style="5" customWidth="1"/>
+    <col min="9" max="9" width="9.54296875" style="5" customWidth="1"/>
+    <col min="10" max="10" width="6.54296875" style="3" customWidth="1"/>
     <col min="11" max="11" width="2" style="3" customWidth="1"/>
-    <col min="12" max="12" width="19.28515625" style="69" customWidth="1"/>
+    <col min="12" max="12" width="19.26953125" style="69" customWidth="1"/>
     <col min="13" max="13" width="51" style="1" customWidth="1"/>
-    <col min="14" max="14" width="9.5703125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="2.7109375" style="6" customWidth="1"/>
-    <col min="16" max="17" width="6.5703125" style="6" customWidth="1"/>
-    <col min="18" max="18" width="9.140625" style="1" customWidth="1"/>
-    <col min="19" max="25" width="9.140625" style="1"/>
-    <col min="26" max="26" width="5.5703125" style="1" customWidth="1"/>
-    <col min="27" max="27" width="2.7109375" style="1" customWidth="1"/>
+    <col min="14" max="14" width="9.54296875" style="1" customWidth="1"/>
+    <col min="15" max="15" width="2.7265625" style="6" customWidth="1"/>
+    <col min="16" max="17" width="6.54296875" style="6" customWidth="1"/>
+    <col min="18" max="18" width="9.1796875" style="1" customWidth="1"/>
+    <col min="19" max="25" width="9.1796875" style="1"/>
+    <col min="26" max="26" width="5.54296875" style="1" customWidth="1"/>
+    <col min="27" max="27" width="2.7265625" style="1" customWidth="1"/>
     <col min="28" max="28" width="7" style="1" customWidth="1"/>
-    <col min="29" max="29" width="6.5703125" style="1" customWidth="1"/>
-    <col min="30" max="30" width="11.140625" style="1" customWidth="1"/>
-    <col min="31" max="31" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="7.5703125" style="1" customWidth="1"/>
-    <col min="33" max="33" width="5.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="37" max="38" width="4.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="7.7109375" style="1" customWidth="1"/>
+    <col min="29" max="29" width="6.54296875" style="1" customWidth="1"/>
+    <col min="30" max="30" width="11.1796875" style="1" customWidth="1"/>
+    <col min="31" max="31" width="6.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="7.54296875" style="1" customWidth="1"/>
+    <col min="33" max="33" width="5.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="6.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="6.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="37" max="38" width="4.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="7.7265625" style="1" customWidth="1"/>
     <col min="40" max="40" width="3" style="1" customWidth="1"/>
-    <col min="41" max="41" width="23.85546875" style="6" customWidth="1"/>
-    <col min="42" max="42" width="10.42578125" style="1" customWidth="1"/>
-    <col min="43" max="43" width="3.5703125" style="1" customWidth="1"/>
-    <col min="44" max="44" width="28.85546875" style="46" customWidth="1"/>
-    <col min="45" max="45" width="17.7109375" style="1" customWidth="1"/>
-    <col min="46" max="16384" width="9.140625" style="1"/>
+    <col min="41" max="41" width="23.81640625" style="6" customWidth="1"/>
+    <col min="42" max="42" width="10.453125" style="1" customWidth="1"/>
+    <col min="43" max="43" width="3.54296875" style="1" customWidth="1"/>
+    <col min="44" max="44" width="28.81640625" style="46" customWidth="1"/>
+    <col min="45" max="45" width="17.7265625" style="1" customWidth="1"/>
+    <col min="46" max="46" width="18.90625" style="1" customWidth="1"/>
+    <col min="47" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:46" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A1" s="41" t="s">
         <v>281</v>
       </c>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:45" ht="5.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="3" spans="1:45" s="19" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:46" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:46" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
         <v>233</v>
       </c>
@@ -2220,7 +2275,7 @@
       </c>
       <c r="AS3" s="29"/>
     </row>
-    <row r="4" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:46" x14ac:dyDescent="0.25">
       <c r="D4" s="5">
         <v>7</v>
       </c>
@@ -2314,13 +2369,16 @@
       <c r="AS4" s="20" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="5" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AT4" s="20" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="5" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="6" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:46" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>37</v>
       </c>
@@ -2451,8 +2509,12 @@
         <f t="shared" ref="AS6:AS19" si="1">CHAR(44)&amp;CHAR(34)&amp;CHAR(32)&amp;B6&amp;CHAR(34)</f>
         <v>," NOP"</v>
       </c>
-    </row>
-    <row r="7" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AT6" s="1" t="str">
+        <f>B6&amp;CHAR(32)&amp;"when"&amp;CHAR(32)&amp;CHAR(34)&amp;RIGHT(AO6,7)&amp;CHAR(34)</f>
+        <v>NOP when "0000000"</v>
+      </c>
+    </row>
+    <row r="7" spans="1:46" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>2</v>
       </c>
@@ -2584,8 +2646,12 @@
         <f t="shared" si="1"/>
         <v>," DROP"</v>
       </c>
-    </row>
-    <row r="8" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AT7" s="1" t="str">
+        <f t="shared" ref="AT7:AT70" si="6">B7&amp;CHAR(32)&amp;"when"&amp;CHAR(32)&amp;CHAR(34)&amp;RIGHT(AO7,7)&amp;CHAR(34)</f>
+        <v>DROP when "0100000"</v>
+      </c>
+    </row>
+    <row r="8" spans="1:46" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>0</v>
       </c>
@@ -2717,8 +2783,12 @@
         <f t="shared" si="1"/>
         <v>," DUP"</v>
       </c>
-    </row>
-    <row r="9" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AT8" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>DUP when "0000000"</v>
+      </c>
+    </row>
+    <row r="9" spans="1:46" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>3</v>
       </c>
@@ -2850,8 +2920,12 @@
         <f t="shared" si="1"/>
         <v>," SWAP"</v>
       </c>
-    </row>
-    <row r="10" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AT9" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>SWAP when "0100000"</v>
+      </c>
+    </row>
+    <row r="10" spans="1:46" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
         <v>4</v>
       </c>
@@ -2983,8 +3057,12 @@
         <f t="shared" si="1"/>
         <v>," OVER"</v>
       </c>
-    </row>
-    <row r="11" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AT10" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>OVER when "0100000"</v>
+      </c>
+    </row>
+    <row r="11" spans="1:46" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
         <v>5</v>
       </c>
@@ -2995,7 +3073,7 @@
         <v>0</v>
       </c>
       <c r="F11" s="3">
-        <f t="shared" ref="F11:F19" si="6">F10+1</f>
+        <f t="shared" ref="F11:F19" si="7">F10+1</f>
         <v>5</v>
       </c>
       <c r="H11" s="5">
@@ -3116,8 +3194,12 @@
         <f t="shared" si="1"/>
         <v>," NIP"</v>
       </c>
-    </row>
-    <row r="12" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AT11" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>NIP when "0000000"</v>
+      </c>
+    </row>
+    <row r="12" spans="1:46" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
         <v>6</v>
       </c>
@@ -3128,7 +3210,7 @@
         <v>0</v>
       </c>
       <c r="F12" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>6</v>
       </c>
       <c r="H12" s="5">
@@ -3249,8 +3331,12 @@
         <f t="shared" si="1"/>
         <v>," ROT"</v>
       </c>
-    </row>
-    <row r="13" spans="1:45" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AT12" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>ROT when "0100001"</v>
+      </c>
+    </row>
+    <row r="13" spans="1:46" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B13" s="8" t="s">
         <v>7</v>
       </c>
@@ -3262,7 +3348,7 @@
         <v>0</v>
       </c>
       <c r="F13" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>7</v>
       </c>
       <c r="G13" s="3"/>
@@ -3388,8 +3474,12 @@
         <f t="shared" si="1"/>
         <v>," &gt;R"</v>
       </c>
-    </row>
-    <row r="14" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AT13" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>&gt;R when "0100000"</v>
+      </c>
+    </row>
+    <row r="14" spans="1:46" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
         <v>8</v>
       </c>
@@ -3400,7 +3490,7 @@
         <v>0</v>
       </c>
       <c r="F14" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>8</v>
       </c>
       <c r="H14" s="5">
@@ -3521,8 +3611,12 @@
         <f t="shared" si="1"/>
         <v>," R@"</v>
       </c>
-    </row>
-    <row r="15" spans="1:45" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AT14" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>R@ when "0100010"</v>
+      </c>
+    </row>
+    <row r="15" spans="1:46" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B15" s="8" t="s">
         <v>9</v>
       </c>
@@ -3534,7 +3628,7 @@
         <v>0</v>
       </c>
       <c r="F15" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>9</v>
       </c>
       <c r="G15" s="3"/>
@@ -3660,8 +3754,12 @@
         <f t="shared" si="1"/>
         <v>," R&gt;"</v>
       </c>
-    </row>
-    <row r="16" spans="1:45" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AT15" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>R&gt; when "0100010"</v>
+      </c>
+    </row>
+    <row r="16" spans="1:46" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B16" s="8" t="s">
         <v>285</v>
       </c>
@@ -3673,7 +3771,7 @@
         <v>0</v>
       </c>
       <c r="F16" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>10</v>
       </c>
       <c r="G16" s="3"/>
@@ -3799,8 +3897,12 @@
         <f t="shared" si="1"/>
         <v>," PSP@"</v>
       </c>
-    </row>
-    <row r="17" spans="1:45" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AT16" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>PSP@ when "0100011"</v>
+      </c>
+    </row>
+    <row r="17" spans="1:46" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B17" s="8" t="s">
         <v>326</v>
       </c>
@@ -3812,7 +3914,7 @@
         <v>0</v>
       </c>
       <c r="F17" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>11</v>
       </c>
       <c r="G17" s="3"/>
@@ -3938,8 +4040,12 @@
         <f t="shared" si="1"/>
         <v>," CATCH"</v>
       </c>
-    </row>
-    <row r="18" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AT17" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>CATCH when "0100000"</v>
+      </c>
+    </row>
+    <row r="18" spans="1:46" x14ac:dyDescent="0.25">
       <c r="B18" s="8" t="s">
         <v>335</v>
       </c>
@@ -3950,7 +4056,7 @@
         <v>0</v>
       </c>
       <c r="F18" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>12</v>
       </c>
       <c r="H18" s="5">
@@ -4072,8 +4178,12 @@
         <f t="shared" si="1"/>
         <v>," RESETSP"</v>
       </c>
-    </row>
-    <row r="19" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AT18" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>RESETSP when "0000000"</v>
+      </c>
+    </row>
+    <row r="19" spans="1:46" x14ac:dyDescent="0.25">
       <c r="B19" s="8" t="s">
         <v>327</v>
       </c>
@@ -4084,7 +4194,7 @@
         <v>0</v>
       </c>
       <c r="F19" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>13</v>
       </c>
       <c r="H19" s="5">
@@ -4205,8 +4315,12 @@
         <f t="shared" si="1"/>
         <v>," THROW"</v>
       </c>
-    </row>
-    <row r="20" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AT19" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>THROW when "0000000"</v>
+      </c>
+    </row>
+    <row r="20" spans="1:46" x14ac:dyDescent="0.25">
       <c r="I20" s="3"/>
       <c r="AB20" s="8"/>
       <c r="AC20" s="8"/>
@@ -4217,8 +4331,12 @@
       </c>
       <c r="AR20" s="56"/>
       <c r="AS20" s="56"/>
-    </row>
-    <row r="21" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AT20" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve"> when ""</v>
+      </c>
+    </row>
+    <row r="21" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>10</v>
       </c>
@@ -4232,8 +4350,12 @@
       </c>
       <c r="AR21" s="56"/>
       <c r="AS21" s="56"/>
-    </row>
-    <row r="22" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AT21" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve"> when ""</v>
+      </c>
+    </row>
+    <row r="22" spans="1:46" x14ac:dyDescent="0.25">
       <c r="B22" s="4" t="s">
         <v>11</v>
       </c>
@@ -4249,15 +4371,15 @@
         <v>14</v>
       </c>
       <c r="H22" s="5">
-        <f t="shared" ref="H22:H29" si="7">F22+E22*64+D22*128</f>
+        <f t="shared" ref="H22:H29" si="8">F22+E22*64+D22*128</f>
         <v>14</v>
       </c>
       <c r="I22" s="3" t="str">
-        <f t="shared" ref="I22:I29" si="8">DEC2BIN(H22,7)</f>
+        <f t="shared" ref="I22:I29" si="9">DEC2BIN(H22,7)</f>
         <v>0001110</v>
       </c>
       <c r="J22" s="3" t="str">
-        <f t="shared" ref="J22:J29" si="9">DEC2HEX(H22)</f>
+        <f t="shared" ref="J22:J29" si="10">DEC2HEX(H22)</f>
         <v>E</v>
       </c>
       <c r="L22" s="69" t="s">
@@ -4360,15 +4482,19 @@
         <v>1282</v>
       </c>
       <c r="AR22" s="56" t="str">
-        <f t="shared" ref="AR22:AR29" si="10">"1 "&amp;H22&amp;" INSTRUCTION _"&amp;B22</f>
+        <f t="shared" ref="AR22:AR29" si="11">"1 "&amp;H22&amp;" INSTRUCTION _"&amp;B22</f>
         <v>1 14 INSTRUCTION _+</v>
       </c>
       <c r="AS22" s="56" t="str">
-        <f t="shared" ref="AS22:AS29" si="11">CHAR(44)&amp;CHAR(34)&amp;CHAR(32)&amp;B22&amp;CHAR(34)</f>
+        <f t="shared" ref="AS22:AS29" si="12">CHAR(44)&amp;CHAR(34)&amp;CHAR(32)&amp;B22&amp;CHAR(34)</f>
         <v>," +"</v>
       </c>
-    </row>
-    <row r="23" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AT22" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>+ when "0000010"</v>
+      </c>
+    </row>
+    <row r="23" spans="1:46" x14ac:dyDescent="0.25">
       <c r="B23" s="4" t="s">
         <v>12</v>
       </c>
@@ -4384,15 +4510,15 @@
         <v>15</v>
       </c>
       <c r="H23" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>15</v>
       </c>
       <c r="I23" s="3" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0001111</v>
       </c>
       <c r="J23" s="3" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>F</v>
       </c>
       <c r="L23" s="69" t="s">
@@ -4495,15 +4621,19 @@
         <v>1283</v>
       </c>
       <c r="AR23" s="56" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1 15 INSTRUCTION _-</v>
       </c>
       <c r="AS23" s="56" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>," -"</v>
       </c>
-    </row>
-    <row r="24" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AT23" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>- when "0000011"</v>
+      </c>
+    </row>
+    <row r="24" spans="1:46" x14ac:dyDescent="0.25">
       <c r="B24" s="3" t="s">
         <v>16</v>
       </c>
@@ -4514,19 +4644,19 @@
         <v>0</v>
       </c>
       <c r="F24" s="3">
-        <f t="shared" ref="F24:F29" si="12">F23+1</f>
+        <f t="shared" ref="F24:F29" si="13">F23+1</f>
         <v>16</v>
       </c>
       <c r="H24" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>16</v>
       </c>
       <c r="I24" s="3" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0010000</v>
       </c>
       <c r="J24" s="3" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>10</v>
       </c>
       <c r="L24" s="69" t="s">
@@ -4629,15 +4759,19 @@
         <v>1</v>
       </c>
       <c r="AR24" s="56" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1 16 INSTRUCTION _NEGATE</v>
       </c>
       <c r="AS24" s="56" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>," NEGATE"</v>
       </c>
-    </row>
-    <row r="25" spans="1:45" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AT24" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>NEGATE when "0000001"</v>
+      </c>
+    </row>
+    <row r="25" spans="1:46" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B25" s="8" t="s">
         <v>47</v>
       </c>
@@ -4649,20 +4783,20 @@
         <v>0</v>
       </c>
       <c r="F25" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>17</v>
       </c>
       <c r="G25" s="3"/>
       <c r="H25" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>17</v>
       </c>
       <c r="I25" s="3" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0010001</v>
       </c>
       <c r="J25" s="3" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>11</v>
       </c>
       <c r="K25" s="3"/>
@@ -4768,15 +4902,19 @@
         <v>6</v>
       </c>
       <c r="AR25" s="56" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1 17 INSTRUCTION _1+</v>
       </c>
       <c r="AS25" s="56" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>," 1+"</v>
       </c>
-    </row>
-    <row r="26" spans="1:45" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AT25" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>1+ when "0000110"</v>
+      </c>
+    </row>
+    <row r="26" spans="1:46" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B26" s="10" t="s">
         <v>48</v>
       </c>
@@ -4788,20 +4926,20 @@
         <v>0</v>
       </c>
       <c r="F26" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>18</v>
       </c>
       <c r="G26" s="3"/>
       <c r="H26" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>18</v>
       </c>
       <c r="I26" s="3" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0010010</v>
       </c>
       <c r="J26" s="3" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>12</v>
       </c>
       <c r="K26" s="3"/>
@@ -4907,15 +5045,19 @@
         <v>7</v>
       </c>
       <c r="AR26" s="56" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1 18 INSTRUCTION _1-</v>
       </c>
       <c r="AS26" s="56" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>," 1-"</v>
       </c>
-    </row>
-    <row r="27" spans="1:45" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AT26" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>1- when "0000111"</v>
+      </c>
+    </row>
+    <row r="27" spans="1:46" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B27" s="10" t="s">
         <v>50</v>
       </c>
@@ -4932,15 +5074,15 @@
       </c>
       <c r="G27" s="3"/>
       <c r="H27" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>19</v>
       </c>
       <c r="I27" s="3" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0010011</v>
       </c>
       <c r="J27" s="3" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>13</v>
       </c>
       <c r="K27" s="3"/>
@@ -5046,15 +5188,19 @@
         <v>23</v>
       </c>
       <c r="AR27" s="56" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1 19 INSTRUCTION _2/</v>
       </c>
       <c r="AS27" s="56" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>," 2/"</v>
       </c>
-    </row>
-    <row r="28" spans="1:45" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AT27" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>2/ when "0010111"</v>
+      </c>
+    </row>
+    <row r="28" spans="1:46" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B28" s="8" t="s">
         <v>203</v>
       </c>
@@ -5071,15 +5217,15 @@
       </c>
       <c r="G28" s="3"/>
       <c r="H28" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>20</v>
       </c>
       <c r="I28" s="3" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0010100</v>
       </c>
       <c r="J28" s="3" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>14</v>
       </c>
       <c r="K28" s="8"/>
@@ -5185,15 +5331,19 @@
         <v>1284</v>
       </c>
       <c r="AR28" s="56" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1 20 INSTRUCTION _ADDX</v>
       </c>
       <c r="AS28" s="56" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>," ADDX"</v>
       </c>
-    </row>
-    <row r="29" spans="1:45" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AT28" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>ADDX when "0000100"</v>
+      </c>
+    </row>
+    <row r="29" spans="1:46" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B29" s="8" t="s">
         <v>204</v>
       </c>
@@ -5205,20 +5355,20 @@
         <v>0</v>
       </c>
       <c r="F29" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>21</v>
       </c>
       <c r="G29" s="3"/>
       <c r="H29" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>21</v>
       </c>
       <c r="I29" s="3" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0010101</v>
       </c>
       <c r="J29" s="3" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>15</v>
       </c>
       <c r="K29" s="8"/>
@@ -5324,15 +5474,19 @@
         <v>1285</v>
       </c>
       <c r="AR29" s="56" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1 21 INSTRUCTION _SUBX</v>
       </c>
       <c r="AS29" s="56" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>," SUBX"</v>
       </c>
-    </row>
-    <row r="30" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AT29" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>SUBX when "0000101"</v>
+      </c>
+    </row>
+    <row r="30" spans="1:46" x14ac:dyDescent="0.25">
       <c r="E30" s="10"/>
       <c r="I30" s="3"/>
       <c r="N30" s="3"/>
@@ -5345,8 +5499,12 @@
       </c>
       <c r="AR30" s="56"/>
       <c r="AS30" s="56"/>
-    </row>
-    <row r="31" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AT30" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve"> when ""</v>
+      </c>
+    </row>
+    <row r="31" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>17</v>
       </c>
@@ -5361,8 +5519,12 @@
       </c>
       <c r="AR31" s="56"/>
       <c r="AS31" s="56"/>
-    </row>
-    <row r="32" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AT31" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve"> when ""</v>
+      </c>
+    </row>
+    <row r="32" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
       <c r="B32" s="4" t="s">
         <v>20</v>
@@ -5379,15 +5541,15 @@
         <v>22</v>
       </c>
       <c r="H32" s="5">
-        <f t="shared" ref="H32:H42" si="13">F32+E32*64+D32*128</f>
+        <f t="shared" ref="H32:H42" si="14">F32+E32*64+D32*128</f>
         <v>22</v>
       </c>
       <c r="I32" s="3" t="str">
-        <f t="shared" ref="I32:I42" si="14">DEC2BIN(H32,7)</f>
+        <f t="shared" ref="I32:I42" si="15">DEC2BIN(H32,7)</f>
         <v>0010110</v>
       </c>
       <c r="J32" s="3" t="str">
-        <f t="shared" ref="J32:J42" si="15">DEC2HEX(H32)</f>
+        <f t="shared" ref="J32:J42" si="16">DEC2HEX(H32)</f>
         <v>16</v>
       </c>
       <c r="L32" s="69" t="s">
@@ -5421,7 +5583,7 @@
         <v>219</v>
       </c>
       <c r="W32" s="8" t="str">
-        <f t="shared" ref="W32:W42" si="16">B32</f>
+        <f t="shared" ref="W32:W42" si="17">B32</f>
         <v>=</v>
       </c>
       <c r="X32" s="8" t="s">
@@ -5491,15 +5653,19 @@
         <v>1328</v>
       </c>
       <c r="AR32" s="56" t="str">
-        <f t="shared" ref="AR32:AR42" si="17">"1 "&amp;H32&amp;" INSTRUCTION _"&amp;B32</f>
+        <f t="shared" ref="AR32:AR42" si="18">"1 "&amp;H32&amp;" INSTRUCTION _"&amp;B32</f>
         <v>1 22 INSTRUCTION _=</v>
       </c>
       <c r="AS32" s="56" t="str">
-        <f t="shared" ref="AS32:AS42" si="18">CHAR(44)&amp;CHAR(34)&amp;CHAR(32)&amp;B32&amp;CHAR(34)</f>
+        <f t="shared" ref="AS32:AS42" si="19">CHAR(44)&amp;CHAR(34)&amp;CHAR(32)&amp;B32&amp;CHAR(34)</f>
         <v>," ="</v>
       </c>
-    </row>
-    <row r="33" spans="1:45" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AT32" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>= when "0110000"</v>
+      </c>
+    </row>
+    <row r="33" spans="1:46" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3"/>
       <c r="B33" s="10" t="s">
         <v>40</v>
@@ -5517,15 +5683,15 @@
       </c>
       <c r="G33" s="8"/>
       <c r="H33" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>23</v>
       </c>
       <c r="I33" s="3" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0010111</v>
       </c>
       <c r="J33" s="3" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>17</v>
       </c>
       <c r="K33" s="8"/>
@@ -5561,7 +5727,7 @@
         <v>219</v>
       </c>
       <c r="W33" s="8" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>&lt;&gt;</v>
       </c>
       <c r="X33" s="8" t="s">
@@ -5631,15 +5797,19 @@
         <v>1329</v>
       </c>
       <c r="AR33" s="56" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1 23 INSTRUCTION _&lt;&gt;</v>
       </c>
       <c r="AS33" s="56" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>," &lt;&gt;"</v>
       </c>
-    </row>
-    <row r="34" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AT33" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>&lt;&gt; when "0110001"</v>
+      </c>
+    </row>
+    <row r="34" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
       <c r="B34" s="4" t="s">
         <v>18</v>
@@ -5651,20 +5821,20 @@
         <v>0</v>
       </c>
       <c r="F34" s="8">
-        <f t="shared" ref="F34:F42" si="19">F33+1</f>
+        <f t="shared" ref="F34:F42" si="20">F33+1</f>
         <v>24</v>
       </c>
       <c r="G34" s="8"/>
       <c r="H34" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>24</v>
       </c>
       <c r="I34" s="3" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0011000</v>
       </c>
       <c r="J34" s="3" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>18</v>
       </c>
       <c r="L34" s="69" t="s">
@@ -5698,7 +5868,7 @@
         <v>219</v>
       </c>
       <c r="W34" s="8" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>&lt;</v>
       </c>
       <c r="X34" s="8" t="s">
@@ -5768,15 +5938,19 @@
         <v>1330</v>
       </c>
       <c r="AR34" s="56" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1 24 INSTRUCTION _&lt;</v>
       </c>
       <c r="AS34" s="56" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>," &lt;"</v>
       </c>
-    </row>
-    <row r="35" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AT34" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>&lt; when "0110010"</v>
+      </c>
+    </row>
+    <row r="35" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A35" s="3"/>
       <c r="B35" s="4" t="s">
         <v>19</v>
@@ -5788,20 +5962,20 @@
         <v>0</v>
       </c>
       <c r="F35" s="8">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>25</v>
       </c>
       <c r="G35" s="8"/>
       <c r="H35" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>25</v>
       </c>
       <c r="I35" s="3" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0011001</v>
       </c>
       <c r="J35" s="3" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>19</v>
       </c>
       <c r="L35" s="69" t="s">
@@ -5835,7 +6009,7 @@
         <v>219</v>
       </c>
       <c r="W35" s="8" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>&gt;</v>
       </c>
       <c r="X35" s="8" t="s">
@@ -5905,15 +6079,19 @@
         <v>1331</v>
       </c>
       <c r="AR35" s="56" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1 25 INSTRUCTION _&gt;</v>
       </c>
       <c r="AS35" s="56" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>," &gt;"</v>
       </c>
-    </row>
-    <row r="36" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AT35" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>&gt; when "0110011"</v>
+      </c>
+    </row>
+    <row r="36" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A36" s="3"/>
       <c r="B36" s="4" t="s">
         <v>27</v>
@@ -5925,20 +6103,20 @@
         <v>0</v>
       </c>
       <c r="F36" s="8">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>26</v>
       </c>
       <c r="G36" s="8"/>
       <c r="H36" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>26</v>
       </c>
       <c r="I36" s="3" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0011010</v>
       </c>
       <c r="J36" s="3" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>1A</v>
       </c>
       <c r="L36" s="69" t="s">
@@ -5972,7 +6150,7 @@
         <v>219</v>
       </c>
       <c r="W36" s="8" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>U&lt;</v>
       </c>
       <c r="X36" s="8" t="s">
@@ -6042,15 +6220,19 @@
         <v>1332</v>
       </c>
       <c r="AR36" s="56" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1 26 INSTRUCTION _U&lt;</v>
       </c>
       <c r="AS36" s="56" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>," U&lt;"</v>
       </c>
-    </row>
-    <row r="37" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AT36" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>U&lt; when "0110100"</v>
+      </c>
+    </row>
+    <row r="37" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A37" s="3"/>
       <c r="B37" s="4" t="s">
         <v>28</v>
@@ -6062,20 +6244,20 @@
         <v>0</v>
       </c>
       <c r="F37" s="8">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>27</v>
       </c>
       <c r="G37" s="8"/>
       <c r="H37" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>27</v>
       </c>
       <c r="I37" s="3" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0011011</v>
       </c>
       <c r="J37" s="3" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>1B</v>
       </c>
       <c r="L37" s="69" t="s">
@@ -6109,7 +6291,7 @@
         <v>219</v>
       </c>
       <c r="W37" s="8" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>U&gt;</v>
       </c>
       <c r="X37" s="8" t="s">
@@ -6179,15 +6361,19 @@
         <v>1333</v>
       </c>
       <c r="AR37" s="56" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1 27 INSTRUCTION _U&gt;</v>
       </c>
       <c r="AS37" s="56" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>," U&gt;"</v>
       </c>
-    </row>
-    <row r="38" spans="1:45" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AT37" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>U&gt; when "0110101"</v>
+      </c>
+    </row>
+    <row r="38" spans="1:46" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3"/>
       <c r="B38" s="10" t="s">
         <v>21</v>
@@ -6200,20 +6386,20 @@
         <v>0</v>
       </c>
       <c r="F38" s="8">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>28</v>
       </c>
       <c r="G38" s="8"/>
       <c r="H38" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>28</v>
       </c>
       <c r="I38" s="3" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0011100</v>
       </c>
       <c r="J38" s="3" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>1C</v>
       </c>
       <c r="K38" s="8"/>
@@ -6249,7 +6435,7 @@
         <v>219</v>
       </c>
       <c r="W38" s="8" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0=</v>
       </c>
       <c r="X38" s="8" t="s">
@@ -6319,15 +6505,19 @@
         <v>54</v>
       </c>
       <c r="AR38" s="56" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1 28 INSTRUCTION _0=</v>
       </c>
       <c r="AS38" s="56" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>," 0="</v>
       </c>
-    </row>
-    <row r="39" spans="1:45" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AT38" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>0= when "0110110"</v>
+      </c>
+    </row>
+    <row r="39" spans="1:46" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3"/>
       <c r="B39" s="10" t="s">
         <v>265</v>
@@ -6340,20 +6530,20 @@
         <v>0</v>
       </c>
       <c r="F39" s="8">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>29</v>
       </c>
       <c r="G39" s="8"/>
       <c r="H39" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>29</v>
       </c>
       <c r="I39" s="3" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0011101</v>
       </c>
       <c r="J39" s="3" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>1D</v>
       </c>
       <c r="K39" s="8"/>
@@ -6389,7 +6579,7 @@
         <v>219</v>
       </c>
       <c r="W39" s="8" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0&lt;&gt;</v>
       </c>
       <c r="X39" s="8" t="s">
@@ -6459,15 +6649,19 @@
         <v>55</v>
       </c>
       <c r="AR39" s="56" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1 29 INSTRUCTION _0&lt;&gt;</v>
       </c>
       <c r="AS39" s="56" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>," 0&lt;&gt;"</v>
       </c>
-    </row>
-    <row r="40" spans="1:45" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AT39" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>0&lt;&gt; when "0110111"</v>
+      </c>
+    </row>
+    <row r="40" spans="1:46" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3"/>
       <c r="B40" s="10" t="s">
         <v>263</v>
@@ -6480,20 +6674,20 @@
         <v>0</v>
       </c>
       <c r="F40" s="8">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>30</v>
       </c>
       <c r="G40" s="8"/>
       <c r="H40" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>30</v>
       </c>
       <c r="I40" s="3" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0011110</v>
       </c>
       <c r="J40" s="3" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>1E</v>
       </c>
       <c r="K40" s="8"/>
@@ -6529,7 +6723,7 @@
         <v>219</v>
       </c>
       <c r="W40" s="8" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0&lt;</v>
       </c>
       <c r="X40" s="8" t="s">
@@ -6599,15 +6793,19 @@
         <v>56</v>
       </c>
       <c r="AR40" s="56" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1 30 INSTRUCTION _0&lt;</v>
       </c>
       <c r="AS40" s="56" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>," 0&lt;"</v>
       </c>
-    </row>
-    <row r="41" spans="1:45" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AT40" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>0&lt; when "0111000"</v>
+      </c>
+    </row>
+    <row r="41" spans="1:46" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3"/>
       <c r="B41" s="4" t="s">
         <v>264</v>
@@ -6620,20 +6818,20 @@
         <v>0</v>
       </c>
       <c r="F41" s="8">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>31</v>
       </c>
       <c r="G41" s="8"/>
       <c r="H41" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>31</v>
       </c>
       <c r="I41" s="3" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0011111</v>
       </c>
       <c r="J41" s="3" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>1F</v>
       </c>
       <c r="K41" s="8"/>
@@ -6669,7 +6867,7 @@
         <v>219</v>
       </c>
       <c r="W41" s="8" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0&gt;</v>
       </c>
       <c r="X41" s="8" t="s">
@@ -6739,15 +6937,19 @@
         <v>57</v>
       </c>
       <c r="AR41" s="56" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1 31 INSTRUCTION _0&gt;</v>
       </c>
       <c r="AS41" s="56" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>," 0&gt;"</v>
       </c>
-    </row>
-    <row r="42" spans="1:45" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AT41" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>0&gt; when "0111001"</v>
+      </c>
+    </row>
+    <row r="42" spans="1:46" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3"/>
       <c r="B42" s="8" t="s">
         <v>308</v>
@@ -6760,20 +6962,20 @@
         <v>0</v>
       </c>
       <c r="F42" s="8">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>32</v>
       </c>
       <c r="G42" s="8"/>
       <c r="H42" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>32</v>
       </c>
       <c r="I42" s="3" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0100000</v>
       </c>
       <c r="J42" s="3" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>20</v>
       </c>
       <c r="K42" s="8"/>
@@ -6809,7 +7011,7 @@
         <v>219</v>
       </c>
       <c r="W42" s="8" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>ZERO</v>
       </c>
       <c r="X42" s="8" t="s">
@@ -6879,15 +7081,19 @@
         <v>2234</v>
       </c>
       <c r="AR42" s="56" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1 32 INSTRUCTION _ZERO</v>
       </c>
       <c r="AS42" s="56" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>," ZERO"</v>
       </c>
-    </row>
-    <row r="43" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AT42" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>ZERO when "0111010"</v>
+      </c>
+    </row>
+    <row r="43" spans="1:46" x14ac:dyDescent="0.25">
       <c r="E43" s="10"/>
       <c r="I43" s="3"/>
       <c r="AB43" s="8"/>
@@ -6899,8 +7105,12 @@
       </c>
       <c r="AR43" s="56"/>
       <c r="AS43" s="56"/>
-    </row>
-    <row r="44" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AT43" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve"> when ""</v>
+      </c>
+    </row>
+    <row r="44" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>22</v>
       </c>
@@ -6915,8 +7125,12 @@
       </c>
       <c r="AR44" s="56"/>
       <c r="AS44" s="56"/>
-    </row>
-    <row r="45" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AT44" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve"> when ""</v>
+      </c>
+    </row>
+    <row r="45" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A45" s="3"/>
       <c r="B45" s="3" t="s">
         <v>23</v>
@@ -6932,15 +7146,15 @@
         <v>33</v>
       </c>
       <c r="H45" s="5">
-        <f t="shared" ref="H45:H52" si="20">F45+E45*64+D45*128</f>
+        <f t="shared" ref="H45:H52" si="21">F45+E45*64+D45*128</f>
         <v>33</v>
       </c>
       <c r="I45" s="3" t="str">
-        <f t="shared" ref="I45:I52" si="21">DEC2BIN(H45,7)</f>
+        <f t="shared" ref="I45:I52" si="22">DEC2BIN(H45,7)</f>
         <v>0100001</v>
       </c>
       <c r="J45" s="3" t="str">
-        <f t="shared" ref="J45:J52" si="22">DEC2HEX(H45)</f>
+        <f t="shared" ref="J45:J52" si="23">DEC2HEX(H45)</f>
         <v>21</v>
       </c>
       <c r="L45" s="69" t="s">
@@ -6980,7 +7194,7 @@
         <v>131</v>
       </c>
       <c r="Y45" s="8" t="str">
-        <f t="shared" ref="Y45:Y50" si="23">B45</f>
+        <f t="shared" ref="Y45:Y50" si="24">B45</f>
         <v>AND</v>
       </c>
       <c r="Z45" s="8" t="s">
@@ -7044,15 +7258,19 @@
         <v>1296</v>
       </c>
       <c r="AR45" s="56" t="str">
-        <f t="shared" ref="AR45:AR52" si="24">"1 "&amp;H45&amp;" INSTRUCTION _"&amp;B45</f>
+        <f t="shared" ref="AR45:AR52" si="25">"1 "&amp;H45&amp;" INSTRUCTION _"&amp;B45</f>
         <v>1 33 INSTRUCTION _AND</v>
       </c>
       <c r="AS45" s="56" t="str">
-        <f t="shared" ref="AS45:AS52" si="25">CHAR(44)&amp;CHAR(34)&amp;CHAR(32)&amp;B45&amp;CHAR(34)</f>
+        <f t="shared" ref="AS45:AS52" si="26">CHAR(44)&amp;CHAR(34)&amp;CHAR(32)&amp;B45&amp;CHAR(34)</f>
         <v>," AND"</v>
       </c>
-    </row>
-    <row r="46" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AT45" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>AND when "0010000"</v>
+      </c>
+    </row>
+    <row r="46" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A46" s="3"/>
       <c r="B46" s="3" t="s">
         <v>24</v>
@@ -7068,15 +7286,15 @@
         <v>34</v>
       </c>
       <c r="H46" s="5">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>34</v>
       </c>
       <c r="I46" s="3" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0100010</v>
       </c>
       <c r="J46" s="3" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>22</v>
       </c>
       <c r="L46" s="69" t="s">
@@ -7116,7 +7334,7 @@
         <v>131</v>
       </c>
       <c r="Y46" s="8" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>OR</v>
       </c>
       <c r="Z46" s="8" t="s">
@@ -7180,15 +7398,19 @@
         <v>1297</v>
       </c>
       <c r="AR46" s="56" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>1 34 INSTRUCTION _OR</v>
       </c>
       <c r="AS46" s="56" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>," OR"</v>
       </c>
-    </row>
-    <row r="47" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AT46" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>OR when "0010001"</v>
+      </c>
+    </row>
+    <row r="47" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A47" s="3"/>
       <c r="B47" s="3" t="s">
         <v>26</v>
@@ -7200,19 +7422,19 @@
         <v>0</v>
       </c>
       <c r="F47" s="3">
-        <f t="shared" ref="F47:F52" si="26">F46+1</f>
+        <f t="shared" ref="F47:F52" si="27">F46+1</f>
         <v>35</v>
       </c>
       <c r="H47" s="5">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>35</v>
       </c>
       <c r="I47" s="3" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0100011</v>
       </c>
       <c r="J47" s="3" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>23</v>
       </c>
       <c r="L47" s="69" t="s">
@@ -7252,7 +7474,7 @@
         <v>131</v>
       </c>
       <c r="Y47" s="8" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>INVERT</v>
       </c>
       <c r="Z47" s="8" t="s">
@@ -7316,15 +7538,19 @@
         <v>18</v>
       </c>
       <c r="AR47" s="56" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>1 35 INSTRUCTION _INVERT</v>
       </c>
       <c r="AS47" s="56" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>," INVERT"</v>
       </c>
-    </row>
-    <row r="48" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AT47" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>INVERT when "0010010"</v>
+      </c>
+    </row>
+    <row r="48" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A48" s="3"/>
       <c r="B48" s="3" t="s">
         <v>25</v>
@@ -7336,19 +7562,19 @@
         <v>0</v>
       </c>
       <c r="F48" s="3">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>36</v>
       </c>
       <c r="H48" s="5">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>36</v>
       </c>
       <c r="I48" s="3" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0100100</v>
       </c>
       <c r="J48" s="3" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>24</v>
       </c>
       <c r="L48" s="69" t="s">
@@ -7388,7 +7614,7 @@
         <v>131</v>
       </c>
       <c r="Y48" s="8" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>XOR</v>
       </c>
       <c r="Z48" s="8" t="s">
@@ -7452,15 +7678,19 @@
         <v>1299</v>
       </c>
       <c r="AR48" s="56" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>1 36 INSTRUCTION _XOR</v>
       </c>
       <c r="AS48" s="56" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>," XOR"</v>
       </c>
-    </row>
-    <row r="49" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AT48" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>XOR when "0010011"</v>
+      </c>
+    </row>
+    <row r="49" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A49" s="3"/>
       <c r="B49" s="3" t="s">
         <v>119</v>
@@ -7472,19 +7702,19 @@
         <v>0</v>
       </c>
       <c r="F49" s="3">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>37</v>
       </c>
       <c r="H49" s="5">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>37</v>
       </c>
       <c r="I49" s="3" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0100101</v>
       </c>
       <c r="J49" s="3" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>25</v>
       </c>
       <c r="L49" s="69" t="s">
@@ -7524,7 +7754,7 @@
         <v>131</v>
       </c>
       <c r="Y49" s="3" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>LSL</v>
       </c>
       <c r="Z49" s="3" t="s">
@@ -7588,15 +7818,19 @@
         <v>20</v>
       </c>
       <c r="AR49" s="56" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>1 37 INSTRUCTION _LSL</v>
       </c>
       <c r="AS49" s="56" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>," LSL"</v>
       </c>
-    </row>
-    <row r="50" spans="1:45" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AT49" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>LSL when "0010100"</v>
+      </c>
+    </row>
+    <row r="50" spans="1:46" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="8"/>
       <c r="B50" s="8" t="s">
         <v>118</v>
@@ -7609,20 +7843,20 @@
         <v>0</v>
       </c>
       <c r="F50" s="8">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>38</v>
       </c>
       <c r="G50" s="8"/>
       <c r="H50" s="44">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>38</v>
       </c>
       <c r="I50" s="3" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0100110</v>
       </c>
       <c r="J50" s="8" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>26</v>
       </c>
       <c r="K50" s="8"/>
@@ -7664,7 +7898,7 @@
         <v>131</v>
       </c>
       <c r="Y50" s="8" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>LSR</v>
       </c>
       <c r="Z50" s="8" t="s">
@@ -7728,15 +7962,19 @@
         <v>21</v>
       </c>
       <c r="AR50" s="58" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>1 38 INSTRUCTION _LSR</v>
       </c>
       <c r="AS50" s="58" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>," LSR"</v>
       </c>
-    </row>
-    <row r="51" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AT50" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>LSR when "0010101"</v>
+      </c>
+    </row>
+    <row r="51" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A51" s="3"/>
       <c r="B51" s="3" t="s">
         <v>249</v>
@@ -7748,19 +7986,19 @@
         <v>0</v>
       </c>
       <c r="F51" s="3">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>39</v>
       </c>
       <c r="H51" s="5">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>39</v>
       </c>
       <c r="I51" s="3" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0100111</v>
       </c>
       <c r="J51" s="3" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>27</v>
       </c>
       <c r="L51" s="69" t="s">
@@ -7864,15 +8102,19 @@
         <v>37</v>
       </c>
       <c r="AR51" s="56" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>1 39 INSTRUCTION _XBYTE</v>
       </c>
       <c r="AS51" s="56" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>," XBYTE"</v>
       </c>
-    </row>
-    <row r="52" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AT51" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>XBYTE when "0100101"</v>
+      </c>
+    </row>
+    <row r="52" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A52" s="3"/>
       <c r="B52" s="3" t="s">
         <v>230</v>
@@ -7884,19 +8126,19 @@
         <v>0</v>
       </c>
       <c r="F52" s="3">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>40</v>
       </c>
       <c r="H52" s="5">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>40</v>
       </c>
       <c r="I52" s="3" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0101000</v>
       </c>
       <c r="J52" s="3" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>28</v>
       </c>
       <c r="L52" s="69" t="s">
@@ -8000,15 +8242,19 @@
         <v>38</v>
       </c>
       <c r="AR52" s="56" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>1 40 INSTRUCTION _XWORD</v>
       </c>
       <c r="AS52" s="56" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>," XWORD"</v>
       </c>
-    </row>
-    <row r="53" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AT52" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>XWORD when "0100110"</v>
+      </c>
+    </row>
+    <row r="53" spans="1:46" x14ac:dyDescent="0.25">
       <c r="E53" s="10"/>
       <c r="I53" s="3"/>
       <c r="AB53" s="8"/>
@@ -8020,8 +8266,12 @@
       </c>
       <c r="AR53" s="56"/>
       <c r="AS53" s="56"/>
-    </row>
-    <row r="54" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AT53" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve"> when ""</v>
+      </c>
+    </row>
+    <row r="54" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A54" s="92" t="s">
         <v>311</v>
       </c>
@@ -8036,8 +8286,12 @@
       </c>
       <c r="AR54" s="56"/>
       <c r="AS54" s="56"/>
-    </row>
-    <row r="55" spans="1:45" s="92" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AT54" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve"> when ""</v>
+      </c>
+    </row>
+    <row r="55" spans="1:46" s="92" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B55" s="93" t="s">
         <v>252</v>
       </c>
@@ -8058,7 +8312,7 @@
         <v>41</v>
       </c>
       <c r="I55" s="3" t="str">
-        <f t="shared" ref="I55:I65" si="27">DEC2BIN(H55,7)</f>
+        <f t="shared" ref="I55:I65" si="28">DEC2BIN(H55,7)</f>
         <v>0101001</v>
       </c>
       <c r="J55" s="93" t="str">
@@ -8165,15 +8419,19 @@
         <v>448</v>
       </c>
       <c r="AR55" s="97" t="str">
-        <f t="shared" ref="AR55:AR65" si="28">"1 "&amp;H55&amp;" INSTRUCTION _"&amp;B55</f>
+        <f t="shared" ref="AR55:AR65" si="29">"1 "&amp;H55&amp;" INSTRUCTION _"&amp;B55</f>
         <v>1 41 INSTRUCTION _MULTS</v>
       </c>
       <c r="AS55" s="97" t="str">
-        <f t="shared" ref="AS55:AS65" si="29">CHAR(44)&amp;CHAR(34)&amp;CHAR(32)&amp;B55&amp;CHAR(34)</f>
+        <f t="shared" ref="AS55:AS65" si="30">CHAR(44)&amp;CHAR(34)&amp;CHAR(32)&amp;B55&amp;CHAR(34)</f>
         <v>," MULTS"</v>
       </c>
-    </row>
-    <row r="56" spans="1:45" s="92" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AT55" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>MULTS when "1000000"</v>
+      </c>
+    </row>
+    <row r="56" spans="1:46" s="92" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B56" s="93" t="s">
         <v>253</v>
       </c>
@@ -8194,7 +8452,7 @@
         <v>42</v>
       </c>
       <c r="I56" s="3" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0101010</v>
       </c>
       <c r="J56" s="93" t="str">
@@ -8301,15 +8559,19 @@
         <v>464</v>
       </c>
       <c r="AR56" s="97" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>1 42 INSTRUCTION _MULTU</v>
       </c>
       <c r="AS56" s="97" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>," MULTU"</v>
       </c>
-    </row>
-    <row r="57" spans="1:45" s="92" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AT56" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>MULTU when "1010000"</v>
+      </c>
+    </row>
+    <row r="57" spans="1:46" s="92" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B57" s="93" t="s">
         <v>254</v>
       </c>
@@ -8321,7 +8583,7 @@
         <v>0</v>
       </c>
       <c r="F57" s="93">
-        <f t="shared" ref="F57:F64" si="30">F56+1</f>
+        <f t="shared" ref="F57:F64" si="31">F56+1</f>
         <v>43</v>
       </c>
       <c r="G57" s="93"/>
@@ -8330,7 +8592,7 @@
         <v>43</v>
       </c>
       <c r="I57" s="3" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0101011</v>
       </c>
       <c r="J57" s="93" t="str">
@@ -8438,15 +8700,19 @@
         <v>480</v>
       </c>
       <c r="AR57" s="97" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>1 43 INSTRUCTION _DIVS</v>
       </c>
       <c r="AS57" s="97" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>," DIVS"</v>
       </c>
-    </row>
-    <row r="58" spans="1:45" s="92" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AT57" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>DIVS when "1100000"</v>
+      </c>
+    </row>
+    <row r="58" spans="1:46" s="92" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B58" s="93" t="s">
         <v>255</v>
       </c>
@@ -8458,7 +8724,7 @@
         <v>0</v>
       </c>
       <c r="F58" s="93">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>44</v>
       </c>
       <c r="G58" s="93"/>
@@ -8467,7 +8733,7 @@
         <v>44</v>
       </c>
       <c r="I58" s="3" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0101100</v>
       </c>
       <c r="J58" s="93" t="str">
@@ -8575,15 +8841,19 @@
         <v>496</v>
       </c>
       <c r="AR58" s="97" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>1 44 INSTRUCTION _DIVU</v>
       </c>
       <c r="AS58" s="97" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>," DIVU"</v>
       </c>
-    </row>
-    <row r="59" spans="1:45" s="92" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AT58" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>DIVU when "1110000"</v>
+      </c>
+    </row>
+    <row r="59" spans="1:46" s="92" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B59" s="93" t="s">
         <v>256</v>
       </c>
@@ -8595,20 +8865,20 @@
         <v>0</v>
       </c>
       <c r="F59" s="93">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>45</v>
       </c>
       <c r="G59" s="93"/>
       <c r="H59" s="94">
-        <f t="shared" ref="H59:H64" si="31">F59+E59*64+D59*128</f>
+        <f t="shared" ref="H59:H64" si="32">F59+E59*64+D59*128</f>
         <v>45</v>
       </c>
       <c r="I59" s="3" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0101101</v>
       </c>
       <c r="J59" s="93" t="str">
-        <f t="shared" ref="J59:J64" si="32">DEC2HEX(H59)</f>
+        <f t="shared" ref="J59:J64" si="33">DEC2HEX(H59)</f>
         <v>2D</v>
       </c>
       <c r="K59" s="93"/>
@@ -8712,15 +8982,19 @@
         <v>0</v>
       </c>
       <c r="AR59" s="97" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>1 45 INSTRUCTION _FETCH.L</v>
       </c>
       <c r="AS59" s="97" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>," FETCH.L"</v>
       </c>
-    </row>
-    <row r="60" spans="1:45" s="92" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AT59" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>FETCH.L when "0000000"</v>
+      </c>
+    </row>
+    <row r="60" spans="1:46" s="92" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B60" s="93" t="s">
         <v>257</v>
       </c>
@@ -8732,20 +9006,20 @@
         <v>0</v>
       </c>
       <c r="F60" s="93">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>46</v>
       </c>
       <c r="G60" s="93"/>
       <c r="H60" s="94">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>46</v>
       </c>
       <c r="I60" s="3" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0101110</v>
       </c>
       <c r="J60" s="93" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>2E</v>
       </c>
       <c r="K60" s="93"/>
@@ -8849,15 +9123,19 @@
         <v>0</v>
       </c>
       <c r="AR60" s="97" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>1 46 INSTRUCTION _STORE.L</v>
       </c>
       <c r="AS60" s="97" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>," STORE.L"</v>
       </c>
-    </row>
-    <row r="61" spans="1:45" s="92" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AT60" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>STORE.L when "0000000"</v>
+      </c>
+    </row>
+    <row r="61" spans="1:46" s="92" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B61" s="93" t="s">
         <v>258</v>
       </c>
@@ -8869,20 +9147,20 @@
         <v>0</v>
       </c>
       <c r="F61" s="93">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>47</v>
       </c>
       <c r="G61" s="93"/>
       <c r="H61" s="94">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>47</v>
       </c>
       <c r="I61" s="3" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0101111</v>
       </c>
       <c r="J61" s="93" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>2F</v>
       </c>
       <c r="K61" s="93"/>
@@ -8986,15 +9264,19 @@
         <v>0</v>
       </c>
       <c r="AR61" s="97" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>1 47 INSTRUCTION _FETCH.W</v>
       </c>
       <c r="AS61" s="97" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>," FETCH.W"</v>
       </c>
-    </row>
-    <row r="62" spans="1:45" s="92" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AT61" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>FETCH.W when "0000000"</v>
+      </c>
+    </row>
+    <row r="62" spans="1:46" s="92" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B62" s="93" t="s">
         <v>259</v>
       </c>
@@ -9006,20 +9288,20 @@
         <v>0</v>
       </c>
       <c r="F62" s="93">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>48</v>
       </c>
       <c r="G62" s="93"/>
       <c r="H62" s="94">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>48</v>
       </c>
       <c r="I62" s="3" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0110000</v>
       </c>
       <c r="J62" s="93" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>30</v>
       </c>
       <c r="K62" s="93"/>
@@ -9123,15 +9405,19 @@
         <v>0</v>
       </c>
       <c r="AR62" s="97" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>1 48 INSTRUCTION _STORE.W</v>
       </c>
       <c r="AS62" s="97" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>," STORE.W"</v>
       </c>
-    </row>
-    <row r="63" spans="1:45" s="92" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AT62" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>STORE.W when "0000000"</v>
+      </c>
+    </row>
+    <row r="63" spans="1:46" s="92" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B63" s="93" t="s">
         <v>260</v>
       </c>
@@ -9143,20 +9429,20 @@
         <v>0</v>
       </c>
       <c r="F63" s="93">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>49</v>
       </c>
       <c r="G63" s="93"/>
       <c r="H63" s="94">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>49</v>
       </c>
       <c r="I63" s="3" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0110001</v>
       </c>
       <c r="J63" s="93" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>31</v>
       </c>
       <c r="K63" s="93"/>
@@ -9260,15 +9546,19 @@
         <v>0</v>
       </c>
       <c r="AR63" s="97" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>1 49 INSTRUCTION _FETCH.B</v>
       </c>
       <c r="AS63" s="97" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>," FETCH.B"</v>
       </c>
-    </row>
-    <row r="64" spans="1:45" s="92" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AT63" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>FETCH.B when "0000000"</v>
+      </c>
+    </row>
+    <row r="64" spans="1:46" s="92" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B64" s="93" t="s">
         <v>266</v>
       </c>
@@ -9280,20 +9570,20 @@
         <v>0</v>
       </c>
       <c r="F64" s="93">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>50</v>
       </c>
       <c r="G64" s="93"/>
       <c r="H64" s="94">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>50</v>
       </c>
       <c r="I64" s="3" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0110010</v>
       </c>
       <c r="J64" s="93" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>32</v>
       </c>
       <c r="K64" s="93"/>
@@ -9397,15 +9687,19 @@
         <v>0</v>
       </c>
       <c r="AR64" s="97" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>1 50 INSTRUCTION _STORE.B</v>
       </c>
       <c r="AS64" s="97" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>," STORE.B"</v>
       </c>
-    </row>
-    <row r="65" spans="1:45" s="92" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AT64" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>STORE.B when "0000000"</v>
+      </c>
+    </row>
+    <row r="65" spans="1:46" s="92" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B65" s="93" t="s">
         <v>1</v>
       </c>
@@ -9426,7 +9720,7 @@
         <v>51</v>
       </c>
       <c r="I65" s="3" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0110011</v>
       </c>
       <c r="J65" s="93" t="str">
@@ -9457,31 +9751,31 @@
         <v>31</v>
       </c>
       <c r="T65" s="93" t="str">
-        <f t="shared" ref="T65:Z65" si="33">T8</f>
+        <f t="shared" ref="T65:Z65" si="34">T8</f>
         <v>PSP + 1</v>
       </c>
       <c r="U65" s="93" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>TOS</v>
       </c>
       <c r="V65" s="93" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>addsub</v>
       </c>
       <c r="W65" s="93" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>X</v>
       </c>
       <c r="X65" s="93" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>TOS</v>
       </c>
       <c r="Y65" s="93" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>X</v>
       </c>
       <c r="Z65" s="93" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>X</v>
       </c>
       <c r="AA65" s="93"/>
@@ -9543,15 +9837,19 @@
         <v>2176</v>
       </c>
       <c r="AR65" s="97" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>1 51 INSTRUCTION _?DUP</v>
       </c>
       <c r="AS65" s="97" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>," ?DUP"</v>
       </c>
-    </row>
-    <row r="66" spans="1:45" s="49" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AT65" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>?DUP when "0000000"</v>
+      </c>
+    </row>
+    <row r="66" spans="1:46" s="49" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B66" s="50"/>
       <c r="C66" s="50"/>
       <c r="D66" s="50"/>
@@ -9578,8 +9876,12 @@
       <c r="AP66" s="1"/>
       <c r="AR66" s="56"/>
       <c r="AS66" s="59"/>
-    </row>
-    <row r="67" spans="1:45" s="49" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AT66" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve"> when ""</v>
+      </c>
+    </row>
+    <row r="67" spans="1:46" s="49" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="87" t="s">
         <v>312</v>
       </c>
@@ -9609,8 +9911,12 @@
       <c r="AP67" s="1"/>
       <c r="AR67" s="56"/>
       <c r="AS67" s="59"/>
-    </row>
-    <row r="68" spans="1:45" s="83" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AT67" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve"> when ""</v>
+      </c>
+    </row>
+    <row r="68" spans="1:46" s="83" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B68" s="84" t="s">
         <v>277</v>
       </c>
@@ -9627,15 +9933,15 @@
       </c>
       <c r="G68" s="84"/>
       <c r="H68" s="85">
-        <f t="shared" ref="H68:H76" si="34">F68+E68*64+D68*128</f>
+        <f t="shared" ref="H68:H76" si="35">F68+E68*64+D68*128</f>
         <v>52</v>
       </c>
       <c r="I68" s="3" t="str">
-        <f t="shared" ref="I68:I76" si="35">DEC2BIN(H68,7)</f>
+        <f t="shared" ref="I68:I76" si="36">DEC2BIN(H68,7)</f>
         <v>0110100</v>
       </c>
       <c r="J68" s="84" t="str">
-        <f t="shared" ref="J68:J76" si="36">DEC2HEX(H68)</f>
+        <f t="shared" ref="J68:J76" si="37">DEC2HEX(H68)</f>
         <v>34</v>
       </c>
       <c r="K68" s="84"/>
@@ -9738,15 +10044,19 @@
         <v>2215</v>
       </c>
       <c r="AR68" s="89" t="str">
-        <f t="shared" ref="AR68:AR76" si="37">"1 "&amp;H68&amp;" INSTRUCTION _"&amp;B68</f>
+        <f t="shared" ref="AR68:AR76" si="38">"1 "&amp;H68&amp;" INSTRUCTION _"&amp;B68</f>
         <v>1 52 INSTRUCTION _#.B</v>
       </c>
       <c r="AS68" s="89" t="str">
         <f>CHAR(44)&amp;CHAR(34)&amp;CHAR(32)&amp;B68&amp;CHAR(34)</f>
         <v>," #.B"</v>
       </c>
-    </row>
-    <row r="69" spans="1:45" s="83" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AT68" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>#.B when "0100111"</v>
+      </c>
+    </row>
+    <row r="69" spans="1:46" s="83" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B69" s="84" t="s">
         <v>276</v>
       </c>
@@ -9758,20 +10068,20 @@
         <v>0</v>
       </c>
       <c r="F69" s="84">
-        <f t="shared" ref="F69:F77" si="38">F68+1</f>
+        <f t="shared" ref="F69:F77" si="39">F68+1</f>
         <v>53</v>
       </c>
       <c r="G69" s="84"/>
       <c r="H69" s="85">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>53</v>
       </c>
       <c r="I69" s="3" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>0110101</v>
       </c>
       <c r="J69" s="84" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>35</v>
       </c>
       <c r="K69" s="84"/>
@@ -9874,15 +10184,19 @@
         <v>2215</v>
       </c>
       <c r="AR69" s="89" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>1 53 INSTRUCTION _#.W</v>
       </c>
       <c r="AS69" s="89" t="str">
         <f>CHAR(44)&amp;CHAR(34)&amp;CHAR(32)&amp;B69&amp;CHAR(34)</f>
         <v>," #.W"</v>
       </c>
-    </row>
-    <row r="70" spans="1:45" s="83" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AT69" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>#.W when "0100111"</v>
+      </c>
+    </row>
+    <row r="70" spans="1:46" s="83" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B70" s="84" t="s">
         <v>275</v>
       </c>
@@ -9894,20 +10208,20 @@
         <v>0</v>
       </c>
       <c r="F70" s="84">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>54</v>
       </c>
       <c r="G70" s="84"/>
       <c r="H70" s="85">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>54</v>
       </c>
       <c r="I70" s="3" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>0110110</v>
       </c>
       <c r="J70" s="84" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>36</v>
       </c>
       <c r="K70" s="84"/>
@@ -10010,15 +10324,19 @@
         <v>2215</v>
       </c>
       <c r="AR70" s="89" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>1 54 INSTRUCTION _#.L</v>
       </c>
       <c r="AS70" s="89" t="str">
         <f>CHAR(44)&amp;CHAR(34)&amp;CHAR(32)&amp;B70&amp;CHAR(34)</f>
         <v>," #.L"</v>
       </c>
-    </row>
-    <row r="71" spans="1:45" s="83" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AT70" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>#.L when "0100111"</v>
+      </c>
+    </row>
+    <row r="71" spans="1:46" s="83" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B71" s="84" t="s">
         <v>46</v>
       </c>
@@ -10030,20 +10348,20 @@
         <v>0</v>
       </c>
       <c r="F71" s="84">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>55</v>
       </c>
       <c r="G71" s="84"/>
       <c r="H71" s="85">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>55</v>
       </c>
       <c r="I71" s="3" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>0110111</v>
       </c>
       <c r="J71" s="84" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>37</v>
       </c>
       <c r="K71" s="84"/>
@@ -10138,7 +10456,7 @@
       </c>
       <c r="AN71" s="84"/>
       <c r="AO71" s="9" t="str">
-        <f t="shared" ref="AO71:AO86" si="39">AB71&amp;AC71&amp;AD71&amp;AE71&amp;AF71&amp;AG71&amp;AH71&amp;AM71</f>
+        <f t="shared" ref="AO71:AO86" si="40">AB71&amp;AC71&amp;AD71&amp;AE71&amp;AF71&amp;AG71&amp;AH71&amp;AM71</f>
         <v>00000010000010100100000</v>
       </c>
       <c r="AP71" s="1">
@@ -10146,15 +10464,19 @@
         <v>66848</v>
       </c>
       <c r="AR71" s="89" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>1 55 INSTRUCTION _JMP</v>
       </c>
       <c r="AS71" s="89" t="str">
         <f>CHAR(44)&amp;CHAR(34)&amp;CHAR(32)&amp;B71&amp;CHAR(34)</f>
         <v>," JMP"</v>
       </c>
-    </row>
-    <row r="72" spans="1:45" s="83" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AT71" s="1" t="str">
+        <f t="shared" ref="AT71:AT87" si="41">B71&amp;CHAR(32)&amp;"when"&amp;CHAR(32)&amp;CHAR(34)&amp;RIGHT(AO71,7)&amp;CHAR(34)</f>
+        <v>JMP when "0100000"</v>
+      </c>
+    </row>
+    <row r="72" spans="1:46" s="83" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B72" s="84" t="s">
         <v>304</v>
       </c>
@@ -10166,20 +10488,20 @@
         <v>0</v>
       </c>
       <c r="F72" s="84">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>56</v>
       </c>
       <c r="G72" s="84"/>
       <c r="H72" s="85">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>56</v>
       </c>
       <c r="I72" s="3" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>0111000</v>
       </c>
       <c r="J72" s="84" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>38</v>
       </c>
       <c r="K72" s="84"/>
@@ -10274,7 +10596,7 @@
       </c>
       <c r="AN72" s="84"/>
       <c r="AO72" s="9" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>00001010100000000000000</v>
       </c>
       <c r="AP72" s="1">
@@ -10282,14 +10604,18 @@
         <v>344064</v>
       </c>
       <c r="AR72" s="89" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>1 56 INSTRUCTION _JSL</v>
       </c>
       <c r="AS72" s="89" t="s">
         <v>306</v>
       </c>
-    </row>
-    <row r="73" spans="1:45" s="83" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AT72" s="1" t="str">
+        <f t="shared" si="41"/>
+        <v>JSL when "0000000"</v>
+      </c>
+    </row>
+    <row r="73" spans="1:46" s="83" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B73" s="84" t="s">
         <v>45</v>
       </c>
@@ -10301,20 +10627,20 @@
         <v>0</v>
       </c>
       <c r="F73" s="84">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>57</v>
       </c>
       <c r="G73" s="84"/>
       <c r="H73" s="85">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>57</v>
       </c>
       <c r="I73" s="3" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>0111001</v>
       </c>
       <c r="J73" s="84" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>39</v>
       </c>
       <c r="K73" s="84"/>
@@ -10409,7 +10735,7 @@
       </c>
       <c r="AN73" s="84"/>
       <c r="AO73" s="9" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>00001010100010100100000</v>
       </c>
       <c r="AP73" s="1">
@@ -10417,15 +10743,19 @@
         <v>345376</v>
       </c>
       <c r="AR73" s="89" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>1 57 INSTRUCTION _JSR</v>
       </c>
       <c r="AS73" s="89" t="str">
         <f>CHAR(44)&amp;CHAR(34)&amp;CHAR(32)&amp;B73&amp;CHAR(34)</f>
         <v>," JSR"</v>
       </c>
-    </row>
-    <row r="74" spans="1:45" s="83" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AT73" s="1" t="str">
+        <f t="shared" si="41"/>
+        <v>JSR when "0100000"</v>
+      </c>
+    </row>
+    <row r="74" spans="1:46" s="83" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B74" s="84" t="s">
         <v>268</v>
       </c>
@@ -10437,20 +10767,20 @@
         <v>0</v>
       </c>
       <c r="F74" s="84">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>58</v>
       </c>
       <c r="G74" s="84"/>
       <c r="H74" s="85">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>58</v>
       </c>
       <c r="I74" s="3" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>0111010</v>
       </c>
       <c r="J74" s="84" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>3A</v>
       </c>
       <c r="K74" s="84"/>
@@ -10545,7 +10875,7 @@
       </c>
       <c r="AN74" s="84"/>
       <c r="AO74" s="9" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>00000000000000000000000</v>
       </c>
       <c r="AP74" s="1">
@@ -10553,15 +10883,19 @@
         <v>0</v>
       </c>
       <c r="AR74" s="89" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>1 58 INSTRUCTION _TRAP</v>
       </c>
       <c r="AS74" s="89" t="str">
         <f>CHAR(44)&amp;CHAR(34)&amp;CHAR(32)&amp;B74&amp;CHAR(34)</f>
         <v>," TRAP"</v>
       </c>
-    </row>
-    <row r="75" spans="1:45" s="83" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AT74" s="1" t="str">
+        <f t="shared" si="41"/>
+        <v>TRAP when "0000000"</v>
+      </c>
+    </row>
+    <row r="75" spans="1:46" s="83" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B75" s="84" t="s">
         <v>309</v>
       </c>
@@ -10573,20 +10907,20 @@
         <v>0</v>
       </c>
       <c r="F75" s="84">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>59</v>
       </c>
       <c r="G75" s="84"/>
       <c r="H75" s="85">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>59</v>
       </c>
       <c r="I75" s="3" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>0111011</v>
       </c>
       <c r="J75" s="84" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>3B</v>
       </c>
       <c r="K75" s="84"/>
@@ -10681,7 +11015,7 @@
       </c>
       <c r="AN75" s="84"/>
       <c r="AO75" s="9" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>00000000000000000000000</v>
       </c>
       <c r="AP75" s="1">
@@ -10689,15 +11023,19 @@
         <v>0</v>
       </c>
       <c r="AR75" s="89" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>1 59 INSTRUCTION _RETRAP</v>
       </c>
       <c r="AS75" s="89" t="str">
         <f>CHAR(44)&amp;CHAR(34)&amp;CHAR(32)&amp;B75&amp;CHAR(34)</f>
         <v>," RETRAP"</v>
       </c>
-    </row>
-    <row r="76" spans="1:45" s="83" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AT75" s="1" t="str">
+        <f t="shared" si="41"/>
+        <v>RETRAP when "0000000"</v>
+      </c>
+    </row>
+    <row r="76" spans="1:46" s="83" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B76" s="84" t="s">
         <v>271</v>
       </c>
@@ -10709,20 +11047,20 @@
         <v>0</v>
       </c>
       <c r="F76" s="84">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>60</v>
       </c>
       <c r="G76" s="84"/>
       <c r="H76" s="85">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>60</v>
       </c>
       <c r="I76" s="3" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>0111100</v>
       </c>
       <c r="J76" s="84" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>3C</v>
       </c>
       <c r="K76" s="84"/>
@@ -10817,7 +11155,7 @@
       </c>
       <c r="AN76" s="84"/>
       <c r="AO76" s="9" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>00000000000000000000000</v>
       </c>
       <c r="AP76" s="1">
@@ -10825,15 +11163,19 @@
         <v>0</v>
       </c>
       <c r="AR76" s="89" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>1 60 INSTRUCTION _RTI</v>
       </c>
       <c r="AS76" s="89" t="str">
         <f>CHAR(44)&amp;CHAR(34)&amp;CHAR(32)&amp;B76&amp;CHAR(34)</f>
         <v>," RTI"</v>
       </c>
-    </row>
-    <row r="77" spans="1:45" s="83" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AT76" s="1" t="str">
+        <f t="shared" si="41"/>
+        <v>RTI when "0000000"</v>
+      </c>
+    </row>
+    <row r="77" spans="1:46" s="83" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B77" s="84" t="s">
         <v>340</v>
       </c>
@@ -10845,20 +11187,20 @@
         <v>0</v>
       </c>
       <c r="F77" s="84">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>61</v>
       </c>
       <c r="G77" s="84"/>
       <c r="H77" s="85">
-        <f t="shared" ref="H77" si="40">F77+E77*64+D77*128</f>
+        <f t="shared" ref="H77" si="42">F77+E77*64+D77*128</f>
         <v>61</v>
       </c>
       <c r="I77" s="3" t="str">
-        <f t="shared" ref="I77" si="41">DEC2BIN(H77,7)</f>
+        <f t="shared" ref="I77" si="43">DEC2BIN(H77,7)</f>
         <v>0111101</v>
       </c>
       <c r="J77" s="84" t="str">
-        <f t="shared" ref="J77" si="42">DEC2HEX(H77)</f>
+        <f t="shared" ref="J77" si="44">DEC2HEX(H77)</f>
         <v>3D</v>
       </c>
       <c r="K77" s="84"/>
@@ -10953,7 +11295,7 @@
       </c>
       <c r="AN77" s="84"/>
       <c r="AO77" s="9" t="str">
-        <f t="shared" ref="AO77" si="43">AB77&amp;AC77&amp;AD77&amp;AE77&amp;AF77&amp;AG77&amp;AH77&amp;AM77</f>
+        <f t="shared" ref="AO77" si="45">AB77&amp;AC77&amp;AD77&amp;AE77&amp;AF77&amp;AG77&amp;AH77&amp;AM77</f>
         <v>10010101101101000100100</v>
       </c>
       <c r="AP77" s="1">
@@ -10961,15 +11303,19 @@
         <v>4905508</v>
       </c>
       <c r="AR77" s="89" t="str">
-        <f t="shared" ref="AR77" si="44">"1 "&amp;H77&amp;" INSTRUCTION _"&amp;B77</f>
+        <f t="shared" ref="AR77" si="46">"1 "&amp;H77&amp;" INSTRUCTION _"&amp;B77</f>
         <v>1 61 INSTRUCTION _PAUSE</v>
       </c>
       <c r="AS77" s="89" t="str">
         <f>CHAR(44)&amp;CHAR(34)&amp;CHAR(32)&amp;B77&amp;CHAR(34)</f>
         <v>," PAUSE"</v>
       </c>
-    </row>
-    <row r="78" spans="1:45" s="83" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AT77" s="1" t="str">
+        <f t="shared" si="41"/>
+        <v>PAUSE when "0100100"</v>
+      </c>
+    </row>
+    <row r="78" spans="1:46" s="83" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B78" s="84"/>
       <c r="C78" s="84"/>
       <c r="D78" s="84"/>
@@ -11011,8 +11357,12 @@
       <c r="AP78" s="1"/>
       <c r="AR78" s="89"/>
       <c r="AS78" s="89"/>
-    </row>
-    <row r="79" spans="1:45" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AT78" s="1" t="str">
+        <f t="shared" si="41"/>
+        <v xml:space="preserve"> when ""</v>
+      </c>
+    </row>
+    <row r="79" spans="1:46" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>338</v>
       </c>
@@ -11056,8 +11406,12 @@
       <c r="AO79" s="9"/>
       <c r="AR79" s="58"/>
       <c r="AS79" s="58"/>
-    </row>
-    <row r="80" spans="1:45" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AT79" s="1" t="str">
+        <f t="shared" si="41"/>
+        <v xml:space="preserve"> when ""</v>
+      </c>
+    </row>
+    <row r="80" spans="1:46" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B80" s="8" t="s">
         <v>337</v>
       </c>
@@ -11077,7 +11431,7 @@
         <v>62</v>
       </c>
       <c r="I80" s="8" t="str">
-        <f t="shared" ref="I80:I81" si="45">DEC2BIN(H80,7)</f>
+        <f t="shared" ref="I80:I81" si="47">DEC2BIN(H80,7)</f>
         <v>0111110</v>
       </c>
       <c r="J80" s="8" t="str">
@@ -11180,15 +11534,19 @@
         <v>0</v>
       </c>
       <c r="AR80" s="89" t="str">
-        <f t="shared" ref="AR80:AR81" si="46">"1 "&amp;H80&amp;" INSTRUCTION _"&amp;B80</f>
+        <f t="shared" ref="AR80:AR81" si="48">"1 "&amp;H80&amp;" INSTRUCTION _"&amp;B80</f>
         <v>1 62 INSTRUCTION _UNUSED</v>
       </c>
       <c r="AS80" s="89" t="str">
-        <f t="shared" ref="AS80:AS81" si="47">CHAR(44)&amp;CHAR(34)&amp;CHAR(32)&amp;B80&amp;CHAR(34)</f>
+        <f t="shared" ref="AS80:AS81" si="49">CHAR(44)&amp;CHAR(34)&amp;CHAR(32)&amp;B80&amp;CHAR(34)</f>
         <v>," UNUSED"</v>
       </c>
-    </row>
-    <row r="81" spans="1:45" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AT80" s="1" t="str">
+        <f t="shared" si="41"/>
+        <v>UNUSED when "0000000"</v>
+      </c>
+    </row>
+    <row r="81" spans="1:46" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B81" s="8" t="s">
         <v>337</v>
       </c>
@@ -11204,15 +11562,15 @@
       </c>
       <c r="G81" s="8"/>
       <c r="H81" s="44">
-        <f t="shared" ref="H81" si="48">F81+E81*64+D81*128</f>
+        <f t="shared" ref="H81" si="50">F81+E81*64+D81*128</f>
         <v>63</v>
       </c>
       <c r="I81" s="8" t="str">
-        <f t="shared" si="45"/>
+        <f t="shared" si="47"/>
         <v>0111111</v>
       </c>
       <c r="J81" s="8" t="str">
-        <f t="shared" ref="J81" si="49">DEC2HEX(H81)</f>
+        <f t="shared" ref="J81" si="51">DEC2HEX(H81)</f>
         <v>3F</v>
       </c>
       <c r="K81" s="8"/>
@@ -11311,15 +11669,19 @@
         <v>0</v>
       </c>
       <c r="AR81" s="89" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="48"/>
         <v>1 63 INSTRUCTION _UNUSED</v>
       </c>
       <c r="AS81" s="89" t="str">
-        <f t="shared" si="47"/>
+        <f t="shared" si="49"/>
         <v>," UNUSED"</v>
       </c>
-    </row>
-    <row r="82" spans="1:45" s="49" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AT81" s="1" t="str">
+        <f t="shared" si="41"/>
+        <v>UNUSED when "0000000"</v>
+      </c>
+    </row>
+    <row r="82" spans="1:46" s="49" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B82" s="84"/>
       <c r="C82" s="50"/>
       <c r="D82" s="43"/>
@@ -11341,8 +11703,12 @@
       <c r="AO82" s="9"/>
       <c r="AP82" s="1"/>
       <c r="AR82" s="53"/>
-    </row>
-    <row r="83" spans="1:45" s="42" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AT82" s="1" t="str">
+        <f t="shared" si="41"/>
+        <v xml:space="preserve"> when ""</v>
+      </c>
+    </row>
+    <row r="83" spans="1:46" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="18" t="s">
         <v>339</v>
       </c>
@@ -11365,12 +11731,16 @@
       <c r="AC83" s="43"/>
       <c r="AF83" s="43"/>
       <c r="AO83" s="18" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="AR83" s="121"/>
-    </row>
-    <row r="84" spans="1:45" s="42" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AT83" s="1" t="str">
+        <f t="shared" si="41"/>
+        <v xml:space="preserve"> when ""</v>
+      </c>
+    </row>
+    <row r="84" spans="1:46" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="18"/>
       <c r="B84" s="43" t="s">
         <v>37</v>
@@ -11387,11 +11757,11 @@
       </c>
       <c r="G84" s="43"/>
       <c r="H84" s="48">
-        <f t="shared" ref="H84" si="50">F84+E84*64+D84*128</f>
+        <f t="shared" ref="H84" si="52">F84+E84*64+D84*128</f>
         <v>64</v>
       </c>
       <c r="I84" s="43" t="str">
-        <f t="shared" ref="I84:I86" si="51">DEC2BIN(H84,7)</f>
+        <f t="shared" ref="I84:I86" si="53">DEC2BIN(H84,7)</f>
         <v>1000000</v>
       </c>
       <c r="J84" s="43" t="str">
@@ -11497,8 +11867,12 @@
         <v>0</v>
       </c>
       <c r="AR84" s="121"/>
-    </row>
-    <row r="85" spans="1:45" s="42" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AT84" s="1" t="str">
+        <f t="shared" si="41"/>
+        <v>NOP when "0000000"</v>
+      </c>
+    </row>
+    <row r="85" spans="1:46" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B85" s="43" t="s">
         <v>332</v>
       </c>
@@ -11518,7 +11892,7 @@
         <v>65</v>
       </c>
       <c r="I85" s="43" t="str">
-        <f t="shared" si="51"/>
+        <f t="shared" si="53"/>
         <v>1000001</v>
       </c>
       <c r="J85" s="43" t="str">
@@ -11617,7 +11991,7 @@
       </c>
       <c r="AN85" s="43"/>
       <c r="AO85" s="18" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>00000001000000000000000</v>
       </c>
       <c r="AP85" s="42">
@@ -11626,8 +12000,12 @@
       </c>
       <c r="AR85" s="91"/>
       <c r="AS85" s="91"/>
-    </row>
-    <row r="86" spans="1:45" s="42" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AT85" s="1" t="str">
+        <f t="shared" si="41"/>
+        <v>THROW2 when "0000000"</v>
+      </c>
+    </row>
+    <row r="86" spans="1:46" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B86" s="43" t="s">
         <v>239</v>
       </c>
@@ -11647,7 +12025,7 @@
         <v>66</v>
       </c>
       <c r="I86" s="43" t="str">
-        <f t="shared" si="51"/>
+        <f t="shared" si="53"/>
         <v>1000010</v>
       </c>
       <c r="J86" s="43" t="str">
@@ -11746,7 +12124,7 @@
       </c>
       <c r="AN86" s="43"/>
       <c r="AO86" s="18" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>00000000000000000100111</v>
       </c>
       <c r="AP86" s="42">
@@ -11755,11 +12133,19 @@
       </c>
       <c r="AR86" s="91"/>
       <c r="AS86" s="91"/>
-    </row>
-    <row r="87" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AT86" s="1" t="str">
+        <f t="shared" si="41"/>
+        <v>REPLACE when "0100111"</v>
+      </c>
+    </row>
+    <row r="87" spans="1:46" x14ac:dyDescent="0.25">
       <c r="N87" s="3"/>
-    </row>
-    <row r="88" spans="1:45" s="99" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AT87" s="1" t="str">
+        <f t="shared" si="41"/>
+        <v xml:space="preserve"> when ""</v>
+      </c>
+    </row>
+    <row r="88" spans="1:46" s="99" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="99" t="s">
         <v>310</v>
       </c>
@@ -11781,7 +12167,7 @@
       <c r="AO88" s="103"/>
       <c r="AR88" s="104"/>
     </row>
-    <row r="89" spans="1:45" s="99" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:46" s="99" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B89" s="100" t="s">
         <v>261</v>
       </c>
@@ -11797,12 +12183,12 @@
       </c>
       <c r="G89" s="100"/>
       <c r="H89" s="101">
-        <f t="shared" ref="H89:H91" si="52">F89+E89*64+D89*128</f>
+        <f t="shared" ref="H89:H91" si="54">F89+E89*64+D89*128</f>
         <v>64</v>
       </c>
       <c r="I89" s="100"/>
       <c r="J89" s="100" t="str">
-        <f t="shared" ref="J89:J91" si="53">DEC2HEX(H89)</f>
+        <f t="shared" ref="J89:J91" si="55">DEC2HEX(H89)</f>
         <v>40</v>
       </c>
       <c r="K89" s="100"/>
@@ -11836,13 +12222,13 @@
       <c r="AM89" s="100"/>
       <c r="AN89" s="100"/>
       <c r="AO89" s="9" t="str">
-        <f t="shared" ref="AO89" si="54">AB89&amp;AC89&amp;AD89&amp;AE89&amp;AF89&amp;AG89&amp;AH89&amp;AM89</f>
+        <f t="shared" ref="AO89" si="56">AB89&amp;AC89&amp;AD89&amp;AE89&amp;AF89&amp;AG89&amp;AH89&amp;AM89</f>
         <v/>
       </c>
       <c r="AR89" s="106"/>
       <c r="AS89" s="106"/>
     </row>
-    <row r="90" spans="1:45" s="99" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:46" s="99" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B90" s="100" t="s">
         <v>43</v>
       </c>
@@ -11858,12 +12244,12 @@
       </c>
       <c r="G90" s="100"/>
       <c r="H90" s="101">
-        <f t="shared" si="52"/>
+        <f t="shared" si="54"/>
         <v>128</v>
       </c>
       <c r="I90" s="100"/>
       <c r="J90" s="100" t="str">
-        <f t="shared" si="53"/>
+        <f t="shared" si="55"/>
         <v>80</v>
       </c>
       <c r="K90" s="100"/>
@@ -11902,7 +12288,7 @@
       <c r="AR90" s="106"/>
       <c r="AS90" s="106"/>
     </row>
-    <row r="91" spans="1:45" s="99" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:46" s="99" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B91" s="100" t="s">
         <v>44</v>
       </c>
@@ -11918,12 +12304,12 @@
       </c>
       <c r="G91" s="100"/>
       <c r="H91" s="101">
-        <f t="shared" si="52"/>
+        <f t="shared" si="54"/>
         <v>192</v>
       </c>
       <c r="I91" s="100"/>
       <c r="J91" s="100" t="str">
-        <f t="shared" si="53"/>
+        <f t="shared" si="55"/>
         <v>C0</v>
       </c>
       <c r="K91" s="100"/>
@@ -11942,7 +12328,7 @@
       <c r="AR91" s="106"/>
       <c r="AS91" s="106"/>
     </row>
-    <row r="92" spans="1:45" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:46" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B92" s="12"/>
       <c r="C92" s="12"/>
       <c r="D92" s="12"/>
@@ -11963,7 +12349,7 @@
       <c r="AR92" s="56"/>
       <c r="AS92" s="57"/>
     </row>
-    <row r="93" spans="1:45" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:46" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B93" s="12"/>
       <c r="C93" s="12"/>
       <c r="D93" s="12"/>
@@ -11986,14 +12372,14 @@
       <c r="AR93" s="56"/>
       <c r="AS93" s="57"/>
     </row>
-    <row r="94" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A94" s="6"/>
     </row>
-    <row r="95" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:46" x14ac:dyDescent="0.25">
       <c r="B95" s="6"/>
       <c r="C95" s="6"/>
     </row>
-    <row r="96" spans="1:45" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:46" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B96" s="7"/>
       <c r="C96" s="7"/>
       <c r="D96" s="36"/>
@@ -12011,16 +12397,16 @@
       <c r="AO96" s="37"/>
       <c r="AR96" s="47"/>
     </row>
-    <row r="97" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="97" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B97" s="49"/>
       <c r="C97" s="18"/>
     </row>
-    <row r="98" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="98" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B98" s="18"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B17" r:id="rId1" display="RSP@"/>
+    <hyperlink ref="B17" r:id="rId1" display="RSP@" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="72" orientation="portrait" r:id="rId2"/>
@@ -12028,27 +12414,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3.28515625" customWidth="1"/>
-    <col min="3" max="4" width="9.140625" style="39"/>
+    <col min="1" max="1" width="3.26953125" customWidth="1"/>
+    <col min="3" max="4" width="9.1796875" style="39"/>
     <col min="5" max="5" width="11" style="39" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="9.140625" style="39"/>
+    <col min="6" max="8" width="9.1796875" style="39"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="21" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B3" s="113"/>
       <c r="C3" s="65" t="s">
         <v>319</v>
@@ -12085,7 +12471,7 @@
       </c>
       <c r="N3" s="66"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B4" s="67">
         <v>0</v>
       </c>
@@ -12126,7 +12512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B5" s="67">
         <v>1</v>
       </c>
@@ -12167,7 +12553,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B6" s="67">
         <v>2</v>
       </c>
@@ -12206,7 +12592,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B7" s="67">
         <v>3</v>
       </c>
@@ -12245,7 +12631,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B8" s="67">
         <v>4</v>
       </c>
@@ -12284,7 +12670,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B9" s="67">
         <v>5</v>
       </c>
@@ -12319,7 +12705,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B10" s="67">
         <v>6</v>
       </c>
@@ -12352,7 +12738,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B11" s="67">
         <v>7</v>
       </c>
@@ -12381,7 +12767,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B12" s="67">
         <v>8</v>
       </c>
@@ -12402,7 +12788,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B13" s="67">
         <v>9</v>
       </c>
@@ -12423,7 +12809,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B14" s="67">
         <v>10</v>
       </c>
@@ -12444,7 +12830,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B15" s="67">
         <v>11</v>
       </c>
@@ -12465,7 +12851,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B16" s="67">
         <v>12</v>
       </c>
@@ -12486,7 +12872,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B17" s="67">
         <v>13</v>
       </c>
@@ -12507,7 +12893,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B18" s="67">
         <v>14</v>
       </c>
@@ -12528,7 +12914,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B19" s="68">
         <v>15</v>
       </c>
@@ -12549,7 +12935,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B21" s="3" t="s">
         <v>235</v>
       </c>
@@ -12587,7 +12973,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B22" s="3" t="s">
         <v>236</v>
       </c>
@@ -12629,7 +13015,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B24" s="3" t="s">
         <v>315</v>
       </c>
@@ -12675,7 +13061,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B25" s="3" t="s">
         <v>223</v>
       </c>
@@ -12720,7 +13106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B27" s="3" t="s">
         <v>315</v>
       </c>
@@ -12758,7 +13144,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B28" s="3" t="s">
         <v>223</v>
       </c>
@@ -12796,10 +13182,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:14" x14ac:dyDescent="0.35">
       <c r="E30" s="120"/>
     </row>
-    <row r="31" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:14" x14ac:dyDescent="0.35">
       <c r="E31" s="120"/>
     </row>
   </sheetData>
@@ -12809,45 +13195,45 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:V42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="10.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="3.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="6.28515625" style="1" customWidth="1"/>
-    <col min="4" max="5" width="8.5703125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="8.5703125" style="20" customWidth="1"/>
-    <col min="7" max="9" width="8.5703125" style="1" customWidth="1"/>
-    <col min="10" max="12" width="10.7109375" style="1" customWidth="1"/>
-    <col min="13" max="15" width="8.5703125" style="1" customWidth="1"/>
-    <col min="16" max="16" width="10.28515625" style="1" customWidth="1"/>
-    <col min="17" max="22" width="8.5703125" style="1" customWidth="1"/>
-    <col min="23" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="2.26953125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="3.453125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.26953125" style="1" customWidth="1"/>
+    <col min="4" max="5" width="8.54296875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="8.54296875" style="20" customWidth="1"/>
+    <col min="7" max="9" width="8.54296875" style="1" customWidth="1"/>
+    <col min="10" max="12" width="10.7265625" style="1" customWidth="1"/>
+    <col min="13" max="15" width="8.54296875" style="1" customWidth="1"/>
+    <col min="16" max="16" width="10.26953125" style="1" customWidth="1"/>
+    <col min="17" max="22" width="8.54296875" style="1" customWidth="1"/>
+    <col min="23" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A1" s="21" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B3" s="19" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B4" s="19"/>
       <c r="C4" s="19" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="5" spans="1:22" s="19" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:22" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D5" s="24" t="s">
         <v>142</v>
       </c>
@@ -12867,7 +13253,7 @@
       <c r="K5" s="5"/>
       <c r="L5" s="5"/>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="D6" s="1">
         <v>2</v>
       </c>
@@ -12889,7 +13275,7 @@
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="D7" s="1">
         <v>2</v>
       </c>
@@ -12909,7 +13295,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D8" s="2">
         <v>2</v>
       </c>
@@ -12929,7 +13315,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="D9" s="26">
         <f>SUM(D6:D8)</f>
         <v>6</v>
@@ -12939,18 +13325,18 @@
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
     </row>
-    <row r="11" spans="1:22" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:22" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="27"/>
       <c r="C11" s="27" t="s">
         <v>144</v>
       </c>
       <c r="F11" s="31"/>
     </row>
-    <row r="12" spans="1:22" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:22" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D12" s="11">
         <v>1</v>
       </c>
@@ -12964,22 +13350,22 @@
         <v>292</v>
       </c>
     </row>
-    <row r="13" spans="1:22" s="11" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:22" s="11" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D13" s="28">
         <f>SUM(D12:D12)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:22" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:22" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K14" s="12"/>
       <c r="L14" s="12"/>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B15" s="19" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="D16" s="24" t="s">
         <v>142</v>
       </c>
@@ -13032,7 +13418,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:22" x14ac:dyDescent="0.25">
       <c r="D17" s="25">
         <v>4</v>
       </c>
@@ -13089,7 +13475,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:22" x14ac:dyDescent="0.25">
       <c r="D18" s="25"/>
       <c r="G18" s="3" t="s">
         <v>189</v>
@@ -13140,7 +13526,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="19" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:22" x14ac:dyDescent="0.25">
       <c r="D19" s="1">
         <v>3</v>
       </c>
@@ -13172,7 +13558,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="20" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:22" x14ac:dyDescent="0.25">
       <c r="D20" s="1">
         <v>3</v>
       </c>
@@ -13204,7 +13590,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="21" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:22" x14ac:dyDescent="0.25">
       <c r="D21" s="1">
         <v>1</v>
       </c>
@@ -13236,7 +13622,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="22" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:22" x14ac:dyDescent="0.25">
       <c r="D22" s="1">
         <v>3</v>
       </c>
@@ -13268,22 +13654,22 @@
         <v>184</v>
       </c>
     </row>
-    <row r="23" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:22" x14ac:dyDescent="0.25">
       <c r="D23" s="26">
         <f>MAX(D17:D21)+D22</f>
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:22" x14ac:dyDescent="0.25">
       <c r="D24" s="32"/>
     </row>
-    <row r="25" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B25" s="19" t="s">
         <v>287</v>
       </c>
       <c r="D25" s="32"/>
     </row>
-    <row r="26" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:22" x14ac:dyDescent="0.25">
       <c r="D26" s="24" t="s">
         <v>142</v>
       </c>
@@ -13301,7 +13687,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:22" x14ac:dyDescent="0.25">
       <c r="D27" s="25">
         <v>1</v>
       </c>
@@ -13318,7 +13704,7 @@
       <c r="I27" s="5"/>
       <c r="J27" s="5"/>
     </row>
-    <row r="28" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:22" x14ac:dyDescent="0.25">
       <c r="D28" s="78">
         <f>SUM(D27)</f>
         <v>1</v>
@@ -13329,7 +13715,7 @@
       <c r="I28" s="5"/>
       <c r="J28" s="5"/>
     </row>
-    <row r="29" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:22" x14ac:dyDescent="0.25">
       <c r="D29" s="25"/>
       <c r="E29" s="19"/>
       <c r="G29" s="3"/>
@@ -13337,7 +13723,7 @@
       <c r="I29" s="5"/>
       <c r="J29" s="5"/>
     </row>
-    <row r="30" spans="2:22" s="22" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:22" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D30" s="34"/>
       <c r="F30" s="33"/>
       <c r="G30" s="23"/>
@@ -13346,7 +13732,7 @@
       <c r="J30" s="23"/>
       <c r="K30" s="23"/>
     </row>
-    <row r="31" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B31" s="19" t="s">
         <v>283</v>
       </c>
@@ -13362,7 +13748,7 @@
       <c r="K31" s="15"/>
       <c r="L31" s="15"/>
     </row>
-    <row r="32" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C32" s="1" t="s">
         <v>220</v>
       </c>
@@ -13382,7 +13768,7 @@
       </c>
       <c r="K32" s="3"/>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C33" s="1" t="s">
         <v>221</v>
       </c>
@@ -13412,7 +13798,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C34" s="1" t="s">
         <v>222</v>
       </c>
@@ -13443,7 +13829,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C35" s="1" t="s">
         <v>288</v>
       </c>
@@ -13463,24 +13849,24 @@
       <c r="K35" s="3"/>
       <c r="L35" s="3"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D36" s="26">
         <f>SUM(D32:D35)</f>
         <v>14</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B38" s="27" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D39" s="28">
         <f>D13</f>
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>13</v>
       </c>
@@ -13488,7 +13874,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="11" t="s">
         <v>294</v>
       </c>
@@ -13503,37 +13889,37 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:T28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="10.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" style="3" customWidth="1"/>
-    <col min="3" max="5" width="9.42578125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="1.5703125" style="1" customWidth="1"/>
-    <col min="7" max="8" width="9.28515625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="1.28515625" style="1" customWidth="1"/>
-    <col min="10" max="11" width="8.85546875" style="1" customWidth="1"/>
-    <col min="12" max="12" width="1.5703125" style="1" customWidth="1"/>
-    <col min="13" max="14" width="10.5703125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="1.7109375" style="1" customWidth="1"/>
-    <col min="16" max="17" width="10.5703125" style="1" customWidth="1"/>
-    <col min="18" max="18" width="1.85546875" style="1" customWidth="1"/>
-    <col min="19" max="20" width="8.7109375" style="1" customWidth="1"/>
-    <col min="21" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="14.453125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="17.26953125" style="3" customWidth="1"/>
+    <col min="3" max="5" width="9.453125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="1.54296875" style="1" customWidth="1"/>
+    <col min="7" max="8" width="9.26953125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="1.26953125" style="1" customWidth="1"/>
+    <col min="10" max="11" width="8.81640625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="1.54296875" style="1" customWidth="1"/>
+    <col min="13" max="14" width="10.54296875" style="1" customWidth="1"/>
+    <col min="15" max="15" width="1.7265625" style="1" customWidth="1"/>
+    <col min="16" max="17" width="10.54296875" style="1" customWidth="1"/>
+    <col min="18" max="18" width="1.81640625" style="1" customWidth="1"/>
+    <col min="19" max="20" width="8.7265625" style="1" customWidth="1"/>
+    <col min="21" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A1" s="21" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C4" s="29" t="s">
         <v>162</v>
       </c>
@@ -13560,7 +13946,7 @@
       </c>
       <c r="T4" s="15"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C5" s="3" t="s">
         <v>164</v>
       </c>
@@ -13601,7 +13987,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
@@ -13624,7 +14010,7 @@
       <c r="S6" s="3"/>
       <c r="T6" s="3"/>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>30</v>
       </c>
@@ -13645,7 +14031,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>29</v>
       </c>
@@ -13672,7 +14058,7 @@
       <c r="S8" s="3"/>
       <c r="T8" s="3"/>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>11</v>
       </c>
@@ -13693,7 +14079,7 @@
       <c r="P9" s="3"/>
       <c r="Q9" s="3"/>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>12</v>
       </c>
@@ -13714,7 +14100,7 @@
       <c r="P10" s="3"/>
       <c r="Q10" s="3"/>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>13</v>
       </c>
@@ -13735,7 +14121,7 @@
       <c r="P11" s="3"/>
       <c r="Q11" s="3"/>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
         <v>14</v>
       </c>
@@ -13752,7 +14138,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
         <v>15</v>
       </c>
@@ -13771,7 +14157,7 @@
       <c r="P13" s="3"/>
       <c r="Q13" s="3"/>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
         <v>38</v>
       </c>
@@ -13790,7 +14176,7 @@
       <c r="M14" s="3"/>
       <c r="N14" s="3"/>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="17" t="s">
         <v>39</v>
       </c>
@@ -13809,7 +14195,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>16</v>
       </c>
@@ -13828,7 +14214,7 @@
       <c r="M16" s="3"/>
       <c r="N16" s="3"/>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>47</v>
       </c>
@@ -13847,7 +14233,7 @@
       <c r="M17" s="3"/>
       <c r="N17" s="3"/>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
         <v>48</v>
       </c>
@@ -13868,7 +14254,7 @@
       <c r="S18" s="3"/>
       <c r="T18" s="3"/>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
         <v>49</v>
       </c>
@@ -13887,7 +14273,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
         <v>50</v>
       </c>
@@ -13906,7 +14292,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>23</v>
       </c>
@@ -13925,7 +14311,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>24</v>
       </c>
@@ -13944,7 +14330,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>25</v>
       </c>
@@ -13963,7 +14349,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>26</v>
       </c>
@@ -13982,7 +14368,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
         <v>133</v>
       </c>
@@ -14001,7 +14387,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
         <v>132</v>
       </c>
@@ -14020,7 +14406,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>203</v>
       </c>
@@ -14037,7 +14423,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>204</v>
       </c>
@@ -14060,22 +14446,22 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A2:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22.5703125" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
-    <col min="3" max="4" width="11.42578125" customWidth="1"/>
+    <col min="1" max="1" width="22.54296875" customWidth="1"/>
+    <col min="2" max="2" width="12.7265625" customWidth="1"/>
+    <col min="3" max="4" width="11.453125" customWidth="1"/>
     <col min="7" max="7" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="21" t="s">
         <v>345</v>
       </c>
@@ -14086,7 +14472,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -14101,7 +14487,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>30</v>
       </c>
@@ -14117,7 +14503,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>32</v>
       </c>
@@ -14133,7 +14519,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>31</v>
       </c>
@@ -14149,7 +14535,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>320</v>
       </c>
@@ -14165,7 +14551,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>323</v>
       </c>
@@ -14181,7 +14567,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B9" s="124">
         <f>SUM(B3:B8)</f>
         <v>96</v>
@@ -14194,74 +14580,74 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="109.42578125" customWidth="1"/>
+    <col min="1" max="1" width="109.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" s="80" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" s="80" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" s="80"/>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" s="80" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" s="80" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="80" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" s="80" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A8" s="81" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" s="80"/>
     </row>
-    <row r="10" spans="1:1" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" ht="58" x14ac:dyDescent="0.35">
       <c r="A10" s="81" t="s">
         <v>302</v>
       </c>

</xml_diff>